<commit_message>
excel change for conversion date tc
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9257EFF-0526-48D0-89ED-4E7509AB63C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FieldSet" sheetId="1" r:id="rId1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="267">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -832,12 +831,18 @@
   </si>
   <si>
     <t>Deal3</t>
+  </si>
+  <si>
+    <t>CDINS3</t>
+  </si>
+  <si>
+    <t>Apex Corp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -992,7 +997,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1269,7 +1274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1367,7 +1372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1428,7 +1433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1485,7 +1490,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1615,7 +1620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1720,7 +1725,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2294,11 +2299,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3436,7 +3441,18 @@
         <v>81</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1003" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3456,7 +3472,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4606,7 +4622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4713,10 +4729,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -5839,7 +5855,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5909,7 +5925,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5958,7 +5974,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
excel for change in Module 2
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ABA63A-A614-45A2-8E0B-636D51B8D921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="FieldSet" sheetId="1" r:id="rId1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="307">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -844,12 +843,126 @@
   </si>
   <si>
     <t>ME1</t>
+  </si>
+  <si>
+    <t>HSRPIP1</t>
+  </si>
+  <si>
+    <t>TCS-Pipeline</t>
+  </si>
+  <si>
+    <t>Patel Sons</t>
+  </si>
+  <si>
+    <t>Samantha Rao</t>
+  </si>
+  <si>
+    <t>Ajio Trand</t>
+  </si>
+  <si>
+    <t>HSRPIP2</t>
+  </si>
+  <si>
+    <t>Reliance Trade</t>
+  </si>
+  <si>
+    <t>HSRPIP3</t>
+  </si>
+  <si>
+    <t>IriesIndia- pipeline</t>
+  </si>
+  <si>
+    <t>LOI</t>
+  </si>
+  <si>
+    <t>Iries India</t>
+  </si>
+  <si>
+    <t>HSRPIP4</t>
+  </si>
+  <si>
+    <t>NIIT-Pipeline</t>
+  </si>
+  <si>
+    <t>NDA Signed</t>
+  </si>
+  <si>
+    <t>Jinu Alex</t>
+  </si>
+  <si>
+    <t>HSRPIP5</t>
+  </si>
+  <si>
+    <t>Patel Property Deal</t>
+  </si>
+  <si>
+    <t>Anuradha Jaiswal</t>
+  </si>
+  <si>
+    <t>Sharda Firms</t>
+  </si>
+  <si>
+    <t>HSRCON1</t>
+  </si>
+  <si>
+    <t>Samantha</t>
+  </si>
+  <si>
+    <t>Rao</t>
+  </si>
+  <si>
+    <t>navatariptesting+33853@gmail.com</t>
+  </si>
+  <si>
+    <t>HSRCON2</t>
+  </si>
+  <si>
+    <t>Jinu</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>navatariptesting+13818@gmail.com</t>
+  </si>
+  <si>
+    <t>HSRCON3</t>
+  </si>
+  <si>
+    <t>Anuradha</t>
+  </si>
+  <si>
+    <t>Jaiswal</t>
+  </si>
+  <si>
+    <t>Kanya Groups</t>
+  </si>
+  <si>
+    <t>navatariptesting+78464@gmail.com</t>
+  </si>
+  <si>
+    <t>HSRINS1</t>
+  </si>
+  <si>
+    <t>Intermediary</t>
+  </si>
+  <si>
+    <t>HSRINS2</t>
+  </si>
+  <si>
+    <t>HSRINS3</t>
+  </si>
+  <si>
+    <t>HSRINS4</t>
+  </si>
+  <si>
+    <t>HSRINS5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -997,7 +1110,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1274,10 +1387,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1372,10 +1485,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" activeCellId="1" sqref="E3 E18"/>
     </sheetView>
   </sheetViews>
@@ -1447,7 +1560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1504,7 +1617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1634,7 +1747,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1739,7 +1852,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2313,11 +2426,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:ALO17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALO23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3480,17 +3593,72 @@
         <v>35</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>304</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>305</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>306</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>302</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:ALR8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALR12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4630,13 +4798,64 @@
         <v>124</v>
       </c>
     </row>
+    <row r="10" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>292</v>
+      </c>
+      <c r="B11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C11" t="s">
+        <v>294</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" t="s">
+        <v>297</v>
+      </c>
+      <c r="C12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D12" t="s">
+        <v>299</v>
+      </c>
+      <c r="E12" t="s">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4743,11 +4962,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AML7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AML14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5862,6 +6081,106 @@
         <v>32</v>
       </c>
     </row>
+    <row r="10" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C10" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>272</v>
+      </c>
+      <c r="F10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" t="s">
+        <v>278</v>
+      </c>
+      <c r="E12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" t="s">
+        <v>281</v>
+      </c>
+      <c r="C13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" t="s">
+        <v>282</v>
+      </c>
+      <c r="E13" t="s">
+        <v>283</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>284</v>
+      </c>
+      <c r="B14" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" t="s">
+        <v>278</v>
+      </c>
+      <c r="E14" t="s">
+        <v>286</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>287</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5869,7 +6188,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5939,7 +6258,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5988,7 +6307,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
excel change for Module 3
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="Commitments" sheetId="9" r:id="rId13"/>
     <sheet name="Task" sheetId="12" r:id="rId14"/>
     <sheet name="UploadImageData" sheetId="17" r:id="rId15"/>
+    <sheet name="Fields" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="387">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1079,6 +1080,126 @@
   </si>
   <si>
     <t>Non-Disclosure Agreement</t>
+  </si>
+  <si>
+    <t>Parent_Field_Name</t>
+  </si>
+  <si>
+    <t>accountId</t>
+  </si>
+  <si>
+    <t>M4SDG1</t>
+  </si>
+  <si>
+    <t>M4SDG2</t>
+  </si>
+  <si>
+    <t>Deal Team</t>
+  </si>
+  <si>
+    <t>Deal_Team__c</t>
+  </si>
+  <si>
+    <t>Pipeline__c</t>
+  </si>
+  <si>
+    <t>APIName</t>
+  </si>
+  <si>
+    <t>Override_Label</t>
+  </si>
+  <si>
+    <t>FieldOrder</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>navpeII__Contact_Referral_Source__c</t>
+  </si>
+  <si>
+    <t>Contact Referral Source</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Attendee_Staff__r.Name</t>
+  </si>
+  <si>
+    <t>Attendee_Staff__r.Title</t>
+  </si>
+  <si>
+    <t>Status__c</t>
+  </si>
+  <si>
+    <t>Notes__c</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>CField1</t>
+  </si>
+  <si>
+    <t>CField2</t>
+  </si>
+  <si>
+    <t>CField3</t>
+  </si>
+  <si>
+    <t>CField4</t>
+  </si>
+  <si>
+    <t>CField5</t>
+  </si>
+  <si>
+    <t>DTField1</t>
+  </si>
+  <si>
+    <t>DTField2</t>
+  </si>
+  <si>
+    <t>AFIeld1</t>
+  </si>
+  <si>
+    <t>AField2</t>
+  </si>
+  <si>
+    <t>AField3</t>
+  </si>
+  <si>
+    <t>AField4</t>
+  </si>
+  <si>
+    <t>DTField3</t>
+  </si>
+  <si>
+    <t>DTField4</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>M4SDG3</t>
+  </si>
+  <si>
+    <t>Attendee</t>
+  </si>
+  <si>
+    <t>Attendee__c</t>
+  </si>
+  <si>
+    <t>Marketing_Event__c</t>
   </si>
 </sst>
 </file>
@@ -1987,9 +2108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2223,6 +2342,230 @@
       </c>
       <c r="I4" t="s">
         <v>337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B6" t="s">
+        <v>361</v>
+      </c>
+      <c r="C6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>380</v>
+      </c>
+      <c r="B9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C9" t="s">
+        <v>360</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>381</v>
+      </c>
+      <c r="B10" t="s">
+        <v>382</v>
+      </c>
+      <c r="C10" t="s">
+        <v>382</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>376</v>
+      </c>
+      <c r="B11" t="s">
+        <v>364</v>
+      </c>
+      <c r="C11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>377</v>
+      </c>
+      <c r="B12" t="s">
+        <v>365</v>
+      </c>
+      <c r="C12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>378</v>
+      </c>
+      <c r="B13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>379</v>
+      </c>
+      <c r="B14" t="s">
+        <v>367</v>
+      </c>
+      <c r="C14" t="s">
+        <v>368</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5446,7 +5789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -6740,10 +7083,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6754,7 +7097,7 @@
     <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -6767,8 +7110,11 @@
       <c r="D1" s="25" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="25" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>158</v>
       </c>
@@ -6780,6 +7126,57 @@
       </c>
       <c r="D2" s="5" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel change for Module 4
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -28,6 +28,8 @@
     <sheet name="Task" sheetId="12" r:id="rId14"/>
     <sheet name="UploadImageData" sheetId="17" r:id="rId15"/>
     <sheet name="Fields" sheetId="19" r:id="rId16"/>
+    <sheet name="Attendees" sheetId="20" r:id="rId17"/>
+    <sheet name="Deal Team" sheetId="21" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="469">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1127,9 +1129,6 @@
     <t>navpeII__Contact_Referral_Source__c</t>
   </si>
   <si>
-    <t>Contact Referral Source</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -1266,6 +1265,189 @@
   </si>
   <si>
     <t>Module3Tc031_RemoveQuickCreateObjectFieldAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M4CON1</t>
+  </si>
+  <si>
+    <t>Test Navatar</t>
+  </si>
+  <si>
+    <t>Test Entity1</t>
+  </si>
+  <si>
+    <t>navatariptesting+77479@gmail.com</t>
+  </si>
+  <si>
+    <t>Investor</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>M4CON2</t>
+  </si>
+  <si>
+    <t>navatariptesting+14649@gmail.com</t>
+  </si>
+  <si>
+    <t>Advisor</t>
+  </si>
+  <si>
+    <t>M4CON3</t>
+  </si>
+  <si>
+    <t>navatariptesting+57115@gmail.com</t>
+  </si>
+  <si>
+    <t>M4CON4</t>
+  </si>
+  <si>
+    <t>navatariptesting+18612@gmail.com</t>
+  </si>
+  <si>
+    <t>M4CON5</t>
+  </si>
+  <si>
+    <t>Contact5</t>
+  </si>
+  <si>
+    <t>M4CON6</t>
+  </si>
+  <si>
+    <t>Contact6</t>
+  </si>
+  <si>
+    <t>M4CON7</t>
+  </si>
+  <si>
+    <t>Contact7</t>
+  </si>
+  <si>
+    <t>M4Deal1</t>
+  </si>
+  <si>
+    <t>Deal 1</t>
+  </si>
+  <si>
+    <t>LastModifiedBy.Name</t>
+  </si>
+  <si>
+    <t>LastModifiedBy.Email</t>
+  </si>
+  <si>
+    <t>LastModifiedBy.UserRoleId</t>
+  </si>
+  <si>
+    <t>LastModifiedBy.UserRole.Nam</t>
+  </si>
+  <si>
+    <t>Attendee_Staff</t>
+  </si>
+  <si>
+    <t>M4Att1</t>
+  </si>
+  <si>
+    <t>PE Admin</t>
+  </si>
+  <si>
+    <t>Invited</t>
+  </si>
+  <si>
+    <t>Event 1</t>
+  </si>
+  <si>
+    <t>Salesforce.com, inc. is an American cloud-based software company headquartered in San Francisco, California. It provides (CRM) customer relationship management service and also sells a complementary suite of enterprise applications focused on customer service, marketing automation, analytics, and application development.</t>
+  </si>
+  <si>
+    <t>M4Att2</t>
+  </si>
+  <si>
+    <t>M4Att3</t>
+  </si>
+  <si>
+    <t>M4Att4</t>
+  </si>
+  <si>
+    <t>M4Att5</t>
+  </si>
+  <si>
+    <t>M4Att6</t>
+  </si>
+  <si>
+    <t>DTID</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>M4DT1</t>
+  </si>
+  <si>
+    <t>DT-0017</t>
+  </si>
+  <si>
+    <t>Our Advisor</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>M4DT2</t>
+  </si>
+  <si>
+    <t>DT-0018</t>
+  </si>
+  <si>
+    <t>Company Team</t>
+  </si>
+  <si>
+    <t>M4DT3</t>
+  </si>
+  <si>
+    <t>Company Advisor</t>
+  </si>
+  <si>
+    <t>M4DT4</t>
+  </si>
+  <si>
+    <t>M4DT5</t>
+  </si>
+  <si>
+    <t>M4DT6</t>
+  </si>
+  <si>
+    <t>M4DT7</t>
+  </si>
+  <si>
+    <t>M4DT8</t>
+  </si>
+  <si>
+    <t>M4DT9</t>
+  </si>
+  <si>
+    <t>M4DT10</t>
+  </si>
+  <si>
+    <t>M4DT11</t>
+  </si>
+  <si>
+    <t>M4ME1</t>
+  </si>
+  <si>
+    <t>M4INS1</t>
+  </si>
+  <si>
+    <t>M4INS2</t>
+  </si>
+  <si>
+    <t>Test Entity4</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1457,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1325,6 +1507,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF080707"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1371,7 +1559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1423,6 +1611,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1706,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1742,13 +1931,13 @@
         <v>338</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>388</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>389</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>14</v>
@@ -1816,103 +2005,103 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B8" t="s">
         <v>324</v>
       </c>
       <c r="G8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="B9" t="s">
         <v>392</v>
       </c>
-      <c r="B9" t="s">
+      <c r="H9" t="s">
         <v>393</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>394</v>
-      </c>
-      <c r="I9" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="B10" t="s">
         <v>396</v>
       </c>
-      <c r="B10" t="s">
+      <c r="G10" t="s">
         <v>397</v>
-      </c>
-      <c r="G10" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>398</v>
+      </c>
+      <c r="B11" t="s">
         <v>399</v>
       </c>
-      <c r="B11" t="s">
+      <c r="J11" t="s">
         <v>400</v>
-      </c>
-      <c r="J11" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="B12" t="s">
+        <v>399</v>
+      </c>
+      <c r="J12" t="s">
         <v>402</v>
-      </c>
-      <c r="B12" t="s">
-        <v>400</v>
-      </c>
-      <c r="J12" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -2027,10 +2216,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,6 +2281,20 @@
       </c>
       <c r="E3" s="5" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>465</v>
+      </c>
+      <c r="B4" t="s">
+        <v>438</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" t="s">
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -2537,7 +2740,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2571,184 +2774,475 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B2" t="s">
         <v>358</v>
       </c>
-      <c r="C2" t="s">
-        <v>358</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B3" t="s">
         <v>359</v>
       </c>
-      <c r="C3" t="s">
-        <v>359</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B4" t="s">
         <v>360</v>
       </c>
-      <c r="C4" t="s">
-        <v>360</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B6" t="s">
         <v>361</v>
       </c>
-      <c r="C6" t="s">
-        <v>362</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B7" t="s">
-        <v>363</v>
-      </c>
-      <c r="C7" t="s">
-        <v>363</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B8" t="s">
-        <v>358</v>
-      </c>
-      <c r="C8" t="s">
-        <v>358</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B9" t="s">
-        <v>360</v>
-      </c>
-      <c r="C9" t="s">
-        <v>360</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
+        <v>431</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>381</v>
-      </c>
-      <c r="B10" t="s">
-        <v>382</v>
-      </c>
-      <c r="C10" t="s">
-        <v>382</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
+        <v>380</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B11" t="s">
-        <v>364</v>
-      </c>
-      <c r="C11" t="s">
-        <v>358</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B12" t="s">
-        <v>365</v>
-      </c>
-      <c r="C12" t="s">
-        <v>359</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B14" t="s">
+        <v>366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="C14" t="s">
-        <v>368</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>435</v>
+      </c>
+      <c r="B2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>440</v>
+      </c>
+      <c r="B3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C3" t="s">
+        <v>437</v>
+      </c>
+      <c r="D3" t="s">
+        <v>438</v>
+      </c>
+      <c r="E3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B4" t="s">
+        <v>436</v>
+      </c>
+      <c r="C4" t="s">
+        <v>437</v>
+      </c>
+      <c r="D4" t="s">
+        <v>438</v>
+      </c>
+      <c r="E4" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C5" t="s">
+        <v>437</v>
+      </c>
+      <c r="D5" t="s">
+        <v>438</v>
+      </c>
+      <c r="E5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>443</v>
+      </c>
+      <c r="B6" t="s">
+        <v>436</v>
+      </c>
+      <c r="C6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D6" t="s">
+        <v>438</v>
+      </c>
+      <c r="E6" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>444</v>
+      </c>
+      <c r="B7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C7" t="s">
+        <v>437</v>
+      </c>
+      <c r="D7" t="s">
+        <v>438</v>
+      </c>
+      <c r="E7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>448</v>
+      </c>
+      <c r="B2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E2" t="s">
+        <v>450</v>
+      </c>
+      <c r="F2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B3" t="s">
+        <v>453</v>
+      </c>
+      <c r="C3" t="s">
+        <v>429</v>
+      </c>
+      <c r="D3" t="s">
+        <v>436</v>
+      </c>
+      <c r="E3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>455</v>
+      </c>
+      <c r="C4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D4" t="s">
+        <v>436</v>
+      </c>
+      <c r="E4" t="s">
+        <v>456</v>
+      </c>
+      <c r="F4" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>457</v>
+      </c>
+      <c r="C5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E5" t="s">
+        <v>450</v>
+      </c>
+      <c r="F5" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>458</v>
+      </c>
+      <c r="C6" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6" t="s">
+        <v>436</v>
+      </c>
+      <c r="E6" t="s">
+        <v>454</v>
+      </c>
+      <c r="F6" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>459</v>
+      </c>
+      <c r="C7" t="s">
+        <v>429</v>
+      </c>
+      <c r="D7" t="s">
+        <v>436</v>
+      </c>
+      <c r="E7" t="s">
+        <v>456</v>
+      </c>
+      <c r="F7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>460</v>
+      </c>
+      <c r="C8" t="s">
+        <v>429</v>
+      </c>
+      <c r="D8" t="s">
+        <v>436</v>
+      </c>
+      <c r="E8" t="s">
+        <v>450</v>
+      </c>
+      <c r="F8" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>461</v>
+      </c>
+      <c r="C9" t="s">
+        <v>429</v>
+      </c>
+      <c r="D9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E9" t="s">
+        <v>454</v>
+      </c>
+      <c r="F9" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>462</v>
+      </c>
+      <c r="C10" t="s">
+        <v>429</v>
+      </c>
+      <c r="D10" t="s">
+        <v>436</v>
+      </c>
+      <c r="E10" t="s">
+        <v>456</v>
+      </c>
+      <c r="F10" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>463</v>
+      </c>
+      <c r="C11" t="s">
+        <v>429</v>
+      </c>
+      <c r="D11" t="s">
+        <v>436</v>
+      </c>
+      <c r="E11" t="s">
+        <v>450</v>
+      </c>
+      <c r="F11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>464</v>
+      </c>
+      <c r="C12" t="s">
+        <v>429</v>
+      </c>
+      <c r="D12" t="s">
+        <v>436</v>
+      </c>
+      <c r="E12" t="s">
+        <v>454</v>
+      </c>
+      <c r="F12" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -3430,10 +3924,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALO23"/>
+  <dimension ref="A1:ALO26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4651,6 +5145,28 @@
         <v>301</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>466</v>
+      </c>
+      <c r="B25" t="s">
+        <v>410</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>467</v>
+      </c>
+      <c r="B26" t="s">
+        <v>468</v>
+      </c>
+      <c r="C26" t="s">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4658,10 +5174,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALR12"/>
+  <dimension ref="A1:ALR20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5852,6 +6368,200 @@
         <v>299</v>
       </c>
     </row>
+    <row r="14" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>408</v>
+      </c>
+      <c r="B14" t="s">
+        <v>409</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
+        <v>410</v>
+      </c>
+      <c r="E14" t="s">
+        <v>411</v>
+      </c>
+      <c r="F14">
+        <v>8435985993</v>
+      </c>
+      <c r="H14" t="s">
+        <v>412</v>
+      </c>
+      <c r="I14" t="s">
+        <v>413</v>
+      </c>
+      <c r="J14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>415</v>
+      </c>
+      <c r="B15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" t="s">
+        <v>410</v>
+      </c>
+      <c r="E15" t="s">
+        <v>416</v>
+      </c>
+      <c r="F15">
+        <v>8435985993</v>
+      </c>
+      <c r="H15" t="s">
+        <v>417</v>
+      </c>
+      <c r="I15" t="s">
+        <v>413</v>
+      </c>
+      <c r="J15" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>418</v>
+      </c>
+      <c r="B16" t="s">
+        <v>409</v>
+      </c>
+      <c r="C16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" t="s">
+        <v>410</v>
+      </c>
+      <c r="E16" t="s">
+        <v>419</v>
+      </c>
+      <c r="F16">
+        <v>8435985993</v>
+      </c>
+      <c r="H16" t="s">
+        <v>412</v>
+      </c>
+      <c r="I16" t="s">
+        <v>413</v>
+      </c>
+      <c r="J16" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>420</v>
+      </c>
+      <c r="B17" t="s">
+        <v>409</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" t="s">
+        <v>410</v>
+      </c>
+      <c r="E17" t="s">
+        <v>421</v>
+      </c>
+      <c r="F17">
+        <v>8435985993</v>
+      </c>
+      <c r="H17" t="s">
+        <v>417</v>
+      </c>
+      <c r="I17" t="s">
+        <v>413</v>
+      </c>
+      <c r="J17" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>422</v>
+      </c>
+      <c r="B18" t="s">
+        <v>409</v>
+      </c>
+      <c r="C18" t="s">
+        <v>423</v>
+      </c>
+      <c r="D18" t="s">
+        <v>410</v>
+      </c>
+      <c r="F18">
+        <v>8435985993</v>
+      </c>
+      <c r="H18" t="s">
+        <v>412</v>
+      </c>
+      <c r="I18" t="s">
+        <v>413</v>
+      </c>
+      <c r="J18" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>424</v>
+      </c>
+      <c r="B19" t="s">
+        <v>409</v>
+      </c>
+      <c r="C19" t="s">
+        <v>425</v>
+      </c>
+      <c r="D19" t="s">
+        <v>410</v>
+      </c>
+      <c r="F19">
+        <v>8435985993</v>
+      </c>
+      <c r="H19" t="s">
+        <v>417</v>
+      </c>
+      <c r="I19" t="s">
+        <v>413</v>
+      </c>
+      <c r="J19" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>426</v>
+      </c>
+      <c r="B20" t="s">
+        <v>409</v>
+      </c>
+      <c r="C20" t="s">
+        <v>427</v>
+      </c>
+      <c r="D20" t="s">
+        <v>410</v>
+      </c>
+      <c r="F20">
+        <v>8435985993</v>
+      </c>
+      <c r="H20" t="s">
+        <v>412</v>
+      </c>
+      <c r="I20" t="s">
+        <v>413</v>
+      </c>
+      <c r="J20" t="s">
+        <v>414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5970,10 +6680,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML14"/>
+  <dimension ref="A1:AML16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7188,6 +7898,20 @@
         <v>286</v>
       </c>
     </row>
+    <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>428</v>
+      </c>
+      <c r="B16" t="s">
+        <v>429</v>
+      </c>
+      <c r="C16" t="s">
+        <v>410</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7347,19 +8071,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>385</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel for Module 3 tc031-tc043
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="480">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1448,6 +1448,39 @@
   </si>
   <si>
     <t>Test Entity4</t>
+  </si>
+  <si>
+    <t>Action_Object</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Module3Tc032_RemoveListViewObjectAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Module3Tc033_RemoveListViewNameAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Module3Tc034_CreateRecordTypeFundAndFundOfFundsForFundObjectAndAddTheFromTheProfiles</t>
+  </si>
+  <si>
+    <t>New Fund</t>
+  </si>
+  <si>
+    <t>navpeII__Fund__c</t>
+  </si>
+  <si>
+    <t>Fund&lt;break&gt;Fund of Funds</t>
+  </si>
+  <si>
+    <t>Module3Tc035_VerifyQuickCreateObjectWhenRecordHasMultipleRecordTypes</t>
+  </si>
+  <si>
+    <t>Module3Tc036_1_UpdateTheRecordTypeAndDescriptionImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Module3Tc036_2_UpdateTheRecordTypeAndDescriptionImpactOnNavigationMenu</t>
   </si>
 </sst>
 </file>
@@ -1893,10 +1926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,9 +1942,10 @@
     <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="66" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>318</v>
       </c>
@@ -1942,8 +1976,11 @@
       <c r="J1" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>323</v>
       </c>
@@ -1954,7 +1991,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>326</v>
       </c>
@@ -1965,7 +2002,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>329</v>
       </c>
@@ -1976,7 +2013,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>339</v>
       </c>
@@ -1984,7 +2021,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>341</v>
       </c>
@@ -1995,7 +2032,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>344</v>
       </c>
@@ -2003,7 +2040,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>389</v>
       </c>
@@ -2014,7 +2051,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>391</v>
       </c>
@@ -2028,7 +2065,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>395</v>
       </c>
@@ -2039,7 +2076,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>398</v>
       </c>
@@ -2050,7 +2087,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>401</v>
       </c>
@@ -2061,7 +2098,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>403</v>
       </c>
@@ -2069,7 +2106,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>404</v>
       </c>
@@ -2077,18 +2114,21 @@
         <v>399</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>405</v>
       </c>
       <c r="B15" t="s">
         <v>399</v>
       </c>
+      <c r="H15" t="s">
+        <v>470</v>
+      </c>
       <c r="I15" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>406</v>
       </c>
@@ -2096,12 +2136,78 @@
         <v>399</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>407</v>
       </c>
       <c r="B17" t="s">
         <v>399</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="B18" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="B19" t="s">
+        <v>399</v>
+      </c>
+      <c r="H19" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="B20" t="s">
+        <v>474</v>
+      </c>
+      <c r="H20" t="s">
+        <v>475</v>
+      </c>
+      <c r="I20" t="s">
+        <v>394</v>
+      </c>
+      <c r="J20" t="s">
+        <v>476</v>
+      </c>
+      <c r="K20" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="B21" t="s">
+        <v>474</v>
+      </c>
+      <c r="K21" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>478</v>
+      </c>
+      <c r="B22" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="B23" t="s">
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -5176,7 +5282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
excel update for Module4
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView activeTab="15" firstSheet="11" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="FilePath" sheetId="18" r:id="rId1"/>
-    <sheet name="FieldSet" sheetId="1" r:id="rId2"/>
-    <sheet name="FieldComponent" sheetId="6" r:id="rId3"/>
-    <sheet name="Entities" sheetId="3" r:id="rId4"/>
-    <sheet name="Contacts" sheetId="2" r:id="rId5"/>
-    <sheet name="Fund" sheetId="7" r:id="rId6"/>
-    <sheet name="Deal" sheetId="4" r:id="rId7"/>
-    <sheet name="DealRequestTracker" sheetId="14" r:id="rId8"/>
-    <sheet name="CustomSDG" sheetId="13" r:id="rId9"/>
-    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId10"/>
-    <sheet name="MarketingEvent" sheetId="15" r:id="rId11"/>
-    <sheet name="Partnerships" sheetId="8" r:id="rId12"/>
-    <sheet name="Commitments" sheetId="9" r:id="rId13"/>
-    <sheet name="Task" sheetId="12" r:id="rId14"/>
-    <sheet name="UploadImageData" sheetId="17" r:id="rId15"/>
-    <sheet name="Fields" sheetId="19" r:id="rId16"/>
-    <sheet name="Attendees" sheetId="20" r:id="rId17"/>
-    <sheet name="Deal Team" sheetId="21" r:id="rId18"/>
+    <sheet name="FilePath" r:id="rId1" sheetId="18"/>
+    <sheet name="FieldSet" r:id="rId2" sheetId="1"/>
+    <sheet name="FieldComponent" r:id="rId3" sheetId="6"/>
+    <sheet name="Entities" r:id="rId4" sheetId="3"/>
+    <sheet name="Contacts" r:id="rId5" sheetId="2"/>
+    <sheet name="Fund" r:id="rId6" sheetId="7"/>
+    <sheet name="Deal" r:id="rId7" sheetId="4"/>
+    <sheet name="DealRequestTracker" r:id="rId8" sheetId="14"/>
+    <sheet name="CustomSDG" r:id="rId9" sheetId="13"/>
+    <sheet name="ToggleButtonCheck" r:id="rId10" sheetId="16"/>
+    <sheet name="MarketingEvent" r:id="rId11" sheetId="15"/>
+    <sheet name="Partnerships" r:id="rId12" sheetId="8"/>
+    <sheet name="Commitments" r:id="rId13" sheetId="9"/>
+    <sheet name="Task" r:id="rId14" sheetId="12"/>
+    <sheet name="UploadImageData" r:id="rId15" sheetId="17"/>
+    <sheet name="Fields" r:id="rId16" sheetId="19"/>
+    <sheet name="Attendees" r:id="rId17" sheetId="20"/>
+    <sheet name="Deal Team" r:id="rId18" sheetId="21"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="500">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1270,9 +1270,6 @@
     <t>M4CON1</t>
   </si>
   <si>
-    <t>Test Navatar</t>
-  </si>
-  <si>
     <t>Test Entity1</t>
   </si>
   <si>
@@ -1333,9 +1330,6 @@
     <t>Deal 1</t>
   </si>
   <si>
-    <t>LastModifiedBy.Name</t>
-  </si>
-  <si>
     <t>LastModifiedBy.Email</t>
   </si>
   <si>
@@ -1481,6 +1475,72 @@
   </si>
   <si>
     <t>Module3Tc036_2_UpdateTheRecordTypeAndDescriptionImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M4Field1</t>
+  </si>
+  <si>
+    <t>Test@%^$%^%^&amp;%^^%^&amp;^%^&amp;%^dhgf</t>
+  </si>
+  <si>
+    <t>Test_dhgf__c</t>
+  </si>
+  <si>
+    <t>Test N1</t>
+  </si>
+  <si>
+    <t>Test Na2</t>
+  </si>
+  <si>
+    <t>Test Nav3</t>
+  </si>
+  <si>
+    <t>Test Nava4</t>
+  </si>
+  <si>
+    <t>Test Navat5</t>
+  </si>
+  <si>
+    <t>Test Navata6</t>
+  </si>
+  <si>
+    <t>Test Navatar7</t>
+  </si>
+  <si>
+    <t>LastModifiedBy.UserRole.Name</t>
+  </si>
+  <si>
+    <t>DT-0019</t>
+  </si>
+  <si>
+    <t>DT-0020</t>
+  </si>
+  <si>
+    <t>DT-0021</t>
+  </si>
+  <si>
+    <t>DT-0022</t>
+  </si>
+  <si>
+    <t>DT-0023</t>
+  </si>
+  <si>
+    <t>DT-0024</t>
+  </si>
+  <si>
+    <t>DT-0025</t>
+  </si>
+  <si>
+    <t>DT-0026</t>
+  </si>
+  <si>
+    <t>DT-0027</t>
+  </si>
+  <si>
+    <t>DT-0028</t>
+  </si>
+  <si>
+    <t>DT-0029</t>
   </si>
 </sst>
 </file>
@@ -1589,69 +1649,69 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="14" quotePrefix="1" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1668,10 +1728,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1706,7 +1766,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1741,7 +1801,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1835,21 +1895,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1866,7 +1926,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1918,31 +1978,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="66" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="89.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="81.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="66.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1977,7 +2037,7 @@
         <v>14</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2122,7 +2182,7 @@
         <v>399</v>
       </c>
       <c r="H15" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I15" t="s">
         <v>394</v>
@@ -2146,7 +2206,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B18" t="s">
         <v>399</v>
@@ -2154,71 +2214,71 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B19" t="s">
         <v>399</v>
       </c>
       <c r="H19" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="B20" t="s">
+        <v>472</v>
+      </c>
+      <c r="H20" t="s">
         <v>473</v>
-      </c>
-      <c r="B20" t="s">
-        <v>474</v>
-      </c>
-      <c r="H20" t="s">
-        <v>475</v>
       </c>
       <c r="I20" t="s">
         <v>394</v>
       </c>
       <c r="J20" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="K20" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B21" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="K21" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B22" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B23" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -2226,13 +2286,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="22.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="32.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="127.5703125" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2316,13 +2376,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -2330,12 +2390,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="21.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="11.0" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2391,27 +2451,27 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>177</v>
       </c>
       <c r="E4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -2419,13 +2479,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2462,13 +2522,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
@@ -2476,26 +2536,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="1" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -2592,20 +2652,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2695,13 +2755,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -2709,18 +2769,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2837,25 +2897,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2931,7 +2991,7 @@
         <v>374</v>
       </c>
       <c r="B8" t="s">
-        <v>430</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2939,7 +2999,7 @@
         <v>379</v>
       </c>
       <c r="B9" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2947,10 +3007,10 @@
         <v>380</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2986,20 +3046,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3007,7 +3067,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>98</v>
@@ -3021,121 +3081,121 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C2" t="s">
         <v>435</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>436</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>437</v>
-      </c>
-      <c r="D2" t="s">
-        <v>438</v>
-      </c>
-      <c r="E2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C3" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3" t="s">
         <v>436</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>437</v>
-      </c>
-      <c r="D3" t="s">
-        <v>438</v>
-      </c>
-      <c r="E3" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D4" t="s">
         <v>436</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>437</v>
-      </c>
-      <c r="D4" t="s">
-        <v>438</v>
-      </c>
-      <c r="E4" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B5" t="s">
+        <v>434</v>
+      </c>
+      <c r="C5" t="s">
+        <v>435</v>
+      </c>
+      <c r="D5" t="s">
         <v>436</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>437</v>
-      </c>
-      <c r="D5" t="s">
-        <v>438</v>
-      </c>
-      <c r="E5" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B6" t="s">
+        <v>434</v>
+      </c>
+      <c r="C6" t="s">
+        <v>435</v>
+      </c>
+      <c r="D6" t="s">
         <v>436</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>437</v>
-      </c>
-      <c r="D6" t="s">
-        <v>438</v>
-      </c>
-      <c r="E6" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C7" t="s">
+        <v>435</v>
+      </c>
+      <c r="D7" t="s">
         <v>436</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>437</v>
       </c>
-      <c r="D7" t="s">
-        <v>438</v>
-      </c>
-      <c r="E7" t="s">
-        <v>439</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3143,16 +3203,16 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>381</v>
@@ -3160,205 +3220,232 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E2" t="s">
         <v>448</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>449</v>
-      </c>
-      <c r="C2" t="s">
-        <v>429</v>
-      </c>
-      <c r="D2" t="s">
-        <v>436</v>
-      </c>
-      <c r="E2" t="s">
-        <v>450</v>
-      </c>
-      <c r="F2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D3" t="s">
+        <v>434</v>
+      </c>
+      <c r="E3" t="s">
         <v>452</v>
       </c>
-      <c r="B3" t="s">
-        <v>453</v>
-      </c>
-      <c r="C3" t="s">
-        <v>429</v>
-      </c>
-      <c r="D3" t="s">
-        <v>436</v>
-      </c>
-      <c r="E3" t="s">
-        <v>454</v>
-      </c>
       <c r="F3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>455</v>
+        <v>453</v>
+      </c>
+      <c r="B4" t="s">
+        <v>491</v>
       </c>
       <c r="C4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D4" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E4" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>457</v>
+        <v>455</v>
+      </c>
+      <c r="B5" t="s">
+        <v>492</v>
       </c>
       <c r="C5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>458</v>
+        <v>456</v>
+      </c>
+      <c r="B6" t="s">
+        <v>493</v>
       </c>
       <c r="C6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>459</v>
+        <v>457</v>
+      </c>
+      <c r="B7" t="s">
+        <v>494</v>
       </c>
       <c r="C7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D7" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>460</v>
+        <v>458</v>
+      </c>
+      <c r="B8" t="s">
+        <v>495</v>
       </c>
       <c r="C8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D8" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E8" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F8" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>461</v>
+        <v>459</v>
+      </c>
+      <c r="B9" t="s">
+        <v>496</v>
       </c>
       <c r="C9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E9" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F9" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>462</v>
+        <v>460</v>
+      </c>
+      <c r="B10" t="s">
+        <v>497</v>
       </c>
       <c r="C10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D10" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>463</v>
+        <v>461</v>
+      </c>
+      <c r="B11" t="s">
+        <v>498</v>
       </c>
       <c r="C11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D11" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F11" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>464</v>
+        <v>462</v>
+      </c>
+      <c r="B12" t="s">
+        <v>499</v>
       </c>
       <c r="C12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F12" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -3366,15 +3453,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -3394,7 +3481,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -3449,30 +3536,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -3491,8 +3578,11 @@
       <c r="F1" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -3512,7 +3602,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -3529,7 +3619,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>202</v>
       </c>
@@ -3546,7 +3636,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>204</v>
       </c>
@@ -3563,7 +3653,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>206</v>
       </c>
@@ -3580,7 +3670,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>208</v>
       </c>
@@ -3597,7 +3687,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>210</v>
       </c>
@@ -3614,7 +3704,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>212</v>
       </c>
@@ -3631,7 +3721,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -3648,7 +3738,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>216</v>
       </c>
@@ -3665,7 +3755,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>218</v>
       </c>
@@ -3682,7 +3772,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>230</v>
       </c>
@@ -3699,7 +3789,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>231</v>
       </c>
@@ -3716,7 +3806,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>232</v>
       </c>
@@ -3733,7 +3823,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -4022,15 +4112,35 @@
         <v>43</v>
       </c>
     </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>478</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>479</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" t="s">
+        <v>480</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALO26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALP26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
@@ -4038,10 +4148,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
@@ -5253,10 +5363,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B25" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
@@ -5264,36 +5374,36 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B26" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C26" t="s">
         <v>301</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALR20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALS20"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -6479,203 +6589,203 @@
         <v>408</v>
       </c>
       <c r="B14" t="s">
-        <v>409</v>
+        <v>481</v>
       </c>
       <c r="C14" t="s">
         <v>111</v>
       </c>
       <c r="D14" t="s">
+        <v>409</v>
+      </c>
+      <c r="E14" t="s">
         <v>410</v>
-      </c>
-      <c r="E14" t="s">
-        <v>411</v>
       </c>
       <c r="F14">
         <v>8435985993</v>
       </c>
       <c r="H14" t="s">
+        <v>411</v>
+      </c>
+      <c r="I14" t="s">
         <v>412</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>413</v>
-      </c>
-      <c r="J14" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B15" t="s">
-        <v>409</v>
+        <v>482</v>
       </c>
       <c r="C15" t="s">
         <v>114</v>
       </c>
       <c r="D15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F15">
         <v>8435985993</v>
       </c>
       <c r="H15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I15" t="s">
+        <v>412</v>
+      </c>
+      <c r="J15" t="s">
         <v>413</v>
-      </c>
-      <c r="J15" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="16" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B16" t="s">
-        <v>409</v>
+        <v>483</v>
       </c>
       <c r="C16" t="s">
         <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F16">
         <v>8435985993</v>
       </c>
       <c r="H16" t="s">
+        <v>411</v>
+      </c>
+      <c r="I16" t="s">
         <v>412</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>413</v>
-      </c>
-      <c r="J16" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B17" t="s">
-        <v>409</v>
+        <v>484</v>
       </c>
       <c r="C17" t="s">
         <v>121</v>
       </c>
       <c r="D17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E17" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F17">
         <v>8435985993</v>
       </c>
       <c r="H17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I17" t="s">
+        <v>412</v>
+      </c>
+      <c r="J17" t="s">
         <v>413</v>
-      </c>
-      <c r="J17" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>421</v>
+      </c>
+      <c r="B18" t="s">
+        <v>485</v>
+      </c>
+      <c r="C18" t="s">
         <v>422</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>409</v>
-      </c>
-      <c r="C18" t="s">
-        <v>423</v>
-      </c>
-      <c r="D18" t="s">
-        <v>410</v>
       </c>
       <c r="F18">
         <v>8435985993</v>
       </c>
       <c r="H18" t="s">
+        <v>411</v>
+      </c>
+      <c r="I18" t="s">
         <v>412</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>413</v>
-      </c>
-      <c r="J18" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>423</v>
+      </c>
+      <c r="B19" t="s">
+        <v>486</v>
+      </c>
+      <c r="C19" t="s">
         <v>424</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>409</v>
-      </c>
-      <c r="C19" t="s">
-        <v>425</v>
-      </c>
-      <c r="D19" t="s">
-        <v>410</v>
       </c>
       <c r="F19">
         <v>8435985993</v>
       </c>
       <c r="H19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I19" t="s">
+        <v>412</v>
+      </c>
+      <c r="J19" t="s">
         <v>413</v>
-      </c>
-      <c r="J19" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>425</v>
+      </c>
+      <c r="B20" t="s">
+        <v>487</v>
+      </c>
+      <c r="C20" t="s">
         <v>426</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>409</v>
-      </c>
-      <c r="C20" t="s">
-        <v>427</v>
-      </c>
-      <c r="D20" t="s">
-        <v>410</v>
       </c>
       <c r="F20">
         <v>8435985993</v>
       </c>
       <c r="H20" t="s">
+        <v>411</v>
+      </c>
+      <c r="I20" t="s">
         <v>412</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>413</v>
       </c>
-      <c r="J20" t="s">
-        <v>414</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
@@ -6683,18 +6793,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -6780,13 +6890,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMM16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -6794,15 +6904,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -8006,13 +8116,13 @@
     </row>
     <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>427</v>
+      </c>
+      <c r="B16" t="s">
         <v>428</v>
       </c>
-      <c r="B16" t="s">
-        <v>429</v>
-      </c>
       <c r="C16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -8020,13 +8130,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:E2"/>
@@ -8034,10 +8144,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="5" width="15.28515625" collapsed="true"/>
+    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8089,25 +8199,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" style="5" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="20.140625" collapsed="true"/>
+    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -8193,6 +8303,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="588">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1698,6 +1698,114 @@
   </si>
   <si>
     <t>/lightning/cmp/c__RedirectCmp?c__coverage=Region</t>
+  </si>
+  <si>
+    <t>M4ME2</t>
+  </si>
+  <si>
+    <t>Event 2</t>
+  </si>
+  <si>
+    <t>M4ME3</t>
+  </si>
+  <si>
+    <t>Event 3</t>
+  </si>
+  <si>
+    <t>M4ME4</t>
+  </si>
+  <si>
+    <t>Event 4</t>
+  </si>
+  <si>
+    <t>M4ME5</t>
+  </si>
+  <si>
+    <t>Event 5</t>
+  </si>
+  <si>
+    <t>M4ME6</t>
+  </si>
+  <si>
+    <t>Event 6</t>
+  </si>
+  <si>
+    <t>M4ME7</t>
+  </si>
+  <si>
+    <t>M4ME8</t>
+  </si>
+  <si>
+    <t>M4ME9</t>
+  </si>
+  <si>
+    <t>M4ME10</t>
+  </si>
+  <si>
+    <t>M4ME11</t>
+  </si>
+  <si>
+    <t>M4ME12</t>
+  </si>
+  <si>
+    <t>M4ME13</t>
+  </si>
+  <si>
+    <t>M4ME14</t>
+  </si>
+  <si>
+    <t>M4ME15</t>
+  </si>
+  <si>
+    <t>M4ME16</t>
+  </si>
+  <si>
+    <t>M4ME17</t>
+  </si>
+  <si>
+    <t>M4ME18</t>
+  </si>
+  <si>
+    <t>M4ME19</t>
+  </si>
+  <si>
+    <t>Event 7</t>
+  </si>
+  <si>
+    <t>Event 8</t>
+  </si>
+  <si>
+    <t>Event 9</t>
+  </si>
+  <si>
+    <t>Event 10</t>
+  </si>
+  <si>
+    <t>Event 11</t>
+  </si>
+  <si>
+    <t>Event 12</t>
+  </si>
+  <si>
+    <t>Event 13</t>
+  </si>
+  <si>
+    <t>Event 14</t>
+  </si>
+  <si>
+    <t>Event 15</t>
+  </si>
+  <si>
+    <t>Event 16</t>
+  </si>
+  <si>
+    <t>Event 17</t>
+  </si>
+  <si>
+    <t>Event 18</t>
+  </si>
+  <si>
+    <t>Event 19</t>
   </si>
 </sst>
 </file>
@@ -2145,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2661,10 +2769,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2739,6 +2847,258 @@
         <v>170</v>
       </c>
       <c r="E4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="B5" t="s">
+        <v>553</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="B6" t="s">
+        <v>555</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="B7" t="s">
+        <v>557</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="B8" t="s">
+        <v>559</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="B9" t="s">
+        <v>561</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E9" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="B10" t="s">
+        <v>575</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>563</v>
+      </c>
+      <c r="B11" t="s">
+        <v>576</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="B12" t="s">
+        <v>577</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="B13" t="s">
+        <v>578</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="B14" t="s">
+        <v>579</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>567</v>
+      </c>
+      <c r="B15" t="s">
+        <v>580</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="B16" t="s">
+        <v>581</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>569</v>
+      </c>
+      <c r="B17" t="s">
+        <v>582</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="B18" t="s">
+        <v>583</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="B19" t="s">
+        <v>584</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E19" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="B20" t="s">
+        <v>585</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="B21" t="s">
+        <v>586</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E21" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="B22" t="s">
+        <v>587</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E22" t="s">
         <v>402</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Excel for Module 3 TC081-095
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498335E4-C2C2-4A23-A27C-EB70D79F1143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -18,20 +17,21 @@
     <sheet name="FieldComponent" sheetId="6" r:id="rId3"/>
     <sheet name="Entities" sheetId="3" r:id="rId4"/>
     <sheet name="Contacts" sheetId="2" r:id="rId5"/>
-    <sheet name="Fund" sheetId="7" r:id="rId6"/>
-    <sheet name="Deal" sheetId="4" r:id="rId7"/>
-    <sheet name="DealRequestTracker" sheetId="14" r:id="rId8"/>
-    <sheet name="CustomSDG" sheetId="13" r:id="rId9"/>
-    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId10"/>
-    <sheet name="MarketingEvent" sheetId="15" r:id="rId11"/>
-    <sheet name="Partnerships" sheetId="8" r:id="rId12"/>
-    <sheet name="Commitments" sheetId="9" r:id="rId13"/>
-    <sheet name="Task" sheetId="12" r:id="rId14"/>
-    <sheet name="UploadImageData" sheetId="17" r:id="rId15"/>
-    <sheet name="Fields" sheetId="19" r:id="rId16"/>
-    <sheet name="Attendees" sheetId="20" r:id="rId17"/>
-    <sheet name="Deal Team" sheetId="21" r:id="rId18"/>
-    <sheet name="Coverages" sheetId="22" r:id="rId19"/>
+    <sheet name="Test Custom Object" sheetId="23" r:id="rId6"/>
+    <sheet name="Fund" sheetId="7" r:id="rId7"/>
+    <sheet name="Deal" sheetId="4" r:id="rId8"/>
+    <sheet name="DealRequestTracker" sheetId="14" r:id="rId9"/>
+    <sheet name="CustomSDG" sheetId="13" r:id="rId10"/>
+    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId11"/>
+    <sheet name="MarketingEvent" sheetId="15" r:id="rId12"/>
+    <sheet name="Partnerships" sheetId="8" r:id="rId13"/>
+    <sheet name="Commitments" sheetId="9" r:id="rId14"/>
+    <sheet name="Task" sheetId="12" r:id="rId15"/>
+    <sheet name="UploadImageData" sheetId="17" r:id="rId16"/>
+    <sheet name="Fields" sheetId="19" r:id="rId17"/>
+    <sheet name="Attendees" sheetId="20" r:id="rId18"/>
+    <sheet name="Deal Team" sheetId="21" r:id="rId19"/>
+    <sheet name="Coverages" sheetId="22" r:id="rId20"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="620">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1822,16 +1822,97 @@
   </si>
   <si>
     <t>Date&lt;breakOn&gt;Type&lt;breakOn&gt;Status&lt;breakOn&gt;Location&lt;breakOn&gt;Main Contact&lt;breakOn&gt;Region</t>
+  </si>
+  <si>
+    <t>Module3Tc081_CreateMultiTaggedLogACallAllNavigationMenuItem</t>
+  </si>
+  <si>
+    <t>Log a Call with Multiple Associations</t>
+  </si>
+  <si>
+    <t>create new</t>
+  </si>
+  <si>
+    <t>Module3Tc085_CreateCustomActionOfTypeTask</t>
+  </si>
+  <si>
+    <t>New Meeting</t>
+  </si>
+  <si>
+    <t>Module3Tc086_CreateNavigationRecordsRelatedToMultiTaggedActions</t>
+  </si>
+  <si>
+    <t>New Task with Multiple Associations</t>
+  </si>
+  <si>
+    <t>Module3Tc091_CreatePredefinendValuesInNavigationRecords</t>
+  </si>
+  <si>
+    <t>New Task with Multiple Associations&lt;break&gt;Log a Call with Multiple Associations&lt;break&gt;New Meeting</t>
+  </si>
+  <si>
+    <t>Module3Tc093_CreateTaskRecordTypesAndPageLayouts</t>
+  </si>
+  <si>
+    <t>Task Type1&lt;break&gt;Task Type2&lt;break&gt;Task Type3</t>
+  </si>
+  <si>
+    <t>Module3Tc094_EditNavigationRecordAndSetRecordTypesInEachRecord</t>
+  </si>
+  <si>
+    <t>Log a Call with Multiple Associations&lt;break&gt;New Task with Multiple Associations&lt;break&gt;New Meeting</t>
+  </si>
+  <si>
+    <t>Module3Tc095_VerifyActionsfromNavigationPageAfterAssigningRecordTypes</t>
+  </si>
+  <si>
+    <t>M3INS1</t>
+  </si>
+  <si>
+    <t>M3TestOmaxe Group</t>
+  </si>
+  <si>
+    <t>M3INS2</t>
+  </si>
+  <si>
+    <t>M3TestAIG Corp</t>
+  </si>
+  <si>
+    <t>M3CON1</t>
+  </si>
+  <si>
+    <t>M3TestAlex</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>navatariptesting+78601@gmail.com</t>
+  </si>
+  <si>
+    <t>M3FUND1</t>
+  </si>
+  <si>
+    <t>M3TestAxis Deal</t>
+  </si>
+  <si>
+    <t>M3TestCst Record1</t>
+  </si>
+  <si>
+    <t>M3CSTOBJ</t>
+  </si>
+  <si>
+    <t>Test_Custom_Object_Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1887,6 +1968,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1929,11 +2018,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1990,10 +2080,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2270,11 +2365,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2659,24 +2754,116 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="B33" t="s">
+        <v>594</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>595</v>
+      </c>
+      <c r="K33" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="B34" t="s">
+        <v>597</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>595</v>
+      </c>
+      <c r="K34" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>598</v>
+      </c>
+      <c r="B35" t="s">
+        <v>599</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>595</v>
+      </c>
+      <c r="K35" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="B36" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="J37" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="B38" t="s">
+        <v>605</v>
+      </c>
+      <c r="J38" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>606</v>
+      </c>
+      <c r="B39" t="s">
+        <v>605</v>
+      </c>
+      <c r="F39" t="s">
+        <v>595</v>
+      </c>
+      <c r="J39" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
         <v>518</v>
       </c>
-      <c r="L33" t="s">
+      <c r="L40" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>537</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M41" t="s">
         <v>538</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L30" r:id="rId1" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L33" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L30" r:id="rId1" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M"/>
+    <hyperlink ref="L40" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2684,7 +2871,110 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2787,8 +3077,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3128,8 +3418,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3185,8 +3475,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3315,8 +3605,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3418,8 +3708,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3560,8 +3850,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3709,8 +3999,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3898,8 +4188,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4155,8 +4445,106 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4252,106 +4640,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -4948,11 +5238,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:ALO31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALO34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6233,17 +6523,39 @@
         <v>292</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>607</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>608</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>609</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>610</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:ALR21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALR23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7645,17 +7957,77 @@
         <v>404</v>
       </c>
     </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>611</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>612</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>613</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>608</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>614</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E23" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>619</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I8"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7756,13 +8128,27 @@
         <v>93</v>
       </c>
     </row>
+    <row r="10" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>615</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>616</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9001,8 +9387,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9072,107 +9458,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>534</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>373</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
excel change after adding module wise
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar.LAP0051\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5525,7 +5525,7 @@
   <dimension ref="A1:ALO39"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:D34"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change tc name of Module 2, Module 3, Module 5
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="6195" firstSheet="2" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="6195"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -988,27 +988,18 @@
     <t>Updated_Order</t>
   </si>
   <si>
-    <t>Module3Tc009_1_UpdateReportsAndDashboardURLWithAnActualReporAndDashboardLink_Action</t>
-  </si>
-  <si>
     <t>Reports&lt;break&gt;Dashboards</t>
   </si>
   <si>
     <t>Account Referrals&lt;break&gt;Dead Deals</t>
   </si>
   <si>
-    <t>Module3Tc011_RenameNavigationLabelAndVerifyImpactOnNavigationMenu</t>
-  </si>
-  <si>
     <t>Fund&lt;break&gt;Contact</t>
   </si>
   <si>
     <t>New Fund&lt;break&gt;New Contact</t>
   </si>
   <si>
-    <t>Module3Tc012_ChangeTheOrderOfTheLabelAndVerifyImpactOnNavigationMenu</t>
-  </si>
-  <si>
     <t>New Contact&lt;break&gt;Reports&lt;break&gt;Fund Manager&lt;break&gt;Institution&lt;break&gt;Partnership</t>
   </si>
   <si>
@@ -1024,24 +1015,15 @@
     <t>Parent</t>
   </si>
   <si>
-    <t>Module3Tc015_1_AddNewNavigationItemsAndVerifyItOnNavigationMenu</t>
-  </si>
-  <si>
     <t>Dashboards</t>
   </si>
   <si>
-    <t>Module3Tc018_CreateSubMenuAndVerify</t>
-  </si>
-  <si>
     <t>Reports</t>
   </si>
   <si>
     <t>Accounts</t>
   </si>
   <si>
-    <t>Module3Tc019_CreateSubMenuForIIndlevelAndVerifyItOnTheNavigationMenu</t>
-  </si>
-  <si>
     <t>Test Label 2,10,Reports,,,,,</t>
   </si>
   <si>
@@ -1174,15 +1156,9 @@
     <t>List_View_Name</t>
   </si>
   <si>
-    <t>Module3Tc021_FillThirdPartyWebsiteToReportAndDashboardAndVerifyTheNavigation</t>
-  </si>
-  <si>
     <t>Accounts/Reports&lt;break&gt;Dashboards</t>
   </si>
   <si>
-    <t>Module3Tc022_CreateListViewAndVerifyTheNavigationForListView</t>
-  </si>
-  <si>
     <t>Marketing Prospects</t>
   </si>
   <si>
@@ -1198,36 +1174,15 @@
     <t>Accounts/Custom Label 2</t>
   </si>
   <si>
-    <t>Module3Tc024_VerifyQuickCreateObjectWhenRecordHasMultipleRecordTypes</t>
-  </si>
-  <si>
     <t>OtherAccount</t>
   </si>
   <si>
     <t>Institution&lt;break&gt;Company&lt;break&gt;Fund Manager&lt;break&gt;Fund Manager’s Fund&lt;break&gt;Individual Investor&lt;break&gt;Intermediary&lt;break&gt;Limited Partner</t>
   </si>
   <si>
-    <t>Module3Tc025_FillTheRecordTypeIDAndVerifyTheImpactOnNavigationMenu</t>
-  </si>
-  <si>
     <t>Intermediary&lt;break&gt;Individual Investor&lt;break&gt;Limited Partner</t>
   </si>
   <si>
-    <t>Module3Tc027_RemoveTheRecordTypeAPIFieldAndVerifyTheImpactOnNavigationMenu</t>
-  </si>
-  <si>
-    <t>Module3Tc028_FillSomeThirdPartyUrlInUrlFieldAndVerifyTheImpactOnNavigationMenu</t>
-  </si>
-  <si>
-    <t>Module3Tc029_CreateAlistViewOfAccountsAndListViewInformationOnNavigationPage</t>
-  </si>
-  <si>
-    <t>Module3Tc030_RemoveTheURLAndVerifyTheImpactOnNavigationMenu</t>
-  </si>
-  <si>
-    <t>Module3Tc031_RemoveQuickCreateObjectFieldAndVerifyTheImpactOnNavigationMenu</t>
-  </si>
-  <si>
     <t>M4CON1</t>
   </si>
   <si>
@@ -1402,15 +1357,6 @@
     <t>Account</t>
   </si>
   <si>
-    <t>Module3Tc032_RemoveListViewObjectAndVerifyTheImpactOnNavigationMenu</t>
-  </si>
-  <si>
-    <t>Module3Tc033_RemoveListViewNameAndVerifyTheImpactOnNavigationMenu</t>
-  </si>
-  <si>
-    <t>Module3Tc034_CreateRecordTypeFundAndFundOfFundsForFundObjectAndAddTheFromTheProfiles</t>
-  </si>
-  <si>
     <t>New Fund</t>
   </si>
   <si>
@@ -1420,15 +1366,6 @@
     <t>Fund&lt;break&gt;Fund of Funds</t>
   </si>
   <si>
-    <t>Module3Tc035_VerifyQuickCreateObjectWhenRecordHasMultipleRecordTypes</t>
-  </si>
-  <si>
-    <t>Module3Tc036_1_UpdateTheRecordTypeAndDescriptionImpactOnNavigationMenu</t>
-  </si>
-  <si>
-    <t>Module3Tc036_2_UpdateTheRecordTypeAndDescriptionImpactOnNavigationMenu</t>
-  </si>
-  <si>
     <t>M4Field1</t>
   </si>
   <si>
@@ -1495,27 +1432,9 @@
     <t>DT-0029</t>
   </si>
   <si>
-    <t>Module3Tc050_CreateNewItemTaskOnNavigationTab</t>
-  </si>
-  <si>
-    <t>Module3Tc051_CreateNewItemsOnNavigationPage</t>
-  </si>
-  <si>
-    <t>Module3Tc055_MakeParentItemAsChildOfOtherItem</t>
-  </si>
-  <si>
     <t>Create New</t>
   </si>
   <si>
-    <t>Module3Tc054_CreateRecordsAfterNavigationThroughNavigationMenu</t>
-  </si>
-  <si>
-    <t>Module3Tc057_DeleteCreateNewItemFromNavigationPage</t>
-  </si>
-  <si>
-    <t>Module3Tc058_Create20ItemsUnderAParentItemAndVerfiyNavigationMenu</t>
-  </si>
-  <si>
     <t>Child1&lt;break&gt;Child2&lt;break&gt;Child3&lt;break&gt;Child4&lt;break&gt;Child5&lt;break&gt;Child6&lt;break&gt;Child7&lt;break&gt;Child8&lt;break&gt;Child9&lt;break&gt;Child10&lt;break&gt;Child11&lt;break&gt;Child12&lt;break&gt;Child13&lt;break&gt;Child14&lt;break&gt;Child15&lt;break&gt;Child16&lt;break&gt;Child17&lt;break&gt;Child18&lt;break&gt;Child19&lt;break&gt;Child20</t>
   </si>
   <si>
@@ -1531,12 +1450,6 @@
     <t>M4Att9</t>
   </si>
   <si>
-    <t>Module3Tc063_2_RemoveTheRecordCreationRightForStandardUser</t>
-  </si>
-  <si>
-    <t>Module3Tc065_CreateMyIndustryMenuItem</t>
-  </si>
-  <si>
     <t>My Industry</t>
   </si>
   <si>
@@ -1660,9 +1573,6 @@
     <t>Contact8</t>
   </si>
   <si>
-    <t>Module3Tc074_CreateMyRegionMenuItem</t>
-  </si>
-  <si>
     <t>My Region</t>
   </si>
   <si>
@@ -1807,48 +1717,27 @@
     <t>Date&lt;breakOn&gt;Type&lt;breakOn&gt;Status&lt;breakOn&gt;Location&lt;breakOn&gt;Main Contact&lt;breakOn&gt;Region</t>
   </si>
   <si>
-    <t>Module3Tc081_CreateMultiTaggedLogACallAllNavigationMenuItem</t>
-  </si>
-  <si>
     <t>Log a Call with Multiple Associations</t>
   </si>
   <si>
     <t>create new</t>
   </si>
   <si>
-    <t>Module3Tc085_CreateCustomActionOfTypeTask</t>
-  </si>
-  <si>
     <t>New Meeting</t>
   </si>
   <si>
-    <t>Module3Tc086_CreateNavigationRecordsRelatedToMultiTaggedActions</t>
-  </si>
-  <si>
     <t>New Task with Multiple Associations</t>
   </si>
   <si>
-    <t>Module3Tc091_CreatePredefinendValuesInNavigationRecords</t>
-  </si>
-  <si>
     <t>New Task with Multiple Associations&lt;break&gt;Log a Call with Multiple Associations&lt;break&gt;New Meeting</t>
   </si>
   <si>
-    <t>Module3Tc093_CreateTaskRecordTypesAndPageLayouts</t>
-  </si>
-  <si>
     <t>Task Type1&lt;break&gt;Task Type2&lt;break&gt;Task Type3</t>
   </si>
   <si>
-    <t>Module3Tc094_EditNavigationRecordAndSetRecordTypesInEachRecord</t>
-  </si>
-  <si>
     <t>Log a Call with Multiple Associations&lt;break&gt;New Task with Multiple Associations&lt;break&gt;New Meeting</t>
   </si>
   <si>
-    <t>Module3Tc095_VerifyActionsfromNavigationPageAfterAssigningRecordTypes</t>
-  </si>
-  <si>
     <t>M3INS1</t>
   </si>
   <si>
@@ -1960,16 +1849,10 @@
     <t>New York</t>
   </si>
   <si>
-    <t>Module3Tc008_VerifyTheitemsForWhichURLAndActionObjectAndLiewViewObjectFieldWasBlank</t>
-  </si>
-  <si>
     <t>Accounts/Custom Label 2&lt;break&gt;Contact/Custom Label 1</t>
   </si>
   <si>
     <t xml:space="preserve">40&lt;break&gt;-10&lt;break&gt;6&lt;break&gt;-10&lt;break&gt; </t>
-  </si>
-  <si>
-    <t>Module3Tc023_2_CreateALightningAppPageAndVerifyTheNavigationForLighteningAppPage</t>
   </si>
   <si>
     <t>Account&lt;break&gt;Fund&lt;break&gt;Task1</t>
@@ -2078,6 +1961,123 @@
   </si>
   <si>
     <t>Type__c</t>
+  </si>
+  <si>
+    <t>M3Tc008_VerifyTheitemsForWhichURLAndActionObjectAndLiewViewObjectFieldWasBlank</t>
+  </si>
+  <si>
+    <t>M3Tc009_1_UpdateReportsAndDashboardURLWithAnActualReporAndDashboardLink_Action</t>
+  </si>
+  <si>
+    <t>M3Tc011_RenameNavigationLabelAndVerifyImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc012_ChangeTheOrderOfTheLabelAndVerifyImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc015_1_AddNewNavigationItemsAndVerifyItOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc018_CreateSubMenuAndVerify</t>
+  </si>
+  <si>
+    <t>M3Tc019_CreateSubMenuForIIndlevelAndVerifyItOnTheNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc021_FillThirdPartyWebsiteToReportAndDashboardAndVerifyTheNavigation</t>
+  </si>
+  <si>
+    <t>M3Tc022_CreateListViewAndVerifyTheNavigationForListView</t>
+  </si>
+  <si>
+    <t>M3Tc023_2_CreateALightningAppPageAndVerifyTheNavigationForLighteningAppPage</t>
+  </si>
+  <si>
+    <t>M3Tc024_VerifyQuickCreateObjectWhenRecordHasMultipleRecordTypes</t>
+  </si>
+  <si>
+    <t>M3Tc025_FillTheRecordTypeIDAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc027_RemoveTheRecordTypeAPIFieldAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc028_FillSomeThirdPartyUrlInUrlFieldAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc029_CreateAlistViewOfAccountsAndListViewInformationOnNavigationPage</t>
+  </si>
+  <si>
+    <t>M3Tc030_RemoveTheURLAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc031_RemoveQuickCreateObjectFieldAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc032_RemoveListViewObjectAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc033_RemoveListViewNameAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc034_CreateRecordTypeFundAndFundOfFundsForFundObjectAndAddTheFromTheProfiles</t>
+  </si>
+  <si>
+    <t>M3Tc035_VerifyQuickCreateObjectWhenRecordHasMultipleRecordTypes</t>
+  </si>
+  <si>
+    <t>M3Tc036_1_UpdateTheRecordTypeAndDescriptionImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc036_2_UpdateTheRecordTypeAndDescriptionImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc050_CreateNewItemTaskOnNavigationTab</t>
+  </si>
+  <si>
+    <t>M3Tc051_CreateNewItemsOnNavigationPage</t>
+  </si>
+  <si>
+    <t>M3Tc055_MakeParentItemAsChildOfOtherItem</t>
+  </si>
+  <si>
+    <t>M3Tc054_CreateRecordsAfterNavigationThroughNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc057_DeleteCreateNewItemFromNavigationPage</t>
+  </si>
+  <si>
+    <t>M3Tc058_Create20ItemsUnderAParentItemAndVerfiyNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc063_2_RemoveTheRecordCreationRightForStandardUser</t>
+  </si>
+  <si>
+    <t>M3Tc065_CreateMyIndustryMenuItem</t>
+  </si>
+  <si>
+    <t>M3Tc074_CreateMyRegionMenuItem</t>
+  </si>
+  <si>
+    <t>M3Tc081_CreateMultiTaggedLogACallAllNavigationMenuItem</t>
+  </si>
+  <si>
+    <t>M3Tc085_CreateCustomActionOfTypeTask</t>
+  </si>
+  <si>
+    <t>M3Tc086_CreateNavigationRecordsRelatedToMultiTaggedActions</t>
+  </si>
+  <si>
+    <t>M3Tc091_CreatePredefinendValuesInNavigationRecords</t>
+  </si>
+  <si>
+    <t>M3Tc093_CreateTaskRecordTypesAndPageLayouts</t>
+  </si>
+  <si>
+    <t>M3Tc094_EditNavigationRecordAndSetRecordTypesInEachRecord</t>
+  </si>
+  <si>
+    <t>M3Tc095_VerifyActionsfromNavigationPageAfterAssigningRecordTypes</t>
   </si>
 </sst>
 </file>
@@ -2614,9 +2614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2648,28 +2646,28 @@
         <v>313</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>534</v>
+        <v>505</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2677,444 +2675,444 @@
         <v>638</v>
       </c>
       <c r="B2" t="s">
-        <v>639</v>
+        <v>601</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
+        <v>639</v>
+      </c>
+      <c r="B3" t="s">
         <v>314</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>315</v>
-      </c>
-      <c r="C3" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="B4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" t="s">
         <v>317</v>
-      </c>
-      <c r="B4" t="s">
-        <v>318</v>
-      </c>
-      <c r="D4" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>320</v>
+        <v>641</v>
       </c>
       <c r="B5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E5" t="s">
-        <v>640</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>326</v>
+        <v>642</v>
       </c>
       <c r="B6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>328</v>
+        <v>643</v>
       </c>
       <c r="B7" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F7" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>331</v>
+        <v>644</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>376</v>
+        <v>645</v>
       </c>
       <c r="B9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G9" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>378</v>
+        <v>646</v>
       </c>
       <c r="B10" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="H10" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="I10" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>641</v>
+        <v>647</v>
       </c>
       <c r="B11" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="G11" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>384</v>
+        <v>648</v>
       </c>
       <c r="B12" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="J12" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>387</v>
+        <v>649</v>
       </c>
       <c r="B13" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="J13" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>389</v>
+        <v>650</v>
       </c>
       <c r="B14" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>390</v>
+        <v>651</v>
       </c>
       <c r="B15" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>391</v>
+        <v>652</v>
       </c>
       <c r="B16" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="H16" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="I16" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>392</v>
+        <v>653</v>
       </c>
       <c r="B17" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>393</v>
+        <v>654</v>
       </c>
       <c r="B18" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>452</v>
+        <v>655</v>
       </c>
       <c r="B19" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>453</v>
+        <v>656</v>
       </c>
       <c r="B20" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="H20" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>454</v>
+        <v>657</v>
       </c>
       <c r="B21" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="H21" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="I21" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="J21" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="K21" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>458</v>
+        <v>658</v>
       </c>
       <c r="B22" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="K22" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>459</v>
+        <v>659</v>
       </c>
       <c r="B23" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>460</v>
+        <v>660</v>
       </c>
       <c r="B24" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>483</v>
+        <v>661</v>
       </c>
       <c r="B25" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E25">
         <v>35</v>
       </c>
       <c r="K25" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>484</v>
+        <v>662</v>
       </c>
       <c r="B26" t="s">
-        <v>642</v>
+        <v>603</v>
       </c>
       <c r="F26" t="s">
-        <v>486</v>
+        <v>462</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>485</v>
+        <v>663</v>
       </c>
       <c r="B27" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="F27" t="s">
-        <v>486</v>
+        <v>462</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>487</v>
+        <v>664</v>
       </c>
       <c r="B28" t="s">
-        <v>643</v>
+        <v>604</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>488</v>
+        <v>665</v>
       </c>
       <c r="B29" t="s">
-        <v>644</v>
+        <v>605</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>489</v>
+        <v>666</v>
       </c>
       <c r="B30" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="F30" t="s">
-        <v>491</v>
+        <v>464</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>495</v>
+        <v>667</v>
       </c>
       <c r="B31" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>496</v>
+        <v>668</v>
       </c>
       <c r="B32" t="s">
-        <v>497</v>
+        <v>468</v>
       </c>
       <c r="E32">
         <v>-20</v>
       </c>
       <c r="L32" t="s">
-        <v>498</v>
+        <v>469</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>538</v>
+        <v>669</v>
       </c>
       <c r="B33" t="s">
-        <v>539</v>
+        <v>509</v>
       </c>
       <c r="E33">
         <v>-25</v>
       </c>
       <c r="L33" t="s">
-        <v>540</v>
+        <v>510</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>587</v>
+        <v>670</v>
       </c>
       <c r="B34" t="s">
-        <v>588</v>
+        <v>557</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>589</v>
+        <v>558</v>
       </c>
       <c r="K34" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>590</v>
+        <v>671</v>
       </c>
       <c r="B35" t="s">
-        <v>591</v>
+        <v>559</v>
       </c>
       <c r="E35">
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>589</v>
+        <v>558</v>
       </c>
       <c r="K35" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>592</v>
+        <v>672</v>
       </c>
       <c r="B36" t="s">
-        <v>593</v>
+        <v>560</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>589</v>
+        <v>558</v>
       </c>
       <c r="K36" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>594</v>
+        <v>673</v>
       </c>
       <c r="B37" t="s">
-        <v>595</v>
+        <v>561</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>596</v>
+        <v>674</v>
       </c>
       <c r="J38" t="s">
-        <v>597</v>
+        <v>562</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>598</v>
+        <v>675</v>
       </c>
       <c r="B39" t="s">
-        <v>599</v>
+        <v>563</v>
       </c>
       <c r="J39" t="s">
-        <v>597</v>
+        <v>562</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>600</v>
+        <v>676</v>
       </c>
       <c r="B40" t="s">
-        <v>599</v>
+        <v>563</v>
       </c>
       <c r="F40" t="s">
-        <v>589</v>
+        <v>558</v>
       </c>
       <c r="J40" t="s">
-        <v>597</v>
+        <v>562</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>512</v>
+        <v>483</v>
       </c>
       <c r="L41" t="s">
-        <v>533</v>
+        <v>504</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>531</v>
+        <v>502</v>
       </c>
       <c r="M42" t="s">
-        <v>532</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -3158,7 +3156,7 @@
         <v>152</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -3171,7 +3169,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>620</v>
+        <v>583</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -3180,7 +3178,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>3</v>
@@ -3192,48 +3190,48 @@
         <v>3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>629</v>
+        <v>592</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -3245,10 +3243,10 @@
         <v>153</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>528</v>
+        <v>499</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>528</v>
+        <v>499</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>154</v>
@@ -3310,7 +3308,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>629</v>
+        <v>592</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -3325,7 +3323,7 @@
         <v>176</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>513</v>
+        <v>484</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>177</v>
@@ -3345,7 +3343,7 @@
         <v>181</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>524</v>
+        <v>495</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>182</v>
@@ -3365,7 +3363,7 @@
         <v>186</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>187</v>
@@ -3428,7 +3426,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
-        <v>614</v>
+        <v>577</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="31"/>
@@ -3457,310 +3455,310 @@
       <c r="A6" s="30"/>
       <c r="B6" s="31"/>
       <c r="C6" s="49" t="s">
-        <v>617</v>
+        <v>580</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="B7" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E7" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>541</v>
+        <v>511</v>
       </c>
       <c r="B8" t="s">
-        <v>542</v>
+        <v>512</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E8" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>543</v>
+        <v>513</v>
       </c>
       <c r="B9" t="s">
-        <v>544</v>
+        <v>514</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E9" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>545</v>
+        <v>515</v>
       </c>
       <c r="B10" t="s">
-        <v>546</v>
+        <v>516</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E10" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>547</v>
+        <v>517</v>
       </c>
       <c r="B11" t="s">
-        <v>548</v>
+        <v>518</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E11" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>549</v>
+        <v>519</v>
       </c>
       <c r="B12" t="s">
-        <v>550</v>
+        <v>520</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E12" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>551</v>
+        <v>521</v>
       </c>
       <c r="B13" t="s">
-        <v>564</v>
+        <v>534</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E13" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>552</v>
+        <v>522</v>
       </c>
       <c r="B14" t="s">
-        <v>565</v>
+        <v>535</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E14" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>553</v>
+        <v>523</v>
       </c>
       <c r="B15" t="s">
-        <v>566</v>
+        <v>536</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E15" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>554</v>
+        <v>524</v>
       </c>
       <c r="B16" t="s">
-        <v>567</v>
+        <v>537</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E16" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>555</v>
+        <v>525</v>
       </c>
       <c r="B17" t="s">
-        <v>568</v>
+        <v>538</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E17" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>556</v>
+        <v>526</v>
       </c>
       <c r="B18" t="s">
-        <v>569</v>
+        <v>539</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E18" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>557</v>
+        <v>527</v>
       </c>
       <c r="B19" t="s">
-        <v>570</v>
+        <v>540</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E19" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>558</v>
+        <v>528</v>
       </c>
       <c r="B20" t="s">
-        <v>571</v>
+        <v>541</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E20" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>559</v>
+        <v>529</v>
       </c>
       <c r="B21" t="s">
-        <v>572</v>
+        <v>542</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E21" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>560</v>
+        <v>530</v>
       </c>
       <c r="B22" t="s">
-        <v>573</v>
+        <v>543</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E22" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>561</v>
+        <v>531</v>
       </c>
       <c r="B23" t="s">
-        <v>574</v>
+        <v>544</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E23" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>562</v>
+        <v>532</v>
       </c>
       <c r="B24" t="s">
-        <v>575</v>
+        <v>545</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E24" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>563</v>
+        <v>533</v>
       </c>
       <c r="B25" t="s">
-        <v>576</v>
+        <v>546</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E25" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>621</v>
+        <v>584</v>
       </c>
       <c r="B26" t="s">
-        <v>622</v>
+        <v>585</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E26" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>623</v>
+        <v>586</v>
       </c>
       <c r="B27" t="s">
-        <v>624</v>
+        <v>587</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E27" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>629</v>
+        <v>592</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -3772,16 +3770,16 @@
         <v>167</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>168</v>
       </c>
       <c r="D30" t="s">
-        <v>530</v>
+        <v>501</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>513</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -3826,7 +3824,7 @@
     <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>614</v>
+        <v>577</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -3856,26 +3854,26 @@
     <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>628</v>
+        <v>591</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>516</v>
+        <v>487</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>517</v>
+        <v>488</v>
       </c>
       <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>518</v>
+        <v>489</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>519</v>
+        <v>490</v>
       </c>
       <c r="C9" s="22"/>
     </row>
@@ -3990,7 +3988,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
       <c r="D3" s="9" t="s">
-        <v>615</v>
+        <v>578</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -4048,7 +4046,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
       <c r="D7" s="9" t="s">
-        <v>629</v>
+        <v>592</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -4069,14 +4067,14 @@
     </row>
     <row r="8" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>520</v>
+        <v>491</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>521</v>
+        <v>492</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
@@ -4090,7 +4088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -4112,13 +4110,13 @@
         <v>141</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>660</v>
+        <v>621</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>661</v>
+        <v>622</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>662</v>
+        <v>623</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -4126,7 +4124,7 @@
       <c r="B2" s="9"/>
       <c r="C2" s="13"/>
       <c r="D2" s="9" t="s">
-        <v>619</v>
+        <v>582</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -4218,7 +4216,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="13"/>
       <c r="D15" s="9" t="s">
-        <v>630</v>
+        <v>593</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -4239,56 +4237,56 @@
     </row>
     <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>646</v>
+        <v>607</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>647</v>
+        <v>608</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>648</v>
+        <v>609</v>
       </c>
       <c r="G16" s="50" t="s">
-        <v>649</v>
+        <v>610</v>
       </c>
       <c r="H16" s="50" t="s">
-        <v>650</v>
+        <v>611</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>651</v>
+        <v>612</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>652</v>
+        <v>613</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>653</v>
+        <v>614</v>
       </c>
       <c r="G17" s="50" t="s">
-        <v>654</v>
+        <v>615</v>
       </c>
       <c r="H17" s="50" t="s">
-        <v>655</v>
+        <v>616</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>656</v>
+        <v>617</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>652</v>
+        <v>613</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>657</v>
+        <v>618</v>
       </c>
       <c r="F18" s="50" t="s">
-        <v>658</v>
+        <v>619</v>
       </c>
       <c r="G18" s="50" t="s">
-        <v>649</v>
+        <v>610</v>
       </c>
       <c r="H18" s="50" t="s">
-        <v>659</v>
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -4343,7 +4341,7 @@
         <v>299</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -4354,7 +4352,7 @@
         <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>578</v>
+        <v>548</v>
       </c>
       <c r="D2" t="s">
         <v>301</v>
@@ -4369,7 +4367,7 @@
         <v>302</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>584</v>
+        <v>554</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
@@ -4398,10 +4396,10 @@
         <v>305</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>585</v>
+        <v>555</v>
       </c>
       <c r="I3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4427,10 +4425,10 @@
         <v>305</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>586</v>
+        <v>556</v>
       </c>
       <c r="I4" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -4460,19 +4458,19 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4486,7 +4484,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>620</v>
+        <v>583</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -4496,31 +4494,31 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B4" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B5" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B6" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -4528,77 +4526,77 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B8" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B9" t="s">
-        <v>676</v>
+        <v>637</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="B10" t="s">
-        <v>675</v>
+        <v>636</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B11" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B13" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="B14" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="B15" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B16" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -4625,7 +4623,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>96</v>
@@ -4634,7 +4632,7 @@
         <v>307</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4647,7 +4645,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>620</v>
+        <v>583</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -4656,169 +4654,169 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="B4" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C4" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D4" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E4" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="B5" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C5" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D5" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E5" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="B6" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C6" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D6" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E6" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="B7" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C7" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D7" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E7" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="B8" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C8" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D8" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E8" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="B9" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C9" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D9" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E9" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="B10" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C10" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D10" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E10" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>493</v>
+        <v>466</v>
       </c>
       <c r="B11" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C11" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D11" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E11" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>494</v>
+        <v>467</v>
       </c>
       <c r="B12" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="C12" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D12" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="E12" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>625</v>
+        <v>588</v>
       </c>
       <c r="B13" t="s">
-        <v>626</v>
+        <v>589</v>
       </c>
       <c r="C13" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="D13" t="s">
-        <v>542</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -4845,25 +4843,25 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9" t="s">
-        <v>620</v>
+        <v>583</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="9"/>
@@ -4872,222 +4870,222 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="B3" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="C3" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D3" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E3" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F3" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="B4" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="C4" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D4" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E4" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="F4" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="B5" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="C5" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D5" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E5" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="F5" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="B6" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
       <c r="C6" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D6" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E6" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F6" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="B7" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="C7" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D7" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E7" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="F7" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="B8" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
       <c r="C8" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D8" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E8" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="F8" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="B9" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
       <c r="C9" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D9" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E9" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F9" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="B10" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="C10" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D10" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E10" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="F10" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="B11" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
       <c r="C11" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D11" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E11" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="F11" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="B12" t="s">
-        <v>481</v>
+        <v>460</v>
       </c>
       <c r="C12" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D12" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E12" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="F12" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="B13" t="s">
-        <v>482</v>
+        <v>461</v>
       </c>
       <c r="C13" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="D13" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="E13" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="F13" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -5213,7 +5211,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>499</v>
+        <v>470</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>14</v>
@@ -5227,7 +5225,7 @@
     <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>630</v>
+        <v>593</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -5236,112 +5234,112 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>500</v>
+        <v>471</v>
       </c>
       <c r="B4" t="s">
-        <v>501</v>
+        <v>472</v>
       </c>
       <c r="C4" t="s">
-        <v>502</v>
+        <v>473</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>503</v>
+        <v>474</v>
       </c>
       <c r="B5" t="s">
-        <v>504</v>
+        <v>475</v>
       </c>
       <c r="C5" t="s">
-        <v>502</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>505</v>
+        <v>476</v>
       </c>
       <c r="B6" t="s">
-        <v>506</v>
+        <v>477</v>
       </c>
       <c r="C6" t="s">
-        <v>502</v>
+        <v>473</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>507</v>
+        <v>478</v>
       </c>
       <c r="B7" t="s">
-        <v>508</v>
+        <v>479</v>
       </c>
       <c r="C7" t="s">
-        <v>502</v>
+        <v>473</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>509</v>
+        <v>480</v>
       </c>
       <c r="B8" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="C8" t="s">
-        <v>502</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>510</v>
+        <v>481</v>
       </c>
       <c r="B9" t="s">
-        <v>511</v>
+        <v>482</v>
       </c>
       <c r="C9" t="s">
-        <v>502</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>631</v>
+        <v>594</v>
       </c>
       <c r="B10" t="s">
-        <v>632</v>
+        <v>595</v>
       </c>
       <c r="C10" t="s">
-        <v>618</v>
+        <v>581</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>633</v>
+        <v>596</v>
       </c>
       <c r="B11" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="C11" t="s">
-        <v>618</v>
+        <v>581</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>634</v>
+        <v>597</v>
       </c>
       <c r="B12" t="s">
-        <v>635</v>
+        <v>598</v>
       </c>
       <c r="C12" t="s">
-        <v>618</v>
+        <v>581</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>636</v>
+        <v>599</v>
       </c>
       <c r="B13" t="s">
-        <v>637</v>
+        <v>600</v>
       </c>
       <c r="C13" t="s">
-        <v>618</v>
+        <v>581</v>
       </c>
     </row>
   </sheetData>
@@ -5370,59 +5368,59 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>663</v>
+        <v>624</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>664</v>
+        <v>625</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>665</v>
+        <v>626</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>666</v>
+        <v>627</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>667</v>
+        <v>628</v>
       </c>
       <c r="B2" t="s">
-        <v>668</v>
+        <v>629</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>669</v>
+        <v>630</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>670</v>
+        <v>631</v>
       </c>
       <c r="F2" t="s">
-        <v>671</v>
+        <v>632</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>672</v>
+        <v>633</v>
       </c>
       <c r="B3" t="s">
-        <v>673</v>
+        <v>634</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>669</v>
+        <v>630</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>674</v>
+        <v>635</v>
       </c>
       <c r="F3" t="s">
-        <v>671</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -5468,7 +5466,7 @@
         <v>40</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6007,7 +6005,7 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>617</v>
+        <v>580</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -6015,7 +6013,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
@@ -6024,13 +6022,13 @@
         <v>44</v>
       </c>
       <c r="D35" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>41</v>
       </c>
       <c r="G35" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -8075,7 +8073,7 @@
     <row r="3" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>614</v>
+        <v>577</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -9084,7 +9082,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>577</v>
+        <v>547</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -9095,7 +9093,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>578</v>
+        <v>548</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -9106,7 +9104,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>579</v>
+        <v>549</v>
       </c>
       <c r="C6" t="s">
         <v>65</v>
@@ -9115,7 +9113,7 @@
     <row r="8" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>616</v>
+        <v>579</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -9277,17 +9275,17 @@
     <row r="24" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>627</v>
+        <v>590</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>601</v>
+        <v>564</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>602</v>
+        <v>565</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>79</v>
@@ -9295,10 +9293,10 @@
     </row>
     <row r="26" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>603</v>
+        <v>566</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>604</v>
+        <v>567</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>79</v>
@@ -9322,17 +9320,17 @@
     <row r="30" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>617</v>
+        <v>580</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="B31" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="C31" t="s">
         <v>33</v>
@@ -9340,10 +9338,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="B32" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="C32" t="s">
         <v>292</v>
@@ -9352,7 +9350,7 @@
     <row r="34" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>628</v>
+        <v>591</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -9362,7 +9360,7 @@
         <v>146</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>513</v>
+        <v>484</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>33</v>
@@ -9370,10 +9368,10 @@
     </row>
     <row r="36" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>514</v>
+        <v>485</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>515</v>
+        <v>486</v>
       </c>
       <c r="C36" s="22"/>
     </row>
@@ -9450,13 +9448,13 @@
         <v>14</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>618</v>
+        <v>581</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>502</v>
+        <v>473</v>
       </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -11467,7 +11465,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>614</v>
+        <v>577</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -12481,10 +12479,10 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>580</v>
+        <v>550</v>
       </c>
       <c r="D4" t="s">
-        <v>577</v>
+        <v>547</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -12500,7 +12498,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>616</v>
+        <v>579</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
@@ -12650,7 +12648,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>627</v>
+        <v>590</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="7"/>
@@ -12662,19 +12660,19 @@
     </row>
     <row r="18" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>605</v>
+        <v>568</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>606</v>
+        <v>569</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>607</v>
+        <v>570</v>
       </c>
       <c r="D18" s="50" t="s">
-        <v>602</v>
+        <v>565</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>608</v>
+        <v>571</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -12684,7 +12682,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>617</v>
+        <v>580</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="7"/>
@@ -12696,213 +12694,213 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>394</v>
+        <v>379</v>
       </c>
       <c r="B21" t="s">
-        <v>464</v>
+        <v>443</v>
       </c>
       <c r="C21" t="s">
         <v>109</v>
       </c>
       <c r="D21" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="E21" t="s">
-        <v>396</v>
+        <v>381</v>
       </c>
       <c r="F21">
         <v>8435985993</v>
       </c>
       <c r="H21" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="I21" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="J21" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="B22" t="s">
-        <v>465</v>
+        <v>444</v>
       </c>
       <c r="C22" t="s">
         <v>112</v>
       </c>
       <c r="D22" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="E22" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
       <c r="F22">
         <v>8435985993</v>
       </c>
       <c r="H22" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="I22" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="J22" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>403</v>
+        <v>388</v>
       </c>
       <c r="B23" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
       <c r="C23" t="s">
         <v>116</v>
       </c>
       <c r="D23" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="E23" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="F23">
         <v>8435985993</v>
       </c>
       <c r="H23" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="I23" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="J23" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="B24" t="s">
-        <v>467</v>
+        <v>446</v>
       </c>
       <c r="C24" t="s">
         <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="E24" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="F24">
         <v>8435985993</v>
       </c>
       <c r="H24" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="I24" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="J24" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="B25" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="C25" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="D25" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="F25">
         <v>8435985993</v>
       </c>
       <c r="H25" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="I25" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="J25" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="B26" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="C26" t="s">
-        <v>410</v>
+        <v>395</v>
       </c>
       <c r="D26" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="F26">
         <v>8435985993</v>
       </c>
       <c r="H26" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
       <c r="I26" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="J26" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="B27" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="C27" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
       <c r="D27" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="F27">
         <v>8435985993</v>
       </c>
       <c r="H27" t="s">
-        <v>397</v>
+        <v>382</v>
       </c>
       <c r="I27" t="s">
-        <v>398</v>
+        <v>383</v>
       </c>
       <c r="J27" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>535</v>
+        <v>506</v>
       </c>
       <c r="B28" t="s">
-        <v>536</v>
+        <v>507</v>
       </c>
       <c r="C28" t="s">
-        <v>537</v>
+        <v>508</v>
       </c>
       <c r="D28" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="H28" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -12948,7 +12946,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>613</v>
+        <v>576</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>14</v>
@@ -12963,7 +12961,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>627</v>
+        <v>590</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -12975,10 +12973,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>612</v>
+        <v>575</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>611</v>
+        <v>574</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -13058,7 +13056,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>614</v>
+        <v>577</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -13072,10 +13070,10 @@
         <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>581</v>
+        <v>551</v>
       </c>
       <c r="C4" t="s">
-        <v>645</v>
+        <v>606</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>
@@ -13089,10 +13087,10 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>582</v>
+        <v>552</v>
       </c>
       <c r="C5" t="s">
-        <v>645</v>
+        <v>606</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -13111,7 +13109,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>627</v>
+        <v>590</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
@@ -13122,10 +13120,10 @@
     </row>
     <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>609</v>
+        <v>572</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>610</v>
+        <v>573</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>60</v>
@@ -13139,7 +13137,7 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>628</v>
+        <v>591</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
@@ -13153,7 +13151,7 @@
         <v>147</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>522</v>
+        <v>493</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>60</v>
@@ -13167,7 +13165,7 @@
         <v>148</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>523</v>
+        <v>494</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>60</v>
@@ -15273,7 +15271,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>615</v>
+        <v>578</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -16304,7 +16302,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>583</v>
+        <v>553</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -16316,7 +16314,7 @@
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>577</v>
+        <v>547</v>
       </c>
     </row>
     <row r="5" spans="1:1026" x14ac:dyDescent="0.25">
@@ -16351,7 +16349,7 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>619</v>
+        <v>582</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -16429,7 +16427,7 @@
         <v>262</v>
       </c>
       <c r="D12" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E12" t="s">
         <v>273</v>
@@ -16465,7 +16463,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>620</v>
+        <v>583</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -16474,13 +16472,13 @@
     </row>
     <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="B16" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
       <c r="C16" t="s">
-        <v>395</v>
+        <v>380</v>
       </c>
       <c r="D16" t="s">
         <v>30</v>
@@ -16490,7 +16488,7 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>629</v>
+        <v>592</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -16502,7 +16500,7 @@
         <v>149</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>524</v>
+        <v>495</v>
       </c>
       <c r="D19" s="50" t="s">
         <v>30</v>
@@ -16554,7 +16552,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>629</v>
+        <v>592</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -16569,7 +16567,7 @@
         <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>525</v>
+        <v>496</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>160</v>
@@ -16586,13 +16584,13 @@
         <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>526</v>
+        <v>497</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>163</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>527</v>
+        <v>498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel update for module 2
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,43 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514448F2-BBA0-4845-B7F6-21852203D5C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="7" firstSheet="1" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="FilePath" sheetId="18" r:id="rId1"/>
-    <sheet name="FieldSet" sheetId="1" r:id="rId2"/>
-    <sheet name="FieldComponent" sheetId="6" r:id="rId3"/>
-    <sheet name="Entities" sheetId="3" r:id="rId4"/>
-    <sheet name="Contacts" sheetId="2" r:id="rId5"/>
-    <sheet name="Test Custom Object" sheetId="23" r:id="rId6"/>
-    <sheet name="Fund" sheetId="7" r:id="rId7"/>
-    <sheet name="Deal" sheetId="4" r:id="rId8"/>
-    <sheet name="DealRequestTracker" sheetId="14" r:id="rId9"/>
-    <sheet name="CustomSDG" sheetId="13" r:id="rId10"/>
-    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId11"/>
-    <sheet name="MarketingEvent" sheetId="15" r:id="rId12"/>
-    <sheet name="Partnerships" sheetId="8" r:id="rId13"/>
-    <sheet name="Commitments" sheetId="9" r:id="rId14"/>
-    <sheet name="Task" sheetId="12" r:id="rId15"/>
-    <sheet name="UploadImageData" sheetId="17" r:id="rId16"/>
-    <sheet name="Fields" sheetId="19" r:id="rId17"/>
-    <sheet name="Attendees" sheetId="20" r:id="rId18"/>
-    <sheet name="Deal Team" sheetId="21" r:id="rId19"/>
-    <sheet name="Coverages" sheetId="22" r:id="rId20"/>
-    <sheet name="SDGActions" sheetId="24" r:id="rId21"/>
+    <sheet name="FilePath" r:id="rId1" sheetId="18"/>
+    <sheet name="FieldSet" r:id="rId2" sheetId="1"/>
+    <sheet name="FieldComponent" r:id="rId3" sheetId="6"/>
+    <sheet name="Entities" r:id="rId4" sheetId="3"/>
+    <sheet name="Contacts" r:id="rId5" sheetId="2"/>
+    <sheet name="Test Custom Object" r:id="rId6" sheetId="23"/>
+    <sheet name="Fund" r:id="rId7" sheetId="7"/>
+    <sheet name="Deal" r:id="rId8" sheetId="4"/>
+    <sheet name="DealRequestTracker" r:id="rId9" sheetId="14"/>
+    <sheet name="CustomSDG" r:id="rId10" sheetId="13"/>
+    <sheet name="ToggleButtonCheck" r:id="rId11" sheetId="16"/>
+    <sheet name="MarketingEvent" r:id="rId12" sheetId="15"/>
+    <sheet name="Partnerships" r:id="rId13" sheetId="8"/>
+    <sheet name="Commitments" r:id="rId14" sheetId="9"/>
+    <sheet name="Task" r:id="rId15" sheetId="12"/>
+    <sheet name="UploadImageData" r:id="rId16" sheetId="17"/>
+    <sheet name="Fields" r:id="rId17" sheetId="19"/>
+    <sheet name="Attendees" r:id="rId18" sheetId="20"/>
+    <sheet name="Deal Team" r:id="rId19" sheetId="21"/>
+    <sheet name="Coverages" r:id="rId20" sheetId="22"/>
+    <sheet name="SDGActions" r:id="rId21" sheetId="24"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="692">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2100,12 +2099,36 @@
   </si>
   <si>
     <t>JPG Minimum size&lt;break&gt;JPG Maximum size&lt;break&gt;PNG Minimum size&lt;break&gt;PNG Maximum size&lt;break&gt;GIF Minimum size&lt;break&gt;GIF Maximum size</t>
+  </si>
+  <si>
+    <t>Updated_Stage</t>
+  </si>
+  <si>
+    <t>HSRPIP6</t>
+  </si>
+  <si>
+    <t>InstDeal</t>
+  </si>
+  <si>
+    <t>navatariptesting+19650@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+26881@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+73144@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+99299@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+44415@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -2234,135 +2257,135 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="58">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="14" quotePrefix="1" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2379,10 +2402,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2417,7 +2440,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2452,7 +2475,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2546,21 +2569,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2577,7 +2600,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2629,31 +2652,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="66" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="89.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="81.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="66.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -3150,7 +3173,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>681</v>
       </c>
@@ -3163,18 +3186,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L41" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L31" r:id="rId2" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B44" r:id="rId3" xr:uid="{9E447F27-0081-418F-ACAF-CCA965A9ED8A}"/>
+    <hyperlink r:id="rId1" ref="L41"/>
+    <hyperlink display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M" r:id="rId2" ref="L31"/>
+    <hyperlink r:id="rId3" ref="B44"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD4"/>
@@ -3182,11 +3205,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" style="5" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="20.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="19.140625" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3206,7 +3229,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3274,7 +3297,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -3300,13 +3323,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -3314,13 +3337,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="22.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="32.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="127.5703125" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3343,7 +3366,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
@@ -3351,7 +3374,7 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
     </row>
-    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -3423,13 +3446,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A5" sqref="A3:XFD5"/>
@@ -3437,12 +3460,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="21.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="11.0" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3462,14 +3485,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
     </row>
-    <row r="3" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
@@ -3801,7 +3824,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="29" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
@@ -3830,14 +3853,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
@@ -3845,13 +3868,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -3865,10 +3888,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
     </row>
-    <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>571</v>
@@ -3898,7 +3921,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>585</v>
@@ -3906,7 +3929,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>486</v>
       </c>
@@ -3915,7 +3938,7 @@
       </c>
       <c r="C8" s="22"/>
     </row>
-    <row r="9" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>488</v>
       </c>
@@ -3925,13 +3948,13 @@
       <c r="C9" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:T9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
@@ -3939,26 +3962,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="1" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -4020,7 +4043,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" t="s">
         <v>673</v>
@@ -4032,7 +4055,7 @@
       <c r="Q2" s="48"/>
       <c r="S2" s="48"/>
     </row>
-    <row r="3" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
@@ -4093,7 +4116,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="7" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
@@ -4117,14 +4140,14 @@
       <c r="S7" s="16"/>
       <c r="T7" s="13"/>
     </row>
-    <row r="8" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>490</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="22"/>
     </row>
-    <row r="9" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>491</v>
       </c>
@@ -4132,13 +4155,13 @@
       <c r="C9" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:T18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -4146,12 +4169,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4171,7 +4194,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="13"/>
@@ -4263,7 +4286,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="15" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="13"/>
@@ -4287,7 +4310,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="13"/>
     </row>
-    <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>601</v>
       </c>
@@ -4304,7 +4327,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>606</v>
       </c>
@@ -4321,7 +4344,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>611</v>
       </c>
@@ -4342,13 +4365,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
@@ -4356,18 +4379,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.7109375" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="29" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="29" width="21.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4484,13 +4507,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -4498,11 +4521,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4652,13 +4675,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -4666,8 +4689,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4872,13 +4895,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -4886,8 +4909,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5141,13 +5164,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -5155,15 +5178,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -5183,7 +5206,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -5238,14 +5261,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
@@ -5253,9 +5276,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5269,12 +5292,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="53"/>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
     </row>
-    <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>587</v>
@@ -5395,13 +5418,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -5409,10 +5432,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5435,7 +5458,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row ht="150" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>622</v>
       </c>
@@ -5455,7 +5478,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row ht="210" r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>627</v>
       </c>
@@ -5476,13 +5499,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -5490,15 +5513,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -6085,24 +6108,24 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:ALO49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALP49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
@@ -7118,7 +7141,7 @@
       <c r="ALN1" s="5"/>
       <c r="ALO1" s="5"/>
     </row>
-    <row r="2" spans="1:1003" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="35"/>
@@ -9324,7 +9347,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="24" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>584</v>
@@ -9332,7 +9355,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>558</v>
       </c>
@@ -9343,7 +9366,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="26" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>560</v>
       </c>
@@ -9354,22 +9377,22 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="27" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="22"/>
     </row>
-    <row r="28" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="28" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="22"/>
     </row>
-    <row r="29" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="29" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="22"/>
     </row>
-    <row r="30" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="30" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
         <v>574</v>
@@ -9399,7 +9422,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="34" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
         <v>585</v>
@@ -9407,7 +9430,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="35" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>145</v>
       </c>
@@ -9418,7 +9441,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="36" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>484</v>
       </c>
@@ -9427,41 +9450,41 @@
       </c>
       <c r="C36" s="22"/>
     </row>
-    <row r="41" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="41" s="50" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="42" s="50" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="43" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="53"/>
       <c r="B43" s="53"/>
       <c r="C43" s="53"/>
       <c r="D43" s="53"/>
     </row>
-    <row r="44" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="44" s="50" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="45" s="50" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="46" s="50" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="47" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="53"/>
       <c r="B47" s="53"/>
       <c r="C47" s="53"/>
       <c r="D47" s="53"/>
     </row>
-    <row r="48" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="48" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="20"/>
       <c r="B48" s="20"/>
       <c r="C48" s="22"/>
     </row>
-    <row r="49" spans="1:3" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="49" s="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:ALR31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALS31"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:XFD18"/>
@@ -9469,12 +9492,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -10505,7 +10528,7 @@
       <c r="ALQ1" s="5"/>
       <c r="ALR1" s="5"/>
     </row>
-    <row r="2" spans="1:1006" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -12574,7 +12597,7 @@
         <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>109</v>
+        <v>687</v>
       </c>
     </row>
     <row r="8" spans="1:1006" x14ac:dyDescent="0.25">
@@ -12591,7 +12614,7 @@
         <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:1006" x14ac:dyDescent="0.25">
@@ -12608,7 +12631,7 @@
         <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>689</v>
       </c>
     </row>
     <row r="10" spans="1:1006" x14ac:dyDescent="0.25">
@@ -12625,7 +12648,7 @@
         <v>101</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>690</v>
       </c>
     </row>
     <row r="11" spans="1:1006" x14ac:dyDescent="0.25">
@@ -12642,7 +12665,7 @@
         <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>121</v>
+        <v>691</v>
       </c>
     </row>
     <row r="13" spans="1:1006" x14ac:dyDescent="0.25">
@@ -12710,7 +12733,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
         <v>562</v>
       </c>
@@ -12727,7 +12750,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="19" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E19" s="54"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -12955,7 +12978,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="30" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="53"/>
       <c r="B30" s="51"/>
       <c r="C30" s="51"/>
@@ -12967,20 +12990,20 @@
       <c r="I30" s="53"/>
       <c r="J30" s="53"/>
     </row>
-    <row r="31" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="31" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E31" s="54"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E18" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink r:id="rId1" ref="E18"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -12988,9 +13011,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -13004,7 +13027,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -13033,13 +13056,13 @@
       <c r="C4" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -13047,19 +13070,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -13091,7 +13114,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -13103,7 +13126,7 @@
       <c r="I2" s="39"/>
       <c r="J2" s="41"/>
     </row>
-    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -13151,12 +13174,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -13170,7 +13193,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>566</v>
       </c>
@@ -13184,7 +13207,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -13198,7 +13221,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>146</v>
       </c>
@@ -13212,7 +13235,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>147</v>
       </c>
@@ -13227,29 +13250,29 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AML19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMM20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -13271,7 +13294,9 @@
       <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="6"/>
+      <c r="H1" s="3" t="s">
+        <v>684</v>
+      </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -14291,7 +14316,7 @@
       <c r="AMK1" s="6"/>
       <c r="AML1" s="6"/>
     </row>
-    <row r="2" spans="1:1026" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="44" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -15319,7 +15344,7 @@
       <c r="AMK2" s="43"/>
       <c r="AML2" s="43"/>
     </row>
-    <row r="3" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -16499,7 +16524,7 @@
         <v>261</v>
       </c>
       <c r="D13" t="s">
-        <v>268</v>
+        <v>495</v>
       </c>
       <c r="E13" t="s">
         <v>275</v>
@@ -16507,66 +16532,89 @@
       <c r="F13" s="22" t="s">
         <v>276</v>
       </c>
+      <c r="H13" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="F14" s="22"/>
+      <c r="A14" t="s">
+        <v>685</v>
+      </c>
+      <c r="B14" t="s">
+        <v>686</v>
+      </c>
+      <c r="C14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E14" t="s">
+        <v>275</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="15" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>397</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>398</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>379</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
+    <row customFormat="1" r="19" s="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row customFormat="1" r="20" s="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B20" s="50" t="s">
         <v>494</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D20" s="50" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -16574,10 +16622,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="5" width="15.28515625" collapsed="true"/>
+    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -16597,10 +16645,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
-    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -16646,7 +16694,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
excel chhange for module 2
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar Guest\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="688">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2110,6 +2110,15 @@
   </si>
   <si>
     <t>7/18/2021</t>
+  </si>
+  <si>
+    <t>HSRPIP6</t>
+  </si>
+  <si>
+    <t>InstDeal</t>
+  </si>
+  <si>
+    <t>Updated_Stage</t>
   </si>
 </sst>
 </file>
@@ -13240,7 +13249,7 @@
   <dimension ref="A1:AML19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13275,7 +13284,9 @@
       <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="6"/>
+      <c r="H1" s="3" t="s">
+        <v>687</v>
+      </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -16503,7 +16514,7 @@
         <v>259</v>
       </c>
       <c r="D13" t="s">
-        <v>266</v>
+        <v>493</v>
       </c>
       <c r="E13" t="s">
         <v>273</v>
@@ -16511,9 +16522,29 @@
       <c r="F13" s="22" t="s">
         <v>274</v>
       </c>
+      <c r="H13" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="F14" s="22"/>
+      <c r="A14" t="s">
+        <v>685</v>
+      </c>
+      <c r="B14" t="s">
+        <v>686</v>
+      </c>
+      <c r="C14" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E14" t="s">
+        <v>273</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="15" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>

</xml_diff>

<commit_message>
Updated Excel For Module 3 Added TC001-TC015
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar Guest\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="764">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2335,6 +2335,21 @@
   </si>
   <si>
     <t>Fund Preferences&lt;break&gt;Existing LP&lt;break&gt;Total Fund Commitments (mn)&lt;break&gt;Total Co-investment Commitments (mn)&lt;break&gt;Industry&lt;break&gt;Region&lt;break&gt;Bank Name&lt;break&gt;City</t>
+  </si>
+  <si>
+    <t>Accounts New</t>
+  </si>
+  <si>
+    <t>M3Tc012_RenameNavigationLabelAndVerifyImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc013_ChangeTheOrderOfTheLabelAndVerifyImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Contact&lt;break&gt;Reports&lt;break&gt;Fund Manager&lt;break&gt;Institution&lt;break&gt;Partnership</t>
+  </si>
+  <si>
+    <t>60&lt;break&gt;-10&lt;break&gt;5&lt;break&gt;-10&lt;break&gt;</t>
   </si>
 </sst>
 </file>
@@ -2882,10 +2897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3404,6 +3419,28 @@
       </c>
       <c r="C44" s="56" t="s">
         <v>669</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>760</v>
+      </c>
+      <c r="B47" t="s">
+        <v>319</v>
+      </c>
+      <c r="D47" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>761</v>
+      </c>
+      <c r="B48" t="s">
+        <v>762</v>
+      </c>
+      <c r="E48" t="s">
+        <v>763</v>
       </c>
     </row>
   </sheetData>
@@ -3676,7 +3713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A5" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Excel for Module 3 TC016-025
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="770">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2350,6 +2350,24 @@
   </si>
   <si>
     <t>60&lt;break&gt;-10&lt;break&gt;5&lt;break&gt;-10&lt;break&gt;</t>
+  </si>
+  <si>
+    <t>M3Tc016_AddNewNavigationItemsAndVerifyItOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M3Tc019_CreateRecordTypeFundAndFundOfFundsForFundObjectAndAddTheFromTheProfiles</t>
+  </si>
+  <si>
+    <t>TestFund&lt;break&gt;TestFund of Funds</t>
+  </si>
+  <si>
+    <t>M3Tc020_VerifyQuickCreateObjectWhenRecordHasMultipleRecordTypes</t>
+  </si>
+  <si>
+    <t>TestCustom Object 1&lt;break&gt;TestCustom Object 2</t>
+  </si>
+  <si>
+    <t>M3Tc023_CreateRecordTypeForCustomObjectAndAddTheFromTheProfiles</t>
   </si>
 </sst>
 </file>
@@ -2897,10 +2915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3441,6 +3459,53 @@
       </c>
       <c r="E48" t="s">
         <v>763</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>764</v>
+      </c>
+      <c r="B49" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>765</v>
+      </c>
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="H50" t="s">
+        <v>432</v>
+      </c>
+      <c r="I50" t="s">
+        <v>367</v>
+      </c>
+      <c r="J50" t="s">
+        <v>766</v>
+      </c>
+      <c r="K50" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>767</v>
+      </c>
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="K51" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>769</v>
+      </c>
+      <c r="J52" t="s">
+        <v>768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tc for module 6 excel update
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="852">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1030,12 +1030,6 @@
     <t>Deal Team</t>
   </si>
   <si>
-    <t>Deal_Team__c</t>
-  </si>
-  <si>
-    <t>Pipeline__c</t>
-  </si>
-  <si>
     <t>APIName</t>
   </si>
   <si>
@@ -1063,18 +1057,6 @@
     <t>Task</t>
   </si>
   <si>
-    <t>Attendee_Staff__r.Name</t>
-  </si>
-  <si>
-    <t>Attendee_Staff__r.Title</t>
-  </si>
-  <si>
-    <t>Status__c</t>
-  </si>
-  <si>
-    <t>Notes__c</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -1124,12 +1106,6 @@
   </si>
   <si>
     <t>Attendee</t>
-  </si>
-  <si>
-    <t>Attendee__c</t>
-  </si>
-  <si>
-    <t>Marketing_Event__c</t>
   </si>
   <si>
     <t>Navigation_Label_With_Parent</t>
@@ -1922,12 +1898,6 @@
     <t>{"entityApiName": "Contact", "defaultFieldValues": {
 "AccountId" : "#parentrecordId#"
 }}</t>
-  </si>
-  <si>
-    <t>Member__r.Name</t>
-  </si>
-  <si>
-    <t>Type__c</t>
   </si>
   <si>
     <t>M3Tc008_VerifyTheitemsForWhichURLAndActionObjectAndLiewViewObjectFieldWasBlank</t>
@@ -2369,6 +2339,282 @@
   <si>
     <t>M3Tc023_CreateRecordTypeForCustomObjectAndAddTheFromTheProfiles</t>
   </si>
+  <si>
+    <t>Module6</t>
+  </si>
+  <si>
+    <t>M6INS1</t>
+  </si>
+  <si>
+    <t>Test Institution</t>
+  </si>
+  <si>
+    <t>M6INS2</t>
+  </si>
+  <si>
+    <t>Test Company1</t>
+  </si>
+  <si>
+    <t>M6INS3</t>
+  </si>
+  <si>
+    <t>Test Company 2</t>
+  </si>
+  <si>
+    <t>M6INS4</t>
+  </si>
+  <si>
+    <t>Test Company 4</t>
+  </si>
+  <si>
+    <t>M6INS5</t>
+  </si>
+  <si>
+    <t>Test Company 5</t>
+  </si>
+  <si>
+    <t>M6INS6</t>
+  </si>
+  <si>
+    <t>Test Company 6</t>
+  </si>
+  <si>
+    <t>M6INS7</t>
+  </si>
+  <si>
+    <t>Test Company 7</t>
+  </si>
+  <si>
+    <t>M6INS8</t>
+  </si>
+  <si>
+    <t>Test Company 8</t>
+  </si>
+  <si>
+    <t>M6INS9</t>
+  </si>
+  <si>
+    <t>Test Company 9</t>
+  </si>
+  <si>
+    <t>M6INS10</t>
+  </si>
+  <si>
+    <t>Test Company 10</t>
+  </si>
+  <si>
+    <t>M6INS11</t>
+  </si>
+  <si>
+    <t>Company Name (),-,_/,\ &amp;*!@#$%^&amp; commitments - Company Name ^0&amp;*@#$%^ &amp;*!@#$%^&amp; commitments - Company Name ^0&amp;*@#$%^ &amp;*!@#$%^&amp; commitments - Company Name ^0&amp;*@#$%^ &amp;*!@#$%^&amp; commitments - Company Name ^0&amp;*@#$%^ &amp;*!@#$%^&amp; commitments - Company Name ^0&amp;*@#$</t>
+  </si>
+  <si>
+    <t>M6INS12</t>
+  </si>
+  <si>
+    <t>Test Company 11</t>
+  </si>
+  <si>
+    <t>M6INS13</t>
+  </si>
+  <si>
+    <t>Test Company 12</t>
+  </si>
+  <si>
+    <t>M6INS14</t>
+  </si>
+  <si>
+    <t>Test Company 13</t>
+  </si>
+  <si>
+    <t>M6INS15</t>
+  </si>
+  <si>
+    <t>Test Company 14</t>
+  </si>
+  <si>
+    <t>M6INS16</t>
+  </si>
+  <si>
+    <t>Test Company 15</t>
+  </si>
+  <si>
+    <t>M6INS17</t>
+  </si>
+  <si>
+    <t>Test Company 16</t>
+  </si>
+  <si>
+    <t>M6INS18</t>
+  </si>
+  <si>
+    <t>Test Company 17</t>
+  </si>
+  <si>
+    <t>Lender</t>
+  </si>
+  <si>
+    <t>M6INS19</t>
+  </si>
+  <si>
+    <t>Test Company 3</t>
+  </si>
+  <si>
+    <t>M6INS20</t>
+  </si>
+  <si>
+    <t>Test Company 20</t>
+  </si>
+  <si>
+    <t>Module 6</t>
+  </si>
+  <si>
+    <t>M6Deal1</t>
+  </si>
+  <si>
+    <t>Institution Deal</t>
+  </si>
+  <si>
+    <t>M6Deal2</t>
+  </si>
+  <si>
+    <t>Test Deal</t>
+  </si>
+  <si>
+    <t>M6Deal3</t>
+  </si>
+  <si>
+    <t>Test Deal 2</t>
+  </si>
+  <si>
+    <t>IOI</t>
+  </si>
+  <si>
+    <t>M6Deal4</t>
+  </si>
+  <si>
+    <t>Test Deal 4</t>
+  </si>
+  <si>
+    <t>M6Deal5</t>
+  </si>
+  <si>
+    <t>Test Deal 5</t>
+  </si>
+  <si>
+    <t>M6Deal6</t>
+  </si>
+  <si>
+    <t>Test Deal 6</t>
+  </si>
+  <si>
+    <t>Due Dilligence</t>
+  </si>
+  <si>
+    <t>M6Deal7</t>
+  </si>
+  <si>
+    <t>Test Deal 7</t>
+  </si>
+  <si>
+    <t>Parked</t>
+  </si>
+  <si>
+    <t>M6Deal8</t>
+  </si>
+  <si>
+    <t>Test Deal 8</t>
+  </si>
+  <si>
+    <t>M6Deal9</t>
+  </si>
+  <si>
+    <t>Test Deal 9</t>
+  </si>
+  <si>
+    <t>M6Deal10</t>
+  </si>
+  <si>
+    <t>Test Deal 10</t>
+  </si>
+  <si>
+    <t>M6Deal11</t>
+  </si>
+  <si>
+    <t>Test Deal 3</t>
+  </si>
+  <si>
+    <t>M6Deal12</t>
+  </si>
+  <si>
+    <t>Test Deal 11</t>
+  </si>
+  <si>
+    <t>M6Deal13</t>
+  </si>
+  <si>
+    <t>Test Deal 12</t>
+  </si>
+  <si>
+    <t>M6Deal14</t>
+  </si>
+  <si>
+    <t>Test Deal 13</t>
+  </si>
+  <si>
+    <t>M6Deal15</t>
+  </si>
+  <si>
+    <t>Test Deal 14</t>
+  </si>
+  <si>
+    <t>M6Deal16</t>
+  </si>
+  <si>
+    <t>Test Deal 15</t>
+  </si>
+  <si>
+    <t>M6Deal17</t>
+  </si>
+  <si>
+    <t>Test Deal 16</t>
+  </si>
+  <si>
+    <t>M6Deal18</t>
+  </si>
+  <si>
+    <t>Test Deal 17</t>
+  </si>
+  <si>
+    <t>M6Deal19</t>
+  </si>
+  <si>
+    <t>Test Deal 20</t>
+  </si>
+  <si>
+    <t>navpeII__Deal_Team__c</t>
+  </si>
+  <si>
+    <t>navpeII__Attendee__c</t>
+  </si>
+  <si>
+    <t>navpeII__Deal_Contact_Type__c</t>
+  </si>
+  <si>
+    <t>navpeII__Team_Member__r.Name</t>
+  </si>
+  <si>
+    <t>navpeII__Attendee_Staff__r.Name</t>
+  </si>
+  <si>
+    <t>navpeII__Attendee_Staff__r.Title</t>
+  </si>
+  <si>
+    <t>navpeII__Status__c</t>
+  </si>
+  <si>
+    <t>navpeII__Notes__c</t>
+  </si>
 </sst>
 </file>
 
@@ -2377,7 +2623,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2447,6 +2693,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF080707"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -2512,7 +2764,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2633,6 +2885,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2917,7 +3170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
@@ -2954,38 +3207,38 @@
         <v>316</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="B2" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="B3" t="s">
         <v>310</v>
@@ -2996,7 +3249,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="B4" t="s">
         <v>312</v>
@@ -3007,18 +3260,18 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="B5" t="s">
         <v>314</v>
       </c>
       <c r="E5" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="B6" t="s">
         <v>317</v>
@@ -3026,7 +3279,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="B7" t="s">
         <v>318</v>
@@ -3037,7 +3290,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
       <c r="B8" t="s">
         <v>320</v>
@@ -3045,425 +3298,425 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="B9" t="s">
         <v>310</v>
       </c>
       <c r="G9" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="B10" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="H10" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="I10" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="B11" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="G11" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="B12" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="J12" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
       <c r="B13" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="J13" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="B14" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="B15" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="B16" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="H16" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="I16" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="B17" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="B18" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="B19" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="B20" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="H20" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="B21" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="H21" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="I21" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="J21" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K21" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>646</v>
+        <v>636</v>
       </c>
       <c r="B22" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="K22" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="B23" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
       <c r="B24" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="B25" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E25">
         <v>35</v>
       </c>
       <c r="K25" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="B26" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="F26" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="B27" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="F27" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="B28" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="B29" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="B30" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="F30" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="B31" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="B32" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="E32">
         <v>-20</v>
       </c>
       <c r="L32" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="B33" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="E33">
         <v>-25</v>
       </c>
       <c r="L33" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="B34" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="K34" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="B35" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="E35">
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="K35" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="B36" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="K36" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="B37" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="J38" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="B39" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="J39" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="B40" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="F40" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="J40" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="L41" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="M42" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>666</v>
+        <v>656</v>
       </c>
       <c r="B43" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
       <c r="B44" s="57" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
       <c r="C44" s="56" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>760</v>
+        <v>750</v>
       </c>
       <c r="B47" t="s">
         <v>319</v>
       </c>
       <c r="D47" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>761</v>
+        <v>751</v>
       </c>
       <c r="B48" t="s">
-        <v>762</v>
+        <v>752</v>
       </c>
       <c r="E48" t="s">
-        <v>763</v>
+        <v>753</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>764</v>
+        <v>754</v>
       </c>
       <c r="B49" t="s">
         <v>317</v>
@@ -3471,41 +3724,41 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>765</v>
+        <v>755</v>
       </c>
       <c r="B50" t="s">
         <v>57</v>
       </c>
       <c r="H50" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="I50" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="J50" t="s">
-        <v>766</v>
+        <v>756</v>
       </c>
       <c r="K50" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>767</v>
+        <v>757</v>
       </c>
       <c r="B51" t="s">
         <v>57</v>
       </c>
       <c r="K51" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="J52" t="s">
-        <v>768</v>
+        <v>758</v>
       </c>
     </row>
   </sheetData>
@@ -3524,7 +3777,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3563,7 +3816,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -3587,7 +3840,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>325</v>
       </c>
@@ -3597,35 +3850,35 @@
       <c r="C6" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>327</v>
+      <c r="D6" s="62" t="s">
+        <v>844</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>359</v>
+        <v>845</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -3637,10 +3890,10 @@
         <v>150</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>151</v>
@@ -3702,7 +3955,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -3717,7 +3970,7 @@
         <v>173</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>174</v>
@@ -3737,7 +3990,7 @@
         <v>178</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>179</v>
@@ -3757,7 +4010,7 @@
         <v>183</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>184</v>
@@ -3820,7 +4073,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="31"/>
@@ -3849,310 +4102,310 @@
       <c r="A6" s="30"/>
       <c r="B6" s="31"/>
       <c r="C6" s="49" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B7" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E7" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B8" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E8" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="B9" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="B10" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E10" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="B11" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E11" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="B12" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E12" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="B13" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E13" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="B14" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E14" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="B15" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E15" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="B16" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E16" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="B17" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="B18" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E18" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="B19" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E19" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="B20" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B21" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E21" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="B22" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E22" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="B23" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E23" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="B24" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E24" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B25" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E25" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="B26" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E26" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="B27" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E27" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -4164,16 +4417,16 @@
         <v>164</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>165</v>
       </c>
       <c r="D30" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -4218,7 +4471,7 @@
     <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -4248,26 +4501,26 @@
     <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="C9" s="22"/>
     </row>
@@ -4370,7 +4623,7 @@
     <row r="2" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" t="s">
-        <v>676</v>
+        <v>666</v>
       </c>
       <c r="K2" s="47"/>
       <c r="L2" s="47"/>
@@ -4384,7 +4637,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
       <c r="D3" s="9" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -4408,7 +4661,7 @@
         <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>675</v>
+        <v>665</v>
       </c>
       <c r="C4" t="s">
         <v>61</v>
@@ -4445,7 +4698,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
       <c r="D7" s="9" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -4466,14 +4719,14 @@
     </row>
     <row r="8" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
@@ -4509,13 +4762,13 @@
         <v>138</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -4523,7 +4776,7 @@
       <c r="B2" s="9"/>
       <c r="C2" s="13"/>
       <c r="D2" s="9" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -4615,7 +4868,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="13"/>
       <c r="D15" s="9" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -4636,56 +4889,56 @@
     </row>
     <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="G16" s="50" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H16" s="50" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="G17" s="50" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
       <c r="H17" s="50" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="F18" s="50" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="G18" s="50" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H18" s="50" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -4748,10 +5001,10 @@
         <v>297</v>
       </c>
       <c r="B2" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="C2" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="D2" t="s">
         <v>298</v>
@@ -4766,10 +5019,10 @@
         <v>299</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="I2" t="s">
-        <v>746</v>
+        <v>736</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4795,7 +5048,7 @@
         <v>299</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>747</v>
+        <v>737</v>
       </c>
       <c r="I3" t="s">
         <v>35</v>
@@ -4824,10 +5077,10 @@
         <v>299</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>748</v>
+        <v>738</v>
       </c>
       <c r="I4" t="s">
-        <v>749</v>
+        <v>739</v>
       </c>
     </row>
   </sheetData>
@@ -4839,8 +5092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4857,16 +5110,16 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>330</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>332</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>322</v>
@@ -4883,7 +5136,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -4893,31 +5146,31 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B7" t="s">
         <v>20</v>
@@ -4925,77 +5178,77 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="B8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B9" t="s">
-        <v>625</v>
+        <v>846</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B10" t="s">
-        <v>624</v>
+        <v>847</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B11" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B13" t="s">
-        <v>338</v>
+        <v>848</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B14" t="s">
-        <v>339</v>
+        <v>849</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B15" t="s">
-        <v>340</v>
+        <v>850</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="B16" t="s">
-        <v>341</v>
+        <v>851</v>
       </c>
     </row>
   </sheetData>
@@ -5022,7 +5275,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>93</v>
@@ -5031,7 +5284,7 @@
         <v>303</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5044,7 +5297,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -5053,169 +5306,169 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="B4" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C4" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D4" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E4" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B5" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C5" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D5" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E5" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B6" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C6" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D6" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E6" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B7" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C7" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D7" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E7" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="B8" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C8" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D8" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E8" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B9" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C9" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D9" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E9" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="B10" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C10" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D10" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E10" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="B11" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C11" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D11" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E11" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="B12" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C12" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D12" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="E12" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="B13" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="C13" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="D13" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
     </row>
   </sheetData>
@@ -5242,25 +5495,25 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="9"/>
@@ -5269,222 +5522,222 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="C3" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D3" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E3" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="F3" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="B4" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="C4" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D4" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E4" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="F4" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B5" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C5" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D5" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E5" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="F5" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B6" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="C6" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D6" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E6" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="F6" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B7" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="C7" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D7" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E7" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="F7" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B8" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="C8" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D8" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E8" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="F8" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="B9" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C9" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D9" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E9" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="F9" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B10" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="C10" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D10" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E10" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="F10" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B11" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="C11" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D11" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E11" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="F11" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="B12" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="C12" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D12" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E12" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="F12" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B13" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C13" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="D13" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="E13" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="F13" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -5544,10 +5797,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>674</v>
+        <v>664</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5564,7 +5817,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5586,36 +5839,36 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>753</v>
+        <v>743</v>
       </c>
       <c r="B5" t="s">
         <v>303</v>
       </c>
       <c r="C5" t="s">
-        <v>749</v>
+        <v>739</v>
       </c>
       <c r="D5" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>755</v>
+        <v>745</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="B6" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="C6" t="s">
-        <v>746</v>
+        <v>736</v>
       </c>
       <c r="D6" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>758</v>
+        <v>748</v>
       </c>
     </row>
   </sheetData>
@@ -5644,7 +5897,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>14</v>
@@ -5658,7 +5911,7 @@
     <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -5667,112 +5920,112 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="B4" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="C4" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="B5" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="C5" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B6" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="C6" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B7" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="C7" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B8" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C8" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="B9" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="C9" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="B10" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="C10" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="B11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C11" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="B12" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="C12" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="B13" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="C13" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -5801,59 +6054,59 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="B2" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="F2" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="B3" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="F3" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -5885,19 +6138,19 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>683</v>
+        <v>673</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>684</v>
+        <v>674</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>685</v>
+        <v>675</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>686</v>
+        <v>676</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -5905,22 +6158,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>688</v>
+        <v>678</v>
       </c>
       <c r="B2" t="s">
-        <v>704</v>
+        <v>694</v>
       </c>
       <c r="C2" t="s">
-        <v>705</v>
+        <v>695</v>
       </c>
       <c r="D2" t="s">
-        <v>689</v>
+        <v>679</v>
       </c>
       <c r="E2" t="s">
-        <v>690</v>
+        <v>680</v>
       </c>
       <c r="F2" t="s">
-        <v>691</v>
+        <v>681</v>
       </c>
     </row>
   </sheetData>
@@ -5955,57 +6208,57 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>692</v>
+        <v>682</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>693</v>
+        <v>683</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>694</v>
+        <v>684</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>695</v>
+        <v>685</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>696</v>
+        <v>686</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>138</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>697</v>
+        <v>687</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>698</v>
+        <v>688</v>
       </c>
       <c r="B2" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
       <c r="C2" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
       <c r="D2" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="E2" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>700</v>
+        <v>690</v>
       </c>
       <c r="G2" t="s">
-        <v>701</v>
+        <v>691</v>
       </c>
       <c r="H2" t="s">
-        <v>702</v>
+        <v>692</v>
       </c>
       <c r="I2" t="s">
-        <v>703</v>
+        <v>693</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6047,28 +6300,28 @@
         <v>138</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>708</v>
+        <v>698</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>709</v>
+        <v>699</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>710</v>
+        <v>700</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>711</v>
+        <v>701</v>
       </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -7084,19 +7337,19 @@
     </row>
     <row r="2" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>717</v>
+        <v>707</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>713</v>
+        <v>703</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>712</v>
+        <v>702</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -8116,21 +8369,21 @@
     </row>
     <row r="3" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>719</v>
+        <v>709</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>713</v>
+        <v>703</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>714</v>
+        <v>704</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>715</v>
+        <v>705</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -9150,19 +9403,19 @@
     </row>
     <row r="4" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>718</v>
+        <v>708</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>713</v>
+        <v>703</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>716</v>
+        <v>706</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -10189,7 +10442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -10223,7 +10476,7 @@
         <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -10758,13 +11011,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="B33" t="s">
         <v>188</v>
       </c>
       <c r="C33" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D33" s="61" t="s">
         <v>299</v>
@@ -10773,13 +11026,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D34" s="61" t="s">
         <v>299</v>
@@ -10788,13 +11041,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>752</v>
+        <v>742</v>
       </c>
       <c r="B35" t="s">
         <v>238</v>
       </c>
       <c r="C35" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D35" s="61" t="s">
         <v>299</v>
@@ -10807,7 +11060,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -10815,7 +11068,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
@@ -10824,13 +11077,13 @@
         <v>42</v>
       </c>
       <c r="D38" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>39</v>
       </c>
       <c r="G38" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -10841,10 +11094,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALO49"/>
+  <dimension ref="A1:ALO68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10870,7 +11123,7 @@
         <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>745</v>
+        <v>735</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -12878,7 +13131,7 @@
     <row r="3" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -13887,7 +14140,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -13898,7 +14151,7 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
@@ -13909,7 +14162,7 @@
         <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="C6" t="s">
         <v>62</v>
@@ -13918,7 +14171,7 @@
     <row r="8" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -14080,17 +14333,17 @@
     <row r="24" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>76</v>
@@ -14098,10 +14351,10 @@
     </row>
     <row r="26" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>76</v>
@@ -14125,17 +14378,17 @@
     <row r="30" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B31" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="C31" t="s">
         <v>32</v>
@@ -14143,10 +14396,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="B32" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="C32" t="s">
         <v>289</v>
@@ -14155,7 +14408,7 @@
     <row r="34" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -14165,7 +14418,7 @@
         <v>143</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>32</v>
@@ -14173,19 +14426,19 @@
     </row>
     <row r="36" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="C36" s="22"/>
     </row>
     <row r="38" spans="1:5" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="59" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="B38" s="59" t="s">
-        <v>721</v>
+        <v>711</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>76</v>
@@ -14193,10 +14446,10 @@
     </row>
     <row r="39" spans="1:5" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="59" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="B39" s="59" t="s">
-        <v>724</v>
+        <v>714</v>
       </c>
       <c r="C39" s="58" t="s">
         <v>32</v>
@@ -14204,10 +14457,10 @@
     </row>
     <row r="40" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="59" t="s">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="B40" s="59" t="s">
-        <v>736</v>
+        <v>726</v>
       </c>
       <c r="C40" s="58" t="s">
         <v>32</v>
@@ -14215,10 +14468,10 @@
     </row>
     <row r="41" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="59" t="s">
-        <v>731</v>
+        <v>721</v>
       </c>
       <c r="B41" s="59" t="s">
-        <v>737</v>
+        <v>727</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>76</v>
@@ -14226,53 +14479,53 @@
     </row>
     <row r="42" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="59" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="B42" s="58" t="s">
-        <v>738</v>
+        <v>728</v>
       </c>
       <c r="C42" s="58" t="s">
-        <v>741</v>
+        <v>731</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="59" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
       <c r="B43" s="58" t="s">
-        <v>744</v>
+        <v>734</v>
       </c>
       <c r="C43" s="58" t="s">
-        <v>742</v>
+        <v>732</v>
       </c>
       <c r="D43" s="53"/>
       <c r="E43" s="32" t="s">
-        <v>738</v>
+        <v>728</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="59" t="s">
-        <v>734</v>
+        <v>724</v>
       </c>
       <c r="B44" s="58" t="s">
-        <v>739</v>
+        <v>729</v>
       </c>
       <c r="C44" s="58" t="s">
-        <v>743</v>
+        <v>733</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="59" t="s">
-        <v>735</v>
+        <v>725</v>
       </c>
       <c r="B45" s="58" t="s">
-        <v>740</v>
+        <v>730</v>
       </c>
       <c r="C45" s="58" t="s">
         <v>62</v>
       </c>
       <c r="E45" s="58" t="s">
-        <v>736</v>
+        <v>726</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -14283,14 +14536,233 @@
       <c r="D47" s="53"/>
     </row>
     <row r="48" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="22"/>
-    </row>
-    <row r="49" spans="1:3" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="22"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
+        <v>761</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>762</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
+        <v>763</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>764</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="50"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
+        <v>765</v>
+      </c>
+      <c r="B51" t="s">
+        <v>766</v>
+      </c>
+      <c r="C51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
+        <v>767</v>
+      </c>
+      <c r="B52" t="s">
+        <v>768</v>
+      </c>
+      <c r="C52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
+        <v>769</v>
+      </c>
+      <c r="B53" t="s">
+        <v>770</v>
+      </c>
+      <c r="C53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
+        <v>771</v>
+      </c>
+      <c r="B54" t="s">
+        <v>772</v>
+      </c>
+      <c r="C54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
+        <v>773</v>
+      </c>
+      <c r="B55" t="s">
+        <v>774</v>
+      </c>
+      <c r="C55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
+        <v>775</v>
+      </c>
+      <c r="B56" t="s">
+        <v>776</v>
+      </c>
+      <c r="C56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
+        <v>777</v>
+      </c>
+      <c r="B57" t="s">
+        <v>778</v>
+      </c>
+      <c r="C57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
+        <v>779</v>
+      </c>
+      <c r="B58" t="s">
+        <v>780</v>
+      </c>
+      <c r="C58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
+        <v>781</v>
+      </c>
+      <c r="B59" t="s">
+        <v>782</v>
+      </c>
+      <c r="C59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
+        <v>783</v>
+      </c>
+      <c r="B60" t="s">
+        <v>784</v>
+      </c>
+      <c r="C60" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>785</v>
+      </c>
+      <c r="B61" t="s">
+        <v>786</v>
+      </c>
+      <c r="C61" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
+        <v>787</v>
+      </c>
+      <c r="B62" t="s">
+        <v>788</v>
+      </c>
+      <c r="C62" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
+        <v>789</v>
+      </c>
+      <c r="B63" t="s">
+        <v>790</v>
+      </c>
+      <c r="C63" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
+        <v>791</v>
+      </c>
+      <c r="B64" t="s">
+        <v>792</v>
+      </c>
+      <c r="C64" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
+        <v>793</v>
+      </c>
+      <c r="B65" t="s">
+        <v>794</v>
+      </c>
+      <c r="C65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
+        <v>795</v>
+      </c>
+      <c r="B66" t="s">
+        <v>796</v>
+      </c>
+      <c r="C66" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
+        <v>798</v>
+      </c>
+      <c r="B67" t="s">
+        <v>799</v>
+      </c>
+      <c r="C67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
+        <v>800</v>
+      </c>
+      <c r="B68" t="s">
+        <v>801</v>
+      </c>
+      <c r="C68" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14338,13 +14810,13 @@
         <v>14</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -16355,7 +16827,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -17369,13 +17841,13 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="D4" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="E4" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>26</v>
@@ -17388,7 +17860,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
@@ -17538,7 +18010,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="7"/>
@@ -17550,19 +18022,19 @@
     </row>
     <row r="18" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="D18" s="50" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -17572,7 +18044,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="7"/>
@@ -17584,213 +18056,213 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="B21" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="C21" t="s">
         <v>106</v>
       </c>
       <c r="D21" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E21" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="F21">
         <v>8435985993</v>
       </c>
       <c r="H21" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="I21" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="J21" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B22" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="C22" t="s">
         <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E22" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="F22">
         <v>8435985993</v>
       </c>
       <c r="H22" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="I22" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="J22" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="B23" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="C23" t="s">
         <v>113</v>
       </c>
       <c r="D23" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E23" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="F23">
         <v>8435985993</v>
       </c>
       <c r="H23" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="I23" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="J23" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="B24" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="C24" t="s">
         <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="E24" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="F24">
         <v>8435985993</v>
       </c>
       <c r="H24" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="I24" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="J24" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="B25" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="C25" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="D25" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F25">
         <v>8435985993</v>
       </c>
       <c r="H25" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="I25" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="J25" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B26" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="C26" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D26" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F26">
         <v>8435985993</v>
       </c>
       <c r="H26" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="I26" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="J26" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="B27" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="C27" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="D27" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F27">
         <v>8435985993</v>
       </c>
       <c r="H27" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="I27" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="J27" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B28" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C28" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="D28" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="H28" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -17807,25 +18279,25 @@
     </row>
     <row r="31" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="58" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>728</v>
+        <v>718</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>729</v>
+        <v>719</v>
       </c>
       <c r="E31" s="60"/>
     </row>
     <row r="32" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="58" t="s">
-        <v>727</v>
+        <v>717</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>725</v>
+        <v>715</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>726</v>
+        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -17856,7 +18328,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>14</v>
@@ -17871,7 +18343,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -17883,10 +18355,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -17966,7 +18438,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -17980,7 +18452,7 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="D4" t="s">
         <v>57</v>
@@ -17994,7 +18466,7 @@
         <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="D5" t="s">
         <v>57</v>
@@ -18013,7 +18485,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
@@ -18024,10 +18496,10 @@
     </row>
     <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>57</v>
@@ -18041,7 +18513,7 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
@@ -18055,7 +18527,7 @@
         <v>144</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>57</v>
@@ -18069,7 +18541,7 @@
         <v>145</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>57</v>
@@ -18085,10 +18557,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML21"/>
+  <dimension ref="A1:AML42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18124,7 +18596,7 @@
         <v>14</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>682</v>
+        <v>672</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -20177,7 +20649,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -21208,19 +21680,19 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
       <c r="E4" t="s">
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
     </row>
     <row r="5" spans="1:1026" x14ac:dyDescent="0.25">
@@ -21234,7 +21706,7 @@
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
     </row>
     <row r="6" spans="1:1026" x14ac:dyDescent="0.25">
@@ -21248,14 +21720,14 @@
         <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
     </row>
     <row r="8" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -21353,7 +21825,7 @@
         <v>259</v>
       </c>
       <c r="D13" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="E13" t="s">
         <v>273</v>
@@ -21362,15 +21834,15 @@
         <v>274</v>
       </c>
       <c r="H13" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>680</v>
+        <v>670</v>
       </c>
       <c r="B14" t="s">
-        <v>681</v>
+        <v>671</v>
       </c>
       <c r="C14" t="s">
         <v>259</v>
@@ -21389,7 +21861,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -21398,52 +21870,332 @@
     </row>
     <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B16" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C16" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="D16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>146</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="D19" s="50" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>723</v>
+        <v>713</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>720</v>
+        <v>710</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>721</v>
+        <v>711</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>722</v>
+        <v>712</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>803</v>
+      </c>
+      <c r="B24" t="s">
+        <v>804</v>
+      </c>
+      <c r="C24" t="s">
+        <v>762</v>
+      </c>
+      <c r="D24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>805</v>
+      </c>
+      <c r="B25" t="s">
+        <v>806</v>
+      </c>
+      <c r="C25" t="s">
+        <v>764</v>
+      </c>
+      <c r="D25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>807</v>
+      </c>
+      <c r="B26" t="s">
+        <v>808</v>
+      </c>
+      <c r="C26" t="s">
+        <v>764</v>
+      </c>
+      <c r="D26" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>810</v>
+      </c>
+      <c r="B27" t="s">
+        <v>811</v>
+      </c>
+      <c r="C27" t="s">
+        <v>768</v>
+      </c>
+      <c r="D27" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>812</v>
+      </c>
+      <c r="B28" t="s">
+        <v>813</v>
+      </c>
+      <c r="C28" t="s">
+        <v>770</v>
+      </c>
+      <c r="D28" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>814</v>
+      </c>
+      <c r="B29" t="s">
+        <v>815</v>
+      </c>
+      <c r="C29" t="s">
+        <v>772</v>
+      </c>
+      <c r="D29" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>817</v>
+      </c>
+      <c r="B30" t="s">
+        <v>818</v>
+      </c>
+      <c r="C30" t="s">
+        <v>774</v>
+      </c>
+      <c r="D30" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>820</v>
+      </c>
+      <c r="B31" t="s">
+        <v>821</v>
+      </c>
+      <c r="C31" t="s">
+        <v>776</v>
+      </c>
+      <c r="D31" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>822</v>
+      </c>
+      <c r="B32" t="s">
+        <v>823</v>
+      </c>
+      <c r="C32" t="s">
+        <v>778</v>
+      </c>
+      <c r="D32" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>824</v>
+      </c>
+      <c r="B33" t="s">
+        <v>825</v>
+      </c>
+      <c r="C33" t="s">
+        <v>780</v>
+      </c>
+      <c r="D33" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>826</v>
+      </c>
+      <c r="B34" t="s">
+        <v>827</v>
+      </c>
+      <c r="C34" t="s">
+        <v>782</v>
+      </c>
+      <c r="D34" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>828</v>
+      </c>
+      <c r="B35" t="s">
+        <v>829</v>
+      </c>
+      <c r="C35" t="s">
+        <v>784</v>
+      </c>
+      <c r="D35" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>830</v>
+      </c>
+      <c r="B36" t="s">
+        <v>831</v>
+      </c>
+      <c r="C36" t="s">
+        <v>786</v>
+      </c>
+      <c r="D36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>832</v>
+      </c>
+      <c r="B37" t="s">
+        <v>833</v>
+      </c>
+      <c r="C37" t="s">
+        <v>788</v>
+      </c>
+      <c r="D37" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>834</v>
+      </c>
+      <c r="B38" t="s">
+        <v>835</v>
+      </c>
+      <c r="C38" t="s">
+        <v>790</v>
+      </c>
+      <c r="D38" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>836</v>
+      </c>
+      <c r="B39" t="s">
+        <v>837</v>
+      </c>
+      <c r="C39" t="s">
+        <v>792</v>
+      </c>
+      <c r="D39" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>838</v>
+      </c>
+      <c r="B40" t="s">
+        <v>839</v>
+      </c>
+      <c r="C40" t="s">
+        <v>794</v>
+      </c>
+      <c r="D40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>840</v>
+      </c>
+      <c r="B41" t="s">
+        <v>841</v>
+      </c>
+      <c r="C41" t="s">
+        <v>796</v>
+      </c>
+      <c r="D41" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>842</v>
+      </c>
+      <c r="B42" t="s">
+        <v>843</v>
+      </c>
+      <c r="C42" t="s">
+        <v>801</v>
+      </c>
+      <c r="D42" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -21493,7 +22245,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -21508,7 +22260,7 @@
         <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>678</v>
+        <v>668</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>157</v>
@@ -21525,13 +22277,13 @@
         <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>679</v>
+        <v>669</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>160</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel updated for Module 3
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363DDE94-6425-4A79-A074-762742BAF24A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="18" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="886">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2144,18 +2143,6 @@
     <t>PE Test Email Body</t>
   </si>
   <si>
-    <t>CustomReportFolder</t>
-  </si>
-  <si>
-    <t>CustomReport</t>
-  </si>
-  <si>
-    <t>PETestEmailFolder</t>
-  </si>
-  <si>
-    <t>PETestCustomEmailTemplate</t>
-  </si>
-  <si>
     <t>Due_Date</t>
   </si>
   <si>
@@ -2309,30 +2296,18 @@
     <t>Fund Preferences&lt;break&gt;Existing LP&lt;break&gt;Total Fund Commitments (mn)&lt;break&gt;Total Co-investment Commitments (mn)&lt;break&gt;Industry&lt;break&gt;Region&lt;break&gt;Bank Name&lt;break&gt;City</t>
   </si>
   <si>
-    <t>Accounts New</t>
-  </si>
-  <si>
     <t>M3Tc012_RenameNavigationLabelAndVerifyImpactOnNavigationMenu</t>
   </si>
   <si>
     <t>M3Tc013_ChangeTheOrderOfTheLabelAndVerifyImpactOnNavigationMenu</t>
   </si>
   <si>
-    <t>Contact&lt;break&gt;Reports&lt;break&gt;Fund Manager&lt;break&gt;Institution&lt;break&gt;Partnership</t>
-  </si>
-  <si>
-    <t>60&lt;break&gt;-10&lt;break&gt;5&lt;break&gt;-10&lt;break&gt;</t>
-  </si>
-  <si>
     <t>M3Tc016_AddNewNavigationItemsAndVerifyItOnNavigationMenu</t>
   </si>
   <si>
     <t>M3Tc019_CreateRecordTypeFundAndFundOfFundsForFundObjectAndAddTheFromTheProfiles</t>
   </si>
   <si>
-    <t>TestFund&lt;break&gt;TestFund of Funds</t>
-  </si>
-  <si>
     <t>M3Tc020_VerifyQuickCreateObjectWhenRecordHasMultipleRecordTypes</t>
   </si>
   <si>
@@ -2673,12 +2648,81 @@
   </si>
   <si>
     <t>VM Ware, Inc. - Penta Mezzanine</t>
+  </si>
+  <si>
+    <t>Partnership</t>
+  </si>
+  <si>
+    <t>Partnership New</t>
+  </si>
+  <si>
+    <t>Contact&lt;break&gt;Reports&lt;break&gt;Fund Manager&lt;break&gt;Institution&lt;break&gt;Partnership New</t>
+  </si>
+  <si>
+    <t>60&lt;break&gt;-10&lt;break&gt;42&lt;break&gt;-10&lt;break&gt;</t>
+  </si>
+  <si>
+    <t>Test1Fund&lt;break&gt;Test1Fund of Funds</t>
+  </si>
+  <si>
+    <t>M3Tc026_1_DeActivateARecordTypeForInstitution_Action</t>
+  </si>
+  <si>
+    <t>M3Tc027_VerifyAndCreateNavigationItemWhichAreRedirectedtoListView</t>
+  </si>
+  <si>
+    <t>Navigation List View Item</t>
+  </si>
+  <si>
+    <t>M3Tc028_CreateRecordthroughnavigationMenuandVerifyitontabsListview</t>
+  </si>
+  <si>
+    <t>Contact&lt;break&gt;Test Custom Object</t>
+  </si>
+  <si>
+    <t>M3Tc032_VerifyWhetherCustomNavigationwillbeaddedintheNavigationMenu</t>
+  </si>
+  <si>
+    <t>Custom Label</t>
+  </si>
+  <si>
+    <t>M3Tc034_VerifyTheFunctionalityByrenamingAndDeletingandRemovingUtilityItemCustomLabelintheCustomnavigationMenu</t>
+  </si>
+  <si>
+    <t>Custom Label New</t>
+  </si>
+  <si>
+    <t>M3INS12</t>
+  </si>
+  <si>
+    <t>M3INS22</t>
+  </si>
+  <si>
+    <t>navatariptesting+75406@gmail.com</t>
+  </si>
+  <si>
+    <t>M3CON12</t>
+  </si>
+  <si>
+    <t>CustomReportFolder69795</t>
+  </si>
+  <si>
+    <t>CustomReport73415</t>
+  </si>
+  <si>
+    <t>PETestEmailFolder70193</t>
+  </si>
+  <si>
+    <t>PETestCustomEmailTemplate9823</t>
+  </si>
+  <si>
+    <t>08/11/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -2950,7 +2994,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3227,11 +3271,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3752,80 +3796,126 @@
         <v>659</v>
       </c>
     </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>745</v>
+      </c>
+      <c r="B45" t="s">
+        <v>863</v>
+      </c>
+      <c r="D45" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>746</v>
+      </c>
+      <c r="B46" t="s">
+        <v>865</v>
+      </c>
+      <c r="E46" t="s">
+        <v>866</v>
+      </c>
+    </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
+        <v>747</v>
+      </c>
+      <c r="B47" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>748</v>
+      </c>
+      <c r="B48" t="s">
+        <v>57</v>
+      </c>
+      <c r="H48" t="s">
+        <v>424</v>
+      </c>
+      <c r="I48" t="s">
+        <v>359</v>
+      </c>
+      <c r="J48" t="s">
+        <v>867</v>
+      </c>
+      <c r="K48" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>749</v>
+      </c>
+      <c r="B49" t="s">
+        <v>57</v>
+      </c>
+      <c r="K49" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>751</v>
+      </c>
+      <c r="J50" t="s">
         <v>750</v>
-      </c>
-      <c r="B47" t="s">
-        <v>319</v>
-      </c>
-      <c r="D47" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>751</v>
-      </c>
-      <c r="B48" t="s">
-        <v>752</v>
-      </c>
-      <c r="E48" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>754</v>
-      </c>
-      <c r="B49" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>755</v>
-      </c>
-      <c r="B50" t="s">
-        <v>57</v>
-      </c>
-      <c r="H50" t="s">
-        <v>424</v>
-      </c>
-      <c r="I50" t="s">
-        <v>359</v>
-      </c>
-      <c r="J50" t="s">
-        <v>756</v>
-      </c>
-      <c r="K50" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>757</v>
-      </c>
-      <c r="B51" t="s">
-        <v>57</v>
-      </c>
-      <c r="K51" t="s">
-        <v>424</v>
+        <v>868</v>
+      </c>
+      <c r="J51" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>759</v>
-      </c>
-      <c r="J52" t="s">
-        <v>758</v>
+        <v>869</v>
+      </c>
+      <c r="B52" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>871</v>
+      </c>
+      <c r="B53" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>873</v>
+      </c>
+      <c r="B54" t="s">
+        <v>874</v>
+      </c>
+      <c r="K54" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>875</v>
+      </c>
+      <c r="B55" t="s">
+        <v>874</v>
+      </c>
+      <c r="D55" t="s">
+        <v>876</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L41" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="L31" r:id="rId2" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B44" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="L41" r:id="rId1"/>
+    <hyperlink ref="L31" r:id="rId2" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M"/>
+    <hyperlink ref="B44" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -3833,7 +3923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3920,7 +4010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3998,7 +4088,7 @@
         <v>326</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>844</v>
+        <v>836</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>331</v>
@@ -4015,7 +4105,7 @@
         <v>352</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>845</v>
+        <v>837</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>331</v>
@@ -4052,7 +4142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4175,7 +4265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -4583,7 +4673,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4677,7 +4767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4884,7 +4974,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5094,7 +5184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5169,7 +5259,7 @@
         <v>655</v>
       </c>
       <c r="I2" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5195,7 +5285,7 @@
         <v>299</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="I3" t="s">
         <v>35</v>
@@ -5224,10 +5314,10 @@
         <v>299</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="I4" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
   </sheetData>
@@ -5236,7 +5326,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5336,7 +5426,7 @@
         <v>342</v>
       </c>
       <c r="B9" t="s">
-        <v>846</v>
+        <v>838</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5344,7 +5434,7 @@
         <v>343</v>
       </c>
       <c r="B10" t="s">
-        <v>847</v>
+        <v>839</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5371,7 +5461,7 @@
         <v>344</v>
       </c>
       <c r="B13" t="s">
-        <v>848</v>
+        <v>840</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5379,7 +5469,7 @@
         <v>345</v>
       </c>
       <c r="B14" t="s">
-        <v>849</v>
+        <v>841</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5387,7 +5477,7 @@
         <v>346</v>
       </c>
       <c r="B15" t="s">
-        <v>850</v>
+        <v>842</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5395,7 +5485,7 @@
         <v>347</v>
       </c>
       <c r="B16" t="s">
-        <v>851</v>
+        <v>843</v>
       </c>
     </row>
   </sheetData>
@@ -5404,7 +5494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5624,7 +5714,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -5717,36 +5807,36 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="B5" t="s">
         <v>303</v>
       </c>
       <c r="C5" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="D5" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="B6" t="s">
         <v>667</v>
       </c>
       <c r="C6" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="D6" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
   </sheetData>
@@ -5756,7 +5846,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6025,7 +6115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6181,7 +6271,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6262,11 +6352,11 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6308,10 +6398,10 @@
         <v>678</v>
       </c>
       <c r="B2" t="s">
-        <v>694</v>
+        <v>881</v>
       </c>
       <c r="C2" t="s">
-        <v>695</v>
+        <v>882</v>
       </c>
       <c r="D2" t="s">
         <v>679</v>
@@ -6330,11 +6420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6384,10 +6474,10 @@
         <v>688</v>
       </c>
       <c r="B2" t="s">
-        <v>696</v>
+        <v>883</v>
       </c>
       <c r="C2" t="s">
-        <v>697</v>
+        <v>884</v>
       </c>
       <c r="D2" t="s">
         <v>689</v>
@@ -6415,25 +6505,25 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMH4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1022" x14ac:dyDescent="0.25">
@@ -6450,7 +6540,7 @@
         <v>331</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>601</v>
@@ -6462,13 +6552,13 @@
         <v>603</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -7484,16 +7574,18 @@
     </row>
     <row r="2" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="E2" t="s">
+        <v>885</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
         <v>590</v>
@@ -8516,18 +8608,18 @@
     </row>
     <row r="3" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>590</v>
@@ -9550,13 +9642,13 @@
     </row>
     <row r="4" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -10586,10 +10678,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -11158,7 +11250,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B33" t="s">
         <v>188</v>
@@ -11173,7 +11265,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -11188,7 +11280,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="B35" t="s">
         <v>238</v>
@@ -11240,11 +11332,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO68"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11270,7 +11362,7 @@
         <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -14487,7 +14579,7 @@
     </row>
     <row r="25" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>545</v>
+        <v>877</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>546</v>
@@ -14498,7 +14590,7 @@
     </row>
     <row r="26" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>547</v>
+        <v>878</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>548</v>
@@ -14585,7 +14677,7 @@
         <v>545</v>
       </c>
       <c r="B38" s="59" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>76</v>
@@ -14596,7 +14688,7 @@
         <v>547</v>
       </c>
       <c r="B39" s="59" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="C39" s="58" t="s">
         <v>32</v>
@@ -14604,10 +14696,10 @@
     </row>
     <row r="40" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="59" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B40" s="59" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="C40" s="58" t="s">
         <v>32</v>
@@ -14615,10 +14707,10 @@
     </row>
     <row r="41" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="59" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="B41" s="59" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="C41" s="23" t="s">
         <v>76</v>
@@ -14626,53 +14718,53 @@
     </row>
     <row r="42" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="59" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="B42" s="58" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="C42" s="58" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="59" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="B43" s="58" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="C43" s="58" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="D43" s="53"/>
       <c r="E43" s="32" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="59" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B44" s="58" t="s">
+        <v>725</v>
+      </c>
+      <c r="C44" s="58" t="s">
         <v>729</v>
-      </c>
-      <c r="C44" s="58" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="59" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="B45" s="58" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="C45" s="58" t="s">
         <v>62</v>
       </c>
       <c r="E45" s="58" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -14685,17 +14777,17 @@
     <row r="48" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>32</v>
@@ -14703,10 +14795,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="C50" s="22" t="s">
         <v>76</v>
@@ -14715,10 +14807,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="B51" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="C51" t="s">
         <v>76</v>
@@ -14726,10 +14818,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="B52" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="C52" t="s">
         <v>76</v>
@@ -14737,10 +14829,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="B53" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="C53" t="s">
         <v>76</v>
@@ -14748,10 +14840,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="B54" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="C54" t="s">
         <v>76</v>
@@ -14759,10 +14851,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="B55" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="C55" t="s">
         <v>76</v>
@@ -14770,10 +14862,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
       <c r="B56" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="C56" t="s">
         <v>76</v>
@@ -14781,10 +14873,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="B57" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="C57" t="s">
         <v>76</v>
@@ -14792,10 +14884,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="B58" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="C58" t="s">
         <v>76</v>
@@ -14803,10 +14895,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="B59" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="C59" t="s">
         <v>76</v>
@@ -14814,10 +14906,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>783</v>
+        <v>775</v>
       </c>
       <c r="B60" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="C60" t="s">
         <v>373</v>
@@ -14825,43 +14917,43 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>785</v>
+        <v>777</v>
       </c>
       <c r="B61" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="C61" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>787</v>
+        <v>779</v>
       </c>
       <c r="B62" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="C62" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="B63" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="C63" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>791</v>
+        <v>783</v>
       </c>
       <c r="B64" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="C64" t="s">
         <v>289</v>
@@ -14869,10 +14961,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
       <c r="B65" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="C65" t="s">
         <v>62</v>
@@ -14880,21 +14972,21 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>795</v>
+        <v>787</v>
       </c>
       <c r="B66" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="C66" t="s">
-        <v>797</v>
+        <v>789</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>798</v>
+        <v>790</v>
       </c>
       <c r="B67" t="s">
-        <v>799</v>
+        <v>791</v>
       </c>
       <c r="C67" t="s">
         <v>76</v>
@@ -14902,10 +14994,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="B68" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="C68" t="s">
         <v>76</v>
@@ -14917,11 +15009,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD36"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18169,7 +18261,7 @@
     </row>
     <row r="18" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>549</v>
+        <v>880</v>
       </c>
       <c r="B18" s="50" t="s">
         <v>550</v>
@@ -18429,29 +18521,32 @@
         <v>549</v>
       </c>
       <c r="B31" s="58" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="E31" s="60"/>
     </row>
     <row r="32" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="58" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B32" s="58" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>716</v>
+        <v>712</v>
+      </c>
+      <c r="E32" t="s">
+        <v>879</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>852</v>
+        <v>844</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="7"/>
@@ -18463,44 +18558,44 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>853</v>
+        <v>845</v>
       </c>
       <c r="B35" t="s">
-        <v>854</v>
+        <v>846</v>
       </c>
       <c r="C35" t="s">
-        <v>855</v>
+        <v>847</v>
       </c>
       <c r="E35" s="63" t="s">
-        <v>856</v>
+        <v>848</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>857</v>
+        <v>849</v>
       </c>
       <c r="B36" t="s">
-        <v>858</v>
+        <v>850</v>
       </c>
       <c r="C36" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
       <c r="E36" s="63" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E18" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E35" r:id="rId2" display="mailto:dealroom1.2+clientcontact01@gmail.com" xr:uid="{98BA426C-325F-42E4-9F5B-5E6B7175D14E}"/>
-    <hyperlink ref="E36" r:id="rId3" display="mailto:dealroom1.2+clientcontact13@gmail.com" xr:uid="{5EC2790C-F5FF-49E5-AA9D-A10A39B602C9}"/>
+    <hyperlink ref="E18" r:id="rId1"/>
+    <hyperlink ref="E35" r:id="rId2" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
+    <hyperlink ref="E36" r:id="rId3" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18559,7 +18654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18747,11 +18842,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AML47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AML49"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD47"/>
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22097,23 +22192,23 @@
     </row>
     <row r="21" spans="1:8" s="58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B21" s="58" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>802</v>
+        <v>794</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -22122,13 +22217,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>803</v>
+        <v>795</v>
       </c>
       <c r="B24" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="C24" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="D24" t="s">
         <v>266</v>
@@ -22136,13 +22231,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>805</v>
+        <v>797</v>
       </c>
       <c r="B25" t="s">
-        <v>806</v>
+        <v>798</v>
       </c>
       <c r="C25" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
@@ -22153,41 +22248,41 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>807</v>
+        <v>799</v>
       </c>
       <c r="B26" t="s">
-        <v>808</v>
+        <v>800</v>
       </c>
       <c r="C26" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="D26" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>810</v>
+        <v>802</v>
       </c>
       <c r="B27" t="s">
-        <v>811</v>
+        <v>803</v>
       </c>
       <c r="C27" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="D27" t="s">
-        <v>809</v>
+        <v>801</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>812</v>
+        <v>804</v>
       </c>
       <c r="B28" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="C28" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="D28" t="s">
         <v>266</v>
@@ -22195,41 +22290,41 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="B29" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="C29" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="D29" t="s">
-        <v>816</v>
+        <v>808</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>817</v>
+        <v>809</v>
       </c>
       <c r="B30" t="s">
-        <v>818</v>
+        <v>810</v>
       </c>
       <c r="C30" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="D30" t="s">
-        <v>819</v>
+        <v>811</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>820</v>
+        <v>812</v>
       </c>
       <c r="B31" t="s">
-        <v>821</v>
+        <v>813</v>
       </c>
       <c r="C31" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="D31" t="s">
         <v>266</v>
@@ -22237,13 +22332,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="B32" t="s">
-        <v>823</v>
+        <v>815</v>
       </c>
       <c r="C32" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="D32" t="s">
         <v>266</v>
@@ -22251,13 +22346,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>824</v>
+        <v>816</v>
       </c>
       <c r="B33" t="s">
-        <v>825</v>
+        <v>817</v>
       </c>
       <c r="C33" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="D33" t="s">
         <v>266</v>
@@ -22265,13 +22360,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>826</v>
+        <v>818</v>
       </c>
       <c r="B34" t="s">
-        <v>827</v>
+        <v>819</v>
       </c>
       <c r="C34" t="s">
-        <v>782</v>
+        <v>774</v>
       </c>
       <c r="D34" t="s">
         <v>266</v>
@@ -22279,13 +22374,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>828</v>
+        <v>820</v>
       </c>
       <c r="B35" t="s">
-        <v>829</v>
+        <v>821</v>
       </c>
       <c r="C35" t="s">
-        <v>784</v>
+        <v>776</v>
       </c>
       <c r="D35" t="s">
         <v>266</v>
@@ -22293,13 +22388,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>830</v>
+        <v>822</v>
       </c>
       <c r="B36" t="s">
-        <v>831</v>
+        <v>823</v>
       </c>
       <c r="C36" t="s">
-        <v>786</v>
+        <v>778</v>
       </c>
       <c r="D36" t="s">
         <v>266</v>
@@ -22307,13 +22402,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>832</v>
+        <v>824</v>
       </c>
       <c r="B37" t="s">
-        <v>833</v>
+        <v>825</v>
       </c>
       <c r="C37" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="D37" t="s">
         <v>266</v>
@@ -22321,13 +22416,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="B38" t="s">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="C38" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="D38" t="s">
         <v>266</v>
@@ -22335,13 +22430,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>836</v>
+        <v>828</v>
       </c>
       <c r="B39" t="s">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="C39" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="D39" t="s">
         <v>266</v>
@@ -22349,13 +22444,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="B40" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="C40" t="s">
-        <v>794</v>
+        <v>786</v>
       </c>
       <c r="D40" t="s">
         <v>266</v>
@@ -22363,13 +22458,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>840</v>
+        <v>832</v>
       </c>
       <c r="B41" t="s">
-        <v>841</v>
+        <v>833</v>
       </c>
       <c r="C41" t="s">
-        <v>796</v>
+        <v>788</v>
       </c>
       <c r="D41" t="s">
         <v>266</v>
@@ -22377,13 +22472,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="B42" t="s">
-        <v>843</v>
+        <v>835</v>
       </c>
       <c r="C42" t="s">
-        <v>801</v>
+        <v>793</v>
       </c>
       <c r="D42" t="s">
         <v>266</v>
@@ -22393,7 +22488,7 @@
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -22402,10 +22497,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="B46" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="C46" t="s">
         <v>47</v>
@@ -22416,16 +22511,30 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="B47" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="C47" t="s">
         <v>47</v>
       </c>
       <c r="D47" t="s">
         <v>663</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="58" t="s">
+        <v>709</v>
+      </c>
+      <c r="B49" s="58" t="s">
+        <v>706</v>
+      </c>
+      <c r="C49" s="58" t="s">
+        <v>707</v>
+      </c>
+      <c r="D49" s="58" t="s">
+        <v>708</v>
       </c>
     </row>
   </sheetData>
@@ -22436,10 +22545,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE8F3F1-4090-4764-95F5-1455E00CEB5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -22456,7 +22565,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>12</v>
@@ -22467,18 +22576,18 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="B2" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="B3" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel update mfor module 6
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="18" activeTab="24"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="888">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2717,6 +2717,12 @@
   </si>
   <si>
     <t>08/11/2021</t>
+  </si>
+  <si>
+    <t>M6Deal20</t>
+  </si>
+  <si>
+    <t>Test Deal New</t>
   </si>
 </sst>
 </file>
@@ -6508,8 +6514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMH4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18845,8 +18851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22484,6 +22490,23 @@
         <v>266</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>886</v>
+      </c>
+      <c r="B43" t="s">
+        <v>887</v>
+      </c>
+      <c r="C43" t="s">
+        <v>791</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
+      </c>
+      <c r="F43" t="s">
+        <v>784</v>
+      </c>
+    </row>
     <row r="45" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>

</xml_diff>

<commit_message>
Updated Excel for Module 5
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" firstSheet="18" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" firstSheet="15" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="843">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1431,9 +1431,6 @@
   </si>
   <si>
     <t>M5Alexa Event 1</t>
-  </si>
-  <si>
-    <t>3/9/2021</t>
   </si>
   <si>
     <t>M4tc028_VerifyBrokenImageInContactProfile</t>
@@ -2505,6 +2502,93 @@
   <si>
     <t>M3INS10</t>
   </si>
+  <si>
+    <t>TestAzAlexa Info</t>
+  </si>
+  <si>
+    <t>TestAzAlexa Deal</t>
+  </si>
+  <si>
+    <t>TOGGLESDG2</t>
+  </si>
+  <si>
+    <t>Test_Third_Party_Event1</t>
+  </si>
+  <si>
+    <t>navpeII__Marketing_Event__c</t>
+  </si>
+  <si>
+    <t>TOGGLESDG3</t>
+  </si>
+  <si>
+    <t>Test_Event_Attendee1</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Entitys Upcoming Event&lt;break&gt;Our Event Invitees</t>
+  </si>
+  <si>
+    <t>TestAzAlexa Event 1</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>M5TBC1</t>
+  </si>
+  <si>
+    <t>TestM5Alexa info</t>
+  </si>
+  <si>
+    <t>M5TBC2</t>
+  </si>
+  <si>
+    <t>M5TBC3</t>
+  </si>
+  <si>
+    <t>TBC11</t>
+  </si>
+  <si>
+    <t>TBC22</t>
+  </si>
+  <si>
+    <t>TBC33</t>
+  </si>
+  <si>
+    <t>8/17/2021</t>
+  </si>
+  <si>
+    <t>SDGField1</t>
+  </si>
+  <si>
+    <t>navpeII__Attendee_Contact__r.Name__c</t>
+  </si>
+  <si>
+    <t>SDGField2</t>
+  </si>
+  <si>
+    <t>navpeII__Attendee_Contact__r.Title</t>
+  </si>
+  <si>
+    <t>SDGField3</t>
+  </si>
+  <si>
+    <t>navpeII__Attendee_Contact__r.Email</t>
+  </si>
+  <si>
+    <t>SDGField4</t>
+  </si>
+  <si>
+    <t>SDGField5</t>
+  </si>
+  <si>
+    <t>SDGField6</t>
+  </si>
+  <si>
+    <t>navpeII__Attendee_Staff__r.MobilePhone</t>
+  </si>
 </sst>
 </file>
 
@@ -2513,7 +2597,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2589,6 +2673,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF080707"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -2654,7 +2744,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2774,6 +2864,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3113,7 +3204,7 @@
         <v>322</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3121,61 +3212,61 @@
         <v>445</v>
       </c>
       <c r="L2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>461</v>
+      </c>
+      <c r="M3" t="s">
         <v>462</v>
-      </c>
-      <c r="M3" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>573</v>
+      </c>
+      <c r="B5" s="57" t="s">
         <v>574</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="C5" s="56" t="s">
         <v>575</v>
-      </c>
-      <c r="C5" s="56" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B6" t="s">
+        <v>775</v>
+      </c>
+      <c r="D6" t="s">
         <v>776</v>
-      </c>
-      <c r="D6" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B7" t="s">
+        <v>777</v>
+      </c>
+      <c r="E7" t="s">
         <v>778</v>
-      </c>
-      <c r="E7" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B8" t="s">
         <v>312</v>
@@ -3183,7 +3274,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B9" t="s">
         <v>57</v>
@@ -3195,7 +3286,7 @@
         <v>347</v>
       </c>
       <c r="J9" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="K9" t="s">
         <v>406</v>
@@ -3203,7 +3294,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
@@ -3214,15 +3305,15 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J11" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="J12" t="s">
         <v>289</v>
@@ -3230,15 +3321,15 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
+        <v>781</v>
+      </c>
+      <c r="B13" t="s">
         <v>782</v>
-      </c>
-      <c r="B13" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -3246,13 +3337,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
+        <v>796</v>
+      </c>
+      <c r="B15" t="s">
         <v>797</v>
       </c>
-      <c r="B15" t="s">
+      <c r="F15" t="s">
         <v>798</v>
-      </c>
-      <c r="F15" t="s">
-        <v>799</v>
       </c>
       <c r="K15" t="s">
         <v>405</v>
@@ -3260,10 +3351,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
+        <v>784</v>
+      </c>
+      <c r="B16" t="s">
         <v>785</v>
-      </c>
-      <c r="B16" t="s">
-        <v>786</v>
       </c>
       <c r="K16" t="s">
         <v>405</v>
@@ -3271,13 +3362,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
+        <v>786</v>
+      </c>
+      <c r="B17" t="s">
+        <v>785</v>
+      </c>
+      <c r="D17" t="s">
         <v>787</v>
-      </c>
-      <c r="B17" t="s">
-        <v>786</v>
-      </c>
-      <c r="D17" t="s">
-        <v>788</v>
       </c>
     </row>
   </sheetData>
@@ -3295,7 +3386,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3330,7 +3421,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -3345,7 +3436,7 @@
         <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>157</v>
@@ -3362,7 +3453,7 @@
         <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>160</v>
@@ -3379,10 +3470,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3421,7 +3512,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -3456,7 +3547,7 @@
         <v>318</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>323</v>
@@ -3473,7 +3564,7 @@
         <v>343</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>323</v>
@@ -3483,7 +3574,7 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -3502,6 +3593,40 @@
       </c>
       <c r="D10" s="5" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>816</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>819</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>820</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>818</v>
       </c>
     </row>
   </sheetData>
@@ -3511,10 +3636,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3560,7 +3685,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -3572,16 +3697,16 @@
         <v>172</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>173</v>
+        <v>583</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>446</v>
+        <v>814</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>174</v>
+        <v>821</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>175</v>
+        <v>822</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>176</v>
@@ -3595,7 +3720,7 @@
         <v>178</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>457</v>
+        <v>815</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>179</v>
@@ -3615,10 +3740,10 @@
         <v>183</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>460</v>
+        <v>823</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>184</v>
+        <v>824</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>185</v>
@@ -3627,7 +3752,132 @@
         <v>186</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>825</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>826</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>821</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>822</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>827</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>828</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>830</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>831</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1" tooltip="TestM5Alexa info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000giqtpQAA/view"/>
+    <hyperlink ref="C5" r:id="rId2" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view"/>
+    <hyperlink ref="C4" r:id="rId3" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3637,7 +3887,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A5" sqref="A3:XFD5"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3678,7 +3928,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="31"/>
@@ -3707,7 +3957,7 @@
       <c r="A6" s="30"/>
       <c r="B6" s="31"/>
       <c r="C6" s="49" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="31"/>
@@ -3728,10 +3978,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B8" t="s">
         <v>469</v>
-      </c>
-      <c r="B8" t="s">
-        <v>470</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>165</v>
@@ -3742,10 +3992,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="B9" t="s">
         <v>471</v>
-      </c>
-      <c r="B9" t="s">
-        <v>472</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>165</v>
@@ -3756,10 +4006,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B10" t="s">
         <v>473</v>
-      </c>
-      <c r="B10" t="s">
-        <v>474</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>165</v>
@@ -3770,10 +4020,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="B11" t="s">
         <v>475</v>
-      </c>
-      <c r="B11" t="s">
-        <v>476</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>165</v>
@@ -3784,10 +4034,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B12" t="s">
         <v>477</v>
-      </c>
-      <c r="B12" t="s">
-        <v>478</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>165</v>
@@ -3798,10 +4048,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>165</v>
@@ -3812,10 +4062,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B14" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>165</v>
@@ -3826,10 +4076,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>165</v>
@@ -3840,10 +4090,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B16" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>165</v>
@@ -3854,10 +4104,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B17" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>165</v>
@@ -3868,10 +4118,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B18" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>165</v>
@@ -3882,10 +4132,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B19" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>165</v>
@@ -3896,10 +4146,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>165</v>
@@ -3910,10 +4160,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B21" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>165</v>
@@ -3924,10 +4174,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B22" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>165</v>
@@ -3938,10 +4188,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B23" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>165</v>
@@ -3952,10 +4202,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B24" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>165</v>
@@ -3966,10 +4216,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B25" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>165</v>
@@ -3980,10 +4230,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="B26" t="s">
         <v>526</v>
-      </c>
-      <c r="B26" t="s">
-        <v>527</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>165</v>
@@ -3994,10 +4244,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="B27" t="s">
         <v>528</v>
-      </c>
-      <c r="B27" t="s">
-        <v>529</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>165</v>
@@ -4010,7 +4260,7 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -4022,16 +4272,16 @@
         <v>164</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>460</v>
+        <v>823</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>165</v>
       </c>
       <c r="D30" t="s">
-        <v>461</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>446</v>
+        <v>832</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>814</v>
       </c>
     </row>
   </sheetData>
@@ -4076,7 +4326,7 @@
     <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -4106,7 +4356,7 @@
     <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -4132,17 +4382,17 @@
     <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C12" s="22"/>
     </row>
@@ -4245,7 +4495,7 @@
     <row r="2" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="K2" s="47"/>
       <c r="L2" s="47"/>
@@ -4259,7 +4509,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
       <c r="D3" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -4283,7 +4533,7 @@
         <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C4" t="s">
         <v>61</v>
@@ -4320,7 +4570,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
       <c r="D7" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -4384,13 +4634,13 @@
         <v>138</v>
       </c>
       <c r="F1" s="32" t="s">
+        <v>556</v>
+      </c>
+      <c r="G1" s="32" t="s">
         <v>557</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>558</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -4398,7 +4648,7 @@
       <c r="B2" s="9"/>
       <c r="C2" s="13"/>
       <c r="D2" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -4490,7 +4740,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="13"/>
       <c r="D15" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -4511,56 +4761,56 @@
     </row>
     <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
+        <v>542</v>
+      </c>
+      <c r="B16" s="50" t="s">
         <v>543</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="C16" s="50" t="s">
         <v>544</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="G16" s="50" t="s">
         <v>545</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="H16" s="50" t="s">
         <v>546</v>
-      </c>
-      <c r="H16" s="50" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="B17" s="50" t="s">
         <v>548</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="C17" s="50" t="s">
         <v>549</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="G17" s="50" t="s">
         <v>550</v>
       </c>
-      <c r="G17" s="50" t="s">
+      <c r="H17" s="50" t="s">
         <v>551</v>
-      </c>
-      <c r="H17" s="50" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
+        <v>552</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>548</v>
+      </c>
+      <c r="C18" s="50" t="s">
         <v>553</v>
       </c>
-      <c r="B18" s="50" t="s">
-        <v>549</v>
-      </c>
-      <c r="C18" s="50" t="s">
+      <c r="F18" s="50" t="s">
         <v>554</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="G18" s="50" t="s">
+        <v>545</v>
+      </c>
+      <c r="H18" s="50" t="s">
         <v>555</v>
-      </c>
-      <c r="G18" s="50" t="s">
-        <v>546</v>
-      </c>
-      <c r="H18" s="50" t="s">
-        <v>556</v>
       </c>
     </row>
   </sheetData>
@@ -4623,10 +4873,10 @@
         <v>297</v>
       </c>
       <c r="B2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D2" t="s">
         <v>298</v>
@@ -4641,10 +4891,10 @@
         <v>299</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4670,7 +4920,7 @@
         <v>299</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I3" t="s">
         <v>35</v>
@@ -4699,10 +4949,10 @@
         <v>299</v>
       </c>
       <c r="H4" s="29" t="s">
+        <v>647</v>
+      </c>
+      <c r="I4" t="s">
         <v>648</v>
-      </c>
-      <c r="I4" t="s">
-        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -4712,10 +4962,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4758,7 +5008,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -4811,7 +5061,7 @@
         <v>333</v>
       </c>
       <c r="B9" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4819,7 +5069,7 @@
         <v>334</v>
       </c>
       <c r="B10" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4846,7 +5096,7 @@
         <v>335</v>
       </c>
       <c r="B13" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4854,7 +5104,7 @@
         <v>336</v>
       </c>
       <c r="B14" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4862,7 +5112,7 @@
         <v>337</v>
       </c>
       <c r="B15" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4870,7 +5120,66 @@
         <v>338</v>
       </c>
       <c r="B16" t="s">
-        <v>756</v>
+        <v>755</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="46"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>833</v>
+      </c>
+      <c r="B19" s="61" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>835</v>
+      </c>
+      <c r="B20" s="61" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>837</v>
+      </c>
+      <c r="B21" s="61" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>839</v>
+      </c>
+      <c r="B22" s="61" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>840</v>
+      </c>
+      <c r="B23" s="61" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>841</v>
+      </c>
+      <c r="B24" s="61" t="s">
+        <v>842</v>
       </c>
     </row>
   </sheetData>
@@ -4919,7 +5228,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -5081,16 +5390,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>529</v>
+      </c>
+      <c r="B13" t="s">
         <v>530</v>
-      </c>
-      <c r="B13" t="s">
-        <v>531</v>
       </c>
       <c r="C13" t="s">
         <v>374</v>
       </c>
       <c r="D13" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -5150,10 +5459,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5170,7 +5479,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5192,36 +5501,36 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B5" t="s">
         <v>303</v>
       </c>
       <c r="C5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D5" t="s">
+        <v>653</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>654</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>655</v>
+      </c>
+      <c r="B6" t="s">
+        <v>583</v>
+      </c>
+      <c r="C6" t="s">
+        <v>645</v>
+      </c>
+      <c r="D6" t="s">
         <v>656</v>
       </c>
-      <c r="B6" t="s">
-        <v>584</v>
-      </c>
-      <c r="C6" t="s">
-        <v>646</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" s="29" t="s">
         <v>657</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>658</v>
       </c>
     </row>
   </sheetData>
@@ -5267,7 +5576,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="9"/>
@@ -5533,7 +5842,7 @@
     <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -5608,46 +5917,46 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>535</v>
+      </c>
+      <c r="B10" t="s">
         <v>536</v>
       </c>
-      <c r="B10" t="s">
-        <v>537</v>
-      </c>
       <c r="C10" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B11" t="s">
         <v>352</v>
       </c>
       <c r="C11" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>538</v>
+      </c>
+      <c r="B12" t="s">
         <v>539</v>
       </c>
-      <c r="B12" t="s">
-        <v>540</v>
-      </c>
       <c r="C12" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>540</v>
+      </c>
+      <c r="B13" t="s">
         <v>541</v>
       </c>
-      <c r="B13" t="s">
-        <v>542</v>
-      </c>
       <c r="C13" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -5679,56 +5988,56 @@
         <v>323</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>562</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>563</v>
+      </c>
+      <c r="B2" t="s">
         <v>564</v>
-      </c>
-      <c r="B2" t="s">
-        <v>565</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E2" s="56" t="s">
         <v>566</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="F2" t="s">
         <v>567</v>
-      </c>
-      <c r="F2" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>568</v>
+      </c>
+      <c r="B3" t="s">
         <v>569</v>
-      </c>
-      <c r="B3" t="s">
-        <v>570</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
   </sheetData>
@@ -5760,19 +6069,19 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>590</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>591</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>592</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>593</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>594</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -5780,22 +6089,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B2" t="s">
+        <v>788</v>
+      </c>
+      <c r="C2" t="s">
+        <v>789</v>
+      </c>
+      <c r="D2" t="s">
         <v>595</v>
       </c>
-      <c r="B2" t="s">
-        <v>789</v>
-      </c>
-      <c r="C2" t="s">
-        <v>790</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>596</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>597</v>
-      </c>
-      <c r="F2" t="s">
-        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -5830,57 +6139,57 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>599</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>600</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>601</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>384</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>602</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>603</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>138</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B2" t="s">
+        <v>790</v>
+      </c>
+      <c r="C2" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2" t="s">
         <v>605</v>
-      </c>
-      <c r="B2" t="s">
-        <v>791</v>
-      </c>
-      <c r="C2" t="s">
-        <v>792</v>
-      </c>
-      <c r="D2" t="s">
-        <v>606</v>
       </c>
       <c r="E2" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s">
+        <v>606</v>
+      </c>
+      <c r="G2" t="s">
         <v>607</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>608</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>609</v>
-      </c>
-      <c r="I2" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5893,7 +6202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMH4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -5925,25 +6234,25 @@
         <v>323</v>
       </c>
       <c r="E1" s="21" t="s">
+        <v>610</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>556</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>557</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>558</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>611</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>557</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>558</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>559</v>
-      </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>612</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>613</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>614</v>
       </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -6959,21 +7268,21 @@
     </row>
     <row r="2" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -7993,21 +8302,21 @@
     </row>
     <row r="3" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>616</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>617</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -9027,19 +9336,19 @@
     </row>
     <row r="4" spans="1:1022" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -10635,7 +10944,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B33" t="s">
         <v>188</v>
@@ -10650,7 +10959,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -10665,7 +10974,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B35" t="s">
         <v>238</v>
@@ -10684,7 +10993,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -10721,7 +11030,7 @@
   <dimension ref="A1:ALO67"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD54"/>
+      <selection activeCell="A43" sqref="A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10747,7 +11056,7 @@
         <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -12755,7 +13064,7 @@
     <row r="3" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -13764,7 +14073,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -13775,7 +14084,7 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
@@ -13786,7 +14095,7 @@
         <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C6" t="s">
         <v>62</v>
@@ -13795,7 +14104,7 @@
     <row r="8" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -13957,17 +14266,17 @@
     <row r="24" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
@@ -13975,10 +14284,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C26" t="s">
         <v>32</v>
@@ -13986,10 +14295,10 @@
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -13997,10 +14306,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C28" t="s">
         <v>76</v>
@@ -14008,74 +14317,74 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C29" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C30" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E30" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C31" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C32" t="s">
         <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C33" t="s">
         <v>62</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C34" t="s">
         <v>76</v>
@@ -14099,7 +14408,7 @@
     <row r="38" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -14129,7 +14438,7 @@
     <row r="42" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -14139,7 +14448,7 @@
         <v>143</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>446</v>
+        <v>814</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>32</v>
@@ -14163,17 +14472,17 @@
     <row r="47" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
+        <v>665</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>666</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>667</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>32</v>
@@ -14181,10 +14490,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
+        <v>667</v>
+      </c>
+      <c r="B49" s="20" t="s">
         <v>668</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>669</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>76</v>
@@ -14193,10 +14502,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="B50" t="s">
         <v>670</v>
-      </c>
-      <c r="B50" t="s">
-        <v>671</v>
       </c>
       <c r="C50" t="s">
         <v>76</v>
@@ -14204,10 +14513,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="B51" t="s">
         <v>672</v>
-      </c>
-      <c r="B51" t="s">
-        <v>673</v>
       </c>
       <c r="C51" t="s">
         <v>76</v>
@@ -14215,10 +14524,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
+        <v>673</v>
+      </c>
+      <c r="B52" t="s">
         <v>674</v>
-      </c>
-      <c r="B52" t="s">
-        <v>675</v>
       </c>
       <c r="C52" t="s">
         <v>76</v>
@@ -14226,10 +14535,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="B53" t="s">
         <v>676</v>
-      </c>
-      <c r="B53" t="s">
-        <v>677</v>
       </c>
       <c r="C53" t="s">
         <v>76</v>
@@ -14237,10 +14546,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="B54" t="s">
         <v>678</v>
-      </c>
-      <c r="B54" t="s">
-        <v>679</v>
       </c>
       <c r="C54" t="s">
         <v>76</v>
@@ -14248,10 +14557,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
+        <v>679</v>
+      </c>
+      <c r="B55" t="s">
         <v>680</v>
-      </c>
-      <c r="B55" t="s">
-        <v>681</v>
       </c>
       <c r="C55" t="s">
         <v>76</v>
@@ -14259,10 +14568,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
+        <v>681</v>
+      </c>
+      <c r="B56" t="s">
         <v>682</v>
-      </c>
-      <c r="B56" t="s">
-        <v>683</v>
       </c>
       <c r="C56" t="s">
         <v>76</v>
@@ -14270,10 +14579,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="B57" t="s">
         <v>684</v>
-      </c>
-      <c r="B57" t="s">
-        <v>685</v>
       </c>
       <c r="C57" t="s">
         <v>76</v>
@@ -14281,10 +14590,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
+        <v>685</v>
+      </c>
+      <c r="B58" t="s">
         <v>686</v>
-      </c>
-      <c r="B58" t="s">
-        <v>687</v>
       </c>
       <c r="C58" t="s">
         <v>76</v>
@@ -14292,10 +14601,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
+        <v>687</v>
+      </c>
+      <c r="B59" t="s">
         <v>688</v>
-      </c>
-      <c r="B59" t="s">
-        <v>689</v>
       </c>
       <c r="C59" t="s">
         <v>356</v>
@@ -14303,43 +14612,43 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
+        <v>689</v>
+      </c>
+      <c r="B60" t="s">
         <v>690</v>
       </c>
-      <c r="B60" t="s">
-        <v>691</v>
-      </c>
       <c r="C60" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
+        <v>691</v>
+      </c>
+      <c r="B61" t="s">
         <v>692</v>
       </c>
-      <c r="B61" t="s">
-        <v>693</v>
-      </c>
       <c r="C61" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
+        <v>693</v>
+      </c>
+      <c r="B62" t="s">
         <v>694</v>
       </c>
-      <c r="B62" t="s">
-        <v>695</v>
-      </c>
       <c r="C62" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
+        <v>695</v>
+      </c>
+      <c r="B63" t="s">
         <v>696</v>
-      </c>
-      <c r="B63" t="s">
-        <v>697</v>
       </c>
       <c r="C63" t="s">
         <v>289</v>
@@ -14347,10 +14656,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
+        <v>697</v>
+      </c>
+      <c r="B64" t="s">
         <v>698</v>
-      </c>
-      <c r="B64" t="s">
-        <v>699</v>
       </c>
       <c r="C64" t="s">
         <v>62</v>
@@ -14358,21 +14667,21 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
+        <v>699</v>
+      </c>
+      <c r="B65" t="s">
         <v>700</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>701</v>
-      </c>
-      <c r="C65" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
+        <v>702</v>
+      </c>
+      <c r="B66" t="s">
         <v>703</v>
-      </c>
-      <c r="B66" t="s">
-        <v>704</v>
       </c>
       <c r="C66" t="s">
         <v>76</v>
@@ -14380,10 +14689,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
+        <v>704</v>
+      </c>
+      <c r="B67" t="s">
         <v>705</v>
-      </c>
-      <c r="B67" t="s">
-        <v>706</v>
       </c>
       <c r="C67" t="s">
         <v>76</v>
@@ -14438,7 +14747,7 @@
         <v>324</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>435</v>
@@ -16452,7 +16761,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -17466,13 +17775,13 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>26</v>
@@ -17485,7 +17794,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
@@ -17635,7 +17944,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="7"/>
@@ -17647,52 +17956,52 @@
     </row>
     <row r="18" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B18" s="50" t="s">
+        <v>627</v>
+      </c>
+      <c r="C18" s="50" t="s">
         <v>628</v>
       </c>
-      <c r="C18" s="50" t="s">
-        <v>629</v>
-      </c>
       <c r="D18" s="50" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B19" s="50" t="s">
+        <v>624</v>
+      </c>
+      <c r="C19" s="50" t="s">
         <v>625</v>
-      </c>
-      <c r="C19" s="50" t="s">
-        <v>626</v>
       </c>
       <c r="E19" s="54"/>
     </row>
     <row r="20" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
+        <v>801</v>
+      </c>
+      <c r="B20" s="50" t="s">
         <v>802</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="C20" s="50" t="s">
         <v>803</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>804</v>
       </c>
       <c r="E20" s="54"/>
     </row>
     <row r="21" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
+        <v>809</v>
+      </c>
+      <c r="B21" s="50" t="s">
         <v>810</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="C21" s="50" t="s">
         <v>811</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>812</v>
       </c>
       <c r="E21" s="54"/>
     </row>
@@ -17703,7 +18012,7 @@
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="7"/>
@@ -17909,13 +18218,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>465</v>
+      </c>
+      <c r="B31" t="s">
         <v>466</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>467</v>
-      </c>
-      <c r="C31" t="s">
-        <v>468</v>
       </c>
       <c r="D31" t="s">
         <v>349</v>
@@ -17940,7 +18249,7 @@
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="7"/>
@@ -17952,30 +18261,30 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>757</v>
+      </c>
+      <c r="B36" t="s">
         <v>758</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>759</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" s="60" t="s">
         <v>760</v>
-      </c>
-      <c r="E36" s="60" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>761</v>
+      </c>
+      <c r="B37" t="s">
         <v>762</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>763</v>
       </c>
-      <c r="C37" t="s">
+      <c r="E37" s="60" t="s">
         <v>764</v>
-      </c>
-      <c r="E37" s="60" t="s">
-        <v>765</v>
       </c>
     </row>
   </sheetData>
@@ -18007,7 +18316,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>14</v>
@@ -18022,7 +18331,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -18034,10 +18343,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -18117,7 +18426,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -18131,7 +18440,7 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D4" t="s">
         <v>57</v>
@@ -18145,7 +18454,7 @@
         <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D5" t="s">
         <v>57</v>
@@ -18164,7 +18473,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
@@ -18175,10 +18484,10 @@
     </row>
     <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>57</v>
@@ -18192,7 +18501,7 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
@@ -18238,8 +18547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18275,7 +18584,7 @@
         <v>14</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -20328,7 +20637,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -21359,19 +21668,19 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E4" t="s">
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:1026" x14ac:dyDescent="0.25">
@@ -21385,7 +21694,7 @@
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="6" spans="1:1026" x14ac:dyDescent="0.25">
@@ -21399,14 +21708,14 @@
         <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="8" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -21518,10 +21827,10 @@
     </row>
     <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>586</v>
+      </c>
+      <c r="B14" t="s">
         <v>587</v>
-      </c>
-      <c r="B14" t="s">
-        <v>588</v>
       </c>
       <c r="C14" t="s">
         <v>259</v>
@@ -21540,7 +21849,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -21565,7 +21874,7 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -21576,8 +21885,8 @@
       <c r="A19" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="50" t="s">
-        <v>457</v>
+      <c r="B19" s="20" t="s">
+        <v>815</v>
       </c>
       <c r="D19" s="50" t="s">
         <v>30</v>
@@ -21587,7 +21896,7 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -21596,13 +21905,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>707</v>
+      </c>
+      <c r="B23" t="s">
         <v>708</v>
       </c>
-      <c r="B23" t="s">
-        <v>709</v>
-      </c>
       <c r="C23" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D23" t="s">
         <v>266</v>
@@ -21610,13 +21919,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>709</v>
+      </c>
+      <c r="B24" t="s">
         <v>710</v>
       </c>
-      <c r="B24" t="s">
-        <v>711</v>
-      </c>
       <c r="C24" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D24" t="s">
         <v>30</v>
@@ -21627,41 +21936,41 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>711</v>
+      </c>
+      <c r="B25" t="s">
         <v>712</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>668</v>
+      </c>
+      <c r="D25" t="s">
         <v>713</v>
-      </c>
-      <c r="C25" t="s">
-        <v>669</v>
-      </c>
-      <c r="D25" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>714</v>
+      </c>
+      <c r="B26" t="s">
         <v>715</v>
       </c>
-      <c r="B26" t="s">
-        <v>716</v>
-      </c>
       <c r="C26" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D26" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>716</v>
+      </c>
+      <c r="B27" t="s">
         <v>717</v>
       </c>
-      <c r="B27" t="s">
-        <v>718</v>
-      </c>
       <c r="C27" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D27" t="s">
         <v>266</v>
@@ -21669,41 +21978,41 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>718</v>
+      </c>
+      <c r="B28" t="s">
         <v>719</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>676</v>
+      </c>
+      <c r="D28" t="s">
         <v>720</v>
-      </c>
-      <c r="C28" t="s">
-        <v>677</v>
-      </c>
-      <c r="D28" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>721</v>
+      </c>
+      <c r="B29" t="s">
         <v>722</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>678</v>
+      </c>
+      <c r="D29" t="s">
         <v>723</v>
-      </c>
-      <c r="C29" t="s">
-        <v>679</v>
-      </c>
-      <c r="D29" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>724</v>
+      </c>
+      <c r="B30" t="s">
         <v>725</v>
       </c>
-      <c r="B30" t="s">
-        <v>726</v>
-      </c>
       <c r="C30" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D30" t="s">
         <v>266</v>
@@ -21711,13 +22020,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>726</v>
+      </c>
+      <c r="B31" t="s">
         <v>727</v>
       </c>
-      <c r="B31" t="s">
-        <v>728</v>
-      </c>
       <c r="C31" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D31" t="s">
         <v>266</v>
@@ -21725,13 +22034,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>728</v>
+      </c>
+      <c r="B32" t="s">
         <v>729</v>
       </c>
-      <c r="B32" t="s">
-        <v>730</v>
-      </c>
       <c r="C32" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D32" t="s">
         <v>266</v>
@@ -21739,13 +22048,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>730</v>
+      </c>
+      <c r="B33" t="s">
         <v>731</v>
       </c>
-      <c r="B33" t="s">
-        <v>732</v>
-      </c>
       <c r="C33" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D33" t="s">
         <v>266</v>
@@ -21753,13 +22062,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>732</v>
+      </c>
+      <c r="B34" t="s">
         <v>733</v>
       </c>
-      <c r="B34" t="s">
-        <v>734</v>
-      </c>
       <c r="C34" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D34" t="s">
         <v>266</v>
@@ -21767,13 +22076,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>734</v>
+      </c>
+      <c r="B35" t="s">
         <v>735</v>
       </c>
-      <c r="B35" t="s">
-        <v>736</v>
-      </c>
       <c r="C35" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D35" t="s">
         <v>266</v>
@@ -21781,13 +22090,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>736</v>
+      </c>
+      <c r="B36" t="s">
         <v>737</v>
       </c>
-      <c r="B36" t="s">
-        <v>738</v>
-      </c>
       <c r="C36" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D36" t="s">
         <v>266</v>
@@ -21795,13 +22104,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>738</v>
+      </c>
+      <c r="B37" t="s">
         <v>739</v>
       </c>
-      <c r="B37" t="s">
-        <v>740</v>
-      </c>
       <c r="C37" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D37" t="s">
         <v>266</v>
@@ -21809,13 +22118,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>740</v>
+      </c>
+      <c r="B38" t="s">
         <v>741</v>
       </c>
-      <c r="B38" t="s">
-        <v>742</v>
-      </c>
       <c r="C38" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D38" t="s">
         <v>266</v>
@@ -21823,13 +22132,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>742</v>
+      </c>
+      <c r="B39" t="s">
         <v>743</v>
       </c>
-      <c r="B39" t="s">
-        <v>744</v>
-      </c>
       <c r="C39" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D39" t="s">
         <v>266</v>
@@ -21837,13 +22146,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>744</v>
+      </c>
+      <c r="B40" t="s">
         <v>745</v>
       </c>
-      <c r="B40" t="s">
-        <v>746</v>
-      </c>
       <c r="C40" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D40" t="s">
         <v>266</v>
@@ -21851,13 +22160,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>746</v>
+      </c>
+      <c r="B41" t="s">
         <v>747</v>
       </c>
-      <c r="B41" t="s">
-        <v>748</v>
-      </c>
       <c r="C41" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D41" t="s">
         <v>266</v>
@@ -21865,26 +22174,26 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>793</v>
+      </c>
+      <c r="B42" t="s">
         <v>794</v>
       </c>
-      <c r="B42" t="s">
-        <v>795</v>
-      </c>
       <c r="C42" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D42" t="s">
         <v>30</v>
       </c>
       <c r="F42" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -21893,30 +22202,30 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>766</v>
+      </c>
+      <c r="B45" t="s">
         <v>767</v>
-      </c>
-      <c r="B45" t="s">
-        <v>768</v>
       </c>
       <c r="C45" t="s">
         <v>47</v>
       </c>
       <c r="D45" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>768</v>
+      </c>
+      <c r="B46" t="s">
         <v>769</v>
-      </c>
-      <c r="B46" t="s">
-        <v>770</v>
       </c>
       <c r="C46" t="s">
         <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
   </sheetData>
@@ -21947,7 +22256,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>12</v>
@@ -21958,25 +22267,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>771</v>
+      </c>
+      <c r="B2" t="s">
         <v>772</v>
-      </c>
-      <c r="B2" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>773</v>
+      </c>
+      <c r="B3" t="s">
         <v>774</v>
-      </c>
-      <c r="B3" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -21985,10 +22294,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B6" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel update for module 6
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" firstSheet="15" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="857">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2588,6 +2588,48 @@
   </si>
   <si>
     <t>navpeII__Attendee_Staff__r.MobilePhone</t>
+  </si>
+  <si>
+    <t>Test Company 18</t>
+  </si>
+  <si>
+    <t>Test Company 19</t>
+  </si>
+  <si>
+    <t>M6INS21</t>
+  </si>
+  <si>
+    <t>M6INS22</t>
+  </si>
+  <si>
+    <t>M6Deal21</t>
+  </si>
+  <si>
+    <t>M6Deal22</t>
+  </si>
+  <si>
+    <t>Test Deal 18</t>
+  </si>
+  <si>
+    <t>Test Deal 19</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>M6LSCFINS1</t>
+  </si>
+  <si>
+    <t>M6LSCFFUND1</t>
+  </si>
+  <si>
+    <t>Extreme FUND</t>
+  </si>
+  <si>
+    <t>M6LSCFUNDR1</t>
+  </si>
+  <si>
+    <t>Reliance JIO Fundraise</t>
   </si>
 </sst>
 </file>
@@ -4964,7 +5006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -11027,10 +11069,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALO67"/>
+  <dimension ref="A1:ALO71"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14696,6 +14738,39 @@
       </c>
       <c r="C67" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
+        <v>845</v>
+      </c>
+      <c r="B68" t="s">
+        <v>843</v>
+      </c>
+      <c r="C68" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="20" t="s">
+        <v>846</v>
+      </c>
+      <c r="B69" t="s">
+        <v>844</v>
+      </c>
+      <c r="C69" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>852</v>
+      </c>
+      <c r="B71" t="s">
+        <v>623</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -18357,10 +18432,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18538,6 +18613,34 @@
         <v>90</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>853</v>
+      </c>
+      <c r="B17" t="s">
+        <v>854</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18545,10 +18648,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML46"/>
+  <dimension ref="A1:AML48"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22189,42 +22292,76 @@
         <v>696</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>847</v>
+      </c>
+      <c r="B43" t="s">
+        <v>849</v>
+      </c>
+      <c r="C43" t="s">
+        <v>843</v>
+      </c>
+      <c r="D43" t="s">
+        <v>266</v>
+      </c>
+      <c r="G43" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>848</v>
+      </c>
+      <c r="B44" t="s">
+        <v>850</v>
+      </c>
+      <c r="C44" t="s">
+        <v>844</v>
+      </c>
+      <c r="D44" t="s">
+        <v>266</v>
+      </c>
+      <c r="G44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4" t="s">
         <v>765</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>766</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>767</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>47</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>768</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
         <v>769</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C48" t="s">
         <v>47</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>579</v>
       </c>
     </row>
@@ -22237,10 +22374,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22300,6 +22437,29 @@
         <v>807</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>855</v>
+      </c>
+      <c r="B9" t="s">
+        <v>856</v>
+      </c>
+      <c r="C9" t="s">
+        <v>623</v>
+      </c>
+      <c r="D9" t="s">
+        <v>854</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Excel for Module 5 TC010-015
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="861">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2630,6 +2630,18 @@
   </si>
   <si>
     <t>Reliance JIO Fundraise</t>
+  </si>
+  <si>
+    <t>TOGGLESDG4</t>
+  </si>
+  <si>
+    <t>Pipeline @#$%^&amp;*@ Custom</t>
+  </si>
+  <si>
+    <t>TOGGLESDG5</t>
+  </si>
+  <si>
+    <t>Portfolio @#$%^&amp;*@ Deal</t>
   </si>
 </sst>
 </file>
@@ -3512,10 +3524,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,6 +3683,34 @@
         <v>818</v>
       </c>
     </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>857</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>859</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3681,7 +3721,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22376,7 +22416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Excel For Module 3
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C55E9D5-DBAC-4CD1-9B5F-092E87E3B696}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="19" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="942">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1576,9 +1575,6 @@
     <t>M3FUND1</t>
   </si>
   <si>
-    <t>M3TestCst Record1</t>
-  </si>
-  <si>
     <t>M3CSTOBJ</t>
   </si>
   <si>
@@ -1678,9 +1674,6 @@
     <t>In Progress</t>
   </si>
   <si>
-    <t>Multitagged Task 1</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -1688,9 +1681,6 @@
   </si>
   <si>
     <t>M3Task3</t>
-  </si>
-  <si>
-    <t>New Meeting 1</t>
   </si>
   <si>
     <t>Monday Morning Meeting</t>
@@ -1884,21 +1874,12 @@
     <t>Updated_Priority</t>
   </si>
   <si>
-    <t>New Interactions- Call</t>
-  </si>
-  <si>
     <t>Not Started</t>
   </si>
   <si>
-    <t>New Interactions- Meeting</t>
-  </si>
-  <si>
     <t>Board Meeting</t>
   </si>
   <si>
-    <t>New Interactions- Task</t>
-  </si>
-  <si>
     <t>M3CALL1</t>
   </si>
   <si>
@@ -1914,18 +1895,12 @@
     <t>Reliance Group</t>
   </si>
   <si>
-    <t>Mukesh</t>
-  </si>
-  <si>
     <t>Ambani</t>
   </si>
   <si>
     <t>M3CON2</t>
   </si>
   <si>
-    <t>Aman</t>
-  </si>
-  <si>
     <t>Kumar</t>
   </si>
   <si>
@@ -2400,24 +2375,9 @@
     <t>Custom Label</t>
   </si>
   <si>
-    <t>M3Tc034_VerifyTheFunctionalityByrenamingAndDeletingandRemovingUtilityItemCustomLabelintheCustomnavigationMenu</t>
-  </si>
-  <si>
     <t>Custom Label New</t>
   </si>
   <si>
-    <t>CustomReportFolder69795</t>
-  </si>
-  <si>
-    <t>CustomReport73415</t>
-  </si>
-  <si>
-    <t>PETestEmailFolder70193</t>
-  </si>
-  <si>
-    <t>PETestCustomEmailTemplate9823</t>
-  </si>
-  <si>
     <t>08/11/2021</t>
   </si>
   <si>
@@ -2439,40 +2399,25 @@
     <t>Parent_Account1&lt;break&gt;Parent_Account2</t>
   </si>
   <si>
-    <t>TestReliance Fund</t>
-  </si>
-  <si>
     <t>Aman Institute</t>
   </si>
   <si>
     <t>M3CON3</t>
   </si>
   <si>
-    <t>Don</t>
-  </si>
-  <si>
     <t>Ton</t>
   </si>
   <si>
     <t>Reliance Digital</t>
   </si>
   <si>
-    <t>Reliance Partner</t>
-  </si>
-  <si>
     <t>M3PS1</t>
   </si>
   <si>
-    <t>Relaince Fundraising</t>
-  </si>
-  <si>
     <t>M3FR1</t>
   </si>
   <si>
     <t>M3CON4</t>
-  </si>
-  <si>
-    <t>Satty</t>
   </si>
   <si>
     <t>Nade</t>
@@ -2884,12 +2829,75 @@
   </si>
   <si>
     <t>Einstein Events Testing 10</t>
+  </si>
+  <si>
+    <t>M3Tc034_1_VerifyTheFunctionalityByrenamingAndDeletingandRemovingUtilityItemCustomLabelintheCustomnavigationMenu</t>
+  </si>
+  <si>
+    <t>AATestAman</t>
+  </si>
+  <si>
+    <t>navatariptesting+15638@gmail.com</t>
+  </si>
+  <si>
+    <t>TestMukesh</t>
+  </si>
+  <si>
+    <t>navatariptesting+8709@gmail.com</t>
+  </si>
+  <si>
+    <t>TestDon</t>
+  </si>
+  <si>
+    <t>TestSatty</t>
+  </si>
+  <si>
+    <t>TestCst Record1</t>
+  </si>
+  <si>
+    <t>TestRelianced Fund</t>
+  </si>
+  <si>
+    <t>TestRelaince Fundraising</t>
+  </si>
+  <si>
+    <t>TestReliance Partner</t>
+  </si>
+  <si>
+    <t>TestCall</t>
+  </si>
+  <si>
+    <t>TestMultitagged Task 1</t>
+  </si>
+  <si>
+    <t>TestNew Meeting 1</t>
+  </si>
+  <si>
+    <t>CustomReportFolder</t>
+  </si>
+  <si>
+    <t>CustomReport</t>
+  </si>
+  <si>
+    <t>PETestEmailFolder</t>
+  </si>
+  <si>
+    <t>PETestCustomEmailTemplate</t>
+  </si>
+  <si>
+    <t>TestNew Interactions- Call</t>
+  </si>
+  <si>
+    <t>TestNew Interactions- Meeting</t>
+  </si>
+  <si>
+    <t>TestNew Interactions- Task</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -3165,7 +3173,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3442,11 +3450,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A6" sqref="A6:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3521,48 +3529,48 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B4" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="B6" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="D6" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>652</v>
+        <v>644</v>
       </c>
       <c r="B7" t="s">
-        <v>770</v>
+        <v>762</v>
       </c>
       <c r="E7" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>653</v>
+        <v>645</v>
       </c>
       <c r="B8" t="s">
         <v>308</v>
@@ -3570,7 +3578,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>654</v>
+        <v>646</v>
       </c>
       <c r="B9" t="s">
         <v>57</v>
@@ -3582,7 +3590,7 @@
         <v>343</v>
       </c>
       <c r="J9" t="s">
-        <v>772</v>
+        <v>764</v>
       </c>
       <c r="K9" t="s">
         <v>402</v>
@@ -3590,7 +3598,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>655</v>
+        <v>647</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
@@ -3601,15 +3609,15 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>656</v>
+        <v>648</v>
       </c>
       <c r="J11" t="s">
-        <v>788</v>
+        <v>775</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="J12" t="s">
         <v>285</v>
@@ -3617,15 +3625,15 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>774</v>
+        <v>766</v>
       </c>
       <c r="B13" t="s">
-        <v>775</v>
+        <v>767</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -3633,13 +3641,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>789</v>
+        <v>776</v>
       </c>
       <c r="B15" t="s">
-        <v>790</v>
+        <v>777</v>
       </c>
       <c r="F15" t="s">
-        <v>791</v>
+        <v>778</v>
       </c>
       <c r="K15" t="s">
         <v>401</v>
@@ -3647,10 +3655,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>777</v>
+        <v>769</v>
       </c>
       <c r="B16" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="K16" t="s">
         <v>401</v>
@@ -3658,19 +3666,19 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>779</v>
+        <v>921</v>
       </c>
       <c r="B17" t="s">
-        <v>778</v>
+        <v>770</v>
       </c>
       <c r="D17" t="s">
-        <v>780</v>
+        <v>771</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -3678,7 +3686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3717,7 +3725,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -3732,7 +3740,7 @@
         <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>157</v>
@@ -3749,7 +3757,7 @@
         <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>160</v>
@@ -3765,11 +3773,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3808,7 +3816,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -3843,7 +3851,7 @@
         <v>314</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>319</v>
@@ -3860,7 +3868,7 @@
         <v>339</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>319</v>
@@ -3870,7 +3878,7 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -3893,47 +3901,47 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>808</v>
+        <v>790</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>809</v>
+        <v>791</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>809</v>
+        <v>791</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>810</v>
+        <v>792</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>811</v>
+        <v>793</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>812</v>
+        <v>794</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>812</v>
+        <v>794</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>810</v>
+        <v>792</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>840</v>
+        <v>822</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>841</v>
+        <v>823</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>841</v>
+        <v>823</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>151</v>
@@ -3941,13 +3949,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>842</v>
+        <v>824</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>151</v>
@@ -3959,7 +3967,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4009,7 +4017,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -4021,16 +4029,16 @@
         <v>172</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>846</v>
+        <v>828</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>813</v>
+        <v>795</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>814</v>
+        <v>796</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>173</v>
@@ -4044,7 +4052,7 @@
         <v>175</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>176</v>
@@ -4064,10 +4072,10 @@
         <v>180</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>849</v>
+        <v>831</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>815</v>
+        <v>797</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>181</v>
@@ -4078,15 +4086,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view"/>
+    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -4131,7 +4139,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="31"/>
@@ -4160,7 +4168,7 @@
       <c r="A6" s="30"/>
       <c r="B6" s="31"/>
       <c r="C6" s="49" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="31"/>
@@ -4433,10 +4441,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="B26" t="s">
         <v>518</v>
-      </c>
-      <c r="B26" t="s">
-        <v>519</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>165</v>
@@ -4447,10 +4455,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="B27" t="s">
         <v>520</v>
-      </c>
-      <c r="B27" t="s">
-        <v>521</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>165</v>
@@ -4463,7 +4471,7 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -4475,16 +4483,16 @@
         <v>164</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>849</v>
+        <v>831</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>165</v>
       </c>
       <c r="D30" t="s">
-        <v>851</v>
+        <v>833</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>846</v>
+        <v>828</v>
       </c>
     </row>
   </sheetData>
@@ -4494,11 +4502,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4529,7 +4537,7 @@
     <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -4559,7 +4567,7 @@
     <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -4585,17 +4593,17 @@
     <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>799</v>
+        <v>783</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>798</v>
+        <v>931</v>
       </c>
       <c r="C12" s="22"/>
     </row>
@@ -4605,7 +4613,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4698,7 +4706,7 @@
     <row r="2" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="K2" s="47"/>
       <c r="L2" s="47"/>
@@ -4712,7 +4720,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
       <c r="D3" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -4736,7 +4744,7 @@
         <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C4" t="s">
         <v>61</v>
@@ -4773,7 +4781,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
       <c r="D7" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -4812,11 +4820,11 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A15" sqref="A15:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4837,13 +4845,13 @@
         <v>138</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
@@ -4851,7 +4859,7 @@
       <c r="B2" s="9"/>
       <c r="C2" s="13"/>
       <c r="D2" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -4943,7 +4951,7 @@
       <c r="B15" s="9"/>
       <c r="C15" s="13"/>
       <c r="D15" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
@@ -4964,56 +4972,56 @@
     </row>
     <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="B16" s="50" t="s">
         <v>535</v>
       </c>
-      <c r="B16" s="50" t="s">
-        <v>536</v>
-      </c>
       <c r="C16" s="50" t="s">
+        <v>932</v>
+      </c>
+      <c r="G16" s="50" t="s">
         <v>537</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="H16" s="50" t="s">
         <v>538</v>
-      </c>
-      <c r="H16" s="50" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
+        <v>539</v>
+      </c>
+      <c r="B17" s="50" t="s">
         <v>540</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="C17" s="50" t="s">
+        <v>933</v>
+      </c>
+      <c r="G17" s="50" t="s">
         <v>541</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="H17" s="50" t="s">
         <v>542</v>
-      </c>
-      <c r="G17" s="50" t="s">
-        <v>543</v>
-      </c>
-      <c r="H17" s="50" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
+        <v>543</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>540</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>934</v>
+      </c>
+      <c r="F18" s="50" t="s">
+        <v>544</v>
+      </c>
+      <c r="G18" s="50" t="s">
+        <v>537</v>
+      </c>
+      <c r="H18" s="50" t="s">
         <v>545</v>
-      </c>
-      <c r="B18" s="50" t="s">
-        <v>541</v>
-      </c>
-      <c r="C18" s="50" t="s">
-        <v>546</v>
-      </c>
-      <c r="F18" s="50" t="s">
-        <v>547</v>
-      </c>
-      <c r="G18" s="50" t="s">
-        <v>538</v>
-      </c>
-      <c r="H18" s="50" t="s">
-        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -5022,7 +5030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5076,7 +5084,7 @@
         <v>293</v>
       </c>
       <c r="B2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="C2" t="s">
         <v>498</v>
@@ -5094,10 +5102,10 @@
         <v>295</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="I2" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5123,7 +5131,7 @@
         <v>295</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="I3" t="s">
         <v>35</v>
@@ -5152,10 +5160,10 @@
         <v>295</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="I4" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -5164,10 +5172,10 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -5211,7 +5219,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -5264,7 +5272,7 @@
         <v>329</v>
       </c>
       <c r="B9" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5272,7 +5280,7 @@
         <v>330</v>
       </c>
       <c r="B10" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5299,7 +5307,7 @@
         <v>331</v>
       </c>
       <c r="B13" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5307,7 +5315,7 @@
         <v>332</v>
       </c>
       <c r="B14" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5315,7 +5323,7 @@
         <v>333</v>
       </c>
       <c r="B15" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5323,13 +5331,13 @@
         <v>334</v>
       </c>
       <c r="B16" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="9"/>
@@ -5339,50 +5347,50 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>816</v>
+        <v>798</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>817</v>
+        <v>799</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>818</v>
+        <v>800</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>819</v>
+        <v>801</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>820</v>
+        <v>802</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>821</v>
+        <v>803</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>822</v>
+        <v>804</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>823</v>
+        <v>805</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>824</v>
+        <v>806</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>825</v>
+        <v>807</v>
       </c>
     </row>
   </sheetData>
@@ -5391,7 +5399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5431,7 +5439,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -5593,10 +5601,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>521</v>
+      </c>
+      <c r="B13" t="s">
         <v>522</v>
-      </c>
-      <c r="B13" t="s">
-        <v>523</v>
       </c>
       <c r="C13" t="s">
         <v>370</v>
@@ -5611,7 +5619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -5662,10 +5670,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>570</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5682,7 +5690,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5704,36 +5712,36 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="B5" t="s">
         <v>299</v>
       </c>
       <c r="C5" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="D5" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
       <c r="B6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="C6" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="D6" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -5743,7 +5751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5779,7 +5787,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="9"/>
@@ -6012,7 +6020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6045,7 +6053,7 @@
     <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -6120,46 +6128,46 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>527</v>
+      </c>
+      <c r="B10" t="s">
         <v>528</v>
       </c>
-      <c r="B10" t="s">
-        <v>529</v>
-      </c>
       <c r="C10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B11" t="s">
         <v>348</v>
       </c>
       <c r="C11" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>530</v>
+      </c>
+      <c r="B12" t="s">
         <v>531</v>
       </c>
-      <c r="B12" t="s">
-        <v>532</v>
-      </c>
       <c r="C12" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>532</v>
+      </c>
+      <c r="B13" t="s">
         <v>533</v>
       </c>
-      <c r="B13" t="s">
-        <v>534</v>
-      </c>
       <c r="C13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -6168,7 +6176,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6191,56 +6199,56 @@
         <v>319</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>552</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>554</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E2" s="56" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="F2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B3" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E3" s="56" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="F3" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -6249,11 +6257,11 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6272,19 +6280,19 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>582</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>583</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>584</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>585</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>586</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -6292,22 +6300,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B2" t="s">
+        <v>935</v>
+      </c>
+      <c r="C2" t="s">
+        <v>936</v>
+      </c>
+      <c r="D2" t="s">
+        <v>585</v>
+      </c>
+      <c r="E2" t="s">
+        <v>586</v>
+      </c>
+      <c r="F2" t="s">
         <v>587</v>
-      </c>
-      <c r="B2" t="s">
-        <v>781</v>
-      </c>
-      <c r="C2" t="s">
-        <v>782</v>
-      </c>
-      <c r="D2" t="s">
-        <v>588</v>
-      </c>
-      <c r="E2" t="s">
-        <v>589</v>
-      </c>
-      <c r="F2" t="s">
-        <v>590</v>
       </c>
     </row>
   </sheetData>
@@ -6317,11 +6325,11 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6342,57 +6350,57 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>380</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>138</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="B2" t="s">
-        <v>783</v>
+        <v>937</v>
       </c>
       <c r="C2" t="s">
-        <v>784</v>
+        <v>938</v>
       </c>
       <c r="D2" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E2" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s">
+        <v>596</v>
+      </c>
+      <c r="G2" t="s">
+        <v>597</v>
+      </c>
+      <c r="H2" t="s">
+        <v>598</v>
+      </c>
+      <c r="I2" t="s">
         <v>599</v>
-      </c>
-      <c r="G2" t="s">
-        <v>600</v>
-      </c>
-      <c r="H2" t="s">
-        <v>601</v>
-      </c>
-      <c r="I2" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6402,11 +6410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6439,31 +6447,31 @@
         <v>319</v>
       </c>
       <c r="E1" s="21" t="s">
+        <v>600</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>845</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>846</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>547</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>546</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>548</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>601</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>602</v>
+      </c>
+      <c r="M1" s="21" t="s">
         <v>603</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>863</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>864</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>550</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>549</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>551</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>604</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>605</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>606</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -7479,22 +7487,22 @@
     </row>
     <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>607</v>
+        <v>939</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" t="s">
-        <v>785</v>
+        <v>772</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -8515,23 +8523,23 @@
     </row>
     <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>609</v>
+        <v>940</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -9551,20 +9559,20 @@
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>611</v>
+        <v>941</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -10585,147 +10593,147 @@
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>865</v>
+        <v>847</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>866</v>
+        <v>848</v>
       </c>
       <c r="E5" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>868</v>
+        <v>850</v>
       </c>
       <c r="G5" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>870</v>
+        <v>852</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>871</v>
+        <v>853</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>872</v>
+        <v>854</v>
       </c>
       <c r="E6" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>873</v>
+        <v>855</v>
       </c>
       <c r="G6" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>874</v>
+        <v>856</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>875</v>
+        <v>857</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>876</v>
+        <v>858</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>877</v>
+        <v>859</v>
       </c>
       <c r="E7" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>878</v>
+        <v>860</v>
       </c>
       <c r="G7" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>879</v>
+        <v>861</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>880</v>
+        <v>862</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>881</v>
+        <v>863</v>
       </c>
       <c r="E8" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>882</v>
+        <v>864</v>
       </c>
       <c r="G8" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>883</v>
+        <v>865</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>884</v>
+        <v>866</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>885</v>
+        <v>867</v>
       </c>
       <c r="E9" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>886</v>
+        <v>868</v>
       </c>
       <c r="G9" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>887</v>
+        <v>869</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>875</v>
+        <v>857</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>888</v>
+        <v>870</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>889</v>
+        <v>871</v>
       </c>
       <c r="E10" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>890</v>
+        <v>872</v>
       </c>
       <c r="G10" t="s">
         <v>369</v>
@@ -10735,22 +10743,22 @@
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>891</v>
+        <v>873</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>892</v>
+        <v>874</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>893</v>
+        <v>875</v>
       </c>
       <c r="E11" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>894</v>
+        <v>876</v>
       </c>
       <c r="G11" t="s">
         <v>369</v>
@@ -10760,22 +10768,22 @@
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>895</v>
+        <v>877</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>896</v>
+        <v>878</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>897</v>
+        <v>879</v>
       </c>
       <c r="E12" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>898</v>
+        <v>880</v>
       </c>
       <c r="G12" t="s">
         <v>369</v>
@@ -10785,22 +10793,22 @@
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>899</v>
+        <v>881</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>875</v>
+        <v>857</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>900</v>
+        <v>882</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>901</v>
+        <v>883</v>
       </c>
       <c r="E13" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>902</v>
+        <v>884</v>
       </c>
       <c r="G13" t="s">
         <v>369</v>
@@ -10810,22 +10818,22 @@
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>903</v>
+        <v>885</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>904</v>
+        <v>886</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>905</v>
+        <v>887</v>
       </c>
       <c r="E14" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>906</v>
+        <v>888</v>
       </c>
       <c r="G14" t="s">
         <v>369</v>
@@ -10835,100 +10843,100 @@
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>907</v>
+        <v>889</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>908</v>
+        <v>890</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>885</v>
+        <v>867</v>
       </c>
       <c r="E15" t="s">
+        <v>833</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>876</v>
+      </c>
+      <c r="G15" t="s">
         <v>851</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>894</v>
-      </c>
-      <c r="G15" t="s">
-        <v>869</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>909</v>
+        <v>891</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>875</v>
+        <v>857</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>910</v>
+        <v>892</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>889</v>
+        <v>871</v>
       </c>
       <c r="E16" t="s">
+        <v>833</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>880</v>
+      </c>
+      <c r="G16" t="s">
         <v>851</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>898</v>
-      </c>
-      <c r="G16" t="s">
-        <v>869</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>911</v>
+        <v>893</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>912</v>
+        <v>894</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>877</v>
+        <v>859</v>
       </c>
       <c r="E17" t="s">
-        <v>913</v>
+        <v>895</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>878</v>
+        <v>860</v>
       </c>
       <c r="G17" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>914</v>
+        <v>896</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>915</v>
+        <v>897</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>881</v>
+        <v>863</v>
       </c>
       <c r="E18" t="s">
-        <v>913</v>
+        <v>895</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>882</v>
+        <v>864</v>
       </c>
       <c r="G18" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
@@ -10939,7 +10947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E5D19F-62EE-447F-8282-B7E4E58FFCE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMD11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10965,22 +10973,22 @@
         <v>138</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>916</v>
+        <v>898</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>917</v>
+        <v>899</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>319</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>863</v>
+        <v>845</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>864</v>
+        <v>846</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>918</v>
+        <v>900</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -11995,262 +12003,262 @@
     </row>
     <row r="2" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>919</v>
+        <v>901</v>
       </c>
       <c r="B2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C2" t="s">
-        <v>920</v>
+        <v>902</v>
       </c>
       <c r="D2" t="s">
-        <v>920</v>
+        <v>902</v>
       </c>
       <c r="E2" t="s">
-        <v>866</v>
+        <v>848</v>
       </c>
       <c r="F2" t="s">
-        <v>868</v>
+        <v>850</v>
       </c>
       <c r="G2" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H2" t="s">
-        <v>921</v>
+        <v>903</v>
       </c>
     </row>
     <row r="3" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>922</v>
+        <v>904</v>
       </c>
       <c r="B3" t="s">
         <v>321</v>
       </c>
       <c r="C3" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="D3" t="s">
-        <v>923</v>
+        <v>905</v>
       </c>
       <c r="E3" t="s">
-        <v>872</v>
+        <v>854</v>
       </c>
       <c r="F3" t="s">
-        <v>873</v>
+        <v>855</v>
       </c>
       <c r="G3" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H3" t="s">
-        <v>921</v>
+        <v>903</v>
       </c>
     </row>
     <row r="4" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>924</v>
+        <v>906</v>
       </c>
       <c r="B4" t="s">
-        <v>925</v>
+        <v>907</v>
       </c>
       <c r="C4" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="D4" t="s">
-        <v>923</v>
+        <v>905</v>
       </c>
       <c r="E4" t="s">
-        <v>877</v>
+        <v>859</v>
       </c>
       <c r="F4" t="s">
-        <v>878</v>
+        <v>860</v>
       </c>
       <c r="G4" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H4" t="s">
-        <v>921</v>
+        <v>903</v>
       </c>
     </row>
     <row r="5" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>926</v>
+        <v>908</v>
       </c>
       <c r="B5" t="s">
-        <v>927</v>
+        <v>909</v>
       </c>
       <c r="C5" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="D5" t="s">
-        <v>923</v>
+        <v>905</v>
       </c>
       <c r="E5" t="s">
-        <v>881</v>
+        <v>863</v>
       </c>
       <c r="F5" t="s">
-        <v>882</v>
+        <v>864</v>
       </c>
       <c r="G5" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H5" t="s">
-        <v>921</v>
+        <v>903</v>
       </c>
     </row>
     <row r="6" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>928</v>
+        <v>910</v>
       </c>
       <c r="B6" t="s">
-        <v>880</v>
+        <v>862</v>
       </c>
       <c r="C6" t="s">
+        <v>849</v>
+      </c>
+      <c r="D6" t="s">
+        <v>905</v>
+      </c>
+      <c r="E6" t="s">
         <v>867</v>
       </c>
-      <c r="D6" t="s">
-        <v>923</v>
-      </c>
-      <c r="E6" t="s">
-        <v>885</v>
-      </c>
       <c r="F6" t="s">
-        <v>886</v>
+        <v>868</v>
       </c>
       <c r="G6" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H6" t="s">
-        <v>921</v>
+        <v>903</v>
       </c>
     </row>
     <row r="7" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>929</v>
+        <v>911</v>
       </c>
       <c r="B7" t="s">
-        <v>884</v>
+        <v>866</v>
       </c>
       <c r="C7" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="D7" t="s">
-        <v>923</v>
+        <v>905</v>
       </c>
       <c r="E7" t="s">
-        <v>889</v>
+        <v>871</v>
       </c>
       <c r="F7" t="s">
-        <v>890</v>
+        <v>872</v>
       </c>
       <c r="G7" t="s">
         <v>369</v>
       </c>
       <c r="H7" t="s">
-        <v>930</v>
+        <v>912</v>
       </c>
     </row>
     <row r="8" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>931</v>
+        <v>913</v>
       </c>
       <c r="B8" t="s">
-        <v>932</v>
+        <v>914</v>
       </c>
       <c r="C8" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="D8" t="s">
-        <v>923</v>
+        <v>905</v>
       </c>
       <c r="E8" t="s">
-        <v>893</v>
+        <v>875</v>
       </c>
       <c r="F8" t="s">
-        <v>894</v>
+        <v>876</v>
       </c>
       <c r="G8" t="s">
         <v>369</v>
       </c>
       <c r="H8" t="s">
-        <v>930</v>
+        <v>912</v>
       </c>
     </row>
     <row r="9" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>933</v>
+        <v>915</v>
       </c>
       <c r="B9" t="s">
-        <v>934</v>
+        <v>916</v>
       </c>
       <c r="C9" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="D9" t="s">
-        <v>923</v>
+        <v>905</v>
       </c>
       <c r="E9" t="s">
-        <v>897</v>
+        <v>879</v>
       </c>
       <c r="F9" t="s">
-        <v>898</v>
+        <v>880</v>
       </c>
       <c r="G9" t="s">
         <v>369</v>
       </c>
       <c r="H9" t="s">
-        <v>930</v>
+        <v>912</v>
       </c>
     </row>
     <row r="10" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>935</v>
+        <v>917</v>
       </c>
       <c r="B10" t="s">
-        <v>936</v>
+        <v>918</v>
       </c>
       <c r="C10" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="D10" t="s">
-        <v>923</v>
+        <v>905</v>
       </c>
       <c r="E10" t="s">
-        <v>901</v>
+        <v>883</v>
       </c>
       <c r="F10" t="s">
-        <v>902</v>
+        <v>884</v>
       </c>
       <c r="G10" t="s">
         <v>369</v>
       </c>
       <c r="H10" t="s">
-        <v>930</v>
+        <v>912</v>
       </c>
     </row>
     <row r="11" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>937</v>
+        <v>919</v>
       </c>
       <c r="B11" t="s">
-        <v>938</v>
+        <v>920</v>
       </c>
       <c r="C11" t="s">
-        <v>867</v>
+        <v>849</v>
       </c>
       <c r="D11" t="s">
-        <v>923</v>
+        <v>905</v>
       </c>
       <c r="E11" t="s">
-        <v>905</v>
+        <v>887</v>
       </c>
       <c r="F11" t="s">
-        <v>906</v>
+        <v>888</v>
       </c>
       <c r="G11" t="s">
-        <v>869</v>
+        <v>851</v>
       </c>
       <c r="H11" t="s">
-        <v>930</v>
+        <v>912</v>
       </c>
     </row>
   </sheetData>
@@ -12259,7 +12267,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12831,7 +12839,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="B33" t="s">
         <v>184</v>
@@ -12846,7 +12854,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -12861,7 +12869,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="B35" t="s">
         <v>234</v>
@@ -12880,7 +12888,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -12913,11 +12921,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12943,7 +12951,7 @@
         <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -14951,7 +14959,7 @@
     <row r="3" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -15991,7 +15999,7 @@
     <row r="8" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -16153,7 +16161,7 @@
     <row r="24" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -16163,7 +16171,7 @@
         <v>504</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>793</v>
+        <v>779</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
@@ -16174,7 +16182,7 @@
         <v>505</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="C26" t="s">
         <v>32</v>
@@ -16182,10 +16190,10 @@
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -16193,10 +16201,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="C28" t="s">
         <v>76</v>
@@ -16204,74 +16212,74 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="C29" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
       <c r="C30" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="E30" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
       <c r="C31" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
       <c r="C32" t="s">
         <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>805</v>
+        <v>787</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>797</v>
+        <v>782</v>
       </c>
       <c r="C33" t="s">
         <v>62</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>793</v>
+        <v>779</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>806</v>
+        <v>788</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="C34" t="s">
         <v>76</v>
@@ -16295,7 +16303,7 @@
     <row r="38" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -16325,7 +16333,7 @@
     <row r="42" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -16335,7 +16343,7 @@
         <v>143</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>846</v>
+        <v>828</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>32</v>
@@ -16359,17 +16367,17 @@
     <row r="47" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>32</v>
@@ -16377,10 +16385,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>76</v>
@@ -16389,10 +16397,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="B50" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="C50" t="s">
         <v>76</v>
@@ -16400,10 +16408,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="B51" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="C51" t="s">
         <v>76</v>
@@ -16411,10 +16419,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="B52" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="C52" t="s">
         <v>76</v>
@@ -16422,10 +16430,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="B53" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="C53" t="s">
         <v>76</v>
@@ -16433,10 +16441,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="B54" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="C54" t="s">
         <v>76</v>
@@ -16444,10 +16452,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="B55" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="C55" t="s">
         <v>76</v>
@@ -16455,10 +16463,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="B56" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="C56" t="s">
         <v>76</v>
@@ -16466,10 +16474,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="B57" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="C57" t="s">
         <v>76</v>
@@ -16477,10 +16485,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="B58" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="C58" t="s">
         <v>76</v>
@@ -16488,10 +16496,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="B59" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="C59" t="s">
         <v>352</v>
@@ -16499,43 +16507,43 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="B60" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="C60" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="B61" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="C61" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="B62" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="C62" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="B63" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="C63" t="s">
         <v>285</v>
@@ -16543,10 +16551,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="B64" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="C64" t="s">
         <v>62</v>
@@ -16554,21 +16562,21 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="B65" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="C65" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="B66" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="C66" t="s">
         <v>76</v>
@@ -16576,10 +16584,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="B67" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="C67" t="s">
         <v>76</v>
@@ -16587,10 +16595,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>828</v>
+        <v>810</v>
       </c>
       <c r="B68" t="s">
-        <v>826</v>
+        <v>808</v>
       </c>
       <c r="C68" t="s">
         <v>76</v>
@@ -16598,10 +16606,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>829</v>
+        <v>811</v>
       </c>
       <c r="B69" t="s">
-        <v>827</v>
+        <v>809</v>
       </c>
       <c r="C69" t="s">
         <v>76</v>
@@ -16609,10 +16617,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>835</v>
+        <v>817</v>
       </c>
       <c r="B71" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>32</v>
@@ -16624,11 +16632,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16671,22 +16679,22 @@
         <v>320</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>431</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>555</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -18693,7 +18701,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -19713,7 +19721,7 @@
         <v>497</v>
       </c>
       <c r="E4" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>26</v>
@@ -19726,7 +19734,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
@@ -19876,7 +19884,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="7"/>
@@ -19891,49 +19899,53 @@
         <v>506</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>620</v>
+        <v>922</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="D18" s="50" t="s">
-        <v>793</v>
-      </c>
-      <c r="E18" s="54"/>
+        <v>779</v>
+      </c>
+      <c r="E18" t="s">
+        <v>923</v>
+      </c>
     </row>
     <row r="19" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>617</v>
+        <v>924</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>618</v>
-      </c>
-      <c r="E19" s="54"/>
+        <v>611</v>
+      </c>
+      <c r="E19" t="s">
+        <v>925</v>
+      </c>
     </row>
     <row r="20" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
-        <v>794</v>
+        <v>780</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>795</v>
+        <v>926</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>796</v>
+        <v>781</v>
       </c>
       <c r="E20" s="54"/>
     </row>
     <row r="21" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
-        <v>802</v>
+        <v>785</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>803</v>
+        <v>927</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>804</v>
+        <v>786</v>
       </c>
       <c r="E21" s="54"/>
     </row>
@@ -19944,7 +19956,7 @@
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="7"/>
@@ -20169,7 +20181,7 @@
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="7"/>
@@ -20181,19 +20193,19 @@
     </row>
     <row r="34" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
-        <v>844</v>
+        <v>826</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>847</v>
+        <v>829</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>845</v>
+        <v>827</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>807</v>
+        <v>789</v>
       </c>
       <c r="E34" t="s">
-        <v>850</v>
+        <v>832</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -20212,7 +20224,7 @@
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="7"/>
@@ -20224,68 +20236,68 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="B38" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
       <c r="C38" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="E38" s="60" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="B39" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="C39" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="E39" s="60" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>852</v>
+        <v>834</v>
       </c>
       <c r="B40" t="s">
-        <v>853</v>
+        <v>835</v>
       </c>
       <c r="E40" s="60"/>
       <c r="K40" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="L40" t="s">
-        <v>854</v>
+        <v>836</v>
       </c>
       <c r="M40" t="s">
-        <v>855</v>
+        <v>837</v>
       </c>
       <c r="N40" t="s">
-        <v>856</v>
+        <v>838</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E38" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E39" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E38" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
+    <hyperlink ref="E39" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20300,7 +20312,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>14</v>
@@ -20315,7 +20327,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -20327,10 +20339,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>508</v>
+        <v>928</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -20340,11 +20352,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20410,7 +20422,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -20457,7 +20469,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
@@ -20471,7 +20483,7 @@
         <v>507</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>792</v>
+        <v>929</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>57</v>
@@ -20485,7 +20497,7 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
@@ -20527,7 +20539,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>657</v>
+        <v>649</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="3"/>
@@ -20538,10 +20550,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>836</v>
+        <v>818</v>
       </c>
       <c r="B17" t="s">
-        <v>837</v>
+        <v>819</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>57</v>
@@ -20556,10 +20568,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML49"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
@@ -20596,19 +20608,19 @@
         <v>14</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>555</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="M1" s="3"/>
       <c r="N1" s="6"/>
@@ -22657,7 +22669,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -23694,7 +23706,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="E4" t="s">
         <v>31</v>
@@ -23714,7 +23726,7 @@
         <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="6" spans="1:1026" x14ac:dyDescent="0.25">
@@ -23728,14 +23740,14 @@
         <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="8" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -23847,10 +23859,10 @@
     </row>
     <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B14" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C14" t="s">
         <v>255</v>
@@ -23869,7 +23881,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -23894,7 +23906,7 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -23906,7 +23918,7 @@
         <v>146</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
       <c r="D19" s="50" t="s">
         <v>30</v>
@@ -23916,7 +23928,7 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -23925,13 +23937,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="B23" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="C23" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
       <c r="D23" t="s">
         <v>262</v>
@@ -23939,13 +23951,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="B24" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="C24" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="D24" t="s">
         <v>30</v>
@@ -23956,41 +23968,41 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="B25" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
       <c r="C25" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="D25" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="B26" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
       <c r="C26" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="D26" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="B27" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="C27" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="D27" t="s">
         <v>262</v>
@@ -23998,41 +24010,41 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="B28" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
       <c r="C28" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="D28" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
       <c r="B29" t="s">
-        <v>715</v>
+        <v>707</v>
       </c>
       <c r="C29" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="D29" t="s">
-        <v>716</v>
+        <v>708</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="B30" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="C30" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="D30" t="s">
         <v>262</v>
@@ -24040,13 +24052,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="B31" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="C31" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="D31" t="s">
         <v>262</v>
@@ -24054,13 +24066,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="B32" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="C32" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="D32" t="s">
         <v>262</v>
@@ -24068,13 +24080,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
       <c r="B33" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="C33" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="D33" t="s">
         <v>262</v>
@@ -24082,13 +24094,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="B34" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="C34" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="D34" t="s">
         <v>262</v>
@@ -24096,13 +24108,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
       <c r="B35" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="C35" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="D35" t="s">
         <v>262</v>
@@ -24110,13 +24122,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="B36" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="C36" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="D36" t="s">
         <v>262</v>
@@ -24124,13 +24136,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B37" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="C37" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="D37" t="s">
         <v>262</v>
@@ -24138,13 +24150,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="B38" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="C38" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="D38" t="s">
         <v>262</v>
@@ -24152,13 +24164,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
       <c r="B39" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="C39" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="D39" t="s">
         <v>262</v>
@@ -24166,13 +24178,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="B40" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="C40" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="D40" t="s">
         <v>262</v>
@@ -24180,13 +24192,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
       <c r="B41" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="C41" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="D41" t="s">
         <v>262</v>
@@ -24194,47 +24206,47 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>786</v>
+        <v>773</v>
       </c>
       <c r="B42" t="s">
-        <v>787</v>
+        <v>774</v>
       </c>
       <c r="C42" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="D42" t="s">
         <v>30</v>
       </c>
       <c r="F42" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>830</v>
+        <v>812</v>
       </c>
       <c r="B43" t="s">
-        <v>832</v>
+        <v>814</v>
       </c>
       <c r="C43" t="s">
-        <v>826</v>
+        <v>808</v>
       </c>
       <c r="D43" t="s">
         <v>262</v>
       </c>
       <c r="G43" t="s">
-        <v>834</v>
+        <v>816</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>831</v>
+        <v>813</v>
       </c>
       <c r="B44" t="s">
-        <v>833</v>
+        <v>815</v>
       </c>
       <c r="C44" t="s">
-        <v>827</v>
+        <v>809</v>
       </c>
       <c r="D44" t="s">
         <v>262</v>
@@ -24247,7 +24259,7 @@
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -24256,50 +24268,50 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
       <c r="B47" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="C47" t="s">
         <v>47</v>
       </c>
       <c r="D47" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="B48" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="C48" t="s">
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>857</v>
+        <v>839</v>
       </c>
       <c r="B49" t="s">
-        <v>858</v>
+        <v>840</v>
       </c>
       <c r="I49" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="J49" t="s">
-        <v>854</v>
+        <v>836</v>
       </c>
       <c r="K49" t="s">
-        <v>855</v>
+        <v>837</v>
       </c>
       <c r="L49" t="s">
-        <v>859</v>
+        <v>841</v>
       </c>
     </row>
   </sheetData>
@@ -24310,11 +24322,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24333,7 +24345,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>12</v>
@@ -24342,59 +24354,59 @@
         <v>48</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>555</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="B2" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>766</v>
+        <v>758</v>
       </c>
       <c r="B3" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>860</v>
+        <v>842</v>
       </c>
       <c r="B4" t="s">
-        <v>861</v>
+        <v>843</v>
       </c>
       <c r="E4" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="F4" t="s">
-        <v>854</v>
+        <v>836</v>
       </c>
       <c r="G4" t="s">
-        <v>855</v>
+        <v>837</v>
       </c>
       <c r="H4" t="s">
-        <v>862</v>
+        <v>844</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -24403,33 +24415,33 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>801</v>
+        <v>784</v>
       </c>
       <c r="B7" t="s">
-        <v>800</v>
+        <v>930</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>838</v>
+        <v>820</v>
       </c>
       <c r="B10" t="s">
-        <v>839</v>
+        <v>821</v>
       </c>
       <c r="C10" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="D10" t="s">
-        <v>837</v>
+        <v>819</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel change for module 6
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="952">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2177,9 +2177,6 @@
     <t>Test Deal 6</t>
   </si>
   <si>
-    <t>Due Dilligence</t>
-  </si>
-  <si>
     <t>M6Deal7</t>
   </si>
   <si>
@@ -2919,6 +2916,12 @@
   </si>
   <si>
     <t>Test locale 3</t>
+  </si>
+  <si>
+    <t>Fund Manager’s Fund</t>
+  </si>
+  <si>
+    <t>Due Diligence</t>
   </si>
 </sst>
 </file>
@@ -3578,10 +3581,10 @@
         <v>643</v>
       </c>
       <c r="B6" t="s">
+        <v>759</v>
+      </c>
+      <c r="D6" t="s">
         <v>760</v>
-      </c>
-      <c r="D6" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3589,10 +3592,10 @@
         <v>644</v>
       </c>
       <c r="B7" t="s">
+        <v>761</v>
+      </c>
+      <c r="E7" t="s">
         <v>762</v>
-      </c>
-      <c r="E7" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -3617,7 +3620,7 @@
         <v>343</v>
       </c>
       <c r="J9" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="K9" t="s">
         <v>402</v>
@@ -3639,12 +3642,12 @@
         <v>648</v>
       </c>
       <c r="J11" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="J12" t="s">
         <v>285</v>
@@ -3652,15 +3655,15 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
+        <v>765</v>
+      </c>
+      <c r="B13" t="s">
         <v>766</v>
-      </c>
-      <c r="B13" t="s">
-        <v>767</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -3668,13 +3671,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
+        <v>775</v>
+      </c>
+      <c r="B15" t="s">
         <v>776</v>
       </c>
-      <c r="B15" t="s">
+      <c r="F15" t="s">
         <v>777</v>
-      </c>
-      <c r="F15" t="s">
-        <v>778</v>
       </c>
       <c r="K15" t="s">
         <v>401</v>
@@ -3682,10 +3685,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
+        <v>768</v>
+      </c>
+      <c r="B16" t="s">
         <v>769</v>
-      </c>
-      <c r="B16" t="s">
-        <v>770</v>
       </c>
       <c r="K16" t="s">
         <v>401</v>
@@ -3693,13 +3696,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B17" t="s">
+        <v>769</v>
+      </c>
+      <c r="D17" t="s">
         <v>770</v>
-      </c>
-      <c r="D17" t="s">
-        <v>771</v>
       </c>
     </row>
   </sheetData>
@@ -3878,7 +3881,7 @@
         <v>314</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>319</v>
@@ -3895,7 +3898,7 @@
         <v>339</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>319</v>
@@ -3928,47 +3931,47 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
+        <v>789</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>790</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>791</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>791</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>734</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
+        <v>792</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>793</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>794</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
+        <v>821</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>823</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>151</v>
@@ -3976,13 +3979,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
+        <v>823</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>825</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>151</v>
@@ -4059,13 +4062,13 @@
         <v>573</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D4" s="24" t="s">
+        <v>794</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>795</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>796</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>173</v>
@@ -4079,7 +4082,7 @@
         <v>175</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>176</v>
@@ -4099,10 +4102,10 @@
         <v>180</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>181</v>
@@ -4510,16 +4513,16 @@
         <v>164</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>165</v>
       </c>
       <c r="D30" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
   </sheetData>
@@ -4627,10 +4630,10 @@
     </row>
     <row r="12" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C12" s="22"/>
     </row>
@@ -5005,7 +5008,7 @@
         <v>535</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="G16" s="50" t="s">
         <v>537</v>
@@ -5022,7 +5025,7 @@
         <v>540</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="G17" s="50" t="s">
         <v>541</v>
@@ -5039,7 +5042,7 @@
         <v>540</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="F18" s="50" t="s">
         <v>544</v>
@@ -5299,7 +5302,7 @@
         <v>329</v>
       </c>
       <c r="B9" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5307,7 +5310,7 @@
         <v>330</v>
       </c>
       <c r="B10" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5334,7 +5337,7 @@
         <v>331</v>
       </c>
       <c r="B13" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5342,7 +5345,7 @@
         <v>332</v>
       </c>
       <c r="B14" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5350,7 +5353,7 @@
         <v>333</v>
       </c>
       <c r="B15" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5358,7 +5361,7 @@
         <v>334</v>
       </c>
       <c r="B16" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5374,50 +5377,50 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>797</v>
+      </c>
+      <c r="B19" s="61" t="s">
         <v>798</v>
-      </c>
-      <c r="B19" s="61" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>799</v>
+      </c>
+      <c r="B20" s="61" t="s">
         <v>800</v>
-      </c>
-      <c r="B20" s="61" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>801</v>
+      </c>
+      <c r="B21" s="61" t="s">
         <v>802</v>
-      </c>
-      <c r="B21" s="61" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>805</v>
+      </c>
+      <c r="B24" s="61" t="s">
         <v>806</v>
-      </c>
-      <c r="B24" s="61" t="s">
-        <v>807</v>
       </c>
     </row>
   </sheetData>
@@ -6330,10 +6333,10 @@
         <v>584</v>
       </c>
       <c r="B2" t="s">
+        <v>934</v>
+      </c>
+      <c r="C2" t="s">
         <v>935</v>
-      </c>
-      <c r="C2" t="s">
-        <v>936</v>
       </c>
       <c r="D2" t="s">
         <v>585</v>
@@ -6406,10 +6409,10 @@
         <v>594</v>
       </c>
       <c r="B2" t="s">
+        <v>936</v>
+      </c>
+      <c r="C2" t="s">
         <v>937</v>
-      </c>
-      <c r="C2" t="s">
-        <v>938</v>
       </c>
       <c r="D2" t="s">
         <v>595</v>
@@ -6477,10 +6480,10 @@
         <v>600</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>844</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>845</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>846</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>547</v>
@@ -7520,11 +7523,11 @@
         <v>604</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -8556,7 +8559,7 @@
         <v>604</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -9592,7 +9595,7 @@
         <v>604</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -10620,7 +10623,7 @@
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>604</v>
@@ -10629,138 +10632,138 @@
         <v>536</v>
       </c>
       <c r="D5" s="19" t="s">
+        <v>847</v>
+      </c>
+      <c r="E5" t="s">
         <v>848</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="19" t="s">
         <v>849</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" t="s">
         <v>850</v>
-      </c>
-      <c r="G5" t="s">
-        <v>851</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>540</v>
       </c>
       <c r="C6" s="19" t="s">
+        <v>852</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>853</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="E6" t="s">
+        <v>848</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>854</v>
       </c>
-      <c r="E6" t="s">
-        <v>849</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>855</v>
-      </c>
       <c r="G6" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
+        <v>855</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>856</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="C7" s="19" t="s">
         <v>857</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="19" t="s">
         <v>858</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="E7" t="s">
+        <v>848</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>859</v>
       </c>
-      <c r="E7" t="s">
-        <v>849</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>860</v>
-      </c>
       <c r="G7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>604</v>
       </c>
       <c r="C8" s="19" t="s">
+        <v>861</v>
+      </c>
+      <c r="D8" s="19" t="s">
         <v>862</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="E8" t="s">
+        <v>848</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>863</v>
       </c>
-      <c r="E8" t="s">
-        <v>849</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>864</v>
-      </c>
       <c r="G8" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>540</v>
       </c>
       <c r="C9" s="19" t="s">
+        <v>865</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>866</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="E9" t="s">
+        <v>848</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>867</v>
       </c>
-      <c r="E9" t="s">
-        <v>849</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>868</v>
-      </c>
       <c r="G9" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
+        <v>868</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>856</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>869</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>857</v>
-      </c>
-      <c r="C10" s="19" t="s">
+      <c r="D10" s="19" t="s">
         <v>870</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="E10" t="s">
+        <v>848</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>871</v>
-      </c>
-      <c r="E10" t="s">
-        <v>849</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>872</v>
       </c>
       <c r="G10" t="s">
         <v>369</v>
@@ -10770,22 +10773,22 @@
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>604</v>
       </c>
       <c r="C11" s="19" t="s">
+        <v>873</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>874</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="E11" t="s">
+        <v>848</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>875</v>
-      </c>
-      <c r="E11" t="s">
-        <v>849</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>876</v>
       </c>
       <c r="G11" t="s">
         <v>369</v>
@@ -10795,22 +10798,22 @@
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>540</v>
       </c>
       <c r="C12" s="19" t="s">
+        <v>877</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>878</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="E12" t="s">
+        <v>848</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>879</v>
-      </c>
-      <c r="E12" t="s">
-        <v>849</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>880</v>
       </c>
       <c r="G12" t="s">
         <v>369</v>
@@ -10820,22 +10823,22 @@
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
+        <v>880</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>856</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>881</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>857</v>
-      </c>
-      <c r="C13" s="19" t="s">
+      <c r="D13" s="19" t="s">
         <v>882</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="E13" t="s">
+        <v>848</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>883</v>
-      </c>
-      <c r="E13" t="s">
-        <v>849</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>884</v>
       </c>
       <c r="G13" t="s">
         <v>369</v>
@@ -10845,22 +10848,22 @@
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>604</v>
       </c>
       <c r="C14" s="19" t="s">
+        <v>885</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>886</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" t="s">
+        <v>848</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>887</v>
-      </c>
-      <c r="E14" t="s">
-        <v>849</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>888</v>
       </c>
       <c r="G14" t="s">
         <v>369</v>
@@ -10870,100 +10873,100 @@
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>540</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E15" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="G15" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
+        <v>890</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>856</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>891</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>857</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>892</v>
-      </c>
       <c r="D16" s="19" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E16" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="G16" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>535</v>
       </c>
       <c r="C17" s="19" t="s">
+        <v>893</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>858</v>
+      </c>
+      <c r="E17" t="s">
         <v>894</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="F17" s="19" t="s">
         <v>859</v>
       </c>
-      <c r="E17" t="s">
-        <v>895</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>860</v>
-      </c>
       <c r="G17" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>535</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D18" s="19" t="s">
+        <v>862</v>
+      </c>
+      <c r="E18" t="s">
+        <v>894</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>863</v>
       </c>
-      <c r="E18" t="s">
-        <v>895</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>864</v>
-      </c>
       <c r="G18" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
@@ -11000,22 +11003,22 @@
         <v>138</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>898</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>899</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>319</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>844</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>845</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>846</v>
-      </c>
       <c r="H1" s="21" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -12030,262 +12033,262 @@
     </row>
     <row r="2" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B2" t="s">
         <v>536</v>
       </c>
       <c r="C2" t="s">
+        <v>901</v>
+      </c>
+      <c r="D2" t="s">
+        <v>901</v>
+      </c>
+      <c r="E2" t="s">
+        <v>847</v>
+      </c>
+      <c r="F2" t="s">
+        <v>849</v>
+      </c>
+      <c r="G2" t="s">
+        <v>850</v>
+      </c>
+      <c r="H2" t="s">
         <v>902</v>
-      </c>
-      <c r="D2" t="s">
-        <v>902</v>
-      </c>
-      <c r="E2" t="s">
-        <v>848</v>
-      </c>
-      <c r="F2" t="s">
-        <v>850</v>
-      </c>
-      <c r="G2" t="s">
-        <v>851</v>
-      </c>
-      <c r="H2" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="3" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B3" t="s">
         <v>321</v>
       </c>
       <c r="C3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E3" t="s">
+        <v>853</v>
+      </c>
+      <c r="F3" t="s">
         <v>854</v>
       </c>
-      <c r="F3" t="s">
-        <v>855</v>
-      </c>
       <c r="G3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="4" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>905</v>
+      </c>
+      <c r="B4" t="s">
         <v>906</v>
       </c>
-      <c r="B4" t="s">
-        <v>907</v>
-      </c>
       <c r="C4" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D4" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E4" t="s">
+        <v>858</v>
+      </c>
+      <c r="F4" t="s">
         <v>859</v>
       </c>
-      <c r="F4" t="s">
-        <v>860</v>
-      </c>
       <c r="G4" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H4" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="5" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>907</v>
+      </c>
+      <c r="B5" t="s">
         <v>908</v>
       </c>
-      <c r="B5" t="s">
-        <v>909</v>
-      </c>
       <c r="C5" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E5" t="s">
+        <v>862</v>
+      </c>
+      <c r="F5" t="s">
         <v>863</v>
       </c>
-      <c r="F5" t="s">
-        <v>864</v>
-      </c>
       <c r="G5" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H5" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="6" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B6" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C6" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E6" t="s">
+        <v>866</v>
+      </c>
+      <c r="F6" t="s">
         <v>867</v>
       </c>
-      <c r="F6" t="s">
-        <v>868</v>
-      </c>
       <c r="G6" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H6" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="7" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B7" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C7" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E7" t="s">
+        <v>870</v>
+      </c>
+      <c r="F7" t="s">
         <v>871</v>
-      </c>
-      <c r="F7" t="s">
-        <v>872</v>
       </c>
       <c r="G7" t="s">
         <v>369</v>
       </c>
       <c r="H7" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="8" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>912</v>
+      </c>
+      <c r="B8" t="s">
         <v>913</v>
       </c>
-      <c r="B8" t="s">
-        <v>914</v>
-      </c>
       <c r="C8" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D8" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E8" t="s">
+        <v>874</v>
+      </c>
+      <c r="F8" t="s">
         <v>875</v>
-      </c>
-      <c r="F8" t="s">
-        <v>876</v>
       </c>
       <c r="G8" t="s">
         <v>369</v>
       </c>
       <c r="H8" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="9" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>914</v>
+      </c>
+      <c r="B9" t="s">
         <v>915</v>
       </c>
-      <c r="B9" t="s">
-        <v>916</v>
-      </c>
       <c r="C9" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E9" t="s">
+        <v>878</v>
+      </c>
+      <c r="F9" t="s">
         <v>879</v>
-      </c>
-      <c r="F9" t="s">
-        <v>880</v>
       </c>
       <c r="G9" t="s">
         <v>369</v>
       </c>
       <c r="H9" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="10" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>916</v>
+      </c>
+      <c r="B10" t="s">
         <v>917</v>
       </c>
-      <c r="B10" t="s">
-        <v>918</v>
-      </c>
       <c r="C10" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D10" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E10" t="s">
+        <v>882</v>
+      </c>
+      <c r="F10" t="s">
         <v>883</v>
-      </c>
-      <c r="F10" t="s">
-        <v>884</v>
       </c>
       <c r="G10" t="s">
         <v>369</v>
       </c>
       <c r="H10" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="11" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>918</v>
+      </c>
+      <c r="B11" t="s">
         <v>919</v>
       </c>
-      <c r="B11" t="s">
-        <v>920</v>
-      </c>
       <c r="C11" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D11" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E11" t="s">
+        <v>886</v>
+      </c>
+      <c r="F11" t="s">
         <v>887</v>
       </c>
-      <c r="F11" t="s">
-        <v>888</v>
-      </c>
       <c r="G11" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H11" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
   </sheetData>
@@ -12951,8 +12954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO71"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16198,7 +16201,7 @@
         <v>504</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
@@ -16289,21 +16292,21 @@
     </row>
     <row r="33" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C33" t="s">
         <v>62</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>609</v>
@@ -16370,7 +16373,7 @@
         <v>143</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>32</v>
@@ -16551,7 +16554,7 @@
         <v>677</v>
       </c>
       <c r="C61" t="s">
-        <v>626</v>
+        <v>950</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -16622,10 +16625,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B68" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C68" t="s">
         <v>76</v>
@@ -16633,10 +16636,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B69" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C69" t="s">
         <v>76</v>
@@ -16644,7 +16647,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B71" t="s">
         <v>610</v>
@@ -19926,16 +19929,16 @@
         <v>506</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C18" s="50" t="s">
         <v>613</v>
       </c>
       <c r="D18" s="50" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E18" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -19943,36 +19946,36 @@
         <v>612</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C19" s="50" t="s">
         <v>611</v>
       </c>
       <c r="E19" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
+        <v>779</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>925</v>
+      </c>
+      <c r="C20" s="50" t="s">
         <v>780</v>
-      </c>
-      <c r="B20" s="50" t="s">
-        <v>926</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>781</v>
       </c>
       <c r="E20" s="54"/>
     </row>
     <row r="21" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
+        <v>784</v>
+      </c>
+      <c r="B21" s="50" t="s">
+        <v>926</v>
+      </c>
+      <c r="C21" s="50" t="s">
         <v>785</v>
-      </c>
-      <c r="B21" s="50" t="s">
-        <v>927</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>786</v>
       </c>
       <c r="E21" s="54"/>
     </row>
@@ -20220,19 +20223,19 @@
     </row>
     <row r="34" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
+        <v>825</v>
+      </c>
+      <c r="B34" s="50" t="s">
+        <v>828</v>
+      </c>
+      <c r="C34" s="50" t="s">
         <v>826</v>
       </c>
-      <c r="B34" s="50" t="s">
-        <v>829</v>
-      </c>
-      <c r="C34" s="50" t="s">
-        <v>827</v>
-      </c>
       <c r="D34" s="20" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E34" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -20251,7 +20254,7 @@
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="7"/>
@@ -20263,51 +20266,51 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>741</v>
+      </c>
+      <c r="B38" t="s">
         <v>742</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>743</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" s="60" t="s">
         <v>744</v>
-      </c>
-      <c r="E38" s="60" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>745</v>
+      </c>
+      <c r="B39" t="s">
         <v>746</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>747</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" s="60" t="s">
         <v>748</v>
-      </c>
-      <c r="E39" s="60" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>833</v>
+      </c>
+      <c r="B40" t="s">
         <v>834</v>
-      </c>
-      <c r="B40" t="s">
-        <v>835</v>
       </c>
       <c r="E40" s="60"/>
       <c r="K40" t="s">
         <v>555</v>
       </c>
       <c r="L40" t="s">
+        <v>835</v>
+      </c>
+      <c r="M40" t="s">
         <v>836</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>837</v>
-      </c>
-      <c r="N40" t="s">
-        <v>838</v>
       </c>
     </row>
   </sheetData>
@@ -20369,7 +20372,7 @@
         <v>508</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -20510,7 +20513,7 @@
         <v>507</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>57</v>
@@ -20577,10 +20580,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>817</v>
+      </c>
+      <c r="B17" t="s">
         <v>818</v>
-      </c>
-      <c r="B17" t="s">
-        <v>819</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>57</v>
@@ -20598,8 +20601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23945,7 +23948,7 @@
         <v>146</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D19" s="50" t="s">
         <v>30</v>
@@ -24046,29 +24049,29 @@
         <v>661</v>
       </c>
       <c r="D28" t="s">
-        <v>705</v>
+        <v>951</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>705</v>
+      </c>
+      <c r="B29" t="s">
         <v>706</v>
-      </c>
-      <c r="B29" t="s">
-        <v>707</v>
       </c>
       <c r="C29" t="s">
         <v>663</v>
       </c>
       <c r="D29" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>708</v>
+      </c>
+      <c r="B30" t="s">
         <v>709</v>
-      </c>
-      <c r="B30" t="s">
-        <v>710</v>
       </c>
       <c r="C30" t="s">
         <v>665</v>
@@ -24079,10 +24082,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>710</v>
+      </c>
+      <c r="B31" t="s">
         <v>711</v>
-      </c>
-      <c r="B31" t="s">
-        <v>712</v>
       </c>
       <c r="C31" t="s">
         <v>667</v>
@@ -24093,10 +24096,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>712</v>
+      </c>
+      <c r="B32" t="s">
         <v>713</v>
-      </c>
-      <c r="B32" t="s">
-        <v>714</v>
       </c>
       <c r="C32" t="s">
         <v>669</v>
@@ -24107,10 +24110,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>714</v>
+      </c>
+      <c r="B33" t="s">
         <v>715</v>
-      </c>
-      <c r="B33" t="s">
-        <v>716</v>
       </c>
       <c r="C33" t="s">
         <v>671</v>
@@ -24121,10 +24124,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>716</v>
+      </c>
+      <c r="B34" t="s">
         <v>717</v>
-      </c>
-      <c r="B34" t="s">
-        <v>718</v>
       </c>
       <c r="C34" t="s">
         <v>673</v>
@@ -24135,10 +24138,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>718</v>
+      </c>
+      <c r="B35" t="s">
         <v>719</v>
-      </c>
-      <c r="B35" t="s">
-        <v>720</v>
       </c>
       <c r="C35" t="s">
         <v>675</v>
@@ -24149,10 +24152,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>720</v>
+      </c>
+      <c r="B36" t="s">
         <v>721</v>
-      </c>
-      <c r="B36" t="s">
-        <v>722</v>
       </c>
       <c r="C36" t="s">
         <v>677</v>
@@ -24163,10 +24166,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>722</v>
+      </c>
+      <c r="B37" t="s">
         <v>723</v>
-      </c>
-      <c r="B37" t="s">
-        <v>724</v>
       </c>
       <c r="C37" t="s">
         <v>679</v>
@@ -24177,10 +24180,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>724</v>
+      </c>
+      <c r="B38" t="s">
         <v>725</v>
-      </c>
-      <c r="B38" t="s">
-        <v>726</v>
       </c>
       <c r="C38" t="s">
         <v>681</v>
@@ -24191,10 +24194,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>726</v>
+      </c>
+      <c r="B39" t="s">
         <v>727</v>
-      </c>
-      <c r="B39" t="s">
-        <v>728</v>
       </c>
       <c r="C39" t="s">
         <v>683</v>
@@ -24205,10 +24208,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>728</v>
+      </c>
+      <c r="B40" t="s">
         <v>729</v>
-      </c>
-      <c r="B40" t="s">
-        <v>730</v>
       </c>
       <c r="C40" t="s">
         <v>685</v>
@@ -24219,10 +24222,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>730</v>
+      </c>
+      <c r="B41" t="s">
         <v>731</v>
-      </c>
-      <c r="B41" t="s">
-        <v>732</v>
       </c>
       <c r="C41" t="s">
         <v>690</v>
@@ -24233,10 +24236,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>772</v>
+      </c>
+      <c r="B42" t="s">
         <v>773</v>
-      </c>
-      <c r="B42" t="s">
-        <v>774</v>
       </c>
       <c r="C42" t="s">
         <v>688</v>
@@ -24250,30 +24253,30 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B43" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C43" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D43" t="s">
         <v>262</v>
       </c>
       <c r="G43" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B44" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C44" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D44" t="s">
         <v>262</v>
@@ -24286,7 +24289,7 @@
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -24295,10 +24298,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>750</v>
+      </c>
+      <c r="B47" t="s">
         <v>751</v>
-      </c>
-      <c r="B47" t="s">
-        <v>752</v>
       </c>
       <c r="C47" t="s">
         <v>47</v>
@@ -24309,10 +24312,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>752</v>
+      </c>
+      <c r="B48" t="s">
         <v>753</v>
-      </c>
-      <c r="B48" t="s">
-        <v>754</v>
       </c>
       <c r="C48" t="s">
         <v>47</v>
@@ -24323,22 +24326,22 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>838</v>
+      </c>
+      <c r="B49" t="s">
         <v>839</v>
-      </c>
-      <c r="B49" t="s">
-        <v>840</v>
       </c>
       <c r="I49" t="s">
         <v>555</v>
       </c>
       <c r="J49" t="s">
+        <v>835</v>
+      </c>
+      <c r="K49" t="s">
         <v>836</v>
       </c>
-      <c r="K49" t="s">
-        <v>837</v>
-      </c>
       <c r="L49" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
   </sheetData>
@@ -24352,7 +24355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:E14"/>
     </sheetView>
   </sheetViews>
@@ -24372,7 +24375,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>12</v>
@@ -24395,38 +24398,38 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>755</v>
+      </c>
+      <c r="B2" t="s">
         <v>756</v>
-      </c>
-      <c r="B2" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>757</v>
+      </c>
+      <c r="B3" t="s">
         <v>758</v>
-      </c>
-      <c r="B3" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>841</v>
+      </c>
+      <c r="B4" t="s">
         <v>842</v>
-      </c>
-      <c r="B4" t="s">
-        <v>843</v>
       </c>
       <c r="E4" t="s">
         <v>555</v>
       </c>
       <c r="F4" t="s">
+        <v>835</v>
+      </c>
+      <c r="G4" t="s">
         <v>836</v>
       </c>
-      <c r="G4" t="s">
-        <v>837</v>
-      </c>
       <c r="H4" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -24442,10 +24445,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B7" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -24459,84 +24462,84 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>819</v>
+      </c>
+      <c r="B10" t="s">
         <v>820</v>
-      </c>
-      <c r="B10" t="s">
-        <v>821</v>
       </c>
       <c r="C10" t="s">
         <v>610</v>
       </c>
       <c r="D10" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>941</v>
+      </c>
+      <c r="B11" t="s">
         <v>942</v>
-      </c>
-      <c r="B11" t="s">
-        <v>943</v>
       </c>
       <c r="C11" t="s">
         <v>610</v>
       </c>
       <c r="D11" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E11" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>944</v>
+      </c>
+      <c r="B12" t="s">
         <v>945</v>
-      </c>
-      <c r="B12" t="s">
-        <v>946</v>
       </c>
       <c r="C12" t="s">
         <v>610</v>
       </c>
       <c r="D12" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E12" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>946</v>
+      </c>
+      <c r="B13" t="s">
         <v>947</v>
-      </c>
-      <c r="B13" t="s">
-        <v>948</v>
       </c>
       <c r="C13" t="s">
         <v>610</v>
       </c>
       <c r="D13" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E13" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>948</v>
+      </c>
+      <c r="B14" t="s">
         <v>949</v>
-      </c>
-      <c r="B14" t="s">
-        <v>950</v>
       </c>
       <c r="C14" t="s">
         <v>610</v>
       </c>
       <c r="D14" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E14" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel upate for module 4 and mdoule 6
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="953">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2922,6 +2922,9 @@
   </si>
   <si>
     <t>Due Diligence</t>
+  </si>
+  <si>
+    <t>Europe</t>
   </si>
 </sst>
 </file>
@@ -3806,14 +3809,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
@@ -3901,7 +3905,7 @@
         <v>733</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>319</v>
+        <v>791</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -12954,7 +12958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO71"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -16665,8 +16669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16677,10 +16681,10 @@
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -20019,7 +20023,7 @@
         <v>347</v>
       </c>
       <c r="I24" t="s">
-        <v>348</v>
+        <v>952</v>
       </c>
       <c r="J24" t="s">
         <v>349</v>
@@ -20048,7 +20052,7 @@
         <v>352</v>
       </c>
       <c r="I25" t="s">
-        <v>348</v>
+        <v>952</v>
       </c>
       <c r="J25" t="s">
         <v>349</v>
@@ -20077,7 +20081,7 @@
         <v>347</v>
       </c>
       <c r="I26" t="s">
-        <v>348</v>
+        <v>952</v>
       </c>
       <c r="J26" t="s">
         <v>349</v>
@@ -20106,7 +20110,7 @@
         <v>352</v>
       </c>
       <c r="I27" t="s">
-        <v>348</v>
+        <v>952</v>
       </c>
       <c r="J27" t="s">
         <v>349</v>
@@ -20132,7 +20136,7 @@
         <v>347</v>
       </c>
       <c r="I28" t="s">
-        <v>348</v>
+        <v>952</v>
       </c>
       <c r="J28" t="s">
         <v>349</v>
@@ -20158,7 +20162,7 @@
         <v>352</v>
       </c>
       <c r="I29" t="s">
-        <v>348</v>
+        <v>952</v>
       </c>
       <c r="J29" t="s">
         <v>349</v>
@@ -20184,7 +20188,7 @@
         <v>347</v>
       </c>
       <c r="I30" t="s">
-        <v>348</v>
+        <v>952</v>
       </c>
       <c r="J30" t="s">
         <v>349</v>
@@ -20601,7 +20605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -24365,9 +24369,9 @@
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Excel for Module 7 TC006-TC011
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="19" activeTab="24"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="979">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2994,6 +2994,15 @@
   </si>
   <si>
     <t>9/4/2021</t>
+  </si>
+  <si>
+    <t>M7Task3</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Task-3</t>
+  </si>
+  <si>
+    <t>8/29/2021</t>
   </si>
 </sst>
 </file>
@@ -6524,10 +6533,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ21"/>
+  <dimension ref="A1:AMJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11088,6 +11097,23 @@
         <v>605</v>
       </c>
     </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>977</v>
+      </c>
+      <c r="E22" t="s">
+        <v>978</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>544</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16801,8 +16827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added TC 17 to 19
Signed-off-by: Ravi kumar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namita\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B15946-2C0D-404D-B19F-AB47332ED6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A99E82-9C14-4CD5-A206-E088ECBC5753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="1227">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3676,6 +3676,78 @@
   </si>
   <si>
     <t>SMOKFund2</t>
+  </si>
+  <si>
+    <t>SMOKINS11</t>
+  </si>
+  <si>
+    <t>SMOKINS12</t>
+  </si>
+  <si>
+    <t>SMOKINS13</t>
+  </si>
+  <si>
+    <t>SMOKINS14</t>
+  </si>
+  <si>
+    <t>SMOKINS15</t>
+  </si>
+  <si>
+    <t>SMOKINS16</t>
+  </si>
+  <si>
+    <t>SMOKINS17</t>
+  </si>
+  <si>
+    <t>SMOKINS18</t>
+  </si>
+  <si>
+    <t>Test Institution-1</t>
+  </si>
+  <si>
+    <t>Entity_Type</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Test Company-1</t>
+  </si>
+  <si>
+    <t>Test Indi-Investor-1</t>
+  </si>
+  <si>
+    <t>Family Office</t>
+  </si>
+  <si>
+    <t>Test LimtedPartner-1</t>
+  </si>
+  <si>
+    <t>Test Fund Manager-1</t>
+  </si>
+  <si>
+    <t>Test Fund Manager's Fund-1</t>
+  </si>
+  <si>
+    <t>Test Advisor-1</t>
+  </si>
+  <si>
+    <t>Test Intermediary-1</t>
+  </si>
+  <si>
+    <t>Test Lender-1</t>
+  </si>
+  <si>
+    <t>Test Portfolio Company-1</t>
+  </si>
+  <si>
+    <t>Portfolio Company</t>
+  </si>
+  <si>
+    <t>SMOKINS19</t>
+  </si>
+  <si>
+    <t>SMOKINS20</t>
   </si>
 </sst>
 </file>
@@ -14354,23 +14426,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:ALO89"/>
+  <dimension ref="A1:ALP99"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="16.25" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="17.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -14387,9 +14460,11 @@
         <v>619</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -15386,8 +15461,9 @@
       <c r="ALM1" s="5"/>
       <c r="ALN1" s="5"/>
       <c r="ALO1" s="5"/>
-    </row>
-    <row r="2" spans="1:1003" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="ALP1" s="5"/>
+    </row>
+    <row r="2" spans="1:1004" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="35"/>
@@ -16390,8 +16466,9 @@
       <c r="ALM2" s="36"/>
       <c r="ALN2" s="36"/>
       <c r="ALO2" s="36"/>
-    </row>
-    <row r="3" spans="1:1003" x14ac:dyDescent="0.25">
+      <c r="ALP2" s="36"/>
+    </row>
+    <row r="3" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>510</v>
@@ -17397,8 +17474,9 @@
       <c r="ALM3" s="5"/>
       <c r="ALN3" s="5"/>
       <c r="ALO3" s="5"/>
-    </row>
-    <row r="4" spans="1:1003" x14ac:dyDescent="0.25">
+      <c r="ALP3" s="5"/>
+    </row>
+    <row r="4" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -17409,7 +17487,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -17420,7 +17498,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -17431,7 +17509,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>512</v>
@@ -17439,7 +17517,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>96</v>
       </c>
@@ -17453,7 +17531,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>98</v>
       </c>
@@ -17467,7 +17545,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>100</v>
       </c>
@@ -17481,7 +17559,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>102</v>
       </c>
@@ -17495,7 +17573,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -17509,7 +17587,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>141</v>
       </c>
@@ -17523,7 +17601,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>249</v>
       </c>
@@ -17695,7 +17773,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>769</v>
       </c>
@@ -17708,8 +17786,9 @@
       <c r="E33" s="22" t="s">
         <v>928</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>770</v>
       </c>
@@ -17720,22 +17799,22 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="20"/>
       <c r="C35" s="22"/>
     </row>
-    <row r="36" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="22"/>
     </row>
-    <row r="37" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
     </row>
-    <row r="38" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>513</v>
@@ -17743,7 +17822,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>397</v>
       </c>
@@ -17754,7 +17833,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>398</v>
       </c>
@@ -17765,7 +17844,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>524</v>
@@ -17773,7 +17852,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>143</v>
       </c>
@@ -17784,7 +17863,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>442</v>
       </c>
@@ -17793,13 +17872,13 @@
       </c>
       <c r="C44" s="22"/>
     </row>
-    <row r="46" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="53"/>
       <c r="B46" s="53"/>
       <c r="C46" s="53"/>
       <c r="D46" s="53"/>
     </row>
-    <row r="47" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>639</v>
@@ -17807,7 +17886,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>640</v>
       </c>
@@ -18132,7 +18211,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1110</v>
       </c>
@@ -18143,7 +18222,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1112</v>
       </c>
@@ -18154,7 +18233,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1114</v>
       </c>
@@ -18165,7 +18244,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1117</v>
       </c>
@@ -18176,7 +18255,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1119</v>
       </c>
@@ -18187,7 +18266,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1121</v>
       </c>
@@ -18198,7 +18277,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1123</v>
       </c>
@@ -18209,7 +18288,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1125</v>
       </c>
@@ -18220,7 +18299,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1187</v>
       </c>
@@ -18230,8 +18309,148 @@
       <c r="C89" t="s">
         <v>352</v>
       </c>
-      <c r="F89">
+      <c r="G89">
         <v>99852101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C90" t="s">
+        <v>32</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C91" t="s">
+        <v>76</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C92" t="s">
+        <v>618</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C93" t="s">
+        <v>62</v>
+      </c>
+      <c r="E93" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C94" t="s">
+        <v>617</v>
+      </c>
+      <c r="E94" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C95" t="s">
+        <v>923</v>
+      </c>
+      <c r="E95" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C96" t="s">
+        <v>352</v>
+      </c>
+      <c r="F96" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C97" t="s">
+        <v>285</v>
+      </c>
+      <c r="G97">
+        <v>9876540123</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C98" t="s">
+        <v>676</v>
+      </c>
+      <c r="E98" t="s">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1224</v>
       </c>
     </row>
   </sheetData>
@@ -26677,7 +26896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update Excel for TC067-TC079 FOR Smoke
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namita\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A99E82-9C14-4CD5-A206-E088ECBC5753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="1240">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3749,11 +3748,50 @@
   <si>
     <t>SMOKINS20</t>
   </si>
+  <si>
+    <t>SMOKEDEALINS1</t>
+  </si>
+  <si>
+    <t>SmokeTestTata Sons</t>
+  </si>
+  <si>
+    <t>SMOKEDEALINS2</t>
+  </si>
+  <si>
+    <t>SmokeTestTCS</t>
+  </si>
+  <si>
+    <t>SMOKEPFINS1</t>
+  </si>
+  <si>
+    <t>SmokeTestNavatar Company1</t>
+  </si>
+  <si>
+    <t>SMOKEPFINS2</t>
+  </si>
+  <si>
+    <t>SmokeTestNavatar Group</t>
+  </si>
+  <si>
+    <t>SMOKEDEALCON1</t>
+  </si>
+  <si>
+    <t>navatariptesting+1388@gmail.com</t>
+  </si>
+  <si>
+    <t>SmokeTestNavatar</t>
+  </si>
+  <si>
+    <t>SMOKEDEAL1</t>
+  </si>
+  <si>
+    <t>SMOKEDEAL2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -4031,7 +4069,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4308,7 +4346,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4317,15 +4355,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="66" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4535,8 +4573,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4544,19 +4582,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.25" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4631,21 +4669,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.75" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.25" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4826,22 +4864,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="127.625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4945,29 +4983,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view"/>
+    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.625" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.75" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5361,7 +5399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5370,8 +5408,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -5482,7 +5520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5491,23 +5529,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5689,7 +5727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -5698,9 +5736,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -5923,7 +5961,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5932,15 +5970,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.25" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.28515625" style="29" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -6065,7 +6103,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -6074,11 +6112,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6292,7 +6330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6301,8 +6339,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6512,7 +6550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -6521,12 +6559,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6644,7 +6682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6653,8 +6691,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6913,7 +6951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6922,9 +6960,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -7069,7 +7107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7078,9 +7116,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -7150,7 +7188,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7159,13 +7197,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="21.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7218,7 +7256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7227,15 +7265,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" collapsed="1"/>
-    <col min="2" max="2" width="28.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.140625" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7303,7 +7341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -7312,18 +7350,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="65.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.75" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="16.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
@@ -12206,7 +12244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMD23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -12215,13 +12253,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="65.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1018" x14ac:dyDescent="0.25">
@@ -13675,7 +13713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
@@ -13684,12 +13722,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.25" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -14425,22 +14463,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:ALP99"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALP103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1004" x14ac:dyDescent="0.25">
@@ -18169,32 +18207,32 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>1093</v>
-      </c>
-      <c r="B77" s="22" t="s">
-        <v>1094</v>
+        <v>1108</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1109</v>
       </c>
       <c r="C77" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B78" s="22" t="s">
-        <v>1096</v>
+        <v>1110</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1111</v>
       </c>
       <c r="C78" t="s">
-        <v>32</v>
+        <v>285</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>1097</v>
-      </c>
-      <c r="B79" s="22" t="s">
-        <v>1098</v>
+        <v>1112</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1113</v>
       </c>
       <c r="C79" t="s">
         <v>32</v>
@@ -18202,255 +18240,299 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>1108</v>
+        <v>1114</v>
       </c>
       <c r="B80" t="s">
-        <v>1109</v>
+        <v>1115</v>
       </c>
       <c r="C80" t="s">
-        <v>76</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>1110</v>
+        <v>1117</v>
       </c>
       <c r="B81" t="s">
-        <v>1111</v>
+        <v>1118</v>
       </c>
       <c r="C81" t="s">
-        <v>285</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>1112</v>
+        <v>1119</v>
       </c>
       <c r="B82" t="s">
-        <v>1113</v>
+        <v>1120</v>
       </c>
       <c r="C82" t="s">
-        <v>32</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>1114</v>
+        <v>1121</v>
       </c>
       <c r="B83" t="s">
-        <v>1115</v>
+        <v>1122</v>
       </c>
       <c r="C83" t="s">
-        <v>1116</v>
+        <v>618</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>1117</v>
+        <v>1123</v>
       </c>
       <c r="B84" t="s">
-        <v>1118</v>
+        <v>1124</v>
       </c>
       <c r="C84" t="s">
-        <v>1116</v>
+        <v>618</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>1119</v>
+        <v>1125</v>
       </c>
       <c r="B85" t="s">
-        <v>1120</v>
+        <v>1126</v>
       </c>
       <c r="C85" t="s">
-        <v>1116</v>
+        <v>618</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>1121</v>
+        <v>1187</v>
       </c>
       <c r="B86" t="s">
-        <v>1122</v>
+        <v>1188</v>
       </c>
       <c r="C86" t="s">
-        <v>618</v>
+        <v>352</v>
+      </c>
+      <c r="G86">
+        <v>99852101</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>1123</v>
+        <v>1203</v>
       </c>
       <c r="B87" t="s">
-        <v>1124</v>
+        <v>1211</v>
       </c>
       <c r="C87" t="s">
-        <v>618</v>
+        <v>32</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1213</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>1125</v>
+        <v>1204</v>
       </c>
       <c r="B88" t="s">
-        <v>1126</v>
+        <v>1214</v>
       </c>
       <c r="C88" t="s">
-        <v>618</v>
+        <v>76</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>1187</v>
+        <v>1205</v>
       </c>
       <c r="B89" t="s">
-        <v>1188</v>
+        <v>1215</v>
       </c>
       <c r="C89" t="s">
-        <v>352</v>
-      </c>
-      <c r="G89">
-        <v>99852101</v>
+        <v>618</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1216</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>1203</v>
+        <v>1206</v>
       </c>
       <c r="B90" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C90" t="s">
+        <v>62</v>
+      </c>
+      <c r="E90" t="s">
         <v>1211</v>
-      </c>
-      <c r="C90" t="s">
-        <v>32</v>
-      </c>
-      <c r="F90" t="s">
-        <v>1213</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>1204</v>
+        <v>1207</v>
       </c>
       <c r="B91" t="s">
-        <v>1214</v>
+        <v>1218</v>
       </c>
       <c r="C91" t="s">
-        <v>76</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>95</v>
+        <v>617</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1211</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>1205</v>
+        <v>1208</v>
       </c>
       <c r="B92" t="s">
-        <v>1215</v>
+        <v>1219</v>
       </c>
       <c r="C92" t="s">
-        <v>618</v>
-      </c>
-      <c r="F92" t="s">
-        <v>1216</v>
+        <v>923</v>
+      </c>
+      <c r="E92" t="s">
+        <v>1218</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>1206</v>
+        <v>1209</v>
       </c>
       <c r="B93" t="s">
-        <v>1217</v>
+        <v>1220</v>
       </c>
       <c r="C93" t="s">
-        <v>62</v>
-      </c>
-      <c r="E93" t="s">
-        <v>1211</v>
+        <v>352</v>
+      </c>
+      <c r="F93" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
       <c r="B94" t="s">
-        <v>1218</v>
+        <v>1221</v>
       </c>
       <c r="C94" t="s">
-        <v>617</v>
-      </c>
-      <c r="E94" t="s">
-        <v>1211</v>
+        <v>285</v>
+      </c>
+      <c r="G94">
+        <v>9876540123</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>1208</v>
+        <v>1225</v>
       </c>
       <c r="B95" t="s">
-        <v>1219</v>
+        <v>1222</v>
       </c>
       <c r="C95" t="s">
-        <v>923</v>
+        <v>676</v>
       </c>
       <c r="E95" t="s">
-        <v>1218</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>1209</v>
+        <v>1226</v>
       </c>
       <c r="B96" t="s">
-        <v>1220</v>
+        <v>1223</v>
       </c>
       <c r="C96" t="s">
-        <v>352</v>
-      </c>
-      <c r="F96" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>1210</v>
-      </c>
-      <c r="B97" t="s">
-        <v>1221</v>
+        <v>1224</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="32" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>1094</v>
       </c>
       <c r="C97" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B98" s="22" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C98" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C99" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C100" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C101" t="s">
         <v>285</v>
       </c>
-      <c r="G97">
-        <v>9876540123</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B98" t="s">
-        <v>1222</v>
-      </c>
-      <c r="C98" t="s">
-        <v>676</v>
-      </c>
-      <c r="E98" t="s">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>1226</v>
-      </c>
-      <c r="B99" t="s">
-        <v>1223</v>
-      </c>
-      <c r="C99" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D99" t="s">
-        <v>1224</v>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B102" s="22" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C102" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C103" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -18460,26 +18542,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:ALR69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALR71"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+      <selection activeCell="A61" sqref="A61:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.75" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.75" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -22415,202 +22497,230 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1099</v>
+        <v>1127</v>
       </c>
       <c r="B61" t="s">
-        <v>1100</v>
+        <v>1128</v>
       </c>
       <c r="C61" t="s">
-        <v>1101</v>
-      </c>
-      <c r="D61" s="22" t="s">
-        <v>1094</v>
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1113</v>
       </c>
       <c r="E61" t="s">
-        <v>1027</v>
+        <v>1129</v>
+      </c>
+      <c r="F61">
+        <v>996582201</v>
+      </c>
+      <c r="O61">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1127</v>
+        <v>1130</v>
       </c>
       <c r="B62" t="s">
-        <v>1128</v>
+        <v>1131</v>
       </c>
       <c r="C62" t="s">
-        <v>3</v>
+        <v>1101</v>
       </c>
       <c r="D62" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="E62" t="s">
-        <v>1129</v>
+        <v>1132</v>
       </c>
       <c r="F62">
-        <v>996582201</v>
-      </c>
-      <c r="O62">
-        <v>1</v>
+        <v>8954321001</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
       <c r="B63" t="s">
         <v>1131</v>
       </c>
       <c r="C63" t="s">
-        <v>1101</v>
+        <v>1134</v>
       </c>
       <c r="D63" t="s">
-        <v>1115</v>
+        <v>1118</v>
       </c>
       <c r="E63" t="s">
-        <v>1132</v>
+        <v>1135</v>
       </c>
       <c r="F63">
-        <v>8954321001</v>
+        <v>8954321002</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1133</v>
+        <v>1136</v>
       </c>
       <c r="B64" t="s">
         <v>1131</v>
       </c>
       <c r="C64" t="s">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="D64" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="E64" t="s">
-        <v>1135</v>
+        <v>1138</v>
       </c>
       <c r="F64">
-        <v>8954321002</v>
+        <v>8954321003</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1136</v>
+        <v>1139</v>
       </c>
       <c r="B65" t="s">
         <v>1131</v>
       </c>
       <c r="C65" t="s">
-        <v>1137</v>
+        <v>1140</v>
       </c>
       <c r="D65" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="E65" t="s">
-        <v>1138</v>
+        <v>1141</v>
       </c>
       <c r="F65">
-        <v>8954321003</v>
+        <v>8954321004</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1139</v>
+        <v>1142</v>
       </c>
       <c r="B66" t="s">
         <v>1131</v>
       </c>
       <c r="C66" t="s">
-        <v>1140</v>
+        <v>1143</v>
       </c>
       <c r="D66" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="E66" t="s">
-        <v>1141</v>
+        <v>1144</v>
       </c>
       <c r="F66">
-        <v>8954321004</v>
+        <v>8954321005</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1142</v>
+        <v>1145</v>
       </c>
       <c r="B67" t="s">
         <v>1131</v>
       </c>
       <c r="C67" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
       <c r="D67" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="E67" t="s">
-        <v>1144</v>
+        <v>1147</v>
       </c>
       <c r="F67">
-        <v>8954321005</v>
+        <v>8954321006</v>
+      </c>
+      <c r="O67">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1145</v>
+        <v>1189</v>
       </c>
       <c r="B68" t="s">
-        <v>1131</v>
+        <v>1190</v>
       </c>
       <c r="C68" t="s">
-        <v>1146</v>
+        <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>1126</v>
-      </c>
-      <c r="E68" t="s">
-        <v>1147</v>
+        <v>1188</v>
       </c>
       <c r="F68">
-        <v>8954321006</v>
-      </c>
-      <c r="O68">
-        <v>1</v>
+        <v>99852556</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>1189</v>
+      <c r="A69" s="32" t="s">
+        <v>1099</v>
       </c>
       <c r="B69" t="s">
-        <v>1190</v>
+        <v>1100</v>
       </c>
       <c r="C69" t="s">
-        <v>3</v>
-      </c>
-      <c r="D69" t="s">
-        <v>1188</v>
-      </c>
-      <c r="F69">
-        <v>99852556</v>
+        <v>1101</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C70" t="s">
+        <v>106</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C71" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71" s="22" t="s">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
+    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
+    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com"/>
+    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com"/>
+    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com"/>
+    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com"/>
+    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com"/>
+    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22619,9 +22729,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -22669,7 +22779,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -22678,16 +22788,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -22909,24 +23019,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMM69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMM71"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1027" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -26885,6 +26995,30 @@
         <v>30</v>
       </c>
     </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="32" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D70" t="s">
+        <v>30</v>
+      </c>
+      <c r="F70" s="22"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D71" t="s">
+        <v>30</v>
+      </c>
+      <c r="F71" s="22"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26893,7 +27027,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26902,14 +27036,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Tc 27 to 30
Signed-off-by: Ravi Kumar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,47 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namita\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{C8D8BF65-5B42-43E7-BF3C-2D1764BE67D7}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" firstSheet="3" activeTab="7"/>
+    <workbookView activeTab="4" firstSheet="3" tabRatio="926" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="FilePath" sheetId="18" r:id="rId1"/>
-    <sheet name="FieldSet" sheetId="1" r:id="rId2"/>
-    <sheet name="FieldComponent" sheetId="6" r:id="rId3"/>
-    <sheet name="Entities" sheetId="3" r:id="rId4"/>
-    <sheet name="Contacts" sheetId="2" r:id="rId5"/>
-    <sheet name="Test Custom Object" sheetId="23" r:id="rId6"/>
-    <sheet name="Fund" sheetId="7" r:id="rId7"/>
-    <sheet name="Deal" sheetId="4" r:id="rId8"/>
-    <sheet name="Fundraisings" sheetId="28" r:id="rId9"/>
-    <sheet name="DealRequestTracker" sheetId="14" r:id="rId10"/>
-    <sheet name="CustomSDG" sheetId="13" r:id="rId11"/>
-    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId12"/>
-    <sheet name="MarketingEvent" sheetId="15" r:id="rId13"/>
-    <sheet name="Partnerships" sheetId="8" r:id="rId14"/>
-    <sheet name="Commitments" sheetId="9" r:id="rId15"/>
-    <sheet name="Task" sheetId="12" r:id="rId16"/>
-    <sheet name="UploadImageData" sheetId="17" r:id="rId17"/>
-    <sheet name="Fields" sheetId="19" r:id="rId18"/>
-    <sheet name="Attendees" sheetId="20" r:id="rId19"/>
-    <sheet name="Deal Team" sheetId="21" r:id="rId20"/>
-    <sheet name="Coverages" sheetId="22" r:id="rId21"/>
-    <sheet name="SDGActions" sheetId="24" r:id="rId22"/>
-    <sheet name="Report" sheetId="25" r:id="rId23"/>
-    <sheet name="CustomEmailFolder" sheetId="26" r:id="rId24"/>
-    <sheet name="Task1" sheetId="27" r:id="rId25"/>
-    <sheet name="Events" sheetId="29" r:id="rId26"/>
+    <sheet name="FilePath" r:id="rId1" sheetId="18"/>
+    <sheet name="FieldSet" r:id="rId2" sheetId="1"/>
+    <sheet name="FieldComponent" r:id="rId3" sheetId="6"/>
+    <sheet name="Entities" r:id="rId4" sheetId="3"/>
+    <sheet name="Contacts" r:id="rId5" sheetId="2"/>
+    <sheet name="Test Custom Object" r:id="rId6" sheetId="23"/>
+    <sheet name="Fund" r:id="rId7" sheetId="7"/>
+    <sheet name="Deal" r:id="rId8" sheetId="4"/>
+    <sheet name="Fundraisings" r:id="rId9" sheetId="28"/>
+    <sheet name="DealRequestTracker" r:id="rId10" sheetId="14"/>
+    <sheet name="CustomSDG" r:id="rId11" sheetId="13"/>
+    <sheet name="ToggleButtonCheck" r:id="rId12" sheetId="16"/>
+    <sheet name="MarketingEvent" r:id="rId13" sheetId="15"/>
+    <sheet name="Partnerships" r:id="rId14" sheetId="8"/>
+    <sheet name="Commitments" r:id="rId15" sheetId="9"/>
+    <sheet name="Task" r:id="rId16" sheetId="12"/>
+    <sheet name="UploadImageData" r:id="rId17" sheetId="17"/>
+    <sheet name="Fields" r:id="rId18" sheetId="19"/>
+    <sheet name="Attendees" r:id="rId19" sheetId="20"/>
+    <sheet name="Deal Team" r:id="rId20" sheetId="21"/>
+    <sheet name="Coverages" r:id="rId21" sheetId="22"/>
+    <sheet name="SDGActions" r:id="rId22" sheetId="24"/>
+    <sheet name="Report" r:id="rId23" sheetId="25"/>
+    <sheet name="CustomEmailFolder" r:id="rId24" sheetId="26"/>
+    <sheet name="Task1" r:id="rId25" sheetId="27"/>
+    <sheet name="Events" r:id="rId26" sheetId="29"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2125" uniqueCount="1246">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3787,11 +3788,29 @@
   <si>
     <t>SMOKEDEAL2</t>
   </si>
+  <si>
+    <t>SMOKCON9</t>
+  </si>
+  <si>
+    <t>Test Instituion-1</t>
+  </si>
+  <si>
+    <t>navatariptesting+61187@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+60618@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+46249@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+6477@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -3938,141 +3957,141 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="64">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="14" quotePrefix="1" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4089,10 +4108,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -4127,7 +4146,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -4162,7 +4181,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -4256,21 +4275,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -4287,7 +4306,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -4339,15 +4358,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -4355,15 +4374,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="66" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="89.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="81.75" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.25" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="30.875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="29.125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="66.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4431,7 +4450,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>563</v>
       </c>
@@ -4573,28 +4592,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="L2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId2" ref="B5" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="18.875" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="5" width="15.25" collapsed="true"/>
+    <col min="5" max="16384" style="5" width="9.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4614,10 +4633,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
-    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -4663,27 +4682,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="11.75" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="27.25" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="20.125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="19.125" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4703,7 +4722,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4737,7 +4756,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>313</v>
       </c>
@@ -4771,7 +4790,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -4859,27 +4878,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="22.875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="18.875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="12.125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="32.125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="127.625" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4902,7 +4921,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
@@ -4910,7 +4929,7 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
     </row>
-    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -4983,29 +5002,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view"/>
-    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view"/>
+    <hyperlink display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" r:id="rId1" ref="C5" tooltip="TestAzAlexa Deal" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" r:id="rId2" ref="C4" tooltip="TestAzAlexa Info" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="21.875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="20.625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="13.75" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="11.0" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5025,14 +5044,14 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
     </row>
-    <row r="3" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
@@ -5364,7 +5383,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="29" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
@@ -5393,14 +5412,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -5408,13 +5427,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -5428,10 +5447,10 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
     </row>
-    <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>510</v>
@@ -5461,7 +5480,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>523</v>
@@ -5469,7 +5488,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>766</v>
       </c>
@@ -5478,17 +5497,17 @@
       </c>
       <c r="C8" s="22"/>
     </row>
-    <row r="9" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
     </row>
-    <row r="10" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="22"/>
     </row>
-    <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>524</v>
@@ -5496,7 +5515,7 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>444</v>
       </c>
@@ -5505,7 +5524,7 @@
       </c>
       <c r="C12" s="22"/>
     </row>
-    <row r="13" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>446</v>
       </c>
@@ -5515,13 +5534,13 @@
       <c r="C13" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
@@ -5529,26 +5548,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.75" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.25" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="27.125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="8.75" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="1" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -5610,7 +5629,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" t="s">
         <v>572</v>
@@ -5622,7 +5641,7 @@
       <c r="Q2" s="48"/>
       <c r="S2" s="48"/>
     </row>
-    <row r="3" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
@@ -5683,7 +5702,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="7" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
@@ -5707,14 +5726,14 @@
       <c r="S7" s="16"/>
       <c r="T7" s="13"/>
     </row>
-    <row r="8" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>448</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="22"/>
     </row>
-    <row r="9" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>449</v>
       </c>
@@ -5722,13 +5741,13 @@
       <c r="C9" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
@@ -5736,12 +5755,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.25" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -5761,7 +5780,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="13"/>
@@ -5853,7 +5872,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="15" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="13"/>
@@ -5877,7 +5896,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="13"/>
     </row>
-    <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>534</v>
       </c>
@@ -5894,7 +5913,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>539</v>
       </c>
@@ -5911,7 +5930,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>543</v>
       </c>
@@ -5931,7 +5950,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="23" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="13"/>
@@ -5956,13 +5975,13 @@
       <c r="T23" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -5970,18 +5989,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.28515625" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="29" width="16.125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="29" width="24.25" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -6098,13 +6117,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -6112,11 +6131,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6325,13 +6344,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -6339,8 +6358,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6545,13 +6564,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -6559,15 +6578,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="77.625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -6587,7 +6606,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -6676,14 +6695,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -6691,8 +6710,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.25" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6946,13 +6965,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
@@ -6960,9 +6979,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.75" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6976,12 +6995,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="53"/>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
     </row>
-    <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>526</v>
@@ -7102,13 +7121,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -7116,10 +7135,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -7142,7 +7161,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row ht="150" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>553</v>
       </c>
@@ -7162,7 +7181,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row ht="210" r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>558</v>
       </c>
@@ -7183,13 +7202,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -7197,13 +7216,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="21.375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7250,14 +7269,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -7265,15 +7284,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.25" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.25" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="29.125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7305,7 +7324,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>594</v>
       </c>
@@ -7334,15 +7353,15 @@
         <v>599</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row customHeight="1" ht="15" r="6" spans="1:9" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <dimension ref="A1:AMK47"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
@@ -7350,18 +7369,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="65.625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.75" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.75" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.25" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="26.375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.625" collapsed="true"/>
+    <col min="12" max="13" bestFit="true" customWidth="true" width="16.25" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
@@ -12158,7 +12177,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="40" s="32" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>1102</v>
@@ -12239,13 +12258,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMD23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <dimension ref="A1:AME23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:XFD24"/>
@@ -12253,13 +12272,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="65.625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.75" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1018" x14ac:dyDescent="0.25">
@@ -13679,7 +13698,7 @@
       <c r="I19" s="62"/>
       <c r="J19" s="62"/>
     </row>
-    <row r="21" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="21" s="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="32" t="s">
         <v>1092</v>
       </c>
@@ -13708,13 +13727,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
@@ -13722,15 +13741,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.25" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.25" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.25" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -14458,27 +14477,27 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALP103"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:ALQ103"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.25" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1004" x14ac:dyDescent="0.25">
@@ -15501,7 +15520,7 @@
       <c r="ALO1" s="5"/>
       <c r="ALP1" s="5"/>
     </row>
-    <row r="2" spans="1:1004" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="35"/>
@@ -17709,7 +17728,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="24" s="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>523</v>
@@ -17739,7 +17758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="13.5" r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>611</v>
       </c>
@@ -17811,7 +17830,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="33" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>769</v>
       </c>
@@ -17837,22 +17856,22 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="35" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="20"/>
       <c r="C35" s="22"/>
     </row>
-    <row r="36" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="36" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="22"/>
     </row>
-    <row r="37" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="37" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
     </row>
-    <row r="38" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="38" s="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>513</v>
@@ -17882,7 +17901,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="42" s="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>524</v>
@@ -17890,7 +17909,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="43" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>143</v>
       </c>
@@ -17901,7 +17920,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="44" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>442</v>
       </c>
@@ -17910,13 +17929,13 @@
       </c>
       <c r="C44" s="22"/>
     </row>
-    <row r="46" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="46" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="53"/>
       <c r="B46" s="53"/>
       <c r="C46" s="53"/>
       <c r="D46" s="53"/>
     </row>
-    <row r="47" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="47" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>639</v>
@@ -17924,7 +17943,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="48" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>640</v>
       </c>
@@ -18178,7 +18197,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="73" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3" t="s">
         <v>953</v>
@@ -18197,7 +18216,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="14.25" r="76" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3" t="s">
         <v>1092</v>
@@ -18537,31 +18556,31 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALR71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:ALS72"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:XFD61"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="17.75" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.75" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.75" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -19602,7 +19621,7 @@
       <c r="ALQ1" s="5"/>
       <c r="ALR1" s="5"/>
     </row>
-    <row r="2" spans="1:1006" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -21807,7 +21826,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
         <v>506</v>
       </c>
@@ -21824,7 +21843,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="19" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>610</v>
       </c>
@@ -21838,7 +21857,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="20" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
         <v>765</v>
       </c>
@@ -21850,7 +21869,7 @@
       </c>
       <c r="E20" s="54"/>
     </row>
-    <row r="21" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="21" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
         <v>768</v>
       </c>
@@ -21862,7 +21881,7 @@
       </c>
       <c r="E21" s="54"/>
     </row>
-    <row r="22" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="22" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E22" s="54"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -22104,7 +22123,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="34" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
         <v>808</v>
       </c>
@@ -22121,7 +22140,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="35" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="53"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
@@ -22147,7 +22166,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="37" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="50" t="s">
         <v>956</v>
       </c>
@@ -22164,7 +22183,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="38" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="50" t="s">
         <v>960</v>
       </c>
@@ -22181,7 +22200,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="39" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="50" t="s">
         <v>964</v>
       </c>
@@ -22198,7 +22217,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="40" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
         <v>985</v>
       </c>
@@ -22215,7 +22234,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="41" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="50" t="s">
         <v>986</v>
       </c>
@@ -22232,7 +22251,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="42" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="50" t="s">
         <v>987</v>
       </c>
@@ -22249,7 +22268,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="43" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="50" t="s">
         <v>1005</v>
       </c>
@@ -22266,7 +22285,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="44" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="50" t="s">
         <v>1010</v>
       </c>
@@ -22283,7 +22302,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="45" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="50" t="s">
         <v>1008</v>
       </c>
@@ -22300,7 +22319,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="46" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="50" t="s">
         <v>1009</v>
       </c>
@@ -22317,7 +22336,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="47" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="50" t="s">
         <v>1018</v>
       </c>
@@ -22334,7 +22353,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="48" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="50" t="s">
         <v>1054</v>
       </c>
@@ -22351,7 +22370,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="49" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="50" t="s">
         <v>1057</v>
       </c>
@@ -22368,7 +22387,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="50" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="50" t="s">
         <v>1060</v>
       </c>
@@ -22385,7 +22404,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="51" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="50" t="s">
         <v>1063</v>
       </c>
@@ -22402,7 +22421,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="52" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="53"/>
       <c r="B52" s="51"/>
       <c r="C52" s="51"/>
@@ -22414,7 +22433,7 @@
       <c r="I52" s="53"/>
       <c r="J52" s="53"/>
     </row>
-    <row r="54" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="54" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
     </row>
@@ -22659,69 +22678,86 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="32" t="s">
-        <v>1099</v>
+      <c r="A69" t="s">
+        <v>1240</v>
       </c>
       <c r="B69" t="s">
-        <v>1100</v>
+        <v>25</v>
       </c>
       <c r="C69" t="s">
         <v>1101</v>
       </c>
-      <c r="D69" s="22" t="s">
-        <v>1094</v>
+      <c r="D69" t="s">
+        <v>1241</v>
       </c>
       <c r="E69" t="s">
-        <v>1027</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>1235</v>
+      <c r="A70" s="32" t="s">
+        <v>1099</v>
       </c>
       <c r="B70" t="s">
         <v>1100</v>
       </c>
       <c r="C70" t="s">
-        <v>106</v>
+        <v>1101</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>1230</v>
+        <v>1094</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B71" t="s">
-        <v>1237</v>
+        <v>1100</v>
       </c>
       <c r="C71" t="s">
         <v>106</v>
       </c>
       <c r="D71" s="22" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C72" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="22" t="s">
         <v>1234</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
-    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
-    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com"/>
-    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com"/>
-    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com"/>
-    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com"/>
-    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com"/>
-    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com"/>
+    <hyperlink display="mailto:dealroom1.2+clientcontact01@gmail.com" r:id="rId1" ref="E56" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink display="mailto:dealroom1.2+clientcontact13@gmail.com" r:id="rId2" ref="E57" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink display="mailto:navatariptesting+11679@gmail.com" r:id="rId3" ref="E37" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink display="mailto:navatariptesting+18785@gmail.com" r:id="rId4" ref="E38" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink display="mailto:navatariptesting+49153@gmail.com" r:id="rId5" ref="E39" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink display="mailto:navatariptesting+11679@gmail.com" r:id="rId6" ref="E40" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink display="mailto:navatariptesting+18785@gmail.com" r:id="rId7" ref="E41" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink display="mailto:navatariptesting+49153@gmail.com" r:id="rId8" ref="E42" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD4"/>
@@ -22729,9 +22765,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -22745,7 +22781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -22774,13 +22810,13 @@
       <c r="C4" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
@@ -22788,19 +22824,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.75" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.25" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.25" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -22832,7 +22868,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -22844,7 +22880,7 @@
       <c r="I2" s="39"/>
       <c r="J2" s="41"/>
     </row>
-    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -22886,12 +22922,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -22905,7 +22941,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>507</v>
       </c>
@@ -22919,7 +22955,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -22933,7 +22969,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>144</v>
       </c>
@@ -22947,7 +22983,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>145</v>
       </c>
@@ -23014,32 +23050,32 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMM71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AMN71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.75" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.75" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.75" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1027" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -24096,7 +24132,7 @@
       <c r="AML1" s="6"/>
       <c r="AMM1" s="6"/>
     </row>
-    <row r="2" spans="1:1027" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="44" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -25125,7 +25161,7 @@
       <c r="AML2" s="43"/>
       <c r="AMM2" s="43"/>
     </row>
-    <row r="3" spans="1:1027" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -26413,7 +26449,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="24" s="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
@@ -26425,7 +26461,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>146</v>
       </c>
@@ -26768,7 +26804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="52" s="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
@@ -26828,7 +26864,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="61" s="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4" t="s">
@@ -27021,14 +27057,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
@@ -27036,17 +27072,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="22.625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -27123,7 +27159,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -27244,6 +27280,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added TC094-095 OF Smoke
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namita\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87891C95-DB84-410E-80F4-5AF18C7948C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" firstSheet="14" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -39,6 +38,7 @@
     <sheet name="CustomEmailFolder" sheetId="26" r:id="rId24"/>
     <sheet name="Task1" sheetId="27" r:id="rId25"/>
     <sheet name="Events" sheetId="29" r:id="rId26"/>
+    <sheet name="MI" sheetId="30" r:id="rId27"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="1246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="1249">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3806,11 +3806,20 @@
   <si>
     <t>SMOKCON9</t>
   </si>
+  <si>
+    <t>Marketing_InitiativeName</t>
+  </si>
+  <si>
+    <t>SmokeMI1</t>
+  </si>
+  <si>
+    <t>M1TestMarketingInitiative</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -4088,7 +4097,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4365,7 +4374,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4374,15 +4383,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="66" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4592,8 +4601,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4601,19 +4610,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.25" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4688,21 +4697,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.75" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.25" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4883,22 +4892,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="127.625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5002,29 +5011,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view"/>
+    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.625" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.75" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5418,7 +5427,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5427,8 +5436,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -5539,7 +5548,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5548,23 +5557,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5746,7 +5755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -5755,9 +5764,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -5980,7 +5989,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5989,15 +5998,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.25" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.28515625" style="29" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -6122,7 +6131,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -6131,11 +6140,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -6349,7 +6358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6358,8 +6367,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6569,7 +6578,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -6578,12 +6587,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6701,7 +6710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6710,8 +6719,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6970,7 +6979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6979,9 +6988,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -7126,7 +7135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7135,9 +7144,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -7207,7 +7216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7216,13 +7225,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="21.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7275,7 +7284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7284,15 +7293,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" collapsed="1"/>
-    <col min="2" max="2" width="28.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.140625" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -7360,7 +7369,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -7369,18 +7378,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="65.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.75" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="16.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
@@ -12263,7 +12272,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMD23"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -12272,13 +12281,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="65.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1018" x14ac:dyDescent="0.25">
@@ -13731,8 +13740,43 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17:K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
@@ -13741,12 +13785,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.25" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -14482,22 +14526,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALP103"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1004" x14ac:dyDescent="0.25">
@@ -18561,26 +18605,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.75" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.75" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -22739,21 +22783,21 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
+    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
+    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com"/>
+    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com"/>
+    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com"/>
+    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com"/>
+    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com"/>
+    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22762,9 +22806,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -22812,7 +22856,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -22821,16 +22865,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -23066,7 +23110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM71"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
@@ -23075,15 +23119,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1027" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -27074,7 +27118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27083,14 +27127,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added FSTG page layout and compact layout field verification  test cases
Signed-off-by: Navatar <rkumar1@navatargroup.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -9,42 +9,44 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
     <sheet name="FSTGListView" sheetId="37" r:id="rId2"/>
-    <sheet name="FSTGVerifyField" sheetId="36" r:id="rId3"/>
-    <sheet name="FieldSet" sheetId="1" r:id="rId4"/>
-    <sheet name="FieldComponent" sheetId="6" r:id="rId5"/>
-    <sheet name="Entities" sheetId="3" r:id="rId6"/>
-    <sheet name="Contacts" sheetId="2" r:id="rId7"/>
-    <sheet name="Test Custom Object" sheetId="23" r:id="rId8"/>
-    <sheet name="Fund" sheetId="7" r:id="rId9"/>
-    <sheet name="FundInvestment" sheetId="34" r:id="rId10"/>
-    <sheet name="FundDistribution" sheetId="33" r:id="rId11"/>
-    <sheet name="FundDrawdown" sheetId="32" r:id="rId12"/>
-    <sheet name="Deal" sheetId="4" r:id="rId13"/>
-    <sheet name="Fundraisings" sheetId="28" r:id="rId14"/>
-    <sheet name="DealRequestTracker" sheetId="14" r:id="rId15"/>
-    <sheet name="CustomSDG" sheetId="13" r:id="rId16"/>
-    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId17"/>
-    <sheet name="MarketingEvent" sheetId="15" r:id="rId18"/>
-    <sheet name="Partnerships" sheetId="8" r:id="rId19"/>
-    <sheet name="AgreementsAmendments" sheetId="35" r:id="rId20"/>
-    <sheet name="Commitments" sheetId="9" r:id="rId21"/>
-    <sheet name="Task" sheetId="12" r:id="rId22"/>
-    <sheet name="UploadImageData" sheetId="17" r:id="rId23"/>
-    <sheet name="Fields" sheetId="19" r:id="rId24"/>
-    <sheet name="Attendees" sheetId="20" r:id="rId25"/>
-    <sheet name="Deal Team" sheetId="21" r:id="rId26"/>
-    <sheet name="Coverages" sheetId="22" r:id="rId27"/>
-    <sheet name="SDGActions" sheetId="24" r:id="rId28"/>
-    <sheet name="Report" sheetId="25" r:id="rId29"/>
-    <sheet name="CustomEmailFolder" sheetId="26" r:id="rId30"/>
-    <sheet name="Task1" sheetId="27" r:id="rId31"/>
-    <sheet name="Events" sheetId="29" r:id="rId32"/>
-    <sheet name="MI" sheetId="30" r:id="rId33"/>
+    <sheet name="FSTGCompactLayoutField" sheetId="39" r:id="rId3"/>
+    <sheet name="FSTGPageLayoutField" sheetId="38" r:id="rId4"/>
+    <sheet name="FSTGVerifyField" sheetId="36" r:id="rId5"/>
+    <sheet name="FieldSet" sheetId="1" r:id="rId6"/>
+    <sheet name="FieldComponent" sheetId="6" r:id="rId7"/>
+    <sheet name="Entities" sheetId="3" r:id="rId8"/>
+    <sheet name="Contacts" sheetId="2" r:id="rId9"/>
+    <sheet name="Test Custom Object" sheetId="23" r:id="rId10"/>
+    <sheet name="Fund" sheetId="7" r:id="rId11"/>
+    <sheet name="FundInvestment" sheetId="34" r:id="rId12"/>
+    <sheet name="FundDistribution" sheetId="33" r:id="rId13"/>
+    <sheet name="FundDrawdown" sheetId="32" r:id="rId14"/>
+    <sheet name="Deal" sheetId="4" r:id="rId15"/>
+    <sheet name="Fundraisings" sheetId="28" r:id="rId16"/>
+    <sheet name="DealRequestTracker" sheetId="14" r:id="rId17"/>
+    <sheet name="CustomSDG" sheetId="13" r:id="rId18"/>
+    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId19"/>
+    <sheet name="MarketingEvent" sheetId="15" r:id="rId20"/>
+    <sheet name="Partnerships" sheetId="8" r:id="rId21"/>
+    <sheet name="AgreementsAmendments" sheetId="35" r:id="rId22"/>
+    <sheet name="Commitments" sheetId="9" r:id="rId23"/>
+    <sheet name="Task" sheetId="12" r:id="rId24"/>
+    <sheet name="UploadImageData" sheetId="17" r:id="rId25"/>
+    <sheet name="Fields" sheetId="19" r:id="rId26"/>
+    <sheet name="Attendees" sheetId="20" r:id="rId27"/>
+    <sheet name="Deal Team" sheetId="21" r:id="rId28"/>
+    <sheet name="Coverages" sheetId="22" r:id="rId29"/>
+    <sheet name="SDGActions" sheetId="24" r:id="rId30"/>
+    <sheet name="Report" sheetId="25" r:id="rId31"/>
+    <sheet name="CustomEmailFolder" sheetId="26" r:id="rId32"/>
+    <sheet name="Task1" sheetId="27" r:id="rId33"/>
+    <sheet name="Events" sheetId="29" r:id="rId34"/>
+    <sheet name="MI" sheetId="30" r:id="rId35"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="1321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2340" uniqueCount="1380">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -4037,7 +4039,202 @@
     <t>All Institutions,All Companies,All Intermediaries,All Fund Manager's Funds</t>
   </si>
   <si>
-    <t>All Institutions&lt;filter&gt;Filter by Owner All Institutions&lt;break&gt;All Companies&lt;filter&gt;Filter by Owner All Institutions#Record type equals Company&lt;break&gt;All Intermediaries&lt;filter&gt;Filter by Owner All Institutions#Institution Type includes Advisors,Bank,Broker,Intermediaries#Record type equals Intermediary&lt;break&gt;All Fund Manager's Funds&lt;fiter&gt;Filter by Owner All Institutions#Record type equals Fund manager's Fund</t>
+    <t>All Institutions&lt;filter&gt;Filter by Owner All Institutions&lt;break&gt;All Companies&lt;filter&gt;Filter by Owner All Institutions#Record type equals Company&lt;break&gt;All Intermediaries&lt;filter&gt;Filter by Owner All Institutions#Institution Type includes Advisors,Bank,Broker,Intermediaries#Record type equals Intermediary&lt;break&gt;All Fund Manager's Funds&lt;filter&gt;Filter by Owner All Institutions#Record type equals Fund manager's Fund</t>
+  </si>
+  <si>
+    <t>Firm Events&lt;pl&gt;Marketing Event Name#Budget#Co-ordinator#Start Date#End Date#Sector#Location#Region#Status#Total Expense#Event Type&lt;break&gt;
+Third Party Events&lt;pl&gt;Marketing Event Name#Main Contact#Organizer#Start Date#End Date#Sector#Location#Region#Event Type</t>
+  </si>
+  <si>
+    <t>Advisor&lt;pl&gt;Entity Type#Sector#Region&lt;break&gt;
+Company&lt;pl&gt;Entity Type#Deal Conversion Date#Introduced By#Introduction Date#Status#Tier#Investment Type#Sector#Region&lt;break&gt;
+Individual Investor&lt;pl&gt;Entity Type#Total Commitments (mn)#Fund Preferences#Sector#Region&lt;break&gt;
+Portfolio Company&lt;pl&gt;Deal Conversion Date#Entity Type#Introduced By#Introduction Date#Status#Investment Type#Sector#Region&lt;break&gt;
+Institution&lt;pl&gt;Entity Type#Total Commitments (mn)#Fund Preferences#Sector#Region&lt;break&gt;
+Intermediary&lt;pl&gt;Entity Type#Tier#Sector#Region&lt;break&gt;
+Lender&lt;pl&gt;Entity Type#Sector#Region&lt;break&gt;
+Fund Manager&lt;pl&gt;Fund Preferences#Sector#Region&lt;break&gt;
+Fund Manager’s Fund&lt;pl&gt;Status#Sector#Region</t>
+  </si>
+  <si>
+    <t>FieldVar5</t>
+  </si>
+  <si>
+    <t>FieldVar6</t>
+  </si>
+  <si>
+    <t>FieldVar7</t>
+  </si>
+  <si>
+    <t>FieldVar8</t>
+  </si>
+  <si>
+    <t>FieldVar9</t>
+  </si>
+  <si>
+    <t>FieldVar10</t>
+  </si>
+  <si>
+    <t>FieldVar11</t>
+  </si>
+  <si>
+    <t>FieldVar12</t>
+  </si>
+  <si>
+    <t>FieldVar13</t>
+  </si>
+  <si>
+    <t>FieldVar14</t>
+  </si>
+  <si>
+    <t>FieldVar15</t>
+  </si>
+  <si>
+    <t>Affiliation</t>
+  </si>
+  <si>
+    <t>Financing</t>
+  </si>
+  <si>
+    <t>Fundraising</t>
+  </si>
+  <si>
+    <t>Fundraising Contact</t>
+  </si>
+  <si>
+    <t>Pipeline Snapshot</t>
+  </si>
+  <si>
+    <t>Request Tracker</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Sortable Data Grid</t>
+  </si>
+  <si>
+    <t>Sortable Data Grid Action</t>
+  </si>
+  <si>
+    <t>Sortable Data Grid Field</t>
+  </si>
+  <si>
+    <t>Sortable Data Grid Prefrence</t>
+  </si>
+  <si>
+    <t>Valuation</t>
+  </si>
+  <si>
+    <t>FieldVar16</t>
+  </si>
+  <si>
+    <t>FieldVar17</t>
+  </si>
+  <si>
+    <t>FieldVar18</t>
+  </si>
+  <si>
+    <t>FieldVar19</t>
+  </si>
+  <si>
+    <t>FieldVar20</t>
+  </si>
+  <si>
+    <t>FieldVar21</t>
+  </si>
+  <si>
+    <t>FieldVar22</t>
+  </si>
+  <si>
+    <t>Affiliation Layout&lt;pl&gt;Start Date#End Date</t>
+  </si>
+  <si>
+    <t>Attendee Layout&lt;pl&gt;Attendee ID#Attendee Contact#Attendee Staff#Marketing Event#Notes#Status</t>
+  </si>
+  <si>
+    <t>Contact Layout&lt;pl&gt;Last Touchpoint#Relationship Classification#Touchpoint Overdue#Profile Image#Sector Expertise#Sector#Region#Average Deal Quality Score#Z_(Internal)_TDS#Total Deals Shown#Industry Focus#Tier#Z_Internal_Current_Date#Next Touchpoint Date</t>
+  </si>
+  <si>
+    <t>Deal Expert</t>
+  </si>
+  <si>
+    <t>Deal Expert Layout&lt;pl&gt;Deal Expert ID#Deal Expert#Expert Fees#Hours Spent#Notes#Deal#Status</t>
+  </si>
+  <si>
+    <t>Deal Team Layout&lt;pl&gt;Deal Team ID#Deal#Deal Contact#Deal Contact Type#Team Member#Team Member Role</t>
+  </si>
+  <si>
+    <t>Financing Layout&lt;pl&gt;Deal#Lender Status#Notes#Date#Exit Date#Ownership</t>
+  </si>
+  <si>
+    <t>Fund Layout&lt;pl&gt;Sector#Region</t>
+  </si>
+  <si>
+    <t>Fundraising Layout&lt;pl&gt;Last Stage Change Date#Closing Date#Reason for Decline</t>
+  </si>
+  <si>
+    <t>Fundraising Contact Layout&lt;pl&gt;Role</t>
+  </si>
+  <si>
+    <t>Navigation Layout&lt;pl&gt;Action Object#Action Record Type#Activities Button API Name#List View Name#List View Object#Navigation Label#Order#Parent#URL</t>
+  </si>
+  <si>
+    <t>Pipeline Layout&lt;pl&gt;Reason for Decline#LOI Due Date#Management Meeting Date#Stage#Platform Company#Reason to Park#Z_(Internal)_DQS#Deal Quality Score#EBITDA / Sales#Multiple#Z_(Internal)_CompanyId</t>
+  </si>
+  <si>
+    <t>Pipeline Snapshot Layout&lt;pl&gt;Stage#Pipeline Snapshot ID#Company Name#Confidentiality Agreement Signed#Industry#Institution#Log In Date#NDA Signed Date#Pipeline#Pipeline Comments#Pipeline Name#Snapshot Date#Snapshot Month#Snapshot Month (Date)#Source Contact#Source Firm#Stage</t>
+  </si>
+  <si>
+    <t>Request Tracker Layout&lt;pl&gt;Request Tracker ID#Date Requested#Deal#Notes#Priority#Request#Response#Status#Request Type</t>
+  </si>
+  <si>
+    <t>Review Layout&lt;pl&gt;Review#Comments#Review Date#Deal#Decision</t>
+  </si>
+  <si>
+    <t>SDG Layout&lt;pl&gt;All Rows#Default Sort#Disable Sharing Rules#Enable Inline Edit#Enable Manage Fields#Filter#Grouping Field API#Highlight Colors#Is Valid#List View Name#My Home#My Records#My Teams Records#Parent Field Name#Related Association Query#Remember Filter#SDG Name#SDG Tag#Show Icon#sObjectName</t>
+  </si>
+  <si>
+    <t>SDG Action Layout&lt;pl&gt;Action Order#Name#Action Type#Event#Event Payload#Icon#Requires Createable#Requires Deletable#Requires Editable#SDG</t>
+  </si>
+  <si>
+    <t>Time Log</t>
+  </si>
+  <si>
+    <t>Time Log Layout&lt;pl&gt;Time Log ID#Function#Fund#Hours#Deal#Staff#Date</t>
+  </si>
+  <si>
+    <t>Valuation Layout&lt;pl&gt;Valuation Name#Company#Valuation Date#Frequency#IRR#Total Dividend#Total Investment#Total Valuation</t>
+  </si>
+  <si>
+    <t>Field Layout&lt;pl&gt;APIName#Color#Custom Renderer#FieldOrder#Filter Sequence#Grouping Query#Hide Filter#Image Field API#Is Hidden#Is Valid#Name#Override Label#Parent Field Name#Redirect URL#sdg#URL</t>
+  </si>
+  <si>
+    <t>Sortable Data Grid Preference Layout&lt;pl&gt;Filters#IsExpanded#Owner#sdgKey#Sortable Data Grid Preferences Name#User</t>
+  </si>
+  <si>
+    <t>Portfolio_Company_Highlight&lt;cl&gt;Phone#Entity Type#Sector#Region#LTM Revenue#LTM EBITDA&lt;break&gt;
+Company_Highlight&lt;cl&gt;Website#Status#Phone#Sector#Region&lt;break&gt;
+Intermediary_Highlight&lt;cl&gt;Total Deals Shown#Average Deal Quality Score#Website#Sector#Region&lt;break&gt;
+Institution_Highlight&lt;cl&gt;Website#Entity Type#Phone#Total Fund Commitments (mn)#Total Co-investment Commitments (mn)&lt;break&gt;
+Limited_Partner_Highlight&lt;cl&gt;Parent Institution#Total Fund Commitments (mn)#Total Co-investment Commitments (mn)#Website#Phone&lt;break&gt;
+Advisor_Highlight&lt;cl&gt;Phone#Website#EntityType#Sector#Region&lt;break&gt;
+Individual_Investor_Highlight&lt;cl&gt;Phone#Total Fund Commitments (mn)#Total Co-investment Commitments (mn)#Sector#Region&lt;break&gt;
+Lender_Highlight&lt;cl&gt;Phone#Website#Annual Revenue#Sector#Region&lt;break&gt;
+Fund_Manager_Highlight&lt;cl&gt;Phone#AUM (in millions)#Fundraising in Next 12 Months?#Employees&lt;break&gt;
+Fund_Manager_Fund_Highlight&lt;cl&gt;Parent Institution#Vintage#Status#Potential Investment#Fund Strategy</t>
+  </si>
+  <si>
+    <t>Contact_Highlight&lt;cl&gt;Legal Name#Tier#Phone#Last Touch Point#Sector</t>
+  </si>
+  <si>
+    <t>Highlight&lt;cl&gt;Stage#Investment Size#Source Firm#Source Contact</t>
+  </si>
+  <si>
+    <t>Highlight&lt;cl&gt;Fund Type#Vinatge Year#Target Commitments (mn)#Total Commitments (mn)#Total Capital Called (mn)</t>
+  </si>
+  <si>
+    <t>Highlight&lt;cl&gt;Legal Name#Stage#Investment Likely Amount (mn)#Target Close Date#Closing</t>
   </si>
 </sst>
 </file>
@@ -4209,7 +4406,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4376,6 +4573,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -4893,6 +5109,350 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>947</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="41"/>
+    </row>
+    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>501</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>502</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>948</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>450</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>451</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>800</v>
+      </c>
+      <c r="B17" t="s">
+        <v>801</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B26" s="50" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML71"/>
   <sheetViews>
@@ -7058,7 +7618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM71"/>
   <sheetViews>
@@ -9271,7 +9831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM71"/>
   <sheetViews>
@@ -11486,7 +12046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM71"/>
   <sheetViews>
@@ -15494,7 +16054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
@@ -15738,7 +16298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -15825,7 +16385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -16020,7 +16580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -16147,7 +16707,178 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="47.26953125" style="84" customWidth="1"/>
+    <col min="4" max="4" width="72.6328125" style="84" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="9.1796875" style="5" collapsed="1"/>
+    <col min="8" max="9" width="9.1796875" style="5"/>
+    <col min="10" max="16384" width="9.1796875" style="5" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="82" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D1" s="82" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="51"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+    </row>
+    <row r="3" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C4" s="81" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D4" s="81" t="s">
+        <v>1318</v>
+      </c>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+    </row>
+    <row r="5" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>573</v>
+      </c>
+      <c r="C5" s="81" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D5" s="81" t="s">
+        <v>1320</v>
+      </c>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+    </row>
+    <row r="6" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="32"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="80"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="80"/>
+    </row>
+    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="80"/>
+      <c r="C10" s="84" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D10" s="84" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+    </row>
+    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" s="80"/>
+      <c r="C13" s="84" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D13" s="81" t="s">
+        <v>1313</v>
+      </c>
+      <c r="H13" s="80"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="80"/>
+      <c r="C14" s="84" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D14" s="81"/>
+      <c r="H14" s="80"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="80"/>
+      <c r="C15" s="84" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D15" s="81"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="80"/>
+      <c r="D16" s="81"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="80"/>
+      <c r="D17" s="81"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="80"/>
+      <c r="D18" s="81"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -16555,7 +17286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -16695,178 +17426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="47.26953125" style="84" customWidth="1"/>
-    <col min="4" max="4" width="72.6328125" style="84" customWidth="1" collapsed="1"/>
-    <col min="5" max="7" width="9.1796875" style="5" collapsed="1"/>
-    <col min="8" max="9" width="9.1796875" style="5"/>
-    <col min="10" max="16384" width="9.1796875" style="5" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="82" t="s">
-        <v>1316</v>
-      </c>
-      <c r="D1" s="82" t="s">
-        <v>1315</v>
-      </c>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-    </row>
-    <row r="3" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>1306</v>
-      </c>
-      <c r="B4" s="80" t="s">
-        <v>1308</v>
-      </c>
-      <c r="C4" s="81" t="s">
-        <v>1317</v>
-      </c>
-      <c r="D4" s="81" t="s">
-        <v>1318</v>
-      </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-    </row>
-    <row r="5" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>1307</v>
-      </c>
-      <c r="B5" s="80" t="s">
-        <v>573</v>
-      </c>
-      <c r="C5" s="81" t="s">
-        <v>1319</v>
-      </c>
-      <c r="D5" s="81" t="s">
-        <v>1320</v>
-      </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-    </row>
-    <row r="6" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="32"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="80"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="80"/>
-    </row>
-    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="80"/>
-      <c r="C10" s="84" t="s">
-        <v>1310</v>
-      </c>
-      <c r="D10" s="84" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="80"/>
-      <c r="D11" s="81"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="80"/>
-      <c r="D12" s="81"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-    </row>
-    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="B13" s="80"/>
-      <c r="C13" s="84" t="s">
-        <v>1312</v>
-      </c>
-      <c r="D13" s="81" t="s">
-        <v>1313</v>
-      </c>
-      <c r="H13" s="80"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="80"/>
-      <c r="C14" s="84" t="s">
-        <v>1309</v>
-      </c>
-      <c r="D14" s="81"/>
-      <c r="H14" s="80"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="80"/>
-      <c r="C15" s="84" t="s">
-        <v>1314</v>
-      </c>
-      <c r="D15" s="81"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="80"/>
-      <c r="D16" s="81"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="80"/>
-      <c r="D17" s="81"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="80"/>
-      <c r="D18" s="81"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM71"/>
   <sheetViews>
@@ -19045,7 +19605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T14"/>
   <sheetViews>
@@ -19296,7 +19856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T23"/>
   <sheetViews>
@@ -19530,7 +20090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -19672,7 +20232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
@@ -19899,7 +20459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -20119,7 +20679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -20388,7 +20948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -20544,7 +21104,190 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="127.6328125" style="6" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.26953125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="9.1796875" style="5" collapsed="1"/>
+    <col min="8" max="10" width="9.1796875" style="5"/>
+    <col min="11" max="16384" width="9.1796875" style="5" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:5" s="86" customFormat="1" ht="147.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="88" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B2" s="88" t="s">
+        <v>573</v>
+      </c>
+      <c r="C2" s="89" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="88" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B3" s="90" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="91" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="88" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B4" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="88" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="88" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B6" s="92" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="90"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="90"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="90"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="90"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="90"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="90"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="90"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="90"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="90"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="90"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="90"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="90"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="90"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="90"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="90"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="90"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="90"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="90"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="90"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="90"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="90"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="90"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="90"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="90"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="90"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="90"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="90"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="90"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="90"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="90"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="90"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="90"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="90"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="90"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="90"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -20625,7 +21368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -20693,122 +21436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="111.08984375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.26953125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="8" width="9.1796875" style="5" collapsed="1"/>
-    <col min="9" max="9" width="9.1796875" style="5"/>
-    <col min="10" max="16384" width="9.1796875" style="5" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-    </row>
-    <row r="2" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51"/>
-    </row>
-    <row r="3" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>1296</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>1297</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>1298</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>1211</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>1299</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>1301</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>1303</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>1300</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>1253</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="Test Institution-1" display="https://navatar-5b--sb17.lightning.force.com/lightning/r/0013J00000JlvfYQAR/view"/>
-    <hyperlink ref="C7" r:id="rId2" tooltip="Test Fund-1" display="https://navatar-5b--sb17.lightning.force.com/lightning/r/a0B3J000001rYbbUAE/view"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -20893,7 +21521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ47"/>
   <sheetViews>
@@ -25796,7 +26424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMD23"/>
   <sheetViews>
@@ -27265,7 +27893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -27301,6 +27929,406 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="127.6328125" style="6" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.26953125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="9.1796875" style="5" collapsed="1"/>
+    <col min="8" max="10" width="9.1796875" style="5"/>
+    <col min="11" max="16384" width="9.1796875" style="5" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:5" s="86" customFormat="1" ht="132.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="88" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B2" s="88" t="s">
+        <v>573</v>
+      </c>
+      <c r="C2" s="89" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="90" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B3" s="90" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="91" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="90" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B4" s="90" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="90" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B5" s="90" t="s">
+        <v>339</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="90" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B6" s="92" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="90" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C7" s="90" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="90" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>314</v>
+      </c>
+      <c r="C8" s="90" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="90" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C9" s="90" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="90" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C10" s="90" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="90" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="90" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="90" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C12" s="90" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="90" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B13" s="74" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C13" s="90" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="90" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="90" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="90" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B15" s="74" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C15" s="90" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="90" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B16" s="74" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C16" s="90" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="90" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B17" s="74" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C17" s="90" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="90" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C18" s="90" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="90" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B19" s="74" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C19" s="90" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="90" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B20" s="74" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C20" s="90" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="90" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B21" s="74" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C21" s="90" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="90" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B22" s="74" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C22" s="90" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="90" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B23" s="74" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C23" s="90" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="90"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.81640625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="111.08984375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.26953125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="9.1796875" style="5" collapsed="1"/>
+    <col min="9" max="9" width="9.1796875" style="5"/>
+    <col min="10" max="16384" width="9.1796875" style="5" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="51"/>
+    </row>
+    <row r="3" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" tooltip="Test Institution-1" display="https://navatar-5b--sb17.lightning.force.com/lightning/r/0013J00000JlvfYQAR/view"/>
+    <hyperlink ref="C7" r:id="rId2" tooltip="Test Fund-1" display="https://navatar-5b--sb17.lightning.force.com/lightning/r/a0B3J000001rYbbUAE/view"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -27432,7 +28460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
@@ -28182,7 +29210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALP103"/>
   <sheetViews>
@@ -32261,7 +33289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR73"/>
   <sheetViews>
@@ -36474,348 +37502,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>509</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>947</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7265625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="41"/>
-    </row>
-    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>501</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>502</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
-        <v>507</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>948</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>450</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>451</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>639</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>800</v>
-      </c>
-      <c r="B17" t="s">
-        <v>801</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>1200</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1253</v>
-      </c>
-      <c r="D24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>1293</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1294</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1295</v>
-      </c>
-      <c r="E25" t="s">
-        <v>57</v>
-      </c>
-      <c r="I25">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>1243</v>
-      </c>
-      <c r="B26" s="50" t="s">
-        <v>1244</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added convert to portfolio testcase
Signed-off-by: Ravi Kumar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namita\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E015E3-787F-490B-A444-70723250CBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA06DE24-33D6-47DB-AFB1-103140563EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="711" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2625" uniqueCount="1537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2648" uniqueCount="1548">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -4707,6 +4707,39 @@
   </si>
   <si>
     <t>Test Contact-2</t>
+  </si>
+  <si>
+    <t>M2DQSINS5</t>
+  </si>
+  <si>
+    <t>M2DQSINS6</t>
+  </si>
+  <si>
+    <t>M2DQSINS7</t>
+  </si>
+  <si>
+    <t>DQSPatel Sons</t>
+  </si>
+  <si>
+    <t>DQSKanya Groups</t>
+  </si>
+  <si>
+    <t>DQSSharda Firms</t>
+  </si>
+  <si>
+    <t>DQSAnuradha</t>
+  </si>
+  <si>
+    <t>DQSPatel Property Deal</t>
+  </si>
+  <si>
+    <t>DQSAnuradha Jaiswal</t>
+  </si>
+  <si>
+    <t>M2DQSPIP6</t>
+  </si>
+  <si>
+    <t>DQSIns Deal</t>
   </si>
 </sst>
 </file>
@@ -12567,10 +12600,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:AMO74"/>
+  <dimension ref="A1:AMO75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15947,7 +15980,7 @@
       </c>
       <c r="G16" s="94"/>
     </row>
-    <row r="17" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="80" t="s">
         <v>1530</v>
       </c>
@@ -15968,365 +16001,385 @@
       </c>
       <c r="G17" s="94"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="80" t="s">
         <v>1531</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="B18" s="80" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C18" s="80" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D18" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="E18" s="80" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>1542</v>
+      </c>
       <c r="G18" s="94"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="80" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C19" s="80" t="s">
+        <v>1540</v>
+      </c>
+      <c r="D19" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="E19" s="80" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>931</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>932</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>910</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>906</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="94"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F21" s="22"/>
       <c r="G21" s="94"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F22" s="22"/>
       <c r="G22" s="94"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23" s="22"/>
+      <c r="G23" s="94"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="93"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>349</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>350</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>331</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
+    <row r="27" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="93"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B28" s="20" t="s">
         <v>794</v>
       </c>
-      <c r="D27" s="50" t="s">
+      <c r="D28" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="95"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4" t="s">
+      <c r="G28" s="95"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>664</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>665</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>623</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>666</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>667</v>
-      </c>
-      <c r="C32" t="s">
-        <v>625</v>
-      </c>
-      <c r="D32" t="s">
-        <v>29</v>
-      </c>
-      <c r="J32" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>668</v>
-      </c>
-      <c r="B33" t="s">
-        <v>669</v>
       </c>
       <c r="C33" t="s">
         <v>625</v>
       </c>
       <c r="D33" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J33" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="B34" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C34" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="D34" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>671</v>
+      </c>
+      <c r="B35" t="s">
+        <v>672</v>
+      </c>
+      <c r="C35" t="s">
+        <v>629</v>
+      </c>
+      <c r="D35" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>673</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>674</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>631</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>675</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>676</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>633</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>677</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>678</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>635</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>680</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>681</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>637</v>
-      </c>
-      <c r="D38" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>682</v>
-      </c>
-      <c r="B39" t="s">
-        <v>683</v>
-      </c>
-      <c r="C39" t="s">
-        <v>639</v>
       </c>
       <c r="D39" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B40" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="C40" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D40" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B41" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="C41" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D41" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B42" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C42" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D42" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B43" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="C43" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D43" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B44" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C44" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D44" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B45" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="C45" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D45" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B46" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C46" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D46" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B47" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="C47" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D47" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B48" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="C48" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D48" t="s">
         <v>258</v>
@@ -16334,13 +16387,13 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B49" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="C49" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="D49" t="s">
         <v>258</v>
@@ -16348,88 +16401,88 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>742</v>
+        <v>702</v>
       </c>
       <c r="B50" t="s">
-        <v>743</v>
+        <v>703</v>
       </c>
       <c r="C50" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="D50" t="s">
-        <v>29</v>
-      </c>
-      <c r="F50" t="s">
-        <v>653</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>776</v>
+        <v>742</v>
       </c>
       <c r="B51" t="s">
-        <v>778</v>
+        <v>743</v>
       </c>
       <c r="C51" t="s">
-        <v>772</v>
+        <v>660</v>
       </c>
       <c r="D51" t="s">
-        <v>258</v>
-      </c>
-      <c r="H51" t="s">
-        <v>780</v>
+        <v>29</v>
+      </c>
+      <c r="F51" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B52" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C52" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D52" t="s">
         <v>258</v>
       </c>
       <c r="H52" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>777</v>
+      </c>
+      <c r="B53" t="s">
+        <v>779</v>
+      </c>
+      <c r="C53" t="s">
+        <v>773</v>
+      </c>
+      <c r="D53" t="s">
+        <v>258</v>
+      </c>
+      <c r="H53" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4" t="s">
+    <row r="55" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4" t="s">
         <v>721</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="93"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>722</v>
-      </c>
-      <c r="B55" t="s">
-        <v>723</v>
-      </c>
-      <c r="C55" t="s">
-        <v>46</v>
-      </c>
-      <c r="D55" t="s">
-        <v>555</v>
-      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="93"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B56" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C56" t="s">
         <v>46</v>
@@ -16440,255 +16493,269 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>724</v>
+      </c>
+      <c r="B57" t="s">
+        <v>725</v>
+      </c>
+      <c r="C57" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>803</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>804</v>
       </c>
-      <c r="L57" t="s">
+      <c r="L58" t="s">
         <v>541</v>
       </c>
-      <c r="M57" t="s">
+      <c r="M58" t="s">
         <v>800</v>
       </c>
-      <c r="N57" t="s">
+      <c r="N58" t="s">
         <v>801</v>
       </c>
-      <c r="O57" t="s">
+      <c r="O58" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4" t="s">
+    <row r="64" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4" t="s">
         <v>1138</v>
       </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="93"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>1141</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1142</v>
-      </c>
-      <c r="D64" t="s">
-        <v>1143</v>
-      </c>
-      <c r="E64" t="s">
-        <v>1144</v>
-      </c>
-      <c r="F64" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G64" s="63">
-        <v>44291</v>
-      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="93"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="B65" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="D65" t="s">
-        <v>555</v>
+        <v>1143</v>
       </c>
       <c r="E65" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="F65" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="G65" s="63">
-        <v>44322</v>
+        <v>44291</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="B66" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="D66" t="s">
-        <v>1150</v>
+        <v>555</v>
       </c>
       <c r="E66" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="F66" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="G66" s="63">
-        <v>44354</v>
+        <v>44322</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="B67" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="D67" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="E67" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="F67" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="G67" s="63">
-        <v>44385</v>
+        <v>44354</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="B68" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="D68" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="E68" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="F68" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="G68" s="63">
-        <v>44417</v>
+        <v>44385</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="B69" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="D69" t="s">
-        <v>258</v>
+        <v>1158</v>
       </c>
       <c r="E69" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="F69" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="G69" s="63">
-        <v>44449</v>
+        <v>44417</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D70" t="s">
+        <v>258</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1162</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G70" s="63">
+        <v>44449</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>1163</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>1164</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>1090</v>
-      </c>
-      <c r="D70" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A71" s="32" t="s">
-        <v>1213</v>
-      </c>
-      <c r="C71" s="22" t="s">
-        <v>1204</v>
       </c>
       <c r="D71" t="s">
         <v>29</v>
       </c>
-      <c r="F71" s="22"/>
-      <c r="J71" t="s">
-        <v>1464</v>
-      </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>1214</v>
+      <c r="A72" s="32" t="s">
+        <v>1213</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="D72" t="s">
         <v>29</v>
       </c>
       <c r="F72" s="22"/>
+      <c r="J72" t="s">
+        <v>1464</v>
+      </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>1461</v>
-      </c>
-      <c r="B73" t="s">
-        <v>1139</v>
-      </c>
-      <c r="C73" t="s">
-        <v>1090</v>
+        <v>1214</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>1208</v>
       </c>
       <c r="D73" t="s">
         <v>29</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" s="22"/>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1461</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D74" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" t="s">
         <v>1134</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F74" t="s">
         <v>1092</v>
       </c>
-      <c r="G73" s="63">
+      <c r="G74" s="63">
         <v>44644</v>
       </c>
-      <c r="I73" s="80">
+      <c r="I74" s="80">
         <v>1000000</v>
       </c>
-      <c r="K73" s="80">
+      <c r="K74" s="80">
         <v>1100000</v>
       </c>
-      <c r="Q73" t="s">
+      <c r="Q74" t="s">
         <v>1140</v>
       </c>
     </row>
-    <row r="74" spans="1:17" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="80" t="s">
+    <row r="75" spans="1:17" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="80" t="s">
         <v>1462</v>
       </c>
-      <c r="B74" s="80" t="s">
+      <c r="B75" s="80" t="s">
         <v>1366</v>
       </c>
-      <c r="C74" s="80" t="s">
+      <c r="C75" s="80" t="s">
         <v>1090</v>
       </c>
-      <c r="D74" s="80" t="s">
+      <c r="D75" s="80" t="s">
         <v>1358</v>
       </c>
-      <c r="E74" s="80" t="s">
+      <c r="E75" s="80" t="s">
         <v>1134</v>
       </c>
-      <c r="F74" s="80" t="s">
+      <c r="F75" s="80" t="s">
         <v>1092</v>
       </c>
-      <c r="G74" s="63">
+      <c r="G75" s="63">
         <v>44639</v>
       </c>
-      <c r="I74" s="80">
+      <c r="I75" s="80">
         <v>23000000</v>
       </c>
     </row>
@@ -30302,10 +30369,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:ALP125"/>
+  <dimension ref="A1:ALP127"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33643,45 +33710,54 @@
       <c r="A33" s="80" t="s">
         <v>1520</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-    </row>
-    <row r="35" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3" t="s">
+      <c r="B33" s="22" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C33" s="80" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="80" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C34" s="80" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="80" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="80" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>490</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B38" s="22" t="s">
         <v>910</v>
-      </c>
-      <c r="C36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>491</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>911</v>
-      </c>
-      <c r="C37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>593</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>912</v>
       </c>
       <c r="C38" t="s">
         <v>31</v>
@@ -33689,229 +33765,229 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>594</v>
+        <v>491</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C40" t="s">
-        <v>599</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C41" t="s">
-        <v>905</v>
-      </c>
-      <c r="E41" t="s">
-        <v>914</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C42" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>905</v>
       </c>
       <c r="E43" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>751</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>918</v>
+        <v>597</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>916</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>910</v>
-      </c>
-      <c r="F44" s="22"/>
+        <v>600</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>598</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>917</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>751</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>918</v>
+      </c>
+      <c r="C46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>910</v>
+      </c>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>752</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B47" s="22" t="s">
         <v>919</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="22"/>
-    </row>
-    <row r="47" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="22"/>
-    </row>
     <row r="48" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
+      <c r="A48" s="34"/>
       <c r="B48" s="20"/>
       <c r="C48" s="22"/>
     </row>
-    <row r="49" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3" t="s">
+    <row r="49" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="22"/>
+    </row>
+    <row r="50" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="22"/>
+    </row>
+    <row r="51" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>383</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>331</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>384</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B53" t="s">
         <v>385</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3" t="s">
+    <row r="55" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B56" s="20" t="s">
         <v>792</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C56" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
+    <row r="57" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
         <v>428</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B57" s="20" t="s">
         <v>429</v>
       </c>
-      <c r="C55" s="22"/>
-    </row>
-    <row r="57" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="53"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-    </row>
-    <row r="58" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3" t="s">
+      <c r="C57" s="22"/>
+    </row>
+    <row r="59" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="53"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+    </row>
+    <row r="60" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="20" t="s">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
         <v>622</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B61" s="20" t="s">
         <v>623</v>
       </c>
-      <c r="C59" s="22" t="s">
+      <c r="C61" s="22" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="20" t="s">
-        <v>624</v>
-      </c>
-      <c r="B60" s="20" t="s">
-        <v>625</v>
-      </c>
-      <c r="C60" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D60" s="50"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="20" t="s">
-        <v>626</v>
-      </c>
-      <c r="B61" t="s">
-        <v>627</v>
-      </c>
-      <c r="C61" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>628</v>
-      </c>
-      <c r="B62" t="s">
-        <v>629</v>
-      </c>
-      <c r="C62" t="s">
+        <v>624</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>625</v>
+      </c>
+      <c r="C62" s="22" t="s">
         <v>75</v>
       </c>
+      <c r="D62" s="50"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B63" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C63" t="s">
         <v>75</v>
@@ -33919,10 +33995,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="B64" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="C64" t="s">
         <v>75</v>
@@ -33930,10 +34006,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B65" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="C65" t="s">
         <v>75</v>
@@ -33941,10 +34017,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B66" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C66" t="s">
         <v>75</v>
@@ -33952,10 +34028,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B67" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="C67" t="s">
         <v>75</v>
@@ -33963,10 +34039,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="B68" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C68" t="s">
         <v>75</v>
@@ -33974,10 +34050,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B69" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C69" t="s">
         <v>75</v>
@@ -33985,109 +34061,109 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B70" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C70" t="s">
-        <v>338</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B71" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="C71" t="s">
-        <v>599</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="B72" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C72" t="s">
-        <v>905</v>
+        <v>338</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B73" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C73" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="B74" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C74" t="s">
-        <v>275</v>
+        <v>905</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B75" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="C75" t="s">
-        <v>61</v>
+        <v>600</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="B76" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="C76" t="s">
-        <v>658</v>
+        <v>275</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="B77" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="C77" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="B78" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="C78" t="s">
-        <v>75</v>
+        <v>658</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
-        <v>774</v>
+        <v>659</v>
       </c>
       <c r="B79" t="s">
-        <v>772</v>
+        <v>660</v>
       </c>
       <c r="C79" t="s">
         <v>75</v>
@@ -34095,103 +34171,103 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
-        <v>775</v>
+        <v>661</v>
       </c>
       <c r="B80" t="s">
-        <v>773</v>
+        <v>662</v>
       </c>
       <c r="C80" t="s">
         <v>75</v>
       </c>
     </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="20" t="s">
+        <v>774</v>
+      </c>
+      <c r="B81" t="s">
+        <v>772</v>
+      </c>
+      <c r="C81" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="20" t="s">
+        <v>775</v>
+      </c>
+      <c r="B82" t="s">
+        <v>773</v>
+      </c>
+      <c r="C82" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>781</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B84" t="s">
         <v>591</v>
       </c>
-      <c r="C82" s="22" t="s">
+      <c r="C84" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3" t="s">
+    <row r="86" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3" t="s">
         <v>935</v>
       </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>936</v>
       </c>
-      <c r="B85" s="22" t="s">
+      <c r="B87" s="22" t="s">
         <v>937</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C87" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3" t="s">
+    <row r="89" spans="1:4" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3" t="s">
         <v>1074</v>
       </c>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>1089</v>
-      </c>
-      <c r="B88" t="s">
-        <v>1090</v>
-      </c>
-      <c r="C88" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B89" t="s">
-        <v>1092</v>
-      </c>
-      <c r="C89" t="s">
-        <v>275</v>
-      </c>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
       <c r="B90" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="C90" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="B91" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="C91" t="s">
-        <v>31</v>
+        <v>275</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="B92" t="s">
-        <v>1098</v>
+        <v>1094</v>
       </c>
       <c r="C92" t="s">
         <v>31</v>
@@ -34199,10 +34275,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="B93" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="C93" t="s">
         <v>31</v>
@@ -34210,32 +34286,32 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="B94" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="C94" t="s">
-        <v>600</v>
+        <v>31</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="B95" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="C95" t="s">
-        <v>600</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="B96" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="C96" t="s">
         <v>600</v>
@@ -34243,252 +34319,252 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>1165</v>
+        <v>1103</v>
       </c>
       <c r="B97" t="s">
-        <v>1166</v>
+        <v>1104</v>
       </c>
       <c r="C97" t="s">
-        <v>338</v>
-      </c>
-      <c r="G97">
-        <v>99852101</v>
+        <v>600</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>1179</v>
+        <v>1105</v>
       </c>
       <c r="B98" t="s">
-        <v>1187</v>
+        <v>1106</v>
       </c>
       <c r="C98" t="s">
-        <v>31</v>
-      </c>
-      <c r="F98" t="s">
-        <v>1189</v>
+        <v>600</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>1180</v>
+        <v>1165</v>
       </c>
       <c r="B99" t="s">
-        <v>1190</v>
+        <v>1166</v>
       </c>
       <c r="C99" t="s">
-        <v>75</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>94</v>
+        <v>338</v>
+      </c>
+      <c r="G99">
+        <v>99852101</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="B100" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="C100" t="s">
-        <v>600</v>
+        <v>31</v>
       </c>
       <c r="F100" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="B101" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="C101" t="s">
-        <v>61</v>
-      </c>
-      <c r="E101" t="s">
-        <v>1187</v>
+        <v>75</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="B102" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="C102" t="s">
-        <v>599</v>
-      </c>
-      <c r="E102" t="s">
-        <v>1187</v>
+        <v>600</v>
+      </c>
+      <c r="F102" t="s">
+        <v>1192</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B103" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C103" t="s">
-        <v>905</v>
+        <v>61</v>
       </c>
       <c r="E103" t="s">
-        <v>1194</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="B104" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="C104" t="s">
-        <v>338</v>
-      </c>
-      <c r="F104" t="s">
-        <v>338</v>
+        <v>599</v>
+      </c>
+      <c r="E104" t="s">
+        <v>1187</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="B105" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="C105" t="s">
-        <v>275</v>
-      </c>
-      <c r="G105">
-        <v>9876540123</v>
+        <v>905</v>
+      </c>
+      <c r="E105" t="s">
+        <v>1194</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>1201</v>
+        <v>1185</v>
       </c>
       <c r="B106" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="C106" t="s">
-        <v>658</v>
-      </c>
-      <c r="E106" t="s">
-        <v>1187</v>
+        <v>338</v>
+      </c>
+      <c r="F106" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>1202</v>
+        <v>1186</v>
       </c>
       <c r="B107" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="C107" t="s">
-        <v>1200</v>
-      </c>
-      <c r="D107" t="s">
-        <v>1200</v>
+        <v>275</v>
+      </c>
+      <c r="G107">
+        <v>9876540123</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="32" t="s">
-        <v>1075</v>
-      </c>
-      <c r="B108" s="22" t="s">
-        <v>1076</v>
+      <c r="A108" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1198</v>
       </c>
       <c r="C108" t="s">
-        <v>31</v>
+        <v>658</v>
+      </c>
+      <c r="E108" t="s">
+        <v>1187</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>1486</v>
-      </c>
-      <c r="B109" s="22" t="s">
-        <v>1078</v>
+        <v>1202</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1199</v>
       </c>
       <c r="C109" t="s">
-        <v>31</v>
+        <v>1200</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1200</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>1077</v>
+      <c r="A110" s="32" t="s">
+        <v>1075</v>
       </c>
       <c r="B110" s="22" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
       <c r="C110" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="80" t="s">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B111" s="22" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C111" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B112" s="22" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C112" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="80" t="s">
         <v>1079</v>
       </c>
-      <c r="B111" s="22" t="s">
+      <c r="B113" s="22" t="s">
         <v>1375</v>
       </c>
-      <c r="C111" s="80" t="s">
+      <c r="C113" s="80" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="80" t="s">
+    <row r="114" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="80" t="s">
         <v>1374</v>
       </c>
-      <c r="B112" s="22" t="s">
+      <c r="B114" s="22" t="s">
         <v>1376</v>
       </c>
-      <c r="C112" s="80" t="s">
+      <c r="C114" s="80" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>1203</v>
-      </c>
-      <c r="B113" s="22" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C113" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>1205</v>
-      </c>
-      <c r="B114" s="22" t="s">
-        <v>1206</v>
-      </c>
-      <c r="C114" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="B115" s="22" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="C115" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="B116" s="22" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="C116" t="s">
         <v>275</v>
@@ -34496,49 +34572,43 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B117" s="22" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C117" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B118" s="22" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C118" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>1386</v>
       </c>
-      <c r="B117" s="22" t="s">
+      <c r="B119" s="22" t="s">
         <v>1387</v>
       </c>
-      <c r="C117" s="80" t="s">
+      <c r="C119" s="80" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="80" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="80" t="s">
         <v>1397</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B120" t="s">
         <v>1394</v>
-      </c>
-      <c r="C118" s="80" t="s">
-        <v>75</v>
-      </c>
-      <c r="D118" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="80" t="s">
-        <v>1398</v>
-      </c>
-      <c r="B119" s="22" t="s">
-        <v>1395</v>
-      </c>
-      <c r="C119" s="80" t="s">
-        <v>75</v>
-      </c>
-      <c r="D119" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>1392</v>
-      </c>
-      <c r="B120" s="22" t="s">
-        <v>1399</v>
       </c>
       <c r="C120" s="80" t="s">
         <v>75</v>
@@ -34549,59 +34619,87 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="80" t="s">
-        <v>1393</v>
+        <v>1398</v>
       </c>
       <c r="B121" s="22" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="C121" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="D121" s="80" t="s">
+      <c r="D121" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="80" t="s">
-        <v>1418</v>
+      <c r="A122" t="s">
+        <v>1392</v>
       </c>
       <c r="B122" s="22" t="s">
-        <v>1471</v>
+        <v>1399</v>
       </c>
       <c r="C122" s="80" t="s">
-        <v>31</v>
+        <v>75</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="80" t="s">
-        <v>1429</v>
+        <v>1393</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>1430</v>
+        <v>1400</v>
       </c>
       <c r="C123" s="80" t="s">
-        <v>31</v>
+        <v>75</v>
+      </c>
+      <c r="D123" s="80" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>1437</v>
+      <c r="A124" s="80" t="s">
+        <v>1418</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>1436</v>
+        <v>1471</v>
       </c>
       <c r="C124" s="80" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="A125" s="80" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B125" s="22" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C125" s="80" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B126" s="22" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C126" s="80" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>1444</v>
       </c>
-      <c r="B125" s="22" t="s">
+      <c r="B127" s="22" t="s">
         <v>1445</v>
       </c>
-      <c r="C125" s="80" t="s">
+      <c r="C127" s="80" t="s">
         <v>31</v>
       </c>
     </row>
@@ -34616,7 +34714,7 @@
   <dimension ref="A1:ALR89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37895,6 +37993,15 @@
       <c r="A18" s="80" t="s">
         <v>1525</v>
       </c>
+      <c r="B18" s="80" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C18" s="80" t="s">
+        <v>272</v>
+      </c>
+      <c r="D18" s="80" t="s">
+        <v>1541</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>

</xml_diff>

<commit_message>
Update average DQS on source firm and contact page
Signed-off-by: Ravi Kumar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -1,57 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namita\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA06DE24-33D6-47DB-AFB1-103140563EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{DA06DE24-33D6-47DB-AFB1-103140563EF2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="711" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="14" firstSheet="7" tabRatio="711" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="FilePath" sheetId="18" r:id="rId1"/>
-    <sheet name="FSTGListView" sheetId="37" r:id="rId2"/>
-    <sheet name="FSTGCompactLayoutField" sheetId="39" r:id="rId3"/>
-    <sheet name="FSTGPageLayoutField" sheetId="38" r:id="rId4"/>
-    <sheet name="FSTGVerifyField" sheetId="36" r:id="rId5"/>
-    <sheet name="FieldSet" sheetId="1" r:id="rId6"/>
-    <sheet name="FieldComponent" sheetId="6" r:id="rId7"/>
-    <sheet name="Entities" sheetId="3" r:id="rId8"/>
-    <sheet name="Contacts" sheetId="2" r:id="rId9"/>
-    <sheet name="Test Custom Object" sheetId="23" r:id="rId10"/>
-    <sheet name="Fund" sheetId="7" r:id="rId11"/>
-    <sheet name="FundInvestment" sheetId="34" r:id="rId12"/>
-    <sheet name="FundDistribution" sheetId="33" r:id="rId13"/>
-    <sheet name="FundDrawdown" sheetId="32" r:id="rId14"/>
-    <sheet name="Deal" sheetId="4" r:id="rId15"/>
-    <sheet name="Fundraisings" sheetId="28" r:id="rId16"/>
-    <sheet name="DealRequestTracker" sheetId="14" r:id="rId17"/>
-    <sheet name="CustomSDG" sheetId="13" r:id="rId18"/>
-    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId19"/>
-    <sheet name="MarketingEvent" sheetId="15" r:id="rId20"/>
-    <sheet name="Partnerships" sheetId="8" r:id="rId21"/>
-    <sheet name="AgreementsAmendments" sheetId="35" r:id="rId22"/>
-    <sheet name="Commitments" sheetId="9" r:id="rId23"/>
-    <sheet name="Task" sheetId="12" r:id="rId24"/>
-    <sheet name="UploadImageData" sheetId="17" r:id="rId25"/>
-    <sheet name="Fields" sheetId="19" r:id="rId26"/>
-    <sheet name="Attendees" sheetId="20" r:id="rId27"/>
-    <sheet name="Deal Team" sheetId="21" r:id="rId28"/>
-    <sheet name="Coverages" sheetId="22" r:id="rId29"/>
-    <sheet name="SDGActions" sheetId="24" r:id="rId30"/>
-    <sheet name="Report" sheetId="25" r:id="rId31"/>
-    <sheet name="CustomEmailFolder" sheetId="26" r:id="rId32"/>
-    <sheet name="Task1" sheetId="27" r:id="rId33"/>
-    <sheet name="Events" sheetId="29" r:id="rId34"/>
-    <sheet name="MI" sheetId="30" r:id="rId35"/>
+    <sheet name="FilePath" r:id="rId1" sheetId="18"/>
+    <sheet name="FSTGListView" r:id="rId2" sheetId="37"/>
+    <sheet name="FSTGCompactLayoutField" r:id="rId3" sheetId="39"/>
+    <sheet name="FSTGPageLayoutField" r:id="rId4" sheetId="38"/>
+    <sheet name="FSTGVerifyField" r:id="rId5" sheetId="36"/>
+    <sheet name="FieldSet" r:id="rId6" sheetId="1"/>
+    <sheet name="FieldComponent" r:id="rId7" sheetId="6"/>
+    <sheet name="Entities" r:id="rId8" sheetId="3"/>
+    <sheet name="Contacts" r:id="rId9" sheetId="2"/>
+    <sheet name="Test Custom Object" r:id="rId10" sheetId="23"/>
+    <sheet name="Fund" r:id="rId11" sheetId="7"/>
+    <sheet name="FundInvestment" r:id="rId12" sheetId="34"/>
+    <sheet name="FundDistribution" r:id="rId13" sheetId="33"/>
+    <sheet name="FundDrawdown" r:id="rId14" sheetId="32"/>
+    <sheet name="Deal" r:id="rId15" sheetId="4"/>
+    <sheet name="Fundraisings" r:id="rId16" sheetId="28"/>
+    <sheet name="DealRequestTracker" r:id="rId17" sheetId="14"/>
+    <sheet name="CustomSDG" r:id="rId18" sheetId="13"/>
+    <sheet name="ToggleButtonCheck" r:id="rId19" sheetId="16"/>
+    <sheet name="MarketingEvent" r:id="rId20" sheetId="15"/>
+    <sheet name="Partnerships" r:id="rId21" sheetId="8"/>
+    <sheet name="AgreementsAmendments" r:id="rId22" sheetId="35"/>
+    <sheet name="Commitments" r:id="rId23" sheetId="9"/>
+    <sheet name="Task" r:id="rId24" sheetId="12"/>
+    <sheet name="UploadImageData" r:id="rId25" sheetId="17"/>
+    <sheet name="Fields" r:id="rId26" sheetId="19"/>
+    <sheet name="Attendees" r:id="rId27" sheetId="20"/>
+    <sheet name="Deal Team" r:id="rId28" sheetId="21"/>
+    <sheet name="Coverages" r:id="rId29" sheetId="22"/>
+    <sheet name="SDGActions" r:id="rId30" sheetId="24"/>
+    <sheet name="Report" r:id="rId31" sheetId="25"/>
+    <sheet name="CustomEmailFolder" r:id="rId32" sheetId="26"/>
+    <sheet name="Task1" r:id="rId33" sheetId="27"/>
+    <sheet name="Events" r:id="rId34" sheetId="29"/>
+    <sheet name="MI" r:id="rId35" sheetId="30"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2648" uniqueCount="1548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="1549">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -4740,6 +4740,9 @@
   </si>
   <si>
     <t>DQSIns Deal</t>
+  </si>
+  <si>
+    <t>navatariptesting+42479@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -4907,209 +4910,209 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="96">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="14" quotePrefix="1" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="2" numFmtId="14" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="6" fontId="2" numFmtId="14" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="2" numFmtId="14" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="1"/>
+    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5126,10 +5129,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -5164,7 +5167,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5199,7 +5202,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5293,21 +5296,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -5324,7 +5327,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -5376,15 +5379,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -5392,15 +5395,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="66" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="89.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="81.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="66.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -5468,7 +5471,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row ht="60" r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>549</v>
       </c>
@@ -5610,17 +5613,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink r:id="rId1" ref="L2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId2" ref="B5" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
@@ -5628,9 +5631,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -5644,7 +5647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -5673,13 +5676,13 @@
       <c r="C4" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:J27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
@@ -5687,19 +5690,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -5731,7 +5734,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -5743,7 +5746,7 @@
       <c r="I2" s="39"/>
       <c r="J2" s="41"/>
     </row>
-    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -5785,12 +5788,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5804,7 +5807,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>493</v>
       </c>
@@ -5818,7 +5821,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -5832,7 +5835,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>143</v>
       </c>
@@ -5846,7 +5849,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>144</v>
       </c>
@@ -5967,7 +5970,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="26" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1219</v>
       </c>
@@ -6000,13 +6003,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:AML71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:AMM71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -6014,18 +6017,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.42578125" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.42578125" style="74" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12.42578125" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="12" width="8.7109375" style="74" collapsed="1"/>
-    <col min="13" max="13" width="16.7109375" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="8.7109375" style="74" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="74" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="74" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="74" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="74" width="25.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="74" width="25.42578125" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" style="74" width="12.42578125" collapsed="true"/>
+    <col min="8" max="12" style="74" width="8.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="74" width="16.7109375" collapsed="true"/>
+    <col min="14" max="16384" style="74" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1026" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="68" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>9</v>
       </c>
@@ -7065,7 +7068,7 @@
       <c r="AMK1" s="67"/>
       <c r="AML1" s="67"/>
     </row>
-    <row r="2" spans="1:1026" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="73" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
         <v>1256</v>
       </c>
@@ -8132,11 +8135,11 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F20" s="75"/>
     </row>
-    <row r="25" spans="1:6" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="76"/>
       <c r="B25" s="76"/>
     </row>
-    <row r="52" spans="1:8" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="52" s="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="65"/>
       <c r="B52" s="65"/>
       <c r="C52" s="65"/>
@@ -8145,7 +8148,7 @@
       <c r="F52" s="65"/>
       <c r="G52" s="66"/>
     </row>
-    <row r="61" spans="1:8" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="61" s="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="65"/>
       <c r="B61" s="65"/>
       <c r="C61" s="65"/>
@@ -8165,14 +8168,14 @@
       <c r="F71" s="75"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:AMM71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:AMN71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -8180,20 +8183,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.42578125" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.85546875" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" style="74" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.42578125" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="13" width="8.7109375" style="74" collapsed="1"/>
-    <col min="14" max="14" width="16.7109375" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16384" width="8.7109375" style="74" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="74" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="74" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="74" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="74" width="25.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="74" width="24.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="74" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="74" width="12.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="74" width="12.42578125" collapsed="true"/>
+    <col min="9" max="13" style="74" width="8.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="74" width="16.7109375" collapsed="true"/>
+    <col min="15" max="16384" style="74" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1027" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="68" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>9</v>
       </c>
@@ -9252,7 +9255,7 @@
       <c r="AML1" s="67"/>
       <c r="AMM1" s="67"/>
     </row>
-    <row r="2" spans="1:1027" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="73" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
         <v>1249</v>
       </c>
@@ -10325,11 +10328,11 @@
       <c r="F20" s="75"/>
       <c r="G20" s="75"/>
     </row>
-    <row r="25" spans="1:7" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="76"/>
       <c r="B25" s="76"/>
     </row>
-    <row r="52" spans="1:9" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="52" s="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="65"/>
       <c r="B52" s="65"/>
       <c r="C52" s="65"/>
@@ -10339,7 +10342,7 @@
       <c r="G52" s="65"/>
       <c r="H52" s="66"/>
     </row>
-    <row r="61" spans="1:9" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="61" s="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="65"/>
       <c r="B61" s="65"/>
       <c r="C61" s="65"/>
@@ -10378,14 +10381,14 @@
       <c r="F71" s="75"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:AMM71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:AMN71"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -10393,18 +10396,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1027" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -11463,7 +11466,7 @@
       <c r="AML1" s="6"/>
       <c r="AMM1" s="6"/>
     </row>
-    <row r="2" spans="1:1027" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="44" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
         <v>1242</v>
       </c>
@@ -12540,11 +12543,11 @@
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
     </row>
-    <row r="25" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
     </row>
-    <row r="52" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="52" s="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -12554,7 +12557,7 @@
       <c r="G52" s="4"/>
       <c r="H52" s="3"/>
     </row>
-    <row r="61" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="61" s="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
@@ -12593,14 +12596,14 @@
       <c r="F71" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:AMO75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:AMP75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -12608,22 +12611,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" style="63" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" style="80" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.7109375" style="80" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="63" width="12.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="80" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="80" width="12.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1029" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:1029" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -13686,7 +13689,7 @@
       <c r="AMN1" s="6"/>
       <c r="AMO1" s="6"/>
     </row>
-    <row r="2" spans="1:1029" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="44" spans="1:1029" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -14717,7 +14720,7 @@
       <c r="AMN2" s="43"/>
       <c r="AMO2" s="43"/>
     </row>
-    <row r="3" spans="1:1029" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:1029" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -15959,7 +15962,7 @@
       </c>
       <c r="G15" s="94"/>
     </row>
-    <row r="16" spans="1:1029" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="80" spans="1:1029" x14ac:dyDescent="0.25">
       <c r="A16" s="80" t="s">
         <v>1529</v>
       </c>
@@ -15980,7 +15983,7 @@
       </c>
       <c r="G16" s="94"/>
     </row>
-    <row r="17" spans="1:9" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="80" t="s">
         <v>1530</v>
       </c>
@@ -16106,7 +16109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="27" s="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
@@ -16119,7 +16122,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="28" s="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>145</v>
       </c>
@@ -16464,7 +16467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="55" s="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4" t="s">
@@ -16525,7 +16528,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="64" s="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
@@ -16733,7 +16736,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="75" spans="1:17" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="75" s="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="80" t="s">
         <v>1462</v>
       </c>
@@ -16761,14 +16764,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:M22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -16776,17 +16779,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -16863,7 +16866,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -16992,7 +16995,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
@@ -17031,7 +17034,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="21" s="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="80" t="s">
         <v>1455</v>
       </c>
@@ -17054,7 +17057,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="22" s="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="80" t="s">
         <v>1456</v>
       </c>
@@ -17070,13 +17073,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
@@ -17084,10 +17087,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="5" width="15.28515625" collapsed="true"/>
+    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -17107,10 +17110,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
-    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -17156,14 +17159,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -17171,12 +17174,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="27.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="20.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="19.140625" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -17196,7 +17199,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -17230,7 +17233,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>299</v>
       </c>
@@ -17264,7 +17267,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -17351,7 +17354,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
@@ -17380,13 +17383,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -17394,13 +17397,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="127.42578125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="22.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="32.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="127.42578125" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -17423,7 +17426,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
@@ -17431,7 +17434,7 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
     </row>
-    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -17521,16 +17524,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
+    <hyperlink display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" r:id="rId1" ref="C5" tooltip="TestAzAlexa Deal" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" r:id="rId2" ref="C4" tooltip="TestAzAlexa Info" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -17538,11 +17541,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="47.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="72.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="84" width="47.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="84" width="72.5703125" collapsed="true"/>
+    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -17560,12 +17563,12 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="C2" s="83"/>
       <c r="D2" s="83"/>
     </row>
-    <row r="3" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="82"/>
@@ -17592,7 +17595,7 @@
       <c r="G4" s="80"/>
       <c r="H4" s="80"/>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1283</v>
       </c>
@@ -17610,7 +17613,7 @@
       <c r="G5" s="80"/>
       <c r="H5" s="80"/>
     </row>
-    <row r="6" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="32"/>
       <c r="C6" s="85"/>
       <c r="D6" s="85"/>
@@ -17633,7 +17636,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="80"/>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="80"/>
       <c r="C10" s="84" t="s">
         <v>1286</v>
@@ -17654,7 +17657,7 @@
       <c r="G12" s="80"/>
       <c r="H12" s="80"/>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="80"/>
       <c r="C13" s="84" t="s">
         <v>1288</v>
@@ -17692,14 +17695,14 @@
       <c r="D18" s="81"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
@@ -17707,12 +17710,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="21.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="11.0" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -17732,14 +17735,14 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
     </row>
-    <row r="3" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
@@ -18071,7 +18074,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="29" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
@@ -18100,14 +18103,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -18115,13 +18118,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -18135,10 +18138,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
     </row>
-    <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>496</v>
@@ -18168,7 +18171,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>509</v>
@@ -18176,7 +18179,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>748</v>
       </c>
@@ -18185,17 +18188,17 @@
       </c>
       <c r="C8" s="22"/>
     </row>
-    <row r="9" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
     </row>
-    <row r="10" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="22"/>
     </row>
-    <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>510</v>
@@ -18203,7 +18206,7 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>430</v>
       </c>
@@ -18212,7 +18215,7 @@
       </c>
       <c r="C12" s="22"/>
     </row>
-    <row r="13" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>432</v>
       </c>
@@ -18221,7 +18224,7 @@
       </c>
       <c r="C13" s="22"/>
     </row>
-    <row r="17" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
         <v>1176</v>
@@ -18241,13 +18244,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:AMM71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <dimension ref="A1:AMN71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -18255,19 +18258,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.5703125" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.7109375" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.42578125" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.42578125" style="74" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="12.42578125" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="13" width="8.7109375" style="74" collapsed="1"/>
-    <col min="14" max="14" width="16.7109375" style="74" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16384" width="8.7109375" style="74" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="74" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="74" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="74" width="22.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="74" width="29.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="74" width="25.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="74" width="25.42578125" collapsed="true"/>
+    <col min="7" max="8" bestFit="true" customWidth="true" style="74" width="12.42578125" collapsed="true"/>
+    <col min="9" max="13" style="74" width="8.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="74" width="16.7109375" collapsed="true"/>
+    <col min="15" max="16384" style="74" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1027" s="68" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="68" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>9</v>
       </c>
@@ -19312,7 +19315,7 @@
       <c r="AML1" s="67"/>
       <c r="AMM1" s="67"/>
     </row>
-    <row r="2" spans="1:1027" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="73" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
         <v>1262</v>
       </c>
@@ -20382,12 +20385,12 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G20" s="75"/>
     </row>
-    <row r="25" spans="1:7" s="77" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="76"/>
       <c r="B25" s="76"/>
       <c r="C25" s="76"/>
     </row>
-    <row r="52" spans="1:9" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="52" s="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="65"/>
       <c r="B52" s="65"/>
       <c r="C52" s="65"/>
@@ -20397,7 +20400,7 @@
       <c r="G52" s="65"/>
       <c r="H52" s="66"/>
     </row>
-    <row r="61" spans="1:9" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="61" s="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="65"/>
       <c r="B61" s="65"/>
       <c r="C61" s="65"/>
@@ -20419,14 +20422,14 @@
       <c r="G71" s="75"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
-  <dimension ref="A1:T14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
@@ -20434,26 +20437,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="1" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -20515,7 +20518,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" t="s">
         <v>558</v>
@@ -20527,7 +20530,7 @@
       <c r="Q2" s="48"/>
       <c r="S2" s="48"/>
     </row>
-    <row r="3" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
@@ -20588,7 +20591,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="7" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
@@ -20612,21 +20615,21 @@
       <c r="S7" s="16"/>
       <c r="T7" s="13"/>
     </row>
-    <row r="8" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>434</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="22"/>
     </row>
-    <row r="9" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>435</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
     </row>
-    <row r="13" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="13" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
         <v>1176</v>
@@ -20671,13 +20674,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <dimension ref="A1:T23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
@@ -20685,12 +20688,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -20710,7 +20713,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="13"/>
@@ -20802,7 +20805,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="15" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="13"/>
@@ -20826,7 +20829,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="13"/>
     </row>
-    <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>520</v>
       </c>
@@ -20843,7 +20846,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>525</v>
       </c>
@@ -20860,7 +20863,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>529</v>
       </c>
@@ -20880,7 +20883,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="23" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="13"/>
@@ -20905,13 +20908,13 @@
       <c r="T23" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -20919,18 +20922,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.28515625" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="29" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="29" width="24.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -21047,13 +21050,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -21061,11 +21064,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -21274,13 +21277,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -21288,8 +21291,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -21494,13 +21497,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -21508,8 +21511,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -21763,13 +21766,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
@@ -21777,9 +21780,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -21793,12 +21796,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="53"/>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
     </row>
-    <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>512</v>
@@ -21919,13 +21922,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -21933,11 +21936,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="127.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="24.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="127.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="15.28515625" collapsed="true"/>
+    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -21953,7 +21956,7 @@
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
     </row>
-    <row r="2" spans="1:5" s="86" customFormat="1" ht="147.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="147.6" r="2" s="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="88" t="s">
         <v>1272</v>
       </c>
@@ -22099,14 +22102,14 @@
       <c r="C24" s="90"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -22114,10 +22117,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -22140,7 +22143,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row ht="90" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>539</v>
       </c>
@@ -22160,7 +22163,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row ht="120" r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>544</v>
       </c>
@@ -22181,13 +22184,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F3"/>
@@ -22195,13 +22198,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -22269,14 +22272,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -22284,15 +22287,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -22324,7 +22327,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>576</v>
       </c>
@@ -22353,15 +22356,15 @@
         <v>581</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row customHeight="1" ht="15" r="6" spans="1:9" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
-  <dimension ref="A1:AMJ55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+  <dimension ref="A1:AMK55"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
@@ -22369,18 +22372,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="65.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="65.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="12" max="13" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
@@ -27177,7 +27180,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row customFormat="1" r="40" s="32" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>1083</v>
@@ -27197,7 +27200,7 @@
       </c>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="42" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>1380</v>
       </c>
@@ -27219,7 +27222,7 @@
       </c>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="43" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>1402</v>
       </c>
@@ -27243,7 +27246,7 @@
       </c>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="44" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>1403</v>
       </c>
@@ -27267,7 +27270,7 @@
       </c>
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="45" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>1404</v>
       </c>
@@ -27284,7 +27287,7 @@
       </c>
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="46" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
         <v>1405</v>
       </c>
@@ -27301,7 +27304,7 @@
       </c>
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="47" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="19" t="s">
         <v>1423</v>
       </c>
@@ -27336,7 +27339,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="49" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
         <v>1379</v>
       </c>
@@ -27352,7 +27355,7 @@
       </c>
       <c r="I49" s="5"/>
     </row>
-    <row r="50" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="50" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>1441</v>
       </c>
@@ -27449,13 +27452,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
-  <dimension ref="A1:AMD28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+  <dimension ref="A1:AME28"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
@@ -27463,13 +27466,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="65.42578125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1018" x14ac:dyDescent="0.25">
@@ -28889,7 +28892,7 @@
       <c r="I19" s="62"/>
       <c r="J19" s="62"/>
     </row>
-    <row r="21" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="21" s="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="32" t="s">
         <v>1074</v>
       </c>
@@ -28917,7 +28920,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="23" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="80" t="s">
         <v>1384</v>
       </c>
@@ -28938,7 +28941,7 @@
       </c>
       <c r="I23" s="62"/>
     </row>
-    <row r="24" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="24" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="80" t="s">
         <v>1414</v>
       </c>
@@ -28956,7 +28959,7 @@
       </c>
       <c r="I24" s="62"/>
     </row>
-    <row r="25" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="80" t="s">
         <v>1415</v>
       </c>
@@ -28977,7 +28980,7 @@
       </c>
       <c r="I25" s="62"/>
     </row>
-    <row r="26" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="26" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="80" t="s">
         <v>1426</v>
       </c>
@@ -28995,7 +28998,7 @@
       </c>
       <c r="I26" s="62"/>
     </row>
-    <row r="27" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="27" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="80" t="s">
         <v>1433</v>
       </c>
@@ -29032,13 +29035,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
@@ -29046,8 +29049,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -29067,13 +29070,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -29081,11 +29084,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="127.5703125" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="24.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="127.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="15.28515625" collapsed="true"/>
+    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -29101,7 +29104,7 @@
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
     </row>
-    <row r="2" spans="1:5" s="86" customFormat="1" ht="132.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="132.6" r="2" s="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="88" t="s">
         <v>1272</v>
       </c>
@@ -29112,7 +29115,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="90" t="s">
         <v>1274</v>
       </c>
@@ -29145,7 +29148,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="90" t="s">
         <v>1298</v>
       </c>
@@ -29233,7 +29236,7 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="90" t="s">
         <v>1306</v>
       </c>
@@ -29244,7 +29247,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="90" t="s">
         <v>1307</v>
       </c>
@@ -29277,7 +29280,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="90" t="s">
         <v>1322</v>
       </c>
@@ -29299,7 +29302,7 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="90" t="s">
         <v>1324</v>
       </c>
@@ -29349,14 +29352,14 @@
       <c r="C24" s="90"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
@@ -29364,12 +29367,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="111.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="15.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="111.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="15.28515625" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -29388,10 +29391,10 @@
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
     </row>
-    <row r="2" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
-    <row r="3" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -29459,17 +29462,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="Test Institution-1" display="https://navatar-5b--sb17.lightning.force.com/lightning/r/0013J00000JlvfYQAR/view" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="C7" r:id="rId2" tooltip="Test Fund-1" display="https://navatar-5b--sb17.lightning.force.com/lightning/r/a0B3J000001rYbbUAE/view" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink display="https://navatar-5b--sb17.lightning.force.com/lightning/r/0013J00000JlvfYQAR/view" r:id="rId1" ref="C5" tooltip="Test Institution-1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink display="https://navatar-5b--sb17.lightning.force.com/lightning/r/a0B3J000001rYbbUAE/view" r:id="rId2" ref="C7" tooltip="Test Fund-1" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -29477,15 +29480,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="77.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -29505,7 +29508,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -29612,14 +29615,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
@@ -29627,15 +29630,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -30363,13 +30366,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:ALP127"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:ALQ127"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
@@ -30377,13 +30380,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1004" x14ac:dyDescent="0.25">
@@ -31406,7 +31409,7 @@
       <c r="ALO1" s="5"/>
       <c r="ALP1" s="5"/>
     </row>
-    <row r="2" spans="1:1004" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="35"/>
@@ -33460,17 +33463,17 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:1004" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="80" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:1004" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="80" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:1004" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="80" spans="1:1004" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="19"/>
       <c r="C11" s="5"/>
@@ -33585,7 +33588,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="22" s="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="80" t="s">
         <v>1497</v>
       </c>
@@ -33596,7 +33599,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="23" s="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="80" t="s">
         <v>1498</v>
       </c>
@@ -33618,7 +33621,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="80" t="s">
         <v>1500</v>
       </c>
@@ -33629,7 +33632,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="26" s="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="80" t="s">
         <v>1505</v>
       </c>
@@ -33673,7 +33676,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="30" s="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="80" t="s">
         <v>1517</v>
       </c>
@@ -33684,7 +33687,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="31" s="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="80" t="s">
         <v>1518</v>
       </c>
@@ -33695,7 +33698,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="32" s="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="80" t="s">
         <v>1519</v>
       </c>
@@ -33706,7 +33709,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="33" s="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="80" t="s">
         <v>1520</v>
       </c>
@@ -33717,7 +33720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="34" s="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="80" t="s">
         <v>1537</v>
       </c>
@@ -33728,7 +33731,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="35" s="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="80" t="s">
         <v>1538</v>
       </c>
@@ -33744,7 +33747,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="37" s="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
         <v>509</v>
@@ -33774,7 +33777,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="13.5" r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>593</v>
       </c>
@@ -33846,7 +33849,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="46" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="46" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>751</v>
       </c>
@@ -33872,22 +33875,22 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="48" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="34"/>
       <c r="B48" s="20"/>
       <c r="C48" s="22"/>
     </row>
-    <row r="49" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="49" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="20"/>
       <c r="B49" s="20"/>
       <c r="C49" s="22"/>
     </row>
-    <row r="50" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="50" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="20"/>
       <c r="B50" s="20"/>
       <c r="C50" s="22"/>
     </row>
-    <row r="51" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="51" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
         <v>499</v>
@@ -33917,7 +33920,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="55" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3" t="s">
         <v>510</v>
@@ -33925,7 +33928,7 @@
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="56" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>142</v>
       </c>
@@ -33936,7 +33939,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="57" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
         <v>428</v>
       </c>
@@ -33945,13 +33948,13 @@
       </c>
       <c r="C57" s="22"/>
     </row>
-    <row r="59" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="59" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="53"/>
       <c r="B59" s="53"/>
       <c r="C59" s="53"/>
       <c r="D59" s="53"/>
     </row>
-    <row r="60" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="60" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3" t="s">
         <v>621</v>
@@ -33959,7 +33962,7 @@
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="61" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
         <v>622</v>
       </c>
@@ -34213,7 +34216,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="86" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3" t="s">
         <v>935</v>
@@ -34232,7 +34235,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="14.25" r="89" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3" t="s">
         <v>1074</v>
@@ -34526,7 +34529,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="113" s="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="80" t="s">
         <v>1079</v>
       </c>
@@ -34537,7 +34540,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="114" spans="1:4" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="114" s="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="80" t="s">
         <v>1374</v>
       </c>
@@ -34705,13 +34708,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:ALR89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:ALS89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -34719,17 +34722,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -35770,7 +35773,7 @@
       <c r="ALQ1" s="5"/>
       <c r="ALR1" s="5"/>
     </row>
-    <row r="2" spans="1:1006" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -37924,7 +37927,7 @@
         <v>255</v>
       </c>
       <c r="E13" t="s">
-        <v>267</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="14" spans="1:1006" x14ac:dyDescent="0.25">
@@ -37961,7 +37964,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:1006" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="80" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A16" s="80" t="s">
         <v>1523</v>
       </c>
@@ -37975,7 +37978,7 @@
         <v>1521</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="80" t="s">
         <v>1524</v>
       </c>
@@ -37989,7 +37992,7 @@
         <v>1533</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="80" t="s">
         <v>1525</v>
       </c>
@@ -38017,7 +38020,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="21" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
         <v>492</v>
       </c>
@@ -38034,7 +38037,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="22" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="50" t="s">
         <v>592</v>
       </c>
@@ -38048,7 +38051,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="23" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="50" t="s">
         <v>747</v>
       </c>
@@ -38060,7 +38063,7 @@
       </c>
       <c r="E23" s="54"/>
     </row>
-    <row r="24" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="24" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="50" t="s">
         <v>750</v>
       </c>
@@ -38072,7 +38075,7 @@
       </c>
       <c r="E24" s="54"/>
     </row>
-    <row r="25" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E25" s="54"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -38314,7 +38317,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="37" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="50" t="s">
         <v>790</v>
       </c>
@@ -38331,7 +38334,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="38" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="53"/>
       <c r="B38" s="51"/>
       <c r="C38" s="51"/>
@@ -38357,7 +38360,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="40" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
         <v>938</v>
       </c>
@@ -38374,7 +38377,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="41" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="50" t="s">
         <v>942</v>
       </c>
@@ -38391,7 +38394,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="42" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="50" t="s">
         <v>946</v>
       </c>
@@ -38408,7 +38411,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="43" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="50" t="s">
         <v>967</v>
       </c>
@@ -38425,7 +38428,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="44" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="50" t="s">
         <v>968</v>
       </c>
@@ -38442,7 +38445,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="45" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="50" t="s">
         <v>969</v>
       </c>
@@ -38459,7 +38462,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="46" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="50" t="s">
         <v>987</v>
       </c>
@@ -38476,7 +38479,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="47" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="50" t="s">
         <v>992</v>
       </c>
@@ -38493,7 +38496,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="48" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="50" t="s">
         <v>990</v>
       </c>
@@ -38510,7 +38513,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="49" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="50" t="s">
         <v>991</v>
       </c>
@@ -38527,7 +38530,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="50" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="50" t="s">
         <v>1000</v>
       </c>
@@ -38544,7 +38547,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="51" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="50" t="s">
         <v>1036</v>
       </c>
@@ -38561,7 +38564,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="52" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="50" t="s">
         <v>1039</v>
       </c>
@@ -38578,7 +38581,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="53" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="50" t="s">
         <v>1042</v>
       </c>
@@ -38595,7 +38598,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="54" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="50" t="s">
         <v>1045</v>
       </c>
@@ -38612,7 +38615,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="55" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="53"/>
       <c r="B55" s="51"/>
       <c r="C55" s="51"/>
@@ -38624,7 +38627,7 @@
       <c r="I55" s="53"/>
       <c r="J55" s="53"/>
     </row>
-    <row r="57" spans="1:15" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="57" s="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D57" s="22"/>
       <c r="E57" s="22"/>
     </row>
@@ -38922,7 +38925,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="75" s="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="32" t="s">
         <v>1377</v>
       </c>
@@ -39155,15 +39158,15 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E59" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="E60" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
-    <hyperlink ref="E40" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
-    <hyperlink ref="E41" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
-    <hyperlink ref="E42" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
-    <hyperlink ref="E43" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
-    <hyperlink ref="E44" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
-    <hyperlink ref="E45" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink display="mailto:dealroom1.2+clientcontact01@gmail.com" r:id="rId1" ref="E59" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink display="mailto:dealroom1.2+clientcontact13@gmail.com" r:id="rId2" ref="E60" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink display="mailto:navatariptesting+11679@gmail.com" r:id="rId3" ref="E40" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink display="mailto:navatariptesting+18785@gmail.com" r:id="rId4" ref="E41" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink display="mailto:navatariptesting+49153@gmail.com" r:id="rId5" ref="E42" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink display="mailto:navatariptesting+11679@gmail.com" r:id="rId6" ref="E43" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink display="mailto:navatariptesting+18785@gmail.com" r:id="rId7" ref="E44" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink display="mailto:navatariptesting+49153@gmail.com" r:id="rId8" ref="E45" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Created 4 new Java Class File FieldAndRelationshipPageBusinessLayer, FieldAndRelationshipPage, LightningAppBuilderPageBusinessLayer, LightningAppBuilderPage 2. Created new function for DeleteContact,CreateAppPage,OpenSDG,
Signed-off-by: sourabhnavatargroup <sourabh@navatargroup.com>
</commit_message>
<xml_diff>
--- a/Phase1DataSheet.xlsx
+++ b/Phase1DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\einstein-code-version-2-pe2(Working)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="711" firstSheet="25" activeTab="32"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="711" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -45,10 +45,11 @@
     <sheet name="Coverages" sheetId="22" r:id="rId31"/>
     <sheet name="SDGActions" sheetId="24" r:id="rId32"/>
     <sheet name="Report" sheetId="25" r:id="rId33"/>
-    <sheet name="CustomEmailFolder" sheetId="26" r:id="rId34"/>
-    <sheet name="Task1" sheetId="27" r:id="rId35"/>
-    <sheet name="Events" sheetId="29" r:id="rId36"/>
-    <sheet name="MI" sheetId="30" r:id="rId37"/>
+    <sheet name="SDGData" sheetId="42" r:id="rId34"/>
+    <sheet name="CustomEmailFolder" sheetId="26" r:id="rId35"/>
+    <sheet name="Task1" sheetId="27" r:id="rId36"/>
+    <sheet name="Events" sheetId="29" r:id="rId37"/>
+    <sheet name="MI" sheetId="30" r:id="rId38"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="1665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3132" uniqueCount="1837">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -5094,6 +5095,522 @@
   </si>
   <si>
     <t>Unfiled Public Reports</t>
+  </si>
+  <si>
+    <t>Account Industry</t>
+  </si>
+  <si>
+    <t>Total Firms</t>
+  </si>
+  <si>
+    <t>Task as per Industries</t>
+  </si>
+  <si>
+    <t>Individuals</t>
+  </si>
+  <si>
+    <t>Fundraising as per Industries</t>
+  </si>
+  <si>
+    <t>SDG_GROUPBY_1 SDG(Phase 4 SDG Sheet (S.no 2 - 23))</t>
+  </si>
+  <si>
+    <t>M9SDGD_1</t>
+  </si>
+  <si>
+    <t>M9SDGD_2</t>
+  </si>
+  <si>
+    <t>Apparel</t>
+  </si>
+  <si>
+    <t>M9SDGD_3</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>M9SDGD_4</t>
+  </si>
+  <si>
+    <t>Biotechnology</t>
+  </si>
+  <si>
+    <t>M9SDGD_5</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>M9SDGD_6</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t>M9SDGD_7</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>M9SDGD_8</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>M9SDGD_9</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>M9SDGD_10</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>M9SDGD_11</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>M9SDGD_12</t>
+  </si>
+  <si>
+    <t>Environmental</t>
+  </si>
+  <si>
+    <t>M9SDGD_13</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>M9SDGD_14</t>
+  </si>
+  <si>
+    <t>Food &amp; Beverage</t>
+  </si>
+  <si>
+    <t>M9SDGD_15</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>M9SDGD_16</t>
+  </si>
+  <si>
+    <t>Hospitality</t>
+  </si>
+  <si>
+    <t>M9SDGD_17</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>M9SDGD_18</t>
+  </si>
+  <si>
+    <t>Retail</t>
+  </si>
+  <si>
+    <t>M9SDGD_19</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>M9SDGD_20</t>
+  </si>
+  <si>
+    <t>Transporation</t>
+  </si>
+  <si>
+    <t>SDG_GROUPBY_1 SDG</t>
+  </si>
+  <si>
+    <t>SDG_GROUPBY_1 SDG(Phase 4 SDG Sheet (S.no 26 - 47))</t>
+  </si>
+  <si>
+    <t>M9SDGD_21</t>
+  </si>
+  <si>
+    <t>M9SDGD_22</t>
+  </si>
+  <si>
+    <t>M9SDGD_23</t>
+  </si>
+  <si>
+    <t>M9SDGD_24</t>
+  </si>
+  <si>
+    <t>M9SDGD_25</t>
+  </si>
+  <si>
+    <t>M9SDGD_26</t>
+  </si>
+  <si>
+    <t>M9SDGD_27</t>
+  </si>
+  <si>
+    <t>M9SDGD_28</t>
+  </si>
+  <si>
+    <t>M9SDGD_29</t>
+  </si>
+  <si>
+    <t>M9SDGD_30</t>
+  </si>
+  <si>
+    <t>M9SDGD_31</t>
+  </si>
+  <si>
+    <t>M9SDGD_32</t>
+  </si>
+  <si>
+    <t>M9SDGD_33</t>
+  </si>
+  <si>
+    <t>M9SDGD_34</t>
+  </si>
+  <si>
+    <t>M9SDGD_35</t>
+  </si>
+  <si>
+    <t>M9SDGD_36</t>
+  </si>
+  <si>
+    <t>M9SDGD_37</t>
+  </si>
+  <si>
+    <t>M9SDGD_38</t>
+  </si>
+  <si>
+    <t>M9SDGD_39</t>
+  </si>
+  <si>
+    <t>M9SDGD_40</t>
+  </si>
+  <si>
+    <t>SDG_GROUPBY_1 SDG(Phase 4 SDG Sheet (S.no 50 - 71))</t>
+  </si>
+  <si>
+    <t>M9SDGD_41</t>
+  </si>
+  <si>
+    <t>M9SDGD_42</t>
+  </si>
+  <si>
+    <t>M9SDGD_43</t>
+  </si>
+  <si>
+    <t>M9SDGD_44</t>
+  </si>
+  <si>
+    <t>BiotechnologyUP</t>
+  </si>
+  <si>
+    <t>M9SDGD_45</t>
+  </si>
+  <si>
+    <t>M9SDGD_46</t>
+  </si>
+  <si>
+    <t>M9SDGD_47</t>
+  </si>
+  <si>
+    <t>M9SDGD_48</t>
+  </si>
+  <si>
+    <t>M9SDGD_49</t>
+  </si>
+  <si>
+    <t>M9SDGD_50</t>
+  </si>
+  <si>
+    <t>M9SDGD_51</t>
+  </si>
+  <si>
+    <t>M9SDGD_52</t>
+  </si>
+  <si>
+    <t>M9SDGD_53</t>
+  </si>
+  <si>
+    <t>M9SDGD_54</t>
+  </si>
+  <si>
+    <t>M9SDGD_55</t>
+  </si>
+  <si>
+    <t>M9SDGD_56</t>
+  </si>
+  <si>
+    <t>M9SDGD_57</t>
+  </si>
+  <si>
+    <t>M9SDGD_58</t>
+  </si>
+  <si>
+    <t>M9SDGD_59</t>
+  </si>
+  <si>
+    <t>M9SDGD_60</t>
+  </si>
+  <si>
+    <t>SDG_GROUPBY_1 SDG(Phase 4 SDG Sheet (S.no 73 - 94))</t>
+  </si>
+  <si>
+    <t>M9SDGD_61</t>
+  </si>
+  <si>
+    <t>M9SDGD_62</t>
+  </si>
+  <si>
+    <t>M9SDGD_63</t>
+  </si>
+  <si>
+    <t>M9SDGD_64</t>
+  </si>
+  <si>
+    <t>M9SDGD_65</t>
+  </si>
+  <si>
+    <t>M9SDGD_66</t>
+  </si>
+  <si>
+    <t>M9SDGD_67</t>
+  </si>
+  <si>
+    <t>M9SDGD_68</t>
+  </si>
+  <si>
+    <t>M9SDGD_69</t>
+  </si>
+  <si>
+    <t>M9SDGD_70</t>
+  </si>
+  <si>
+    <t>M9SDGD_71</t>
+  </si>
+  <si>
+    <t>M9SDGD_72</t>
+  </si>
+  <si>
+    <t>M9SDGD_73</t>
+  </si>
+  <si>
+    <t>M9SDGD_74</t>
+  </si>
+  <si>
+    <t>M9SDGD_75</t>
+  </si>
+  <si>
+    <t>M9SDGD_76</t>
+  </si>
+  <si>
+    <t>M9SDGD_77</t>
+  </si>
+  <si>
+    <t>M9SDGD_78</t>
+  </si>
+  <si>
+    <t>M9SDGD_79</t>
+  </si>
+  <si>
+    <t>M9SDGD_80</t>
+  </si>
+  <si>
+    <t>SDG_GROUPBY_1 SDG(Phase 4 SDG Sheet (S.no 96 - 116))</t>
+  </si>
+  <si>
+    <t>M9SDGD_81</t>
+  </si>
+  <si>
+    <t>M9SDGD_82</t>
+  </si>
+  <si>
+    <t>M9SDGD_83</t>
+  </si>
+  <si>
+    <t>M9SDGD_84</t>
+  </si>
+  <si>
+    <t>M9SDGD_85</t>
+  </si>
+  <si>
+    <t>M9SDGD_86</t>
+  </si>
+  <si>
+    <t>M9SDGD_87</t>
+  </si>
+  <si>
+    <t>M9SDGD_88</t>
+  </si>
+  <si>
+    <t>M9SDGD_89</t>
+  </si>
+  <si>
+    <t>M9SDGD_90</t>
+  </si>
+  <si>
+    <t>M9SDGD_91</t>
+  </si>
+  <si>
+    <t>M9SDGD_92</t>
+  </si>
+  <si>
+    <t>M9SDGD_93</t>
+  </si>
+  <si>
+    <t>M9SDGD_94</t>
+  </si>
+  <si>
+    <t>M9SDGD_95</t>
+  </si>
+  <si>
+    <t>M9SDGD_96</t>
+  </si>
+  <si>
+    <t>M9SDGD_97</t>
+  </si>
+  <si>
+    <t>M9SDGD_98</t>
+  </si>
+  <si>
+    <t>M9SDGD_99</t>
+  </si>
+  <si>
+    <t>SDG_GROUPBY_1 SDG(Phase 4 SDG Sheet (S.no 118 - 137))</t>
+  </si>
+  <si>
+    <t>M9SDGD_100</t>
+  </si>
+  <si>
+    <t>M9SDGD_101</t>
+  </si>
+  <si>
+    <t>M9SDGD_102</t>
+  </si>
+  <si>
+    <t>M9SDGD_103</t>
+  </si>
+  <si>
+    <t>M9SDGD_104</t>
+  </si>
+  <si>
+    <t>M9SDGD_105</t>
+  </si>
+  <si>
+    <t>M9SDGD_106</t>
+  </si>
+  <si>
+    <t>M9SDGD_107</t>
+  </si>
+  <si>
+    <t>M9SDGD_108</t>
+  </si>
+  <si>
+    <t>M9SDGD_109</t>
+  </si>
+  <si>
+    <t>M9SDGD_110</t>
+  </si>
+  <si>
+    <t>M9SDGD_111</t>
+  </si>
+  <si>
+    <t>M9SDGD_112</t>
+  </si>
+  <si>
+    <t>M9SDGD_113</t>
+  </si>
+  <si>
+    <t>M9SDGD_114</t>
+  </si>
+  <si>
+    <t>M9SDGD_115</t>
+  </si>
+  <si>
+    <t>M9SDGD_116</t>
+  </si>
+  <si>
+    <t>M9SDGD_117</t>
+  </si>
+  <si>
+    <t>SDG_GROUPBY_1 SDG(Phase 4 SDG Sheet (S.no 139 - 158))</t>
+  </si>
+  <si>
+    <t>M9SDGD_118</t>
+  </si>
+  <si>
+    <t>M9SDGD_119</t>
+  </si>
+  <si>
+    <t>M9SDGD_120</t>
+  </si>
+  <si>
+    <t>M9SDGD_121</t>
+  </si>
+  <si>
+    <t>M9SDGD_122</t>
+  </si>
+  <si>
+    <t>M9SDGD_123</t>
+  </si>
+  <si>
+    <t>M9SDGD_124</t>
+  </si>
+  <si>
+    <t>M9SDGD_125</t>
+  </si>
+  <si>
+    <t>M9SDGD_126</t>
+  </si>
+  <si>
+    <t>M9SDGD_127</t>
+  </si>
+  <si>
+    <t>M9SDGD_128</t>
+  </si>
+  <si>
+    <t>M9SDGD_129</t>
+  </si>
+  <si>
+    <t>M9SDGD_130</t>
+  </si>
+  <si>
+    <t>M9SDGD_131</t>
+  </si>
+  <si>
+    <t>M9SDGD_132</t>
+  </si>
+  <si>
+    <t>M9SDGD_133</t>
+  </si>
+  <si>
+    <t>M9SDGD_134</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>M9SDGD_135</t>
+  </si>
+  <si>
+    <t>M9CON1</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Falcon -1</t>
   </si>
 </sst>
 </file>
@@ -5278,7 +5795,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5499,6 +6016,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6018,10 +6541,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALR89"/>
+  <dimension ref="A1:ALR90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10457,7 +10980,36 @@
       <c r="A88" s="80"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A89" s="80"/>
+      <c r="A89" s="3"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D89" s="4"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="3"/>
+      <c r="H89" s="3"/>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A90" s="80" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B90" s="80" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C90" s="80" t="s">
+        <v>1836</v>
+      </c>
+      <c r="D90" s="80"/>
+      <c r="E90" s="80"/>
+      <c r="F90" s="80"/>
+      <c r="G90" s="80"/>
+      <c r="H90" s="80"/>
+      <c r="I90" s="80"/>
+      <c r="J90" s="80"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -27290,7 +27842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -27465,6 +28017,2945 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F157"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1666</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1668</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="107"/>
+      <c r="C3" s="9" t="s">
+        <v>1646</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="109" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="108"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="68" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B5" s="110" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C5" s="68">
+        <v>1</v>
+      </c>
+      <c r="D5" s="68">
+        <v>0</v>
+      </c>
+      <c r="E5" s="68">
+        <v>3</v>
+      </c>
+      <c r="F5" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="68" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B6" s="110" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C6" s="68">
+        <v>1</v>
+      </c>
+      <c r="D6" s="68">
+        <v>0</v>
+      </c>
+      <c r="E6" s="68">
+        <v>3</v>
+      </c>
+      <c r="F6" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="68" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B7" s="110" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C7" s="68">
+        <v>1</v>
+      </c>
+      <c r="D7" s="68">
+        <v>0</v>
+      </c>
+      <c r="E7" s="68">
+        <v>3</v>
+      </c>
+      <c r="F7" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="68" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B8" s="110" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C8" s="68">
+        <v>1</v>
+      </c>
+      <c r="D8" s="68">
+        <v>0</v>
+      </c>
+      <c r="E8" s="68">
+        <v>3</v>
+      </c>
+      <c r="F8" s="68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="68" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B9" s="110" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C9" s="68">
+        <v>1</v>
+      </c>
+      <c r="D9" s="68">
+        <v>0</v>
+      </c>
+      <c r="E9" s="68">
+        <v>3</v>
+      </c>
+      <c r="F9" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="68" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B10" s="110" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C10" s="68">
+        <v>1</v>
+      </c>
+      <c r="D10" s="68">
+        <v>0</v>
+      </c>
+      <c r="E10" s="68">
+        <v>2</v>
+      </c>
+      <c r="F10" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="68" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B11" s="110" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C11" s="68">
+        <v>1</v>
+      </c>
+      <c r="D11" s="68">
+        <v>0</v>
+      </c>
+      <c r="E11" s="68">
+        <v>2</v>
+      </c>
+      <c r="F11" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="68" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B12" s="110" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C12" s="68">
+        <v>1</v>
+      </c>
+      <c r="D12" s="68">
+        <v>0</v>
+      </c>
+      <c r="E12" s="68">
+        <v>2</v>
+      </c>
+      <c r="F12" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="68" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B13" s="110" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C13" s="68">
+        <v>1</v>
+      </c>
+      <c r="D13" s="68">
+        <v>0</v>
+      </c>
+      <c r="E13" s="68">
+        <v>2</v>
+      </c>
+      <c r="F13" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="68" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B14" s="110" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C14" s="68">
+        <v>1</v>
+      </c>
+      <c r="D14" s="68">
+        <v>0</v>
+      </c>
+      <c r="E14" s="68">
+        <v>2</v>
+      </c>
+      <c r="F14" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="68" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B15" s="110" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C15" s="68">
+        <v>1</v>
+      </c>
+      <c r="D15" s="68">
+        <v>0</v>
+      </c>
+      <c r="E15" s="68">
+        <v>0</v>
+      </c>
+      <c r="F15" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="68" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B16" s="110" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C16" s="68">
+        <v>1</v>
+      </c>
+      <c r="D16" s="68">
+        <v>0</v>
+      </c>
+      <c r="E16" s="68">
+        <v>0</v>
+      </c>
+      <c r="F16" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="68" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B17" s="110" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C17" s="68">
+        <v>1</v>
+      </c>
+      <c r="D17" s="68">
+        <v>0</v>
+      </c>
+      <c r="E17" s="68">
+        <v>0</v>
+      </c>
+      <c r="F17" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="68" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B18" s="110" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C18" s="68">
+        <v>1</v>
+      </c>
+      <c r="D18" s="68">
+        <v>0</v>
+      </c>
+      <c r="E18" s="68">
+        <v>0</v>
+      </c>
+      <c r="F18" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="68" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B19" s="110" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C19" s="68">
+        <v>2</v>
+      </c>
+      <c r="D19" s="68">
+        <v>0</v>
+      </c>
+      <c r="E19" s="68">
+        <v>0</v>
+      </c>
+      <c r="F19" s="110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="68" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B20" s="110" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C20" s="68">
+        <v>2</v>
+      </c>
+      <c r="D20" s="68">
+        <v>0</v>
+      </c>
+      <c r="E20" s="68">
+        <v>0</v>
+      </c>
+      <c r="F20" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="68" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B21" s="110" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C21" s="68">
+        <v>2</v>
+      </c>
+      <c r="D21" s="68">
+        <v>0</v>
+      </c>
+      <c r="E21" s="68">
+        <v>0</v>
+      </c>
+      <c r="F21" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="68" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B22" s="110" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C22" s="68">
+        <v>2</v>
+      </c>
+      <c r="D22" s="68">
+        <v>0</v>
+      </c>
+      <c r="E22" s="68">
+        <v>0</v>
+      </c>
+      <c r="F22" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="68" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B23" s="110" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C23" s="68">
+        <v>1</v>
+      </c>
+      <c r="D23" s="68">
+        <v>0</v>
+      </c>
+      <c r="E23" s="68">
+        <v>0</v>
+      </c>
+      <c r="F23" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="68" t="s">
+        <v>1708</v>
+      </c>
+      <c r="B24" s="110" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C24" s="68">
+        <v>2</v>
+      </c>
+      <c r="D24" s="68">
+        <v>0</v>
+      </c>
+      <c r="E24" s="68">
+        <v>0</v>
+      </c>
+      <c r="F24" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="9"/>
+      <c r="B26" s="107"/>
+      <c r="C26" s="109" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="9"/>
+      <c r="B27" s="107"/>
+      <c r="C27" s="109" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="68" t="s">
+        <v>1712</v>
+      </c>
+      <c r="B28" s="110" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C28" s="68">
+        <v>1</v>
+      </c>
+      <c r="D28" s="68">
+        <v>0</v>
+      </c>
+      <c r="E28" s="68">
+        <v>2</v>
+      </c>
+      <c r="F28" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="68" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B29" s="110" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C29" s="68">
+        <v>1</v>
+      </c>
+      <c r="D29" s="68">
+        <v>0</v>
+      </c>
+      <c r="E29" s="68">
+        <v>3</v>
+      </c>
+      <c r="F29" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="68" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B30" s="110" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C30" s="68">
+        <v>1</v>
+      </c>
+      <c r="D30" s="68">
+        <v>0</v>
+      </c>
+      <c r="E30" s="68">
+        <v>3</v>
+      </c>
+      <c r="F30" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="68" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B31" s="110" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C31" s="68">
+        <v>1</v>
+      </c>
+      <c r="D31" s="68">
+        <v>0</v>
+      </c>
+      <c r="E31" s="68">
+        <v>3</v>
+      </c>
+      <c r="F31" s="68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="68" t="s">
+        <v>1716</v>
+      </c>
+      <c r="B32" s="110" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C32" s="68">
+        <v>1</v>
+      </c>
+      <c r="D32" s="68">
+        <v>0</v>
+      </c>
+      <c r="E32" s="68">
+        <v>3</v>
+      </c>
+      <c r="F32" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="68" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B33" s="110" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C33" s="68">
+        <v>1</v>
+      </c>
+      <c r="D33" s="68">
+        <v>0</v>
+      </c>
+      <c r="E33" s="68">
+        <v>2</v>
+      </c>
+      <c r="F33" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="68" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B34" s="110" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C34" s="68">
+        <v>1</v>
+      </c>
+      <c r="D34" s="68">
+        <v>0</v>
+      </c>
+      <c r="E34" s="68">
+        <v>2</v>
+      </c>
+      <c r="F34" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="68" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B35" s="110" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C35" s="68">
+        <v>1</v>
+      </c>
+      <c r="D35" s="68">
+        <v>0</v>
+      </c>
+      <c r="E35" s="68">
+        <v>2</v>
+      </c>
+      <c r="F35" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="68" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B36" s="110" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C36" s="68">
+        <v>1</v>
+      </c>
+      <c r="D36" s="68">
+        <v>0</v>
+      </c>
+      <c r="E36" s="68">
+        <v>2</v>
+      </c>
+      <c r="F36" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="68" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B37" s="110" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C37" s="68">
+        <v>1</v>
+      </c>
+      <c r="D37" s="68">
+        <v>0</v>
+      </c>
+      <c r="E37" s="68">
+        <v>2</v>
+      </c>
+      <c r="F37" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="68" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B38" s="110" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C38" s="68">
+        <v>1</v>
+      </c>
+      <c r="D38" s="68">
+        <v>0</v>
+      </c>
+      <c r="E38" s="68">
+        <v>0</v>
+      </c>
+      <c r="F38" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="68" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B39" s="110" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C39" s="68">
+        <v>1</v>
+      </c>
+      <c r="D39" s="68">
+        <v>0</v>
+      </c>
+      <c r="E39" s="68">
+        <v>0</v>
+      </c>
+      <c r="F39" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="68" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B40" s="110" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C40" s="68">
+        <v>1</v>
+      </c>
+      <c r="D40" s="68">
+        <v>0</v>
+      </c>
+      <c r="E40" s="68">
+        <v>0</v>
+      </c>
+      <c r="F40" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="68" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B41" s="110" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C41" s="68">
+        <v>1</v>
+      </c>
+      <c r="D41" s="68">
+        <v>0</v>
+      </c>
+      <c r="E41" s="68">
+        <v>0</v>
+      </c>
+      <c r="F41" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="68" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B42" s="110" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C42" s="68">
+        <v>2</v>
+      </c>
+      <c r="D42" s="68">
+        <v>0</v>
+      </c>
+      <c r="E42" s="68">
+        <v>0</v>
+      </c>
+      <c r="F42" s="110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="68" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B43" s="110" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C43" s="68">
+        <v>2</v>
+      </c>
+      <c r="D43" s="68">
+        <v>0</v>
+      </c>
+      <c r="E43" s="68">
+        <v>0</v>
+      </c>
+      <c r="F43" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="68" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B44" s="110" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C44" s="68">
+        <v>2</v>
+      </c>
+      <c r="D44" s="68">
+        <v>0</v>
+      </c>
+      <c r="E44" s="68">
+        <v>0</v>
+      </c>
+      <c r="F44" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="68" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B45" s="110" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C45" s="68">
+        <v>2</v>
+      </c>
+      <c r="D45" s="68">
+        <v>0</v>
+      </c>
+      <c r="E45" s="68">
+        <v>0</v>
+      </c>
+      <c r="F45" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="68" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B46" s="110" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C46" s="68">
+        <v>1</v>
+      </c>
+      <c r="D46" s="68">
+        <v>0</v>
+      </c>
+      <c r="E46" s="68">
+        <v>0</v>
+      </c>
+      <c r="F46" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="68" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B47" s="110" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C47" s="68">
+        <v>2</v>
+      </c>
+      <c r="D47" s="68">
+        <v>0</v>
+      </c>
+      <c r="E47" s="68">
+        <v>0</v>
+      </c>
+      <c r="F47" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="9"/>
+      <c r="B49" s="107"/>
+      <c r="C49" s="109" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" s="108"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="9"/>
+      <c r="B50" s="107"/>
+      <c r="C50" s="109" t="s">
+        <v>1732</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="108"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="68" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B51" s="110" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C51" s="68">
+        <v>1</v>
+      </c>
+      <c r="D51" s="68">
+        <v>0</v>
+      </c>
+      <c r="E51" s="68">
+        <v>3</v>
+      </c>
+      <c r="F51" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="68" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B52" s="110" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C52" s="68">
+        <v>1</v>
+      </c>
+      <c r="D52" s="68">
+        <v>0</v>
+      </c>
+      <c r="E52" s="68">
+        <v>3</v>
+      </c>
+      <c r="F52" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="68" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B53" s="110" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C53" s="68">
+        <v>1</v>
+      </c>
+      <c r="D53" s="68">
+        <v>0</v>
+      </c>
+      <c r="E53" s="68">
+        <v>3</v>
+      </c>
+      <c r="F53" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="68" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B54" s="110" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C54" s="68">
+        <v>0</v>
+      </c>
+      <c r="D54" s="68">
+        <v>0</v>
+      </c>
+      <c r="E54" s="68">
+        <v>0</v>
+      </c>
+      <c r="F54" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="68" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B55" s="110" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C55" s="68">
+        <v>1</v>
+      </c>
+      <c r="D55" s="68">
+        <v>0</v>
+      </c>
+      <c r="E55" s="68">
+        <v>3</v>
+      </c>
+      <c r="F55" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="68" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B56" s="110" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C56" s="68">
+        <v>1</v>
+      </c>
+      <c r="D56" s="68">
+        <v>0</v>
+      </c>
+      <c r="E56" s="68">
+        <v>2</v>
+      </c>
+      <c r="F56" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="68" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B57" s="110" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C57" s="68">
+        <v>1</v>
+      </c>
+      <c r="D57" s="68">
+        <v>0</v>
+      </c>
+      <c r="E57" s="68">
+        <v>2</v>
+      </c>
+      <c r="F57" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="68" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B58" s="110" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C58" s="68">
+        <v>1</v>
+      </c>
+      <c r="D58" s="68">
+        <v>0</v>
+      </c>
+      <c r="E58" s="68">
+        <v>2</v>
+      </c>
+      <c r="F58" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="68" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B59" s="110" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C59" s="68">
+        <v>1</v>
+      </c>
+      <c r="D59" s="68">
+        <v>0</v>
+      </c>
+      <c r="E59" s="68">
+        <v>2</v>
+      </c>
+      <c r="F59" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="68" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B60" s="110" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C60" s="68">
+        <v>1</v>
+      </c>
+      <c r="D60" s="68">
+        <v>0</v>
+      </c>
+      <c r="E60" s="68">
+        <v>2</v>
+      </c>
+      <c r="F60" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="68" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B61" s="110" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C61" s="68">
+        <v>1</v>
+      </c>
+      <c r="D61" s="68">
+        <v>0</v>
+      </c>
+      <c r="E61" s="68">
+        <v>0</v>
+      </c>
+      <c r="F61" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="68" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B62" s="110" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C62" s="68">
+        <v>1</v>
+      </c>
+      <c r="D62" s="68">
+        <v>0</v>
+      </c>
+      <c r="E62" s="68">
+        <v>0</v>
+      </c>
+      <c r="F62" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="68" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B63" s="110" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C63" s="68">
+        <v>1</v>
+      </c>
+      <c r="D63" s="68">
+        <v>0</v>
+      </c>
+      <c r="E63" s="68">
+        <v>0</v>
+      </c>
+      <c r="F63" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="68" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B64" s="110" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C64" s="68">
+        <v>1</v>
+      </c>
+      <c r="D64" s="68">
+        <v>0</v>
+      </c>
+      <c r="E64" s="68">
+        <v>0</v>
+      </c>
+      <c r="F64" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" s="68" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B65" s="110" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C65" s="68">
+        <v>2</v>
+      </c>
+      <c r="D65" s="68">
+        <v>0</v>
+      </c>
+      <c r="E65" s="68">
+        <v>0</v>
+      </c>
+      <c r="F65" s="110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" s="68" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B66" s="110" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C66" s="68">
+        <v>2</v>
+      </c>
+      <c r="D66" s="68">
+        <v>0</v>
+      </c>
+      <c r="E66" s="68">
+        <v>0</v>
+      </c>
+      <c r="F66" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="68" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B67" s="110" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C67" s="68">
+        <v>2</v>
+      </c>
+      <c r="D67" s="68">
+        <v>0</v>
+      </c>
+      <c r="E67" s="68">
+        <v>0</v>
+      </c>
+      <c r="F67" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" s="68" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B68" s="110" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C68" s="68">
+        <v>2</v>
+      </c>
+      <c r="D68" s="68">
+        <v>0</v>
+      </c>
+      <c r="E68" s="68">
+        <v>0</v>
+      </c>
+      <c r="F68" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" s="68" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B69" s="110" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C69" s="68">
+        <v>1</v>
+      </c>
+      <c r="D69" s="68">
+        <v>0</v>
+      </c>
+      <c r="E69" s="68">
+        <v>0</v>
+      </c>
+      <c r="F69" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="68" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B70" s="110" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C70" s="68">
+        <v>2</v>
+      </c>
+      <c r="D70" s="68">
+        <v>0</v>
+      </c>
+      <c r="E70" s="68">
+        <v>0</v>
+      </c>
+      <c r="F70" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A72" s="9"/>
+      <c r="B72" s="107"/>
+      <c r="C72" s="109" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D72" s="9"/>
+      <c r="E72" s="108"/>
+      <c r="F72" s="4"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" s="9"/>
+      <c r="B73" s="107"/>
+      <c r="C73" s="109" t="s">
+        <v>1754</v>
+      </c>
+      <c r="D73" s="9"/>
+      <c r="E73" s="108"/>
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" s="68" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B74" s="110" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C74" s="68">
+        <v>1</v>
+      </c>
+      <c r="D74" s="68">
+        <v>0</v>
+      </c>
+      <c r="E74" s="68">
+        <v>3</v>
+      </c>
+      <c r="F74" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" s="68" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B75" s="110" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C75" s="68">
+        <v>1</v>
+      </c>
+      <c r="D75" s="68">
+        <v>0</v>
+      </c>
+      <c r="E75" s="68">
+        <v>3</v>
+      </c>
+      <c r="F75" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" s="68" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B76" s="110" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C76" s="68">
+        <v>1</v>
+      </c>
+      <c r="D76" s="68">
+        <v>0</v>
+      </c>
+      <c r="E76" s="68">
+        <v>3</v>
+      </c>
+      <c r="F76" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" s="68" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B77" s="110" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C77" s="68">
+        <v>1</v>
+      </c>
+      <c r="D77" s="68">
+        <v>0</v>
+      </c>
+      <c r="E77" s="68">
+        <v>3</v>
+      </c>
+      <c r="F77" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" s="68" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B78" s="110" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C78" s="68">
+        <v>1</v>
+      </c>
+      <c r="D78" s="68">
+        <v>0</v>
+      </c>
+      <c r="E78" s="68">
+        <v>2</v>
+      </c>
+      <c r="F78" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79" s="68" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B79" s="110" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C79" s="68">
+        <v>1</v>
+      </c>
+      <c r="D79" s="68">
+        <v>0</v>
+      </c>
+      <c r="E79" s="68">
+        <v>2</v>
+      </c>
+      <c r="F79" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A80" s="68" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B80" s="110" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C80" s="68">
+        <v>1</v>
+      </c>
+      <c r="D80" s="68">
+        <v>0</v>
+      </c>
+      <c r="E80" s="68">
+        <v>2</v>
+      </c>
+      <c r="F80" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A81" s="68" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B81" s="110" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C81" s="68">
+        <v>1</v>
+      </c>
+      <c r="D81" s="68">
+        <v>0</v>
+      </c>
+      <c r="E81" s="68">
+        <v>2</v>
+      </c>
+      <c r="F81" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" s="68" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B82" s="110" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C82" s="68">
+        <v>1</v>
+      </c>
+      <c r="D82" s="68">
+        <v>0</v>
+      </c>
+      <c r="E82" s="68">
+        <v>2</v>
+      </c>
+      <c r="F82" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" s="68" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B83" s="110" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C83" s="68">
+        <v>1</v>
+      </c>
+      <c r="D83" s="68">
+        <v>0</v>
+      </c>
+      <c r="E83" s="68">
+        <v>0</v>
+      </c>
+      <c r="F83" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84" s="68" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B84" s="110" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C84" s="68">
+        <v>1</v>
+      </c>
+      <c r="D84" s="68">
+        <v>0</v>
+      </c>
+      <c r="E84" s="68">
+        <v>0</v>
+      </c>
+      <c r="F84" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" s="68" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B85" s="110" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C85" s="68">
+        <v>1</v>
+      </c>
+      <c r="D85" s="68">
+        <v>0</v>
+      </c>
+      <c r="E85" s="68">
+        <v>0</v>
+      </c>
+      <c r="F85" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86" s="68" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B86" s="110" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C86" s="68">
+        <v>1</v>
+      </c>
+      <c r="D86" s="68">
+        <v>0</v>
+      </c>
+      <c r="E86" s="68">
+        <v>0</v>
+      </c>
+      <c r="F86" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87" s="68" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B87" s="110" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C87" s="68">
+        <v>2</v>
+      </c>
+      <c r="D87" s="68">
+        <v>0</v>
+      </c>
+      <c r="E87" s="68">
+        <v>0</v>
+      </c>
+      <c r="F87" s="110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A88" s="68" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B88" s="110" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C88" s="68">
+        <v>2</v>
+      </c>
+      <c r="D88" s="68">
+        <v>0</v>
+      </c>
+      <c r="E88" s="68">
+        <v>0</v>
+      </c>
+      <c r="F88" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89" s="68" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B89" s="110" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C89" s="68">
+        <v>2</v>
+      </c>
+      <c r="D89" s="68">
+        <v>0</v>
+      </c>
+      <c r="E89" s="68">
+        <v>0</v>
+      </c>
+      <c r="F89" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A90" s="68" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B90" s="110" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C90" s="68">
+        <v>2</v>
+      </c>
+      <c r="D90" s="68">
+        <v>0</v>
+      </c>
+      <c r="E90" s="68">
+        <v>0</v>
+      </c>
+      <c r="F90" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A91" s="68" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B91" s="110" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C91" s="68">
+        <v>1</v>
+      </c>
+      <c r="D91" s="68">
+        <v>0</v>
+      </c>
+      <c r="E91" s="68">
+        <v>0</v>
+      </c>
+      <c r="F91" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A92" s="68" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B92" s="110" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C92" s="68">
+        <v>0</v>
+      </c>
+      <c r="D92" s="68">
+        <v>0</v>
+      </c>
+      <c r="E92" s="68">
+        <v>0</v>
+      </c>
+      <c r="F92" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A93" s="68" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B93" s="110" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C93" s="68">
+        <v>2</v>
+      </c>
+      <c r="D93" s="68">
+        <v>0</v>
+      </c>
+      <c r="E93" s="68">
+        <v>0</v>
+      </c>
+      <c r="F93" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A95" s="9"/>
+      <c r="B95" s="107"/>
+      <c r="C95" s="109" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D95" s="9"/>
+      <c r="E95" s="108"/>
+      <c r="F95" s="4"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A96" s="9"/>
+      <c r="B96" s="107"/>
+      <c r="C96" s="109" t="s">
+        <v>1775</v>
+      </c>
+      <c r="D96" s="9"/>
+      <c r="E96" s="108"/>
+      <c r="F96" s="4"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A97" s="68" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B97" s="110" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C97" s="68">
+        <v>1</v>
+      </c>
+      <c r="D97" s="68">
+        <v>0</v>
+      </c>
+      <c r="E97" s="68">
+        <v>3</v>
+      </c>
+      <c r="F97" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98" s="68" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B98" s="110" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C98" s="68">
+        <v>1</v>
+      </c>
+      <c r="D98" s="68">
+        <v>0</v>
+      </c>
+      <c r="E98" s="68">
+        <v>3</v>
+      </c>
+      <c r="F98" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99" s="68" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B99" s="110" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C99" s="68">
+        <v>1</v>
+      </c>
+      <c r="D99" s="68">
+        <v>0</v>
+      </c>
+      <c r="E99" s="68">
+        <v>3</v>
+      </c>
+      <c r="F99" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100" s="68" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B100" s="110" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C100" s="68">
+        <v>1</v>
+      </c>
+      <c r="D100" s="68">
+        <v>0</v>
+      </c>
+      <c r="E100" s="68">
+        <v>2</v>
+      </c>
+      <c r="F100" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A101" s="68" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B101" s="110" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C101" s="68">
+        <v>1</v>
+      </c>
+      <c r="D101" s="68">
+        <v>0</v>
+      </c>
+      <c r="E101" s="68">
+        <v>2</v>
+      </c>
+      <c r="F101" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A102" s="68" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B102" s="110" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C102" s="68">
+        <v>2</v>
+      </c>
+      <c r="D102" s="68">
+        <v>0</v>
+      </c>
+      <c r="E102" s="68">
+        <v>5</v>
+      </c>
+      <c r="F102" s="110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A103" s="68" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B103" s="110" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C103" s="68">
+        <v>1</v>
+      </c>
+      <c r="D103" s="68">
+        <v>0</v>
+      </c>
+      <c r="E103" s="68">
+        <v>2</v>
+      </c>
+      <c r="F103" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A104" s="68" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B104" s="110" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C104" s="68">
+        <v>1</v>
+      </c>
+      <c r="D104" s="68">
+        <v>0</v>
+      </c>
+      <c r="E104" s="68">
+        <v>2</v>
+      </c>
+      <c r="F104" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A105" s="68" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B105" s="110" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C105" s="68">
+        <v>1</v>
+      </c>
+      <c r="D105" s="68">
+        <v>0</v>
+      </c>
+      <c r="E105" s="68">
+        <v>0</v>
+      </c>
+      <c r="F105" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A106" s="68" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B106" s="110" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C106" s="68">
+        <v>1</v>
+      </c>
+      <c r="D106" s="68">
+        <v>0</v>
+      </c>
+      <c r="E106" s="68">
+        <v>0</v>
+      </c>
+      <c r="F106" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A107" s="68" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B107" s="110" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C107" s="68">
+        <v>1</v>
+      </c>
+      <c r="D107" s="68">
+        <v>0</v>
+      </c>
+      <c r="E107" s="68">
+        <v>0</v>
+      </c>
+      <c r="F107" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108" s="68" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B108" s="110" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C108" s="68">
+        <v>1</v>
+      </c>
+      <c r="D108" s="68">
+        <v>0</v>
+      </c>
+      <c r="E108" s="68">
+        <v>0</v>
+      </c>
+      <c r="F108" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109" s="68" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B109" s="110" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C109" s="68">
+        <v>2</v>
+      </c>
+      <c r="D109" s="68">
+        <v>0</v>
+      </c>
+      <c r="E109" s="68">
+        <v>0</v>
+      </c>
+      <c r="F109" s="110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" s="68" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B110" s="110" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C110" s="68">
+        <v>2</v>
+      </c>
+      <c r="D110" s="68">
+        <v>0</v>
+      </c>
+      <c r="E110" s="68">
+        <v>0</v>
+      </c>
+      <c r="F110" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111" s="68" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B111" s="110" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C111" s="68">
+        <v>2</v>
+      </c>
+      <c r="D111" s="68">
+        <v>0</v>
+      </c>
+      <c r="E111" s="68">
+        <v>0</v>
+      </c>
+      <c r="F111" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112" s="68" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B112" s="110" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C112" s="68">
+        <v>2</v>
+      </c>
+      <c r="D112" s="68">
+        <v>0</v>
+      </c>
+      <c r="E112" s="68">
+        <v>0</v>
+      </c>
+      <c r="F112" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A113" s="68" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B113" s="110" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C113" s="68">
+        <v>1</v>
+      </c>
+      <c r="D113" s="68">
+        <v>0</v>
+      </c>
+      <c r="E113" s="68">
+        <v>0</v>
+      </c>
+      <c r="F113" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A114" s="68" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B114" s="110" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C114" s="68">
+        <v>0</v>
+      </c>
+      <c r="D114" s="68">
+        <v>0</v>
+      </c>
+      <c r="E114" s="68">
+        <v>0</v>
+      </c>
+      <c r="F114" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115" s="68" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B115" s="110" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C115" s="68">
+        <v>2</v>
+      </c>
+      <c r="D115" s="68">
+        <v>0</v>
+      </c>
+      <c r="E115" s="68">
+        <v>0</v>
+      </c>
+      <c r="F115" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A117" s="9"/>
+      <c r="B117" s="107"/>
+      <c r="C117" s="109" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D117" s="9"/>
+      <c r="E117" s="108"/>
+      <c r="F117" s="4"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A118" s="9"/>
+      <c r="B118" s="107"/>
+      <c r="C118" s="109" t="s">
+        <v>1795</v>
+      </c>
+      <c r="D118" s="9"/>
+      <c r="E118" s="108"/>
+      <c r="F118" s="4"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A119" s="68" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B119" s="110" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C119" s="68">
+        <v>1</v>
+      </c>
+      <c r="D119" s="68">
+        <v>0</v>
+      </c>
+      <c r="E119" s="68">
+        <v>3</v>
+      </c>
+      <c r="F119" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A120" s="68" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B120" s="110" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C120" s="68">
+        <v>1</v>
+      </c>
+      <c r="D120" s="68">
+        <v>0</v>
+      </c>
+      <c r="E120" s="68">
+        <v>3</v>
+      </c>
+      <c r="F120" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A121" s="68" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B121" s="110" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C121" s="68">
+        <v>1</v>
+      </c>
+      <c r="D121" s="68">
+        <v>0</v>
+      </c>
+      <c r="E121" s="68">
+        <v>2</v>
+      </c>
+      <c r="F121" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A122" s="68" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B122" s="110" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C122" s="68">
+        <v>1</v>
+      </c>
+      <c r="D122" s="68">
+        <v>0</v>
+      </c>
+      <c r="E122" s="68">
+        <v>2</v>
+      </c>
+      <c r="F122" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A123" s="68" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B123" s="110" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C123" s="68">
+        <v>2</v>
+      </c>
+      <c r="D123" s="68">
+        <v>0</v>
+      </c>
+      <c r="E123" s="68">
+        <v>5</v>
+      </c>
+      <c r="F123" s="110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A124" s="68" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B124" s="110" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C124" s="68">
+        <v>1</v>
+      </c>
+      <c r="D124" s="68">
+        <v>0</v>
+      </c>
+      <c r="E124" s="68">
+        <v>2</v>
+      </c>
+      <c r="F124" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A125" s="68" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B125" s="110" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C125" s="68">
+        <v>1</v>
+      </c>
+      <c r="D125" s="68">
+        <v>0</v>
+      </c>
+      <c r="E125" s="68">
+        <v>2</v>
+      </c>
+      <c r="F125" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A126" s="68" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B126" s="110" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C126" s="68">
+        <v>1</v>
+      </c>
+      <c r="D126" s="68">
+        <v>0</v>
+      </c>
+      <c r="E126" s="68">
+        <v>0</v>
+      </c>
+      <c r="F126" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A127" s="68" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B127" s="110" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C127" s="68">
+        <v>1</v>
+      </c>
+      <c r="D127" s="68">
+        <v>0</v>
+      </c>
+      <c r="E127" s="68">
+        <v>0</v>
+      </c>
+      <c r="F127" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A128" s="68" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B128" s="110" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C128" s="68">
+        <v>1</v>
+      </c>
+      <c r="D128" s="68">
+        <v>0</v>
+      </c>
+      <c r="E128" s="68">
+        <v>0</v>
+      </c>
+      <c r="F128" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A129" s="68" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B129" s="110" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C129" s="68">
+        <v>1</v>
+      </c>
+      <c r="D129" s="68">
+        <v>0</v>
+      </c>
+      <c r="E129" s="68">
+        <v>0</v>
+      </c>
+      <c r="F129" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130" s="68" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B130" s="110" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C130" s="68">
+        <v>2</v>
+      </c>
+      <c r="D130" s="68">
+        <v>0</v>
+      </c>
+      <c r="E130" s="68">
+        <v>0</v>
+      </c>
+      <c r="F130" s="110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A131" s="68" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B131" s="110" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C131" s="68">
+        <v>2</v>
+      </c>
+      <c r="D131" s="68">
+        <v>0</v>
+      </c>
+      <c r="E131" s="68">
+        <v>0</v>
+      </c>
+      <c r="F131" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132" s="68" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B132" s="110" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C132" s="68">
+        <v>2</v>
+      </c>
+      <c r="D132" s="68">
+        <v>0</v>
+      </c>
+      <c r="E132" s="68">
+        <v>0</v>
+      </c>
+      <c r="F132" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133" s="68" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B133" s="110" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C133" s="68">
+        <v>2</v>
+      </c>
+      <c r="D133" s="68">
+        <v>0</v>
+      </c>
+      <c r="E133" s="68">
+        <v>0</v>
+      </c>
+      <c r="F133" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134" s="68" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B134" s="110" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C134" s="68">
+        <v>1</v>
+      </c>
+      <c r="D134" s="68">
+        <v>0</v>
+      </c>
+      <c r="E134" s="68">
+        <v>0</v>
+      </c>
+      <c r="F134" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" s="68" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B135" s="110" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C135" s="68">
+        <v>0</v>
+      </c>
+      <c r="D135" s="68">
+        <v>0</v>
+      </c>
+      <c r="E135" s="68">
+        <v>0</v>
+      </c>
+      <c r="F135" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136" s="68" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B136" s="110" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C136" s="68">
+        <v>2</v>
+      </c>
+      <c r="D136" s="68">
+        <v>0</v>
+      </c>
+      <c r="E136" s="68">
+        <v>0</v>
+      </c>
+      <c r="F136" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="1"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A138" s="9"/>
+      <c r="B138" s="107"/>
+      <c r="C138" s="109" t="s">
+        <v>1710</v>
+      </c>
+      <c r="D138" s="9"/>
+      <c r="E138" s="108"/>
+      <c r="F138" s="4"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A139" s="9"/>
+      <c r="B139" s="107"/>
+      <c r="C139" s="109" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D139" s="9"/>
+      <c r="E139" s="108"/>
+      <c r="F139" s="4"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" s="68" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B140" s="110" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C140" s="68">
+        <v>1</v>
+      </c>
+      <c r="D140" s="68">
+        <v>0</v>
+      </c>
+      <c r="E140" s="68">
+        <v>3</v>
+      </c>
+      <c r="F140" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141" s="68" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B141" s="110" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C141" s="68">
+        <v>1</v>
+      </c>
+      <c r="D141" s="68">
+        <v>0</v>
+      </c>
+      <c r="E141" s="68">
+        <v>3</v>
+      </c>
+      <c r="F141" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142" s="68" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B142" s="110" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C142" s="68">
+        <v>1</v>
+      </c>
+      <c r="D142" s="68">
+        <v>0</v>
+      </c>
+      <c r="E142" s="68">
+        <v>2</v>
+      </c>
+      <c r="F142" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143" s="68" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B143" s="110" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C143" s="68">
+        <v>1</v>
+      </c>
+      <c r="D143" s="68">
+        <v>0</v>
+      </c>
+      <c r="E143" s="68">
+        <v>2</v>
+      </c>
+      <c r="F143" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144" s="68" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B144" s="110" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C144" s="68">
+        <v>2</v>
+      </c>
+      <c r="D144" s="68">
+        <v>0</v>
+      </c>
+      <c r="E144" s="68">
+        <v>5</v>
+      </c>
+      <c r="F144" s="110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A145" s="68" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B145" s="110" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C145" s="68">
+        <v>1</v>
+      </c>
+      <c r="D145" s="68">
+        <v>0</v>
+      </c>
+      <c r="E145" s="68">
+        <v>2</v>
+      </c>
+      <c r="F145" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A146" s="68" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B146" s="110" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C146" s="68">
+        <v>1</v>
+      </c>
+      <c r="D146" s="68">
+        <v>0</v>
+      </c>
+      <c r="E146" s="68">
+        <v>0</v>
+      </c>
+      <c r="F146" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A147" s="68" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B147" s="110" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C147" s="68">
+        <v>1</v>
+      </c>
+      <c r="D147" s="68">
+        <v>0</v>
+      </c>
+      <c r="E147" s="68">
+        <v>0</v>
+      </c>
+      <c r="F147" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A148" s="68" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B148" s="110" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C148" s="68">
+        <v>1</v>
+      </c>
+      <c r="D148" s="68">
+        <v>0</v>
+      </c>
+      <c r="E148" s="68">
+        <v>0</v>
+      </c>
+      <c r="F148" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A149" s="68" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B149" s="110" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C149" s="68">
+        <v>1</v>
+      </c>
+      <c r="D149" s="68">
+        <v>0</v>
+      </c>
+      <c r="E149" s="68">
+        <v>0</v>
+      </c>
+      <c r="F149" s="110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A150" s="68" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B150" s="110" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C150" s="68">
+        <v>2</v>
+      </c>
+      <c r="D150" s="68">
+        <v>0</v>
+      </c>
+      <c r="E150" s="68">
+        <v>0</v>
+      </c>
+      <c r="F150" s="110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A151" s="68" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B151" s="110" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C151" s="68">
+        <v>2</v>
+      </c>
+      <c r="D151" s="68">
+        <v>0</v>
+      </c>
+      <c r="E151" s="68">
+        <v>0</v>
+      </c>
+      <c r="F151" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A152" s="68" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B152" s="110" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C152" s="68">
+        <v>2</v>
+      </c>
+      <c r="D152" s="68">
+        <v>0</v>
+      </c>
+      <c r="E152" s="68">
+        <v>0</v>
+      </c>
+      <c r="F152" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A153" s="68" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B153" s="110" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C153" s="68">
+        <v>2</v>
+      </c>
+      <c r="D153" s="68">
+        <v>0</v>
+      </c>
+      <c r="E153" s="68">
+        <v>0</v>
+      </c>
+      <c r="F153" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A154" s="68" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B154" s="110" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C154" s="68">
+        <v>1</v>
+      </c>
+      <c r="D154" s="68">
+        <v>0</v>
+      </c>
+      <c r="E154" s="68">
+        <v>0</v>
+      </c>
+      <c r="F154" s="110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A155" s="68" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B155" s="110" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C155" s="68">
+        <v>0</v>
+      </c>
+      <c r="D155" s="68">
+        <v>0</v>
+      </c>
+      <c r="E155" s="68">
+        <v>0</v>
+      </c>
+      <c r="F155" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A156" s="68" t="s">
+        <v>1831</v>
+      </c>
+      <c r="B156" s="110" t="s">
+        <v>1832</v>
+      </c>
+      <c r="C156" s="68">
+        <v>1</v>
+      </c>
+      <c r="D156" s="68">
+        <v>0</v>
+      </c>
+      <c r="E156" s="68">
+        <v>2</v>
+      </c>
+      <c r="F156" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A157" s="68" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B157" s="110" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C157" s="68">
+        <v>2</v>
+      </c>
+      <c r="D157" s="68">
+        <v>0</v>
+      </c>
+      <c r="E157" s="68">
+        <v>0</v>
+      </c>
+      <c r="F157" s="110">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -27549,7 +31040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ55"/>
   <sheetViews>
@@ -32643,7 +36134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMD28"/>
   <sheetViews>
@@ -34226,7 +37717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>